<commit_message>
-m the template state builder now working great on all the sheet but the grand total footer doesnt seem to genrate the value. Summary footer is missing also
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -20,7 +20,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="35">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -221,6 +221,20 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <sz val="10"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -230,7 +244,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -344,11 +358,12 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -429,6 +444,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -519,6 +537,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1282,103 +1333,112 @@
         <v/>
       </c>
     </row>
-    <row r="23" ht="61.5" customHeight="1">
+    <row r="23" ht="42" customHeight="1">
       <c r="A23" s="33" t="inlineStr">
         <is>
+          <t>Country of Original Cambodia</t>
+        </is>
+      </c>
+      <c r="E23" s="8" t="n"/>
+      <c r="F23" s="8" t="n"/>
+      <c r="G23" s="2" t="n"/>
+    </row>
+    <row r="24" ht="61.5" customHeight="1">
+      <c r="A24" s="34" t="inlineStr">
+        <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B23" s="34" t="inlineStr">
+      <c r="B24" s="35" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="E23" s="34" t="n"/>
-      <c r="F23" s="8" t="n"/>
-      <c r="G23" s="2" t="n"/>
-    </row>
-    <row r="24" ht="42" customHeight="1">
-      <c r="A24" s="35" t="inlineStr">
+      <c r="E24" s="35" t="n"/>
+      <c r="F24" s="8" t="n"/>
+      <c r="G24" s="2" t="n"/>
+    </row>
+    <row r="25" ht="42" customHeight="1">
+      <c r="A25" s="36" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                                   /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="E24" s="35" t="n"/>
-      <c r="F24" s="35" t="n"/>
-      <c r="G24" s="2" t="n"/>
-    </row>
-    <row r="25" ht="24.75" customHeight="1">
-      <c r="A25" s="36" t="inlineStr">
+      <c r="E25" s="36" t="n"/>
+      <c r="F25" s="36" t="n"/>
+      <c r="G25" s="2" t="n"/>
+    </row>
+    <row r="26" ht="24.75" customHeight="1">
+      <c r="A26" s="37" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="27" customHeight="1">
-      <c r="A26" s="36" t="inlineStr">
+    <row r="27" ht="27" customHeight="1">
+      <c r="A27" s="37" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
       </c>
-    </row>
-    <row r="27" ht="35.1" customHeight="1">
-      <c r="A27" s="11" t="n"/>
-      <c r="B27" s="11" t="n"/>
-      <c r="C27" s="11" t="n"/>
-      <c r="D27" s="11" t="n"/>
-      <c r="E27" s="13" t="n"/>
-      <c r="F27" s="37" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
-      <c r="G27" s="2" t="n"/>
     </row>
     <row r="28" ht="35.1" customHeight="1">
       <c r="A28" s="11" t="n"/>
       <c r="B28" s="11" t="n"/>
       <c r="C28" s="11" t="n"/>
       <c r="D28" s="11" t="n"/>
-      <c r="E28" s="8" t="n"/>
+      <c r="E28" s="13" t="n"/>
       <c r="F28" s="38" t="inlineStr">
         <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="G28" s="2" t="n"/>
+    </row>
+    <row r="29" ht="35.1" customHeight="1">
+      <c r="A29" s="11" t="n"/>
+      <c r="B29" s="11" t="n"/>
+      <c r="C29" s="11" t="n"/>
+      <c r="D29" s="11" t="n"/>
+      <c r="E29" s="8" t="n"/>
+      <c r="F29" s="39" t="inlineStr">
+        <is>
           <t>Sign &amp; Stamp</t>
         </is>
       </c>
-      <c r="G28" s="11" t="n"/>
-    </row>
-    <row r="29" ht="42" customHeight="1">
-      <c r="A29" s="11" t="n"/>
-      <c r="E29" s="8" t="n"/>
-      <c r="F29" s="8" t="n"/>
       <c r="G29" s="11" t="n"/>
     </row>
-    <row r="30" ht="61.5" customHeight="1">
+    <row r="30" ht="42" customHeight="1">
       <c r="A30" s="11" t="n"/>
-      <c r="B30" s="11" t="n"/>
       <c r="E30" s="8" t="n"/>
-      <c r="F30" s="39" t="n"/>
-      <c r="G30" s="39" t="n"/>
-    </row>
-    <row r="31" ht="42" customHeight="1">
+      <c r="F30" s="8" t="n"/>
+      <c r="G30" s="11" t="n"/>
+    </row>
+    <row r="31" ht="61.5" customHeight="1">
       <c r="A31" s="11" t="n"/>
-      <c r="E31" s="11" t="n"/>
-      <c r="F31" s="39" t="inlineStr">
+      <c r="B31" s="11" t="n"/>
+      <c r="E31" s="8" t="n"/>
+      <c r="F31" s="40" t="n"/>
+      <c r="G31" s="40" t="n"/>
+    </row>
+    <row r="32" ht="42" customHeight="1">
+      <c r="A32" s="11" t="n"/>
+      <c r="E32" s="11" t="n"/>
+      <c r="F32" s="40" t="inlineStr">
         <is>
           <t>ZENG XUELI</t>
         </is>
       </c>
-      <c r="G31" s="11" t="n"/>
-    </row>
-    <row r="32" ht="24.75" customHeight="1">
-      <c r="A32" s="11" t="n"/>
-    </row>
-    <row r="33" ht="27" customHeight="1">
+      <c r="G32" s="11" t="n"/>
+    </row>
+    <row r="33" ht="24.75" customHeight="1">
       <c r="A33" s="11" t="n"/>
     </row>
-    <row r="34"/>
+    <row r="34" ht="27" customHeight="1">
+      <c r="A34" s="11" t="n"/>
+    </row>
     <row r="35"/>
     <row r="36"/>
     <row r="37"/>
@@ -1550,22 +1610,23 @@
     <row r="203"/>
     <row r="204"/>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A32:G32"/>
+  <mergeCells count="17">
+    <mergeCell ref="A23:D23"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="A27:G27"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A25:D25"/>
     <mergeCell ref="B22"/>
     <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1602,43 +1663,43 @@
   </cols>
   <sheetData>
     <row r="1" ht="38.25" customHeight="1">
-      <c r="A1" s="40" t="inlineStr">
+      <c r="A1" s="41" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="L1" s="41" t="n"/>
+      <c r="L1" s="42" t="n"/>
       <c r="M1" s="11" t="n"/>
     </row>
     <row r="2" ht="24" customHeight="1">
-      <c r="A2" s="42" t="inlineStr">
+      <c r="A2" s="43" t="inlineStr">
         <is>
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
         </is>
       </c>
-      <c r="L2" s="43" t="n"/>
+      <c r="L2" s="44" t="n"/>
       <c r="M2" s="11" t="n"/>
     </row>
     <row r="3" ht="25.5" customHeight="1">
-      <c r="A3" s="44" t="inlineStr">
+      <c r="A3" s="45" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
       </c>
-      <c r="L3" s="45" t="n"/>
+      <c r="L3" s="46" t="n"/>
       <c r="M3" s="11" t="n"/>
     </row>
     <row r="4" ht="25.5" customHeight="1">
-      <c r="A4" s="42" t="inlineStr">
+      <c r="A4" s="43" t="inlineStr">
         <is>
           <t>VAT:L001-901903209</t>
         </is>
       </c>
-      <c r="L4" s="45" t="n"/>
+      <c r="L4" s="46" t="n"/>
       <c r="M4" s="11" t="n"/>
     </row>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="46" t="inlineStr">
+      <c r="A5" s="47" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
@@ -1653,11 +1714,11 @@
       <c r="I5" s="5" t="n"/>
       <c r="J5" s="5" t="n"/>
       <c r="K5" s="5" t="n"/>
-      <c r="L5" s="45" t="n"/>
+      <c r="L5" s="46" t="n"/>
       <c r="M5" s="11" t="n"/>
     </row>
     <row r="6" ht="54" customHeight="1">
-      <c r="A6" s="47" t="inlineStr">
+      <c r="A6" s="48" t="inlineStr">
         <is>
           <t>PACKING LIST</t>
         </is>
@@ -1672,20 +1733,20 @@
       <c r="I6" s="7" t="n"/>
       <c r="J6" s="7" t="n"/>
       <c r="K6" s="7" t="n"/>
-      <c r="L6" s="48" t="n"/>
+      <c r="L6" s="49" t="n"/>
       <c r="M6" s="11" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="49" t="n"/>
+      <c r="A7" s="50" t="n"/>
       <c r="B7" s="11" t="n"/>
-      <c r="C7" s="49" t="n"/>
-      <c r="D7" s="49" t="n"/>
-      <c r="E7" s="49" t="n"/>
-      <c r="F7" s="49" t="n"/>
-      <c r="G7" s="49" t="n"/>
-      <c r="H7" s="49" t="n"/>
+      <c r="C7" s="50" t="n"/>
+      <c r="D7" s="50" t="n"/>
+      <c r="E7" s="50" t="n"/>
+      <c r="F7" s="50" t="n"/>
+      <c r="G7" s="50" t="n"/>
+      <c r="H7" s="50" t="n"/>
       <c r="I7" s="11" t="n"/>
-      <c r="J7" s="50" t="inlineStr">
+      <c r="J7" s="51" t="inlineStr">
         <is>
           <t>Ref No.:</t>
         </is>
@@ -1699,21 +1760,21 @@
       <c r="M7" s="11" t="n"/>
     </row>
     <row r="8" ht="30" customHeight="1">
-      <c r="A8" s="51" t="inlineStr">
+      <c r="A8" s="52" t="inlineStr">
         <is>
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="52" t="inlineStr">
+      <c r="B8" s="53" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
       <c r="F8" s="11" t="n"/>
-      <c r="G8" s="53" t="n"/>
-      <c r="H8" s="53" t="n"/>
+      <c r="G8" s="54" t="n"/>
+      <c r="H8" s="54" t="n"/>
       <c r="I8" s="11" t="n"/>
-      <c r="J8" s="54" t="inlineStr">
+      <c r="J8" s="55" t="inlineStr">
         <is>
           <t>INVOICE NO :</t>
         </is>
@@ -1727,17 +1788,17 @@
       <c r="M8" s="11" t="n"/>
     </row>
     <row r="9" ht="21" customHeight="1">
-      <c r="A9" s="49" t="n"/>
-      <c r="B9" s="55" t="inlineStr">
+      <c r="A9" s="50" t="n"/>
+      <c r="B9" s="56" t="inlineStr">
         <is>
           <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages,</t>
         </is>
       </c>
       <c r="F9" s="11" t="n"/>
-      <c r="G9" s="49" t="n"/>
-      <c r="H9" s="49" t="n"/>
+      <c r="G9" s="50" t="n"/>
+      <c r="H9" s="50" t="n"/>
       <c r="I9" s="11" t="n"/>
-      <c r="J9" s="54" t="inlineStr">
+      <c r="J9" s="55" t="inlineStr">
         <is>
           <t>Date:</t>
         </is>
@@ -1751,17 +1812,17 @@
       <c r="M9" s="11" t="n"/>
     </row>
     <row r="10" ht="22.5" customHeight="1">
-      <c r="A10" s="49" t="n"/>
-      <c r="B10" s="55" t="inlineStr">
+      <c r="A10" s="50" t="n"/>
+      <c r="B10" s="56" t="inlineStr">
         <is>
           <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
         </is>
       </c>
       <c r="F10" s="11" t="n"/>
-      <c r="G10" s="49" t="n"/>
-      <c r="H10" s="49" t="n"/>
+      <c r="G10" s="50" t="n"/>
+      <c r="H10" s="50" t="n"/>
       <c r="I10" s="11" t="n"/>
-      <c r="J10" s="54">
+      <c r="J10" s="55">
         <f>Invoice!F10</f>
         <v/>
       </c>
@@ -1774,17 +1835,17 @@
       <c r="M10" s="11" t="n"/>
     </row>
     <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="49" t="n"/>
-      <c r="B11" s="55" t="inlineStr">
+      <c r="A11" s="50" t="n"/>
+      <c r="B11" s="56" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
       <c r="F11" s="11" t="n"/>
-      <c r="G11" s="49" t="n"/>
-      <c r="H11" s="49" t="n"/>
+      <c r="G11" s="50" t="n"/>
+      <c r="H11" s="50" t="n"/>
       <c r="I11" s="11" t="n"/>
-      <c r="J11" s="54" t="inlineStr">
+      <c r="J11" s="55" t="inlineStr">
         <is>
           <t>ETD：</t>
         </is>
@@ -1793,20 +1854,20 @@
         <f>K9</f>
         <v/>
       </c>
-      <c r="L11" s="43" t="n"/>
+      <c r="L11" s="44" t="n"/>
       <c r="M11" s="11" t="n"/>
     </row>
     <row r="12" ht="20.1" customHeight="1">
-      <c r="A12" s="49" t="n"/>
+      <c r="A12" s="50" t="n"/>
       <c r="B12" s="11" t="n"/>
-      <c r="C12" s="49" t="n"/>
-      <c r="D12" s="49" t="n"/>
-      <c r="E12" s="49" t="n"/>
-      <c r="F12" s="49" t="n"/>
-      <c r="G12" s="49" t="n"/>
-      <c r="H12" s="49" t="n"/>
+      <c r="C12" s="50" t="n"/>
+      <c r="D12" s="50" t="n"/>
+      <c r="E12" s="50" t="n"/>
+      <c r="F12" s="50" t="n"/>
+      <c r="G12" s="50" t="n"/>
+      <c r="H12" s="50" t="n"/>
       <c r="I12" s="11" t="n"/>
-      <c r="J12" s="54" t="inlineStr">
+      <c r="J12" s="55" t="inlineStr">
         <is>
           <t>ETA:</t>
         </is>
@@ -1815,68 +1876,68 @@
         <f>K11+1</f>
         <v/>
       </c>
-      <c r="L12" s="43" t="n"/>
+      <c r="L12" s="44" t="n"/>
       <c r="M12" s="11" t="n"/>
     </row>
     <row r="13" ht="25.5" customHeight="1">
-      <c r="A13" s="56" t="inlineStr">
+      <c r="A13" s="57" t="inlineStr">
         <is>
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="57" t="inlineStr">
+      <c r="B13" s="58" t="inlineStr">
         <is>
           <t>Wanek Furniture Co., LTD</t>
         </is>
       </c>
       <c r="F13" s="11" t="n"/>
-      <c r="G13" s="58" t="n"/>
-      <c r="H13" s="58" t="n"/>
-      <c r="I13" s="58" t="n"/>
-      <c r="J13" s="59" t="n"/>
+      <c r="G13" s="59" t="n"/>
+      <c r="H13" s="59" t="n"/>
+      <c r="I13" s="59" t="n"/>
+      <c r="J13" s="60" t="n"/>
       <c r="K13" s="11" t="n"/>
-      <c r="L13" s="43" t="n"/>
+      <c r="L13" s="44" t="n"/>
       <c r="M13" s="11" t="n"/>
     </row>
     <row r="14" ht="25.5" customHeight="1">
-      <c r="A14" s="49" t="n"/>
-      <c r="B14" s="60" t="inlineStr">
+      <c r="A14" s="50" t="n"/>
+      <c r="B14" s="61" t="inlineStr">
         <is>
           <t>Lot D_5A_CN, D_5C_CN, D_5E_CN, My Phuoc 3 Industrial Park, Thoi Hoa Ward, Ho Chi Minh City, Vietnam.</t>
         </is>
       </c>
-      <c r="F14" s="61" t="n"/>
-      <c r="G14" s="61" t="n"/>
-      <c r="H14" s="61" t="n"/>
-      <c r="I14" s="61" t="n"/>
+      <c r="F14" s="62" t="n"/>
+      <c r="G14" s="62" t="n"/>
+      <c r="H14" s="62" t="n"/>
+      <c r="I14" s="62" t="n"/>
       <c r="J14" s="11" t="n"/>
       <c r="K14" s="11" t="n"/>
-      <c r="L14" s="43" t="n"/>
+      <c r="L14" s="44" t="n"/>
       <c r="M14" s="11" t="n"/>
     </row>
     <row r="15" ht="17.25" customHeight="1">
-      <c r="A15" s="49" t="n"/>
-      <c r="B15" s="50" t="inlineStr">
+      <c r="A15" s="50" t="n"/>
+      <c r="B15" s="51" t="inlineStr">
         <is>
           <t>P+84 650 3655 200 EXT:7074 MS EMILY(C&amp;L)/MS DOROTHY(CR) EXT:7036 MS JANE (PURCHASING)</t>
         </is>
       </c>
-      <c r="F15" s="62" t="n"/>
-      <c r="G15" s="62" t="n"/>
-      <c r="H15" s="62" t="n"/>
-      <c r="I15" s="62" t="n"/>
+      <c r="F15" s="63" t="n"/>
+      <c r="G15" s="63" t="n"/>
+      <c r="H15" s="63" t="n"/>
+      <c r="I15" s="63" t="n"/>
       <c r="J15" s="11" t="n"/>
       <c r="K15" s="11" t="n"/>
-      <c r="L15" s="43" t="n"/>
+      <c r="L15" s="44" t="n"/>
       <c r="M15" s="11" t="n"/>
     </row>
     <row r="16" ht="27.75" customHeight="1">
-      <c r="A16" s="63" t="inlineStr">
+      <c r="A16" s="64" t="inlineStr">
         <is>
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B16" s="55" t="inlineStr">
+      <c r="B16" s="56" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO HO CHI MINH, VIETNAM.</t>
         </is>
@@ -1884,17 +1945,17 @@
       <c r="F16" s="11" t="n"/>
       <c r="G16" s="11" t="n"/>
       <c r="H16" s="11" t="n"/>
-      <c r="I16" s="64" t="n"/>
+      <c r="I16" s="65" t="n"/>
       <c r="J16" s="11" t="n"/>
       <c r="K16" s="11" t="n"/>
       <c r="L16" s="11" t="n"/>
       <c r="M16" s="11" t="n"/>
     </row>
     <row r="17" ht="24" customHeight="1">
-      <c r="A17" s="65" t="n"/>
+      <c r="A17" s="66" t="n"/>
       <c r="B17" s="11" t="n"/>
-      <c r="C17" s="65" t="n"/>
-      <c r="D17" s="65" t="n"/>
+      <c r="C17" s="66" t="n"/>
+      <c r="D17" s="66" t="n"/>
       <c r="E17" s="11" t="n"/>
       <c r="F17" s="11" t="n"/>
       <c r="G17" s="11" t="n"/>
@@ -1905,7 +1966,7 @@
       <c r="L17" s="11" t="n"/>
       <c r="M17" s="11" t="n"/>
     </row>
-    <row r="18" ht="31.05" customHeight="1">
+    <row r="18" ht="31.1" customHeight="1">
       <c r="A18" s="29" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
@@ -1937,7 +1998,7 @@
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G18" s="66" t="n"/>
+      <c r="G18" s="67" t="n"/>
       <c r="H18" s="29" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -1958,15 +2019,13 @@
           <t>REMARKS</t>
         </is>
       </c>
-      <c r="L18" s="11" t="n"/>
-      <c r="M18" s="11" t="n"/>
-    </row>
-    <row r="19" ht="31.05" customHeight="1">
-      <c r="A19" s="67" t="n"/>
-      <c r="B19" s="67" t="n"/>
-      <c r="C19" s="67" t="n"/>
-      <c r="D19" s="67" t="n"/>
-      <c r="E19" s="67" t="n"/>
+    </row>
+    <row r="19" ht="31.1" customHeight="1">
+      <c r="A19" s="68" t="n"/>
+      <c r="B19" s="68" t="n"/>
+      <c r="C19" s="68" t="n"/>
+      <c r="D19" s="68" t="n"/>
+      <c r="E19" s="68" t="n"/>
       <c r="F19" s="29" t="inlineStr">
         <is>
           <t>PCS</t>
@@ -1977,68 +2036,1629 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="H19" s="67" t="n"/>
-      <c r="I19" s="67" t="n"/>
-      <c r="J19" s="67" t="n"/>
-      <c r="K19" s="67" t="n"/>
-      <c r="L19" s="11" t="n"/>
-      <c r="M19" s="11" t="n"/>
-    </row>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
+      <c r="H19" s="68" t="n"/>
+      <c r="I19" s="68" t="n"/>
+      <c r="J19" s="68" t="n"/>
+      <c r="K19" s="68" t="n"/>
+    </row>
+    <row r="20" ht="31.1" customHeight="1">
+      <c r="A20" s="69" t="inlineStr">
+        <is>
+          <t>VENDOR#:</t>
+        </is>
+      </c>
+      <c r="C20" s="31" t="inlineStr">
+        <is>
+          <t>PT1ZX64</t>
+        </is>
+      </c>
+      <c r="D20" s="70" t="n">
+        <v>140499</v>
+      </c>
+      <c r="E20" s="31" t="inlineStr">
+        <is>
+          <t>L DAHLMOORE ALMOND U13200</t>
+        </is>
+      </c>
+      <c r="F20" s="31" t="n">
+        <v>206</v>
+      </c>
+      <c r="G20" s="32" t="n">
+        <v>10801.1</v>
+      </c>
+      <c r="H20" s="32" t="n">
+        <v>1016.5</v>
+      </c>
+      <c r="I20" s="32" t="n">
+        <v>1061.5</v>
+      </c>
+      <c r="J20" s="32" t="n">
+        <v>2.772</v>
+      </c>
+      <c r="K20" s="31" t="n"/>
+    </row>
+    <row r="21" ht="31.1" customHeight="1">
+      <c r="A21" s="69" t="inlineStr">
+        <is>
+          <t>Des: L MINDANAO BUFFALO STEELU59504</t>
+        </is>
+      </c>
+      <c r="C21" s="31" t="inlineStr">
+        <is>
+          <t>PT1ZX64</t>
+        </is>
+      </c>
+      <c r="D21" s="70" t="n">
+        <v>140499</v>
+      </c>
+      <c r="E21" s="31" t="inlineStr">
+        <is>
+          <t>L DAHLMOORE ALMOND U13200</t>
+        </is>
+      </c>
+      <c r="F21" s="31" t="n">
+        <v>198</v>
+      </c>
+      <c r="G21" s="32" t="n">
+        <v>11008.5</v>
+      </c>
+      <c r="H21" s="32" t="n">
+        <v>1038.5</v>
+      </c>
+      <c r="I21" s="32" t="n">
+        <v>1083.5</v>
+      </c>
+      <c r="J21" s="32" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="K21" s="31" t="n"/>
+    </row>
+    <row r="22" ht="31.1" customHeight="1">
+      <c r="A22" s="69" t="inlineStr">
+        <is>
+          <t>Case Qty:</t>
+        </is>
+      </c>
+      <c r="C22" s="31" t="inlineStr">
+        <is>
+          <t>PT1ZX64</t>
+        </is>
+      </c>
+      <c r="D22" s="70" t="n">
+        <v>140499</v>
+      </c>
+      <c r="E22" s="31" t="inlineStr">
+        <is>
+          <t>L DAHLMOORE ALMOND U13200</t>
+        </is>
+      </c>
+      <c r="F22" s="31" t="n">
+        <v>176</v>
+      </c>
+      <c r="G22" s="32" t="n">
+        <v>10005.8</v>
+      </c>
+      <c r="H22" s="32" t="n">
+        <v>937.5</v>
+      </c>
+      <c r="I22" s="32" t="n">
+        <v>982.5</v>
+      </c>
+      <c r="J22" s="32" t="n">
+        <v>2.8512</v>
+      </c>
+      <c r="K22" s="31" t="n"/>
+    </row>
+    <row r="23" ht="31.1" customHeight="1">
+      <c r="A23" s="69" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="C23" s="31" t="inlineStr">
+        <is>
+          <t>PT1ZX64</t>
+        </is>
+      </c>
+      <c r="D23" s="70" t="n">
+        <v>140499</v>
+      </c>
+      <c r="E23" s="31" t="inlineStr">
+        <is>
+          <t>L DAHLMOORE ALMOND U13200</t>
+        </is>
+      </c>
+      <c r="F23" s="31" t="n">
+        <v>180</v>
+      </c>
+      <c r="G23" s="32" t="n">
+        <v>10109.1</v>
+      </c>
+      <c r="H23" s="70" t="n">
+        <v>973</v>
+      </c>
+      <c r="I23" s="70" t="n">
+        <v>1018</v>
+      </c>
+      <c r="J23" s="32" t="n">
+        <v>2.772</v>
+      </c>
+      <c r="K23" s="31" t="n"/>
+    </row>
+    <row r="24" ht="31.1" customHeight="1">
+      <c r="C24" s="31" t="inlineStr">
+        <is>
+          <t>PT1ZX64</t>
+        </is>
+      </c>
+      <c r="D24" s="70" t="n">
+        <v>140499</v>
+      </c>
+      <c r="E24" s="31" t="inlineStr">
+        <is>
+          <t>L DAHLMOORE ALMOND U13200</t>
+        </is>
+      </c>
+      <c r="F24" s="31" t="n">
+        <v>115</v>
+      </c>
+      <c r="G24" s="32" t="n">
+        <v>6503.8</v>
+      </c>
+      <c r="H24" s="32" t="n">
+        <v>602.7754</v>
+      </c>
+      <c r="I24" s="32" t="n">
+        <v>646.6314</v>
+      </c>
+      <c r="J24" s="32" t="n">
+        <v>2.1226</v>
+      </c>
+      <c r="K24" s="31" t="n"/>
+    </row>
+    <row r="25" ht="31.1" customHeight="1">
+      <c r="C25" s="31" t="inlineStr">
+        <is>
+          <t>PT1ZX64</t>
+        </is>
+      </c>
+      <c r="D25" s="70" t="n">
+        <v>140499</v>
+      </c>
+      <c r="E25" s="31" t="inlineStr">
+        <is>
+          <t>L DAHLMOORE ALMOND U13200</t>
+        </is>
+      </c>
+      <c r="F25" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="G25" s="32" t="n">
+        <v>157.2</v>
+      </c>
+      <c r="H25" s="32" t="n">
+        <v>15.7246</v>
+      </c>
+      <c r="I25" s="32" t="n">
+        <v>16.8686</v>
+      </c>
+      <c r="J25" s="32" t="n">
+        <v>0.0554</v>
+      </c>
+      <c r="K25" s="31" t="inlineStr">
+        <is>
+          <t>Low selection if yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="31.1" customHeight="1">
+      <c r="C26" s="31" t="inlineStr">
+        <is>
+          <t>PT1ZX64</t>
+        </is>
+      </c>
+      <c r="D26" s="70" t="n">
+        <v>140499</v>
+      </c>
+      <c r="E26" s="31" t="inlineStr">
+        <is>
+          <t>L DAHLMOORE ALMOND U13200</t>
+        </is>
+      </c>
+      <c r="F26" s="31" t="n">
+        <v>190</v>
+      </c>
+      <c r="G26" s="32" t="n">
+        <v>10038.5</v>
+      </c>
+      <c r="H26" s="70" t="n">
+        <v>940</v>
+      </c>
+      <c r="I26" s="70" t="n">
+        <v>985</v>
+      </c>
+      <c r="J26" s="32" t="n">
+        <v>2.8908</v>
+      </c>
+      <c r="K26" s="31" t="n"/>
+    </row>
+    <row r="27" ht="31.1" customHeight="1">
+      <c r="C27" s="31" t="inlineStr">
+        <is>
+          <t>PT1ZX64</t>
+        </is>
+      </c>
+      <c r="D27" s="70" t="n">
+        <v>140499</v>
+      </c>
+      <c r="E27" s="31" t="inlineStr">
+        <is>
+          <t>L DAHLMOORE ALMOND U13200</t>
+        </is>
+      </c>
+      <c r="F27" s="31" t="n">
+        <v>185</v>
+      </c>
+      <c r="G27" s="32" t="n">
+        <v>10023.9</v>
+      </c>
+      <c r="H27" s="32" t="n">
+        <v>940.5</v>
+      </c>
+      <c r="I27" s="32" t="n">
+        <v>985.5</v>
+      </c>
+      <c r="J27" s="32" t="n">
+        <v>2.6532</v>
+      </c>
+      <c r="K27" s="31" t="n"/>
+    </row>
+    <row r="28" ht="31.1" customHeight="1">
+      <c r="C28" s="31" t="inlineStr">
+        <is>
+          <t>PT1ZX64</t>
+        </is>
+      </c>
+      <c r="D28" s="70" t="n">
+        <v>140499</v>
+      </c>
+      <c r="E28" s="31" t="inlineStr">
+        <is>
+          <t>L DAHLMOORE ALMOND U13200</t>
+        </is>
+      </c>
+      <c r="F28" s="31" t="n">
+        <v>182</v>
+      </c>
+      <c r="G28" s="32" t="n">
+        <v>9867.200000000001</v>
+      </c>
+      <c r="H28" s="70" t="n">
+        <v>925</v>
+      </c>
+      <c r="I28" s="70" t="n">
+        <v>970</v>
+      </c>
+      <c r="J28" s="32" t="n">
+        <v>2.6928</v>
+      </c>
+      <c r="K28" s="31" t="n"/>
+    </row>
+    <row r="29" ht="31.1" customHeight="1">
+      <c r="C29" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D29" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E29" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F29" s="31" t="n">
+        <v>290</v>
+      </c>
+      <c r="G29" s="32" t="n">
+        <v>10310.7</v>
+      </c>
+      <c r="H29" s="32" t="n">
+        <v>682.5</v>
+      </c>
+      <c r="I29" s="32" t="n">
+        <v>727.5</v>
+      </c>
+      <c r="J29" s="32" t="n">
+        <v>2.2176</v>
+      </c>
+      <c r="K29" s="31" t="n"/>
+    </row>
+    <row r="30" ht="31.1" customHeight="1">
+      <c r="C30" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D30" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E30" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F30" s="31" t="n">
+        <v>290</v>
+      </c>
+      <c r="G30" s="32" t="n">
+        <v>10360.1</v>
+      </c>
+      <c r="H30" s="70" t="n">
+        <v>680</v>
+      </c>
+      <c r="I30" s="70" t="n">
+        <v>725</v>
+      </c>
+      <c r="J30" s="32" t="n">
+        <v>2.376</v>
+      </c>
+      <c r="K30" s="31" t="n"/>
+    </row>
+    <row r="31" ht="31.1" customHeight="1">
+      <c r="C31" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D31" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E31" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F31" s="31" t="n">
+        <v>290</v>
+      </c>
+      <c r="G31" s="32" t="n">
+        <v>10420.2</v>
+      </c>
+      <c r="H31" s="70" t="n">
+        <v>681</v>
+      </c>
+      <c r="I31" s="70" t="n">
+        <v>726</v>
+      </c>
+      <c r="J31" s="32" t="n">
+        <v>2.376</v>
+      </c>
+      <c r="K31" s="31" t="n"/>
+    </row>
+    <row r="32" ht="31.1" customHeight="1">
+      <c r="C32" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D32" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E32" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F32" s="31" t="n">
+        <v>290</v>
+      </c>
+      <c r="G32" s="32" t="n">
+        <v>10160.8</v>
+      </c>
+      <c r="H32" s="32" t="n">
+        <v>681.5</v>
+      </c>
+      <c r="I32" s="32" t="n">
+        <v>726.5</v>
+      </c>
+      <c r="J32" s="32" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="K32" s="31" t="n"/>
+    </row>
+    <row r="33" ht="31.1" customHeight="1">
+      <c r="C33" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D33" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E33" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F33" s="31" t="n">
+        <v>290</v>
+      </c>
+      <c r="G33" s="32" t="n">
+        <v>10254.5</v>
+      </c>
+      <c r="H33" s="32" t="n">
+        <v>673.5</v>
+      </c>
+      <c r="I33" s="32" t="n">
+        <v>718.5</v>
+      </c>
+      <c r="J33" s="32" t="n">
+        <v>2.376</v>
+      </c>
+      <c r="K33" s="31" t="n"/>
+    </row>
+    <row r="34" ht="31.1" customHeight="1">
+      <c r="C34" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D34" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E34" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F34" s="31" t="n">
+        <v>290</v>
+      </c>
+      <c r="G34" s="32" t="n">
+        <v>10477.6</v>
+      </c>
+      <c r="H34" s="32" t="n">
+        <v>687.5</v>
+      </c>
+      <c r="I34" s="32" t="n">
+        <v>732.5</v>
+      </c>
+      <c r="J34" s="32" t="n">
+        <v>2.376</v>
+      </c>
+      <c r="K34" s="31" t="n"/>
+    </row>
+    <row r="35" ht="31.1" customHeight="1">
+      <c r="C35" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D35" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E35" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F35" s="31" t="n">
+        <v>290</v>
+      </c>
+      <c r="G35" s="32" t="n">
+        <v>10183.1</v>
+      </c>
+      <c r="H35" s="32" t="n">
+        <v>683.5</v>
+      </c>
+      <c r="I35" s="32" t="n">
+        <v>728.5</v>
+      </c>
+      <c r="J35" s="32" t="n">
+        <v>2.574</v>
+      </c>
+      <c r="K35" s="31" t="n"/>
+    </row>
+    <row r="36" ht="31.1" customHeight="1">
+      <c r="C36" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D36" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E36" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F36" s="31" t="n">
+        <v>273</v>
+      </c>
+      <c r="G36" s="32" t="n">
+        <v>9825.6</v>
+      </c>
+      <c r="H36" s="32" t="n">
+        <v>657.5</v>
+      </c>
+      <c r="I36" s="32" t="n">
+        <v>702.5</v>
+      </c>
+      <c r="J36" s="32" t="n">
+        <v>2.376</v>
+      </c>
+      <c r="K36" s="31" t="n"/>
+    </row>
+    <row r="37" ht="31.1" customHeight="1">
+      <c r="C37" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D37" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E37" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F37" s="31" t="n">
+        <v>205</v>
+      </c>
+      <c r="G37" s="32" t="n">
+        <v>6995.2</v>
+      </c>
+      <c r="H37" s="32" t="n">
+        <v>463.3165</v>
+      </c>
+      <c r="I37" s="32" t="n">
+        <v>500.5141</v>
+      </c>
+      <c r="J37" s="32" t="n">
+        <v>1.6367</v>
+      </c>
+      <c r="K37" s="31" t="n"/>
+    </row>
+    <row r="38" ht="31.1" customHeight="1">
+      <c r="C38" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D38" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E38" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F38" s="31" t="n">
+        <v>43</v>
+      </c>
+      <c r="G38" s="32" t="n">
+        <v>1372.3</v>
+      </c>
+      <c r="H38" s="32" t="n">
+        <v>97.1835</v>
+      </c>
+      <c r="I38" s="32" t="n">
+        <v>104.9859</v>
+      </c>
+      <c r="J38" s="32" t="n">
+        <v>0.3433</v>
+      </c>
+      <c r="K38" s="31" t="inlineStr">
+        <is>
+          <t>Low selection if yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="31.1" customHeight="1">
+      <c r="C39" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D39" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E39" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F39" s="31" t="n">
+        <v>290</v>
+      </c>
+      <c r="G39" s="32" t="n">
+        <v>10321.1</v>
+      </c>
+      <c r="H39" s="32" t="n">
+        <v>694.5</v>
+      </c>
+      <c r="I39" s="32" t="n">
+        <v>739.5</v>
+      </c>
+      <c r="J39" s="32" t="n">
+        <v>2.178</v>
+      </c>
+      <c r="K39" s="31" t="n"/>
+    </row>
+    <row r="40" ht="31.1" customHeight="1">
+      <c r="C40" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D40" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E40" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F40" s="31" t="n">
+        <v>263</v>
+      </c>
+      <c r="G40" s="32" t="n">
+        <v>9318.799999999999</v>
+      </c>
+      <c r="H40" s="70" t="n">
+        <v>629</v>
+      </c>
+      <c r="I40" s="70" t="n">
+        <v>674</v>
+      </c>
+      <c r="J40" s="32" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="K40" s="31" t="n"/>
+    </row>
+    <row r="41" ht="31.1" customHeight="1">
+      <c r="C41" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D41" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E41" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F41" s="31" t="n">
+        <v>290</v>
+      </c>
+      <c r="G41" s="32" t="n">
+        <v>10255.8</v>
+      </c>
+      <c r="H41" s="70" t="n">
+        <v>681</v>
+      </c>
+      <c r="I41" s="70" t="n">
+        <v>726</v>
+      </c>
+      <c r="J41" s="32" t="n">
+        <v>2.4156</v>
+      </c>
+      <c r="K41" s="31" t="n"/>
+    </row>
+    <row r="42" ht="31.1" customHeight="1">
+      <c r="C42" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D42" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E42" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F42" s="31" t="n">
+        <v>205</v>
+      </c>
+      <c r="G42" s="32" t="n">
+        <v>7487.2</v>
+      </c>
+      <c r="H42" s="32" t="n">
+        <v>453.2778</v>
+      </c>
+      <c r="I42" s="32" t="n">
+        <v>494.2778</v>
+      </c>
+      <c r="J42" s="32" t="n">
+        <v>1.9844</v>
+      </c>
+      <c r="K42" s="31" t="n"/>
+    </row>
+    <row r="43" ht="31.1" customHeight="1">
+      <c r="C43" s="31" t="inlineStr">
+        <is>
+          <t>PT26792</t>
+        </is>
+      </c>
+      <c r="D43" s="70" t="n">
+        <v>140519</v>
+      </c>
+      <c r="E43" s="31" t="inlineStr">
+        <is>
+          <t>L ModMax (Buffalo) Black 
+74305</t>
+        </is>
+      </c>
+      <c r="F43" s="31" t="n">
+        <v>20</v>
+      </c>
+      <c r="G43" s="32" t="n">
+        <v>625.8</v>
+      </c>
+      <c r="H43" s="32" t="n">
+        <v>44.2222</v>
+      </c>
+      <c r="I43" s="32" t="n">
+        <v>48.2222</v>
+      </c>
+      <c r="J43" s="32" t="n">
+        <v>0.1936</v>
+      </c>
+      <c r="K43" s="31" t="inlineStr">
+        <is>
+          <t>Low selection if yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="31.1" customHeight="1">
+      <c r="C44" s="31" t="inlineStr">
+        <is>
+          <t>PT26F87</t>
+        </is>
+      </c>
+      <c r="D44" s="70" t="n">
+        <v>140522</v>
+      </c>
+      <c r="E44" s="31" t="inlineStr">
+        <is>
+          <t>L MOSSANO CANYON 72907</t>
+        </is>
+      </c>
+      <c r="F44" s="31" t="n">
+        <v>175</v>
+      </c>
+      <c r="G44" s="32" t="n">
+        <v>8744.4</v>
+      </c>
+      <c r="H44" s="70" t="n">
+        <v>640</v>
+      </c>
+      <c r="I44" s="70" t="n">
+        <v>685</v>
+      </c>
+      <c r="J44" s="32" t="n">
+        <v>2.2176</v>
+      </c>
+      <c r="K44" s="31" t="n"/>
+    </row>
+    <row r="45" ht="31.1" customHeight="1">
+      <c r="C45" s="31" t="inlineStr">
+        <is>
+          <t>PT26F87</t>
+        </is>
+      </c>
+      <c r="D45" s="70" t="n">
+        <v>140522</v>
+      </c>
+      <c r="E45" s="31" t="inlineStr">
+        <is>
+          <t>L MOSSANO CANYON 72907</t>
+        </is>
+      </c>
+      <c r="F45" s="31" t="n">
+        <v>90</v>
+      </c>
+      <c r="G45" s="32" t="n">
+        <v>4504.3</v>
+      </c>
+      <c r="H45" s="70" t="n">
+        <v>332</v>
+      </c>
+      <c r="I45" s="70" t="n">
+        <v>377</v>
+      </c>
+      <c r="J45" s="32" t="n">
+        <v>1.584</v>
+      </c>
+      <c r="K45" s="31" t="n"/>
+    </row>
+    <row r="46" ht="31.1" customHeight="1">
+      <c r="C46" s="31" t="inlineStr">
+        <is>
+          <t>PT27781</t>
+        </is>
+      </c>
+      <c r="D46" s="70" t="n">
+        <v>140491</v>
+      </c>
+      <c r="E46" s="31" t="inlineStr">
+        <is>
+          <t>L LEESWORTH BUFFALO OCEAN U43809</t>
+        </is>
+      </c>
+      <c r="F46" s="31" t="n">
+        <v>163</v>
+      </c>
+      <c r="G46" s="32" t="n">
+        <v>6024.9</v>
+      </c>
+      <c r="H46" s="70" t="n">
+        <v>388</v>
+      </c>
+      <c r="I46" s="70" t="n">
+        <v>433</v>
+      </c>
+      <c r="J46" s="32" t="n">
+        <v>1.2672</v>
+      </c>
+      <c r="K46" s="31" t="n"/>
+    </row>
+    <row r="47" ht="31.1" customHeight="1">
+      <c r="A47" s="69" t="n"/>
+      <c r="B47" s="71" t="inlineStr">
+        <is>
+          <t>LEATHER (HS.CODE: 4107.12.00)</t>
+        </is>
+      </c>
+      <c r="C47" s="67" t="n"/>
+      <c r="D47" s="31" t="n"/>
+      <c r="E47" s="31" t="n"/>
+      <c r="F47" s="31" t="n"/>
+      <c r="G47" s="31" t="n"/>
+      <c r="H47" s="31" t="n"/>
+      <c r="I47" s="31" t="n"/>
+      <c r="J47" s="31" t="n"/>
+      <c r="K47" s="31" t="n"/>
+    </row>
+    <row r="48" ht="31.1" customHeight="1">
+      <c r="A48" s="72" t="n"/>
+      <c r="B48" s="31" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C48" s="31" t="n"/>
+      <c r="D48" s="31" t="n"/>
+      <c r="E48" s="31" t="inlineStr">
+        <is>
+          <t>24 PALLETS</t>
+        </is>
+      </c>
+      <c r="F48" s="31">
+        <f>SUM(F20:F46)</f>
+        <v/>
+      </c>
+      <c r="G48" s="31">
+        <f>SUM(G20:G46)</f>
+        <v/>
+      </c>
+      <c r="H48" s="31">
+        <f>SUM(H20:H46)</f>
+        <v/>
+      </c>
+      <c r="I48" s="31">
+        <f>SUM(I20:I46)</f>
+        <v/>
+      </c>
+      <c r="J48" s="31">
+        <f>SUM(J20:J46)</f>
+        <v/>
+      </c>
+      <c r="K48" s="31" t="n"/>
+    </row>
+    <row r="49" ht="31.1" customHeight="1">
+      <c r="A49" s="29" t="inlineStr">
+        <is>
+          <t>Mark &amp; Nº</t>
+        </is>
+      </c>
+      <c r="B49" s="29" t="inlineStr">
+        <is>
+          <t>Pallet
+NO.</t>
+        </is>
+      </c>
+      <c r="C49" s="29" t="inlineStr">
+        <is>
+          <t>P.O Nº</t>
+        </is>
+      </c>
+      <c r="D49" s="29" t="inlineStr">
+        <is>
+          <t>ITEM Nº</t>
+        </is>
+      </c>
+      <c r="E49" s="29" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F49" s="29" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="G49" s="67" t="n"/>
+      <c r="H49" s="29" t="inlineStr">
+        <is>
+          <t>N.W (kgs)</t>
+        </is>
+      </c>
+      <c r="I49" s="29" t="inlineStr">
+        <is>
+          <t>G.W (kgs)</t>
+        </is>
+      </c>
+      <c r="J49" s="29" t="inlineStr">
+        <is>
+          <t>CBM</t>
+        </is>
+      </c>
+      <c r="K49" s="29" t="inlineStr">
+        <is>
+          <t>REMARKS</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" ht="31.1" customHeight="1">
+      <c r="A50" s="68" t="n"/>
+      <c r="B50" s="68" t="n"/>
+      <c r="C50" s="68" t="n"/>
+      <c r="D50" s="68" t="n"/>
+      <c r="E50" s="68" t="n"/>
+      <c r="F50" s="29" t="inlineStr">
+        <is>
+          <t>PCS</t>
+        </is>
+      </c>
+      <c r="G50" s="29" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="H50" s="68" t="n"/>
+      <c r="I50" s="68" t="n"/>
+      <c r="J50" s="68" t="n"/>
+      <c r="K50" s="68" t="n"/>
+    </row>
+    <row r="51" ht="31.1" customHeight="1">
+      <c r="A51" s="69" t="inlineStr">
+        <is>
+          <t>VENDOR#:</t>
+        </is>
+      </c>
+      <c r="C51" s="31" t="inlineStr">
+        <is>
+          <t>PT27779</t>
+        </is>
+      </c>
+      <c r="D51" s="70" t="n">
+        <v>140491</v>
+      </c>
+      <c r="E51" s="31" t="inlineStr">
+        <is>
+          <t>L LEESWORTH BUFFALO OCEAN U43809</t>
+        </is>
+      </c>
+      <c r="F51" s="31" t="n">
+        <v>270</v>
+      </c>
+      <c r="G51" s="70" t="n">
+        <v>10074</v>
+      </c>
+      <c r="H51" s="70" t="n">
+        <v>660</v>
+      </c>
+      <c r="I51" s="70" t="n">
+        <v>705</v>
+      </c>
+      <c r="J51" s="32" t="n">
+        <v>2.2176</v>
+      </c>
+      <c r="K51" s="31" t="n"/>
+    </row>
+    <row r="52" ht="31.1" customHeight="1">
+      <c r="A52" s="69" t="inlineStr">
+        <is>
+          <t>Des: L MINDANAO BUFFALO STEELU59504</t>
+        </is>
+      </c>
+      <c r="C52" s="31" t="inlineStr">
+        <is>
+          <t>PT27779</t>
+        </is>
+      </c>
+      <c r="D52" s="70" t="n">
+        <v>140491</v>
+      </c>
+      <c r="E52" s="31" t="inlineStr">
+        <is>
+          <t>L LEESWORTH BUFFALO OCEAN U43809</t>
+        </is>
+      </c>
+      <c r="F52" s="31" t="n">
+        <v>175</v>
+      </c>
+      <c r="G52" s="32" t="n">
+        <v>6420.5</v>
+      </c>
+      <c r="H52" s="32" t="n">
+        <v>657.5</v>
+      </c>
+      <c r="I52" s="32" t="n">
+        <v>702.5</v>
+      </c>
+      <c r="J52" s="32" t="n">
+        <v>1.7424</v>
+      </c>
+      <c r="K52" s="31" t="n"/>
+    </row>
+    <row r="53" ht="31.1" customHeight="1">
+      <c r="A53" s="69" t="inlineStr">
+        <is>
+          <t>Case Qty:</t>
+        </is>
+      </c>
+      <c r="C53" s="31" t="inlineStr">
+        <is>
+          <t>PT27784</t>
+        </is>
+      </c>
+      <c r="D53" s="70" t="n">
+        <v>140491</v>
+      </c>
+      <c r="E53" s="31" t="inlineStr">
+        <is>
+          <t>L LEESWORTH BUFFALO OCEAN U43809</t>
+        </is>
+      </c>
+      <c r="F53" s="31" t="n">
+        <v>280</v>
+      </c>
+      <c r="G53" s="32" t="n">
+        <v>10554.4</v>
+      </c>
+      <c r="H53" s="70" t="n">
+        <v>625</v>
+      </c>
+      <c r="I53" s="70" t="n">
+        <v>670</v>
+      </c>
+      <c r="J53" s="32" t="n">
+        <v>2.6532</v>
+      </c>
+      <c r="K53" s="31" t="n"/>
+    </row>
+    <row r="54" ht="31.1" customHeight="1">
+      <c r="A54" s="69" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="C54" s="31" t="inlineStr">
+        <is>
+          <t>PT27784</t>
+        </is>
+      </c>
+      <c r="D54" s="70" t="n">
+        <v>140491</v>
+      </c>
+      <c r="E54" s="31" t="inlineStr">
+        <is>
+          <t>L LEESWORTH BUFFALO OCEAN U43809</t>
+        </is>
+      </c>
+      <c r="F54" s="31" t="n">
+        <v>287</v>
+      </c>
+      <c r="G54" s="32" t="n">
+        <v>10579.5</v>
+      </c>
+      <c r="H54" s="70" t="n">
+        <v>644</v>
+      </c>
+      <c r="I54" s="70" t="n">
+        <v>689</v>
+      </c>
+      <c r="J54" s="32" t="n">
+        <v>2.7324</v>
+      </c>
+      <c r="K54" s="31" t="n"/>
+    </row>
+    <row r="55" ht="31.1" customHeight="1">
+      <c r="C55" s="31" t="inlineStr">
+        <is>
+          <t>PT27T94</t>
+        </is>
+      </c>
+      <c r="D55" s="70" t="n">
+        <v>140478</v>
+      </c>
+      <c r="E55" s="31" t="inlineStr">
+        <is>
+          <t>L LEESWORTH BUFFALO DARK BROWN</t>
+        </is>
+      </c>
+      <c r="F55" s="31" t="n">
+        <v>245</v>
+      </c>
+      <c r="G55" s="32" t="n">
+        <v>10217.3</v>
+      </c>
+      <c r="H55" s="70" t="n">
+        <v>707</v>
+      </c>
+      <c r="I55" s="70" t="n">
+        <v>752</v>
+      </c>
+      <c r="J55" s="32" t="n">
+        <v>2.3364</v>
+      </c>
+      <c r="K55" s="31" t="n"/>
+    </row>
+    <row r="56" ht="31.1" customHeight="1">
+      <c r="C56" s="31" t="inlineStr">
+        <is>
+          <t>PT27T94</t>
+        </is>
+      </c>
+      <c r="D56" s="70" t="n">
+        <v>140478</v>
+      </c>
+      <c r="E56" s="31" t="inlineStr">
+        <is>
+          <t>L LEESWORTH BUFFALO DARK BROWN</t>
+        </is>
+      </c>
+      <c r="F56" s="31" t="n">
+        <v>260</v>
+      </c>
+      <c r="G56" s="32" t="n">
+        <v>10982.6</v>
+      </c>
+      <c r="H56" s="70" t="n">
+        <v>762</v>
+      </c>
+      <c r="I56" s="70" t="n">
+        <v>807</v>
+      </c>
+      <c r="J56" s="32" t="n">
+        <v>2.574</v>
+      </c>
+      <c r="K56" s="31" t="n"/>
+    </row>
+    <row r="57" ht="31.1" customHeight="1">
+      <c r="C57" s="31" t="inlineStr">
+        <is>
+          <t>PT27T94</t>
+        </is>
+      </c>
+      <c r="D57" s="70" t="n">
+        <v>140478</v>
+      </c>
+      <c r="E57" s="31" t="inlineStr">
+        <is>
+          <t>L LEESWORTH BUFFALO DARK BROWN</t>
+        </is>
+      </c>
+      <c r="F57" s="31" t="n">
+        <v>270</v>
+      </c>
+      <c r="G57" s="32" t="n">
+        <v>11221.2</v>
+      </c>
+      <c r="H57" s="70" t="n">
+        <v>777</v>
+      </c>
+      <c r="I57" s="70" t="n">
+        <v>822</v>
+      </c>
+      <c r="J57" s="32" t="n">
+        <v>2.574</v>
+      </c>
+      <c r="K57" s="31" t="n"/>
+    </row>
+    <row r="58" ht="31.1" customHeight="1">
+      <c r="C58" s="31" t="inlineStr">
+        <is>
+          <t>PT27T94</t>
+        </is>
+      </c>
+      <c r="D58" s="70" t="n">
+        <v>140478</v>
+      </c>
+      <c r="E58" s="31" t="inlineStr">
+        <is>
+          <t>L LEESWORTH BUFFALO DARK BROWN</t>
+        </is>
+      </c>
+      <c r="F58" s="31" t="n">
+        <v>255</v>
+      </c>
+      <c r="G58" s="70" t="n">
+        <v>10497</v>
+      </c>
+      <c r="H58" s="32" t="n">
+        <v>723.5</v>
+      </c>
+      <c r="I58" s="32" t="n">
+        <v>768.5</v>
+      </c>
+      <c r="J58" s="32" t="n">
+        <v>2.376</v>
+      </c>
+      <c r="K58" s="31" t="n"/>
+    </row>
+    <row r="59" ht="31.1" customHeight="1">
+      <c r="C59" s="31" t="inlineStr">
+        <is>
+          <t>PT27T94</t>
+        </is>
+      </c>
+      <c r="D59" s="70" t="n">
+        <v>140478</v>
+      </c>
+      <c r="E59" s="31" t="inlineStr">
+        <is>
+          <t>L LEESWORTH BUFFALO DARK BROWN</t>
+        </is>
+      </c>
+      <c r="F59" s="31" t="n">
+        <v>195</v>
+      </c>
+      <c r="G59" s="32" t="n">
+        <v>8273.700000000001</v>
+      </c>
+      <c r="H59" s="70" t="n">
+        <v>568</v>
+      </c>
+      <c r="I59" s="70" t="n">
+        <v>613</v>
+      </c>
+      <c r="J59" s="32" t="n">
+        <v>2.2968</v>
+      </c>
+      <c r="K59" s="31" t="n"/>
+    </row>
+    <row r="60" ht="31.1" customHeight="1">
+      <c r="C60" s="31" t="inlineStr">
+        <is>
+          <t>PT28714</t>
+        </is>
+      </c>
+      <c r="D60" s="70" t="n">
+        <v>140467</v>
+      </c>
+      <c r="E60" s="31" t="inlineStr">
+        <is>
+          <t>L GENOA  COCONUT 47704</t>
+        </is>
+      </c>
+      <c r="F60" s="31" t="n">
+        <v>115</v>
+      </c>
+      <c r="G60" s="32" t="n">
+        <v>6042.1</v>
+      </c>
+      <c r="H60" s="32" t="n">
+        <v>473.3836</v>
+      </c>
+      <c r="I60" s="32" t="n">
+        <v>517.9957000000001</v>
+      </c>
+      <c r="J60" s="32" t="n">
+        <v>2.0807</v>
+      </c>
+      <c r="K60" s="31" t="n"/>
+    </row>
+    <row r="61" ht="31.1" customHeight="1">
+      <c r="C61" s="31" t="inlineStr">
+        <is>
+          <t>PT28714</t>
+        </is>
+      </c>
+      <c r="D61" s="70" t="n">
+        <v>140467</v>
+      </c>
+      <c r="E61" s="31" t="inlineStr">
+        <is>
+          <t>L GENOA  COCONUT 47704</t>
+        </is>
+      </c>
+      <c r="F61" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="G61" s="32" t="n">
+        <v>55.1</v>
+      </c>
+      <c r="H61" s="32" t="n">
+        <v>4.1164</v>
+      </c>
+      <c r="I61" s="32" t="n">
+        <v>4.5043</v>
+      </c>
+      <c r="J61" s="32" t="n">
+        <v>0.0181</v>
+      </c>
+      <c r="K61" s="31" t="inlineStr">
+        <is>
+          <t>Low selection if yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="31.1" customHeight="1">
+      <c r="C62" s="31" t="inlineStr">
+        <is>
+          <t>PT28714</t>
+        </is>
+      </c>
+      <c r="D62" s="70" t="n">
+        <v>140467</v>
+      </c>
+      <c r="E62" s="31" t="inlineStr">
+        <is>
+          <t>L GENOA  COCONUT 47704</t>
+        </is>
+      </c>
+      <c r="F62" s="31" t="n">
+        <v>115</v>
+      </c>
+      <c r="G62" s="32" t="n">
+        <v>6145.4</v>
+      </c>
+      <c r="H62" s="70" t="n">
+        <v>576</v>
+      </c>
+      <c r="I62" s="70" t="n">
+        <v>621</v>
+      </c>
+      <c r="J62" s="32" t="n">
+        <v>2.376</v>
+      </c>
+      <c r="K62" s="31" t="n"/>
+    </row>
+    <row r="63" ht="31.1" customHeight="1">
+      <c r="A63" s="69" t="n"/>
+      <c r="B63" s="71" t="inlineStr">
+        <is>
+          <t>LEATHER (HS.CODE: 4107.12.00)</t>
+        </is>
+      </c>
+      <c r="C63" s="67" t="n"/>
+      <c r="D63" s="31" t="n"/>
+      <c r="E63" s="31" t="n"/>
+      <c r="F63" s="31" t="n"/>
+      <c r="G63" s="31" t="n"/>
+      <c r="H63" s="31" t="n"/>
+      <c r="I63" s="31" t="n"/>
+      <c r="J63" s="31" t="n"/>
+      <c r="K63" s="31" t="n"/>
+    </row>
+    <row r="64" ht="31.1" customHeight="1">
+      <c r="A64" s="72" t="n"/>
+      <c r="B64" s="31" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C64" s="31" t="n"/>
+      <c r="D64" s="31" t="n"/>
+      <c r="E64" s="31" t="inlineStr">
+        <is>
+          <t>11 PALLETS</t>
+        </is>
+      </c>
+      <c r="F64" s="31">
+        <f>SUM(F51:F62)</f>
+        <v/>
+      </c>
+      <c r="G64" s="31">
+        <f>SUM(G51:G62)</f>
+        <v/>
+      </c>
+      <c r="H64" s="31">
+        <f>SUM(H51:H62)</f>
+        <v/>
+      </c>
+      <c r="I64" s="31">
+        <f>SUM(I51:I62)</f>
+        <v/>
+      </c>
+      <c r="J64" s="31">
+        <f>SUM(J51:J62)</f>
+        <v/>
+      </c>
+      <c r="K64" s="31" t="n"/>
+    </row>
+    <row r="65" ht="31.1" customHeight="1">
+      <c r="A65" s="72" t="n"/>
+      <c r="B65" s="31" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C65" s="31" t="n"/>
+      <c r="D65" s="31" t="n"/>
+      <c r="E65" s="31" t="inlineStr">
+        <is>
+          <t>35 PALLETS</t>
+        </is>
+      </c>
+      <c r="F65" s="31" t="n"/>
+      <c r="G65" s="31" t="n"/>
+      <c r="H65" s="31" t="n"/>
+      <c r="I65" s="31" t="n"/>
+      <c r="J65" s="31" t="n"/>
+      <c r="K65" s="31" t="n"/>
+    </row>
+    <row r="66" ht="42" customHeight="1">
+      <c r="A66" s="73" t="inlineStr">
+        <is>
+          <t>Country of Original Cambodia</t>
+        </is>
+      </c>
+      <c r="F66" s="73" t="n"/>
+      <c r="G66" s="50" t="n"/>
+      <c r="H66" s="50" t="n"/>
+      <c r="I66" s="50" t="n"/>
+      <c r="J66" s="43" t="n"/>
+      <c r="K66" s="11" t="n"/>
+      <c r="L66" s="44" t="n"/>
+      <c r="M66" s="74" t="n"/>
+    </row>
+    <row r="67" ht="61.5" customHeight="1">
+      <c r="A67" s="75" t="inlineStr">
+        <is>
+          <t>Manufacture:</t>
+        </is>
+      </c>
+      <c r="B67" s="76" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
+XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="F67" s="76" t="n"/>
+      <c r="G67" s="76" t="n"/>
+      <c r="H67" s="76" t="n"/>
+      <c r="I67" s="50" t="n"/>
+      <c r="J67" s="43" t="n"/>
+      <c r="K67" s="11" t="n"/>
+      <c r="L67" s="44" t="n"/>
+      <c r="M67" s="74" t="n"/>
+    </row>
+    <row r="68" ht="44.1" customHeight="1">
+      <c r="A68" s="77" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+                                          /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="F68" s="77" t="n"/>
+      <c r="G68" s="77" t="n"/>
+      <c r="H68" s="77" t="n"/>
+      <c r="I68" s="77" t="n"/>
+      <c r="J68" s="43" t="n"/>
+      <c r="K68" s="78" t="n"/>
+      <c r="L68" s="46" t="n"/>
+      <c r="M68" s="74" t="n"/>
+    </row>
+    <row r="69" ht="24.75" customHeight="1">
+      <c r="A69" s="78" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+      <c r="M69" s="11" t="n"/>
+    </row>
+    <row r="70" ht="27" customHeight="1">
+      <c r="A70" s="78" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="M70" s="11" t="n"/>
+    </row>
+    <row r="71" ht="31.05" customHeight="1">
+      <c r="A71" s="11" t="n"/>
+      <c r="B71" s="11" t="n"/>
+      <c r="C71" s="11" t="n"/>
+      <c r="D71" s="11" t="n"/>
+      <c r="E71" s="11" t="n"/>
+      <c r="F71" s="11" t="n"/>
+      <c r="G71" s="50" t="n"/>
+      <c r="H71" s="50" t="n"/>
+      <c r="I71" s="74" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="J71" s="43" t="n"/>
+      <c r="K71" s="11" t="n"/>
+      <c r="L71" s="11" t="n"/>
+      <c r="M71" s="11" t="n"/>
+    </row>
+    <row r="72" ht="31.05" customHeight="1">
+      <c r="A72" s="11" t="n"/>
+      <c r="B72" s="11" t="n"/>
+      <c r="C72" s="11" t="n"/>
+      <c r="D72" s="11" t="n"/>
+      <c r="E72" s="11" t="n"/>
+      <c r="F72" s="11" t="n"/>
+      <c r="G72" s="50" t="n"/>
+      <c r="H72" s="50" t="n"/>
+      <c r="I72" s="43" t="n"/>
+      <c r="J72" s="11" t="n"/>
+      <c r="K72" s="11" t="n"/>
+      <c r="L72" s="11" t="n"/>
+      <c r="M72" s="11" t="n"/>
+    </row>
+    <row r="73" ht="31.05" customHeight="1">
+      <c r="A73" s="11" t="n"/>
+      <c r="B73" s="11" t="n"/>
+      <c r="C73" s="11" t="n"/>
+      <c r="D73" s="11" t="n"/>
+      <c r="E73" s="11" t="n"/>
+      <c r="F73" s="11" t="n"/>
+      <c r="G73" s="50" t="n"/>
+      <c r="H73" s="50" t="n"/>
+      <c r="I73" s="50" t="n"/>
+      <c r="J73" s="11" t="n"/>
+      <c r="K73" s="11" t="n"/>
+      <c r="L73" s="11" t="n"/>
+      <c r="M73" s="11" t="n"/>
+    </row>
+    <row r="74" ht="31.05" customHeight="1">
+      <c r="A74" s="11" t="n"/>
+      <c r="B74" s="11" t="n"/>
+      <c r="C74" s="11" t="n"/>
+      <c r="D74" s="11" t="n"/>
+      <c r="E74" s="11" t="n"/>
+      <c r="F74" s="11" t="n"/>
+      <c r="G74" s="50" t="n"/>
+      <c r="H74" s="50" t="n"/>
+      <c r="I74" s="79" t="inlineStr">
+        <is>
+          <t>ZENG XUELI</t>
+        </is>
+      </c>
+      <c r="J74" s="11" t="n"/>
+      <c r="K74" s="11" t="n"/>
+      <c r="L74" s="11" t="n"/>
+      <c r="M74" s="11" t="n"/>
+    </row>
     <row r="75"/>
     <row r="76"/>
     <row r="77"/>
@@ -2166,30 +3786,50 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="44">
     <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="C48"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B15:E15"/>
+    <mergeCell ref="H49:H50"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="B10:E10"/>
+    <mergeCell ref="J49:J50"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="I18:I19"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="E49:E50"/>
     <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B49:B50"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="J18:J19"/>
+    <mergeCell ref="C64"/>
     <mergeCell ref="A2:K2"/>
+    <mergeCell ref="C65"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="H18:H19"/>
+    <mergeCell ref="B67:E67"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="E18:E19"/>
+    <mergeCell ref="K49:K50"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="A70:L70"/>
     <mergeCell ref="C18:C19"/>
+    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="A69:L69"/>
     <mergeCell ref="K18:K19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adding logging to every of the code file
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -18,14 +18,139 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="24"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Book Antiqua"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Book Antiqua"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Book Antiqua"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <sz val="17"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <sz val="17"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <sz val="15"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -36,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -44,12 +169,168 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,21 +703,179 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17.6640625" customWidth="1" min="1" max="1"/>
+    <col width="33.109375" customWidth="1" min="2" max="2"/>
+    <col width="42.5546875" customWidth="1" min="3" max="3"/>
+    <col width="34.5546875" customWidth="1" min="4" max="4"/>
+    <col width="47.5546875" customWidth="1" min="5" max="5"/>
+    <col width="28.6640625" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
+    <row r="1" ht="45.9" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SALES CONTRACT</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="n"/>
+    </row>
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" s="3" t="n"/>
+      <c r="B2" s="3" t="n"/>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="3" t="n"/>
+      <c r="F2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="27" customHeight="1">
+      <c r="A3" s="2" t="n"/>
+      <c r="B3" s="4" t="n"/>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DATE:</t>
+        </is>
+      </c>
+      <c r="E3" s="6">
+        <f>Invoice!G9</f>
+        <v/>
+      </c>
+      <c r="F3" s="2" t="n"/>
+    </row>
+    <row r="4" ht="30" customHeight="1">
+      <c r="A4" s="4" t="n"/>
+      <c r="B4" s="4" t="n"/>
+      <c r="C4" s="4" t="n"/>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>CONTRACT NO.:</t>
+        </is>
+      </c>
+      <c r="E4" s="7">
+        <f>Invoice!G8</f>
+        <v/>
+      </c>
+      <c r="F4" s="2" t="n"/>
+    </row>
+    <row r="5" ht="32.1" customHeight="1">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Seller:   </t>
+        </is>
+      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="2" t="n"/>
+      <c r="F5" s="2" t="n"/>
+    </row>
+    <row r="6" ht="32.1" customHeight="1">
+      <c r="A6" s="2" t="n"/>
+      <c r="B6" s="9" t="inlineStr">
+        <is>
+          <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District,</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" s="2" t="n"/>
+    </row>
+    <row r="7" ht="32.1" customHeight="1">
+      <c r="A7" s="2" t="n"/>
+      <c r="B7" s="9" t="inlineStr">
+        <is>
+          <t>Svay Rieng Province, Kingdom of Cambodia.</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
+      <c r="F7" s="2" t="n"/>
+    </row>
+    <row r="8" ht="32.1" customHeight="1">
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>TEL:</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="inlineStr">
+        <is>
+          <t>+855   975910636</t>
+        </is>
+      </c>
+      <c r="C8" s="11" t="n"/>
+      <c r="D8" s="11" t="n"/>
+      <c r="E8" s="11" t="n"/>
+      <c r="F8" s="2" t="n"/>
+    </row>
+    <row r="9" ht="32.1" customHeight="1">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Buyer:  </t>
+        </is>
+      </c>
+      <c r="B9" s="9" t="inlineStr">
+        <is>
+          <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
+      <c r="F9" s="2" t="n"/>
+    </row>
+    <row r="10" ht="45" customHeight="1">
+      <c r="A10" s="8" t="n"/>
+      <c r="B10" s="12" t="inlineStr">
+        <is>
+          <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n"/>
+    </row>
+    <row r="11" ht="32.1" customHeight="1">
+      <c r="A11" s="8" t="n"/>
+      <c r="B11" s="12" t="inlineStr">
+        <is>
+          <t>BINH PHUOC WARD, DONG NAI PROVINCE, VIETNAM</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n"/>
+    </row>
+    <row r="12" ht="30" customHeight="1">
+      <c r="A12" s="9" t="inlineStr">
+        <is>
+          <t>Contact Person : Contact Person : Mr. Thuy   Tel: 0379367084</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="8" t="n"/>
+      <c r="F12" s="2" t="n"/>
+    </row>
+    <row r="13" ht="60.9" customHeight="1">
+      <c r="A13" s="13" t="inlineStr">
+        <is>
+          <t>EMAll:jyangbin4720@dingtalk.com jialy@kukahome.com dailin@kukahome.com huanggf@kukahome.com zhangzp@kukahome.com</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n"/>
+    </row>
+    <row r="14" ht="54.9" customHeight="1">
+      <c r="A14" s="14" t="inlineStr">
+        <is>
+          <t>The undersigned Sellers 、Buyers and Beneficiary have agreed to close the  following transactions according to the terms and conditions Stipulated below:</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="n"/>
+    </row>
     <row r="15"/>
     <row r="16"/>
     <row r="17"/>
@@ -624,6 +1063,13 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="B10:E10"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -659,26 +1105,431 @@
     <col width="13" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
+    <row r="1" ht="38.25" customHeight="1">
+      <c r="A1" s="15" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+    </row>
+    <row r="2" ht="24" customHeight="1">
+      <c r="A2" s="16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="17.25" customHeight="1">
+      <c r="A3" s="17" t="inlineStr">
+        <is>
+          <t>Svay Rieng Province, Kingdom of Cambodia.</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n"/>
+      <c r="I3" s="2" t="n"/>
+      <c r="J3" s="2" t="n"/>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="n"/>
+      <c r="O3" s="2" t="n"/>
+    </row>
+    <row r="4" ht="17.25" customHeight="1">
+      <c r="A4" s="16" t="inlineStr">
+        <is>
+          <t>VAT:L001-901903209</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n"/>
+      <c r="I4" s="2" t="n"/>
+      <c r="J4" s="2" t="n"/>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+      <c r="M4" s="2" t="n"/>
+      <c r="N4" s="2" t="n"/>
+      <c r="O4" s="2" t="n"/>
+    </row>
+    <row r="5" ht="25.5" customHeight="1">
+      <c r="A5" s="18" t="inlineStr">
+        <is>
+          <t>Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="B5" s="19" t="n"/>
+      <c r="C5" s="19" t="n"/>
+      <c r="D5" s="19" t="n"/>
+      <c r="E5" s="19" t="n"/>
+      <c r="F5" s="19" t="n"/>
+      <c r="G5" s="19" t="n"/>
+      <c r="H5" s="2" t="n"/>
+      <c r="I5" s="2" t="n"/>
+      <c r="J5" s="2" t="n"/>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+      <c r="M5" s="2" t="n"/>
+      <c r="N5" s="2" t="n"/>
+      <c r="O5" s="2" t="n"/>
+    </row>
+    <row r="6" ht="83.25" customHeight="1">
+      <c r="A6" s="20" t="inlineStr">
+        <is>
+          <t>INVOICE</t>
+        </is>
+      </c>
+      <c r="B6" s="21" t="n"/>
+      <c r="C6" s="21" t="n"/>
+      <c r="D6" s="21" t="n"/>
+      <c r="E6" s="21" t="n"/>
+      <c r="F6" s="21" t="n"/>
+      <c r="G6" s="21" t="n"/>
+      <c r="H6" s="2" t="n"/>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="2" t="n"/>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
+      <c r="N6" s="2" t="n"/>
+      <c r="O6" s="2" t="n"/>
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="22" t="n"/>
+      <c r="B7" s="22" t="n"/>
+      <c r="C7" s="22" t="n"/>
+      <c r="D7" s="22" t="n"/>
+      <c r="E7" s="22" t="n"/>
+      <c r="F7" s="23" t="inlineStr">
+        <is>
+          <t>Ref No.:</t>
+        </is>
+      </c>
+      <c r="G7" s="24">
+        <f>'Packing list'!I7</f>
+        <v/>
+      </c>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
+      <c r="J7" s="2" t="n"/>
+      <c r="K7" s="2" t="n"/>
+      <c r="L7" s="2" t="n"/>
+      <c r="M7" s="2" t="n"/>
+      <c r="N7" s="2" t="n"/>
+      <c r="O7" s="2" t="n"/>
+    </row>
+    <row r="8" ht="30" customHeight="1">
+      <c r="A8" s="25" t="inlineStr">
+        <is>
+          <t>EXPORTER:</t>
+        </is>
+      </c>
+      <c r="B8" s="26" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="26" t="n"/>
+      <c r="F8" s="27" t="inlineStr">
+        <is>
+          <t>INVOICE NO :</t>
+        </is>
+      </c>
+      <c r="G8" s="28">
+        <f>'Packing list'!I8</f>
+        <v/>
+      </c>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="2" t="n"/>
+      <c r="K8" s="2" t="n"/>
+      <c r="L8" s="2" t="n"/>
+      <c r="M8" s="2" t="n"/>
+      <c r="N8" s="2" t="n"/>
+      <c r="O8" s="2" t="n"/>
+    </row>
+    <row r="9" ht="21" customHeight="1">
+      <c r="A9" s="22" t="n"/>
+      <c r="B9" s="22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, </t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="22" t="n"/>
+      <c r="F9" s="27" t="inlineStr">
+        <is>
+          <t>Date:</t>
+        </is>
+      </c>
+      <c r="G9" s="29">
+        <f>'Packing list'!I9</f>
+        <v/>
+      </c>
+      <c r="H9" s="2" t="n"/>
+      <c r="I9" s="2" t="n"/>
+      <c r="J9" s="2" t="n"/>
+      <c r="K9" s="2" t="n"/>
+      <c r="L9" s="2" t="n"/>
+      <c r="M9" s="2" t="n"/>
+      <c r="N9" s="2" t="n"/>
+      <c r="O9" s="2" t="n"/>
+    </row>
+    <row r="10" ht="22.5" customHeight="1">
+      <c r="A10" s="22" t="n"/>
+      <c r="B10" s="22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia </t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="22" t="n"/>
+      <c r="F10" s="30" t="inlineStr">
+        <is>
+          <t>FCA :</t>
+        </is>
+      </c>
+      <c r="G10" s="31" t="inlineStr">
+        <is>
+          <t>BAVET, SVAYRIENG</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="n"/>
+      <c r="I10" s="2" t="n"/>
+      <c r="J10" s="2" t="n"/>
+      <c r="K10" s="2" t="n"/>
+      <c r="L10" s="2" t="n"/>
+      <c r="M10" s="2" t="n"/>
+      <c r="N10" s="2" t="n"/>
+      <c r="O10" s="2" t="n"/>
+    </row>
+    <row r="11" ht="20.25" customHeight="1">
+      <c r="A11" s="22" t="n"/>
+      <c r="B11" s="22" t="inlineStr">
+        <is>
+          <t>Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="2" t="n"/>
+      <c r="E11" s="22" t="n"/>
+      <c r="F11" s="22" t="n"/>
+      <c r="G11" s="16" t="n"/>
+      <c r="H11" s="2" t="n"/>
+      <c r="I11" s="2" t="n"/>
+      <c r="J11" s="2" t="n"/>
+      <c r="K11" s="2" t="n"/>
+      <c r="L11" s="2" t="n"/>
+      <c r="M11" s="2" t="n"/>
+      <c r="N11" s="2" t="n"/>
+      <c r="O11" s="2" t="n"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="22" t="n"/>
+      <c r="B12" s="22" t="n"/>
+      <c r="C12" s="22" t="n"/>
+      <c r="D12" s="22" t="n"/>
+      <c r="E12" s="22" t="n"/>
+      <c r="F12" s="22" t="n"/>
+      <c r="G12" s="16" t="n"/>
+      <c r="H12" s="2" t="n"/>
+      <c r="I12" s="2" t="n"/>
+      <c r="J12" s="2" t="n"/>
+      <c r="K12" s="2" t="n"/>
+      <c r="L12" s="2" t="n"/>
+      <c r="M12" s="2" t="n"/>
+      <c r="N12" s="2" t="n"/>
+      <c r="O12" s="2" t="n"/>
+    </row>
+    <row r="13" ht="25.5" customHeight="1">
+      <c r="A13" s="32" t="inlineStr">
+        <is>
+          <t>CONSIGNEE :</t>
+        </is>
+      </c>
+      <c r="B13" s="33" t="inlineStr">
+        <is>
+          <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="34" t="n"/>
+      <c r="F13" s="34" t="n"/>
+      <c r="G13" s="35" t="n"/>
+      <c r="H13" s="2" t="n"/>
+      <c r="I13" s="2" t="n"/>
+      <c r="J13" s="2" t="n"/>
+      <c r="K13" s="2" t="n"/>
+      <c r="L13" s="2" t="n"/>
+      <c r="M13" s="2" t="n"/>
+      <c r="N13" s="2" t="n"/>
+      <c r="O13" s="2" t="n"/>
+    </row>
+    <row r="14" ht="25.5" customHeight="1">
+      <c r="A14" s="22" t="n"/>
+      <c r="B14" s="36" t="inlineStr">
+        <is>
+          <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
+        </is>
+      </c>
+      <c r="C14" s="37" t="n"/>
+      <c r="D14" s="37" t="n"/>
+      <c r="E14" s="37" t="n"/>
+      <c r="F14" s="37" t="n"/>
+      <c r="G14" s="2" t="n"/>
+      <c r="H14" s="2" t="n"/>
+      <c r="I14" s="2" t="n"/>
+      <c r="J14" s="2" t="n"/>
+      <c r="K14" s="2" t="n"/>
+      <c r="L14" s="2" t="n"/>
+      <c r="M14" s="2" t="n"/>
+      <c r="N14" s="2" t="n"/>
+      <c r="O14" s="2" t="n"/>
+    </row>
+    <row r="15" ht="25.5" customHeight="1">
+      <c r="A15" s="22" t="n"/>
+      <c r="B15" s="38" t="inlineStr">
+        <is>
+          <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
+        </is>
+      </c>
+      <c r="C15" s="39" t="n"/>
+      <c r="D15" s="39" t="n"/>
+      <c r="E15" s="39" t="n"/>
+      <c r="F15" s="35" t="n"/>
+      <c r="G15" s="2" t="n"/>
+      <c r="H15" s="2" t="n"/>
+      <c r="I15" s="2" t="n"/>
+      <c r="J15" s="2" t="n"/>
+      <c r="K15" s="2" t="n"/>
+      <c r="L15" s="2" t="n"/>
+      <c r="M15" s="2" t="n"/>
+      <c r="N15" s="2" t="n"/>
+      <c r="O15" s="2" t="n"/>
+    </row>
+    <row r="16" ht="25.5" customHeight="1">
+      <c r="A16" s="22" t="n"/>
+      <c r="B16" s="40" t="inlineStr">
+        <is>
+          <t>Contact Person : Mr. Thuy   TEl: 0379367084</t>
+        </is>
+      </c>
+      <c r="C16" s="39" t="n"/>
+      <c r="D16" s="39" t="n"/>
+      <c r="E16" s="39" t="n"/>
+      <c r="F16" s="39" t="n"/>
+      <c r="G16" s="2" t="n"/>
+      <c r="H16" s="2" t="n"/>
+      <c r="I16" s="2" t="n"/>
+      <c r="J16" s="2" t="n"/>
+      <c r="K16" s="2" t="n"/>
+      <c r="L16" s="2" t="n"/>
+      <c r="M16" s="2" t="n"/>
+      <c r="N16" s="2" t="n"/>
+      <c r="O16" s="2" t="n"/>
+    </row>
+    <row r="17" ht="25.5" customHeight="1">
+      <c r="A17" s="22" t="n"/>
+      <c r="B17" s="40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EMAlL:jyangbin4720@dingtalk.com jialy@kukahome.com </t>
+        </is>
+      </c>
+      <c r="C17" s="39" t="n"/>
+      <c r="D17" s="39" t="n"/>
+      <c r="E17" s="39" t="n"/>
+      <c r="F17" s="35" t="n"/>
+      <c r="G17" s="2" t="n"/>
+      <c r="H17" s="2" t="n"/>
+      <c r="I17" s="2" t="n"/>
+      <c r="J17" s="2" t="n"/>
+      <c r="K17" s="2" t="n"/>
+      <c r="L17" s="2" t="n"/>
+      <c r="M17" s="2" t="n"/>
+      <c r="N17" s="2" t="n"/>
+      <c r="O17" s="2" t="n"/>
+    </row>
+    <row r="18" ht="25.5" customHeight="1">
+      <c r="A18" s="22" t="n"/>
+      <c r="B18" s="40" t="inlineStr">
+        <is>
+          <t>dailin@kukahome.com huanggf@kukahome.com zhangzp@kukahome.com</t>
+        </is>
+      </c>
+      <c r="C18" s="22" t="n"/>
+      <c r="D18" s="22" t="n"/>
+      <c r="E18" s="22" t="n"/>
+      <c r="F18" s="16" t="n"/>
+      <c r="G18" s="2" t="n"/>
+      <c r="H18" s="2" t="n"/>
+      <c r="I18" s="2" t="n"/>
+      <c r="J18" s="2" t="n"/>
+      <c r="K18" s="2" t="n"/>
+      <c r="L18" s="2" t="n"/>
+      <c r="M18" s="2" t="n"/>
+      <c r="N18" s="2" t="n"/>
+      <c r="O18" s="2" t="n"/>
+    </row>
+    <row r="19" ht="27.75" customHeight="1">
+      <c r="A19" s="41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SHIP: </t>
+        </is>
+      </c>
+      <c r="B19" s="22" t="inlineStr">
+        <is>
+          <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n"/>
+      <c r="E19" s="2" t="n"/>
+      <c r="F19" s="42" t="n"/>
+      <c r="G19" s="2" t="n"/>
+      <c r="H19" s="2" t="n"/>
+      <c r="I19" s="2" t="n"/>
+      <c r="J19" s="2" t="n"/>
+      <c r="K19" s="2" t="n"/>
+      <c r="L19" s="2" t="n"/>
+      <c r="M19" s="2" t="n"/>
+      <c r="N19" s="2" t="n"/>
+      <c r="O19" s="2" t="n"/>
+    </row>
+    <row r="20" ht="27.75" customHeight="1">
+      <c r="A20" s="43" t="n"/>
+      <c r="B20" s="43" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
+      <c r="F20" s="2" t="n"/>
+      <c r="G20" s="2" t="n"/>
+      <c r="H20" s="2" t="n"/>
+      <c r="I20" s="2" t="n"/>
+      <c r="J20" s="2" t="n"/>
+      <c r="K20" s="2" t="n"/>
+      <c r="L20" s="2" t="n"/>
+      <c r="M20" s="2" t="n"/>
+      <c r="N20" s="2" t="n"/>
+      <c r="O20" s="2" t="n"/>
+    </row>
     <row r="21"/>
     <row r="22"/>
     <row r="23"/>
@@ -860,6 +1711,14 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A5:G5"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -877,27 +1736,318 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25.44140625" customWidth="1" min="1" max="1"/>
+    <col width="22.88671875" customWidth="1" min="2" max="2"/>
+    <col width="19.44140625" customWidth="1" min="3" max="3"/>
+    <col width="26.6640625" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="13.6640625" customWidth="1" min="7" max="7"/>
+    <col width="15.5546875" customWidth="1" min="8" max="8"/>
+    <col width="23.6640625" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
+    <row r="1" ht="38.25" customHeight="1">
+      <c r="A1" s="15" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="24" customHeight="1">
+      <c r="A2" s="16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="25.5" customHeight="1">
+      <c r="A3" s="17" t="inlineStr">
+        <is>
+          <t>Svay Rieng Province, Kingdom of Cambodia.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="25.5" customHeight="1">
+      <c r="A4" s="16" t="inlineStr">
+        <is>
+          <t>VAT:L001-901903209</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="25.5" customHeight="1">
+      <c r="A5" s="18" t="inlineStr">
+        <is>
+          <t>Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="B5" s="19" t="n"/>
+      <c r="C5" s="19" t="n"/>
+      <c r="D5" s="19" t="n"/>
+      <c r="E5" s="19" t="n"/>
+      <c r="F5" s="19" t="n"/>
+      <c r="G5" s="19" t="n"/>
+      <c r="H5" s="19" t="n"/>
+      <c r="I5" s="19" t="n"/>
+    </row>
+    <row r="6" ht="54" customHeight="1">
+      <c r="A6" s="20" t="inlineStr">
+        <is>
+          <t>PACKING LIST</t>
+        </is>
+      </c>
+      <c r="B6" s="21" t="n"/>
+      <c r="C6" s="21" t="n"/>
+      <c r="D6" s="21" t="n"/>
+      <c r="E6" s="21" t="n"/>
+      <c r="F6" s="21" t="n"/>
+      <c r="G6" s="21" t="n"/>
+      <c r="H6" s="21" t="n"/>
+      <c r="I6" s="21" t="n"/>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="A7" s="22" t="n"/>
+      <c r="B7" s="44" t="n"/>
+      <c r="C7" s="22" t="n"/>
+      <c r="D7" s="22" t="n"/>
+      <c r="E7" s="16" t="n"/>
+      <c r="F7" s="16" t="n"/>
+      <c r="G7" s="16" t="n"/>
+      <c r="H7" s="23" t="inlineStr">
+        <is>
+          <t>Ref No.:</t>
+        </is>
+      </c>
+      <c r="I7" s="45" t="inlineStr">
+        <is>
+          <t>JFREF</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1">
+      <c r="A8" s="25" t="inlineStr">
+        <is>
+          <t>EXPORTER:</t>
+        </is>
+      </c>
+      <c r="B8" s="46" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="27" t="n"/>
+      <c r="G8" s="27" t="n"/>
+      <c r="H8" s="27" t="inlineStr">
+        <is>
+          <t>INVOICE NO :</t>
+        </is>
+      </c>
+      <c r="I8" s="47" t="inlineStr">
+        <is>
+          <t>JFINV</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="21" customHeight="1">
+      <c r="A9" s="22" t="n"/>
+      <c r="B9" s="44" t="inlineStr">
+        <is>
+          <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages,</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
+      <c r="F9" s="16" t="n"/>
+      <c r="G9" s="16" t="n"/>
+      <c r="H9" s="27" t="inlineStr">
+        <is>
+          <t>Date:</t>
+        </is>
+      </c>
+      <c r="I9" s="29" t="inlineStr">
+        <is>
+          <t>JFTIME</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="22.5" customHeight="1">
+      <c r="A10" s="22" t="n"/>
+      <c r="B10" s="44" t="inlineStr">
+        <is>
+          <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
+      <c r="F10" s="16" t="n"/>
+      <c r="G10" s="16" t="n"/>
+      <c r="H10" s="30" t="inlineStr">
+        <is>
+          <t>FCA :</t>
+        </is>
+      </c>
+      <c r="I10" s="48" t="inlineStr">
+        <is>
+          <t>BAVET, SVAY RIENG</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="20.25" customHeight="1">
+      <c r="A11" s="22" t="n"/>
+      <c r="B11" s="44" t="inlineStr">
+        <is>
+          <t>Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="2" t="n"/>
+      <c r="E11" s="2" t="n"/>
+      <c r="F11" s="16" t="n"/>
+      <c r="G11" s="16" t="n"/>
+      <c r="H11" s="16" t="n"/>
+      <c r="I11" s="16" t="n"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="22" t="n"/>
+      <c r="B12" s="44" t="n"/>
+      <c r="C12" s="22" t="n"/>
+      <c r="D12" s="22" t="n"/>
+      <c r="E12" s="16" t="n"/>
+      <c r="F12" s="16" t="n"/>
+      <c r="G12" s="16" t="n"/>
+      <c r="H12" s="16" t="n"/>
+      <c r="I12" s="16" t="n"/>
+    </row>
+    <row r="13" ht="25.5" customHeight="1">
+      <c r="A13" s="32" t="inlineStr">
+        <is>
+          <t>CONSIGNEE :</t>
+        </is>
+      </c>
+      <c r="B13" s="49" t="inlineStr">
+        <is>
+          <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" s="50" t="n"/>
+      <c r="G13" s="50" t="n"/>
+      <c r="H13" s="50" t="n"/>
+      <c r="I13" s="35" t="n"/>
+    </row>
+    <row r="14" ht="25.5" customHeight="1">
+      <c r="A14" s="22" t="n"/>
+      <c r="B14" s="51" t="inlineStr">
+        <is>
+          <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
+        </is>
+      </c>
+      <c r="C14" s="37" t="n"/>
+      <c r="D14" s="37" t="n"/>
+      <c r="E14" s="52" t="n"/>
+      <c r="F14" s="52" t="n"/>
+      <c r="G14" s="52" t="n"/>
+      <c r="H14" s="52" t="n"/>
+      <c r="I14" s="2" t="n"/>
+    </row>
+    <row r="15" ht="21" customHeight="1">
+      <c r="A15" s="22" t="n"/>
+      <c r="B15" s="53" t="inlineStr">
+        <is>
+          <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
+        </is>
+      </c>
+      <c r="C15" s="39" t="n"/>
+      <c r="D15" s="39" t="n"/>
+      <c r="E15" s="35" t="n"/>
+      <c r="F15" s="35" t="n"/>
+      <c r="G15" s="35" t="n"/>
+      <c r="H15" s="35" t="n"/>
+      <c r="I15" s="2" t="n"/>
+    </row>
+    <row r="16" ht="21" customHeight="1">
+      <c r="A16" s="22" t="n"/>
+      <c r="B16" s="38" t="inlineStr">
+        <is>
+          <t>Contact Person : Mr. Thuy   TEl: 0379367084</t>
+        </is>
+      </c>
+      <c r="C16" s="39" t="n"/>
+      <c r="D16" s="39" t="n"/>
+      <c r="E16" s="35" t="n"/>
+      <c r="F16" s="35" t="n"/>
+      <c r="G16" s="35" t="n"/>
+      <c r="H16" s="35" t="n"/>
+      <c r="I16" s="2" t="n"/>
+    </row>
+    <row r="17" ht="21" customHeight="1">
+      <c r="A17" s="22" t="n"/>
+      <c r="B17" s="38" t="inlineStr">
+        <is>
+          <t>EMAlL:jyangbin4720@dingtalk.com jialy@kukahome.com</t>
+        </is>
+      </c>
+      <c r="C17" s="39" t="n"/>
+      <c r="D17" s="39" t="n"/>
+      <c r="E17" s="35" t="n"/>
+      <c r="F17" s="35" t="n"/>
+      <c r="G17" s="35" t="n"/>
+      <c r="H17" s="35" t="n"/>
+      <c r="I17" s="2" t="n"/>
+    </row>
+    <row r="18" ht="21" customHeight="1">
+      <c r="A18" s="22" t="n"/>
+      <c r="B18" s="38" t="inlineStr">
+        <is>
+          <t>dailin@kukahome.com huanggf@kukahome.com zhangzp@kukahome.com</t>
+        </is>
+      </c>
+      <c r="C18" s="22" t="n"/>
+      <c r="D18" s="22" t="n"/>
+      <c r="E18" s="16" t="n"/>
+      <c r="F18" s="16" t="n"/>
+      <c r="G18" s="16" t="n"/>
+      <c r="H18" s="16" t="n"/>
+      <c r="I18" s="2" t="n"/>
+    </row>
+    <row r="19" ht="27.75" customHeight="1">
+      <c r="A19" s="41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SHIP: </t>
+        </is>
+      </c>
+      <c r="B19" s="44" t="inlineStr">
+        <is>
+          <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n"/>
+      <c r="E19" s="2" t="n"/>
+      <c r="F19" s="2" t="n"/>
+      <c r="G19" s="2" t="n"/>
+      <c r="H19" s="2" t="n"/>
+      <c r="I19" s="2" t="n"/>
+    </row>
+    <row r="20" ht="27.75" customHeight="1">
+      <c r="A20" s="43" t="n"/>
+      <c r="B20" s="54" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
+      <c r="F20" s="2" t="n"/>
+      <c r="G20" s="2" t="n"/>
+      <c r="H20" s="2" t="n"/>
+      <c r="I20" s="2" t="n"/>
+    </row>
     <row r="21"/>
     <row r="22"/>
     <row r="23"/>
@@ -1079,6 +2229,14 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A4:I4"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed data table filling conflict with the footer template at the packing list
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -21,7 +21,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="29">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -127,6 +127,41 @@
     </font>
     <font>
       <name val="Times New Roman"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
       <charset val="134"/>
       <sz val="20"/>
     </font>
@@ -148,20 +183,43 @@
     </font>
     <font>
       <name val="Times New Roman"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="16"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
       <charset val="134"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -187,50 +245,152 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -306,8 +466,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -325,12 +526,33 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -876,33 +1098,435 @@
       </c>
       <c r="F14" s="2" t="n"/>
     </row>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
+    <row r="15">
+      <c r="A15" s="15" t="inlineStr">
+        <is>
+          <t>No.</t>
+        </is>
+      </c>
+      <c r="B15" s="15" t="inlineStr">
+        <is>
+          <t>ITEM Nº</t>
+        </is>
+      </c>
+      <c r="C15" s="15" t="inlineStr">
+        <is>
+          <t>Quantity(SF)</t>
+        </is>
+      </c>
+      <c r="D15" s="15" t="inlineStr">
+        <is>
+          <t>Unit Price(USD)</t>
+        </is>
+      </c>
+      <c r="E15" s="15" t="inlineStr">
+        <is>
+          <t>Total value(USD)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>01.10.W653191</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>6461.7</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E16">
+        <f>D16*C16</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>01.10.W653191</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>77.90000000000001</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E17">
+        <f>D17*C17</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>01.10.U756071</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>20949.5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E18">
+        <f>D18*C18</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>01.10.U756071</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>241.9</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E19">
+        <f>D19*C19</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>28156.8</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="E20">
+        <f>D20*C20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>711.1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E21">
+        <f>D21*C21</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1301.4</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E22">
+        <f>D22*C22</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>18717.9</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="E23">
+        <f>D23*C23</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>106711.7</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E24">
+        <f>D24*C24</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>1320.6</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E25">
+        <f>D25*C25</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>367.3</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="E26">
+        <f>D26*C26</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>101424.8</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E27">
+        <f>D27*C27</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>1205.1</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E28">
+        <f>D28*C28</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>01.10.L2924</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>5345</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E29">
+        <f>D29*C29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>01.10.L2924</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>121</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E30">
+        <f>D30*C30</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" ht="36" customHeight="1">
+      <c r="A31" s="16" t="n"/>
+      <c r="B31" s="16" t="n"/>
+      <c r="C31" s="16" t="n"/>
+      <c r="D31" s="16" t="n"/>
+      <c r="E31" s="16" t="n"/>
+    </row>
+    <row r="32" ht="30" customHeight="1">
+      <c r="A32" s="8" t="inlineStr">
+        <is>
+          <t>Term of Payment: 100% TT after shipment</t>
+        </is>
+      </c>
+      <c r="B32" s="8" t="n"/>
+      <c r="C32" s="8" t="n"/>
+      <c r="D32" s="8" t="n"/>
+      <c r="E32" s="8" t="n"/>
+      <c r="F32" s="2" t="n"/>
+    </row>
+    <row r="33" ht="36" customHeight="1">
+      <c r="A33" s="8" t="inlineStr">
+        <is>
+          <t>Transaction method: FCA(USD)</t>
+        </is>
+      </c>
+      <c r="B33" s="8" t="n"/>
+      <c r="C33" s="8" t="n"/>
+      <c r="D33" s="8" t="n"/>
+      <c r="E33" s="8" t="n"/>
+      <c r="F33" s="2" t="n"/>
+    </row>
+    <row r="34" ht="20.4" customHeight="1">
+      <c r="A34" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beneficiary bank information: </t>
+        </is>
+      </c>
+      <c r="B34" s="8" t="n"/>
+      <c r="C34" s="8" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
+        </is>
+      </c>
+      <c r="D34" s="8" t="n"/>
+      <c r="E34" s="8" t="n"/>
+      <c r="F34" s="2" t="n"/>
+    </row>
+    <row r="35" ht="45.9" customHeight="1">
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beneficiary Bank' s Name: </t>
+        </is>
+      </c>
+      <c r="B35" s="8" t="n"/>
+      <c r="C35" s="14" t="inlineStr">
+        <is>
+          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+ /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="n"/>
+    </row>
+    <row r="36" ht="41.1" customHeight="1">
+      <c r="A36" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bank Address:  </t>
+        </is>
+      </c>
+      <c r="B36" s="8" t="n"/>
+      <c r="C36" s="14" t="inlineStr">
+        <is>
+          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.
+PHNOM PEMH,CAMBODIA.</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="n"/>
+    </row>
+    <row r="37" ht="29.1" customHeight="1">
+      <c r="A37" s="8" t="inlineStr">
+        <is>
+          <t>Bank account :</t>
+        </is>
+      </c>
+      <c r="B37" s="8" t="n"/>
+      <c r="C37" s="17" t="inlineStr">
+        <is>
+          <t>100001100764430</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="n"/>
+    </row>
+    <row r="38" ht="19.2" customHeight="1">
+      <c r="A38" s="8" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：</t>
+        </is>
+      </c>
+      <c r="B38" s="8" t="n"/>
+      <c r="C38" s="8" t="inlineStr">
+        <is>
+          <t>BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="D38" s="8" t="n"/>
+      <c r="E38" s="8" t="n"/>
+      <c r="F38" s="2" t="n"/>
+    </row>
+    <row r="39" ht="45.9" customHeight="1">
+      <c r="A39" s="8" t="n"/>
+      <c r="B39" s="8" t="n"/>
+      <c r="C39" s="8" t="n"/>
+      <c r="D39" s="8" t="n"/>
+      <c r="E39" s="8" t="n"/>
+      <c r="F39" s="8" t="n"/>
+    </row>
+    <row r="40" ht="41.1" customHeight="1">
+      <c r="A40" s="18" t="inlineStr">
+        <is>
+          <t>The Buyer:</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="n"/>
+      <c r="C40" s="2" t="n"/>
+      <c r="D40" s="19" t="inlineStr">
+        <is>
+          <t>The Seller:</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n"/>
+      <c r="F40" s="2" t="n"/>
+    </row>
+    <row r="41" ht="29.1" customHeight="1">
+      <c r="A41" s="20" t="inlineStr">
+        <is>
+          <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
+        </is>
+      </c>
+      <c r="B41" s="21" t="n"/>
+      <c r="C41" s="22" t="n"/>
+      <c r="D41" s="20" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
+        </is>
+      </c>
+      <c r="E41" s="20" t="n"/>
+      <c r="F41" s="2" t="n"/>
+    </row>
     <row r="42"/>
     <row r="43"/>
     <row r="44"/>
@@ -1063,12 +1687,15 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="B10:E10"/>
+    <mergeCell ref="C35:E35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1106,7 +1733,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="38.25" customHeight="1">
-      <c r="A1" s="15" t="inlineStr">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
@@ -1121,7 +1748,7 @@
       <c r="O1" s="2" t="n"/>
     </row>
     <row r="2" ht="24" customHeight="1">
-      <c r="A2" s="16" t="inlineStr">
+      <c r="A2" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
         </is>
@@ -1136,7 +1763,7 @@
       <c r="O2" s="2" t="n"/>
     </row>
     <row r="3" ht="17.25" customHeight="1">
-      <c r="A3" s="17" t="inlineStr">
+      <c r="A3" s="25" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
@@ -1151,7 +1778,7 @@
       <c r="O3" s="2" t="n"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" s="16" t="inlineStr">
+      <c r="A4" s="24" t="inlineStr">
         <is>
           <t>VAT:L001-901903209</t>
         </is>
@@ -1166,17 +1793,17 @@
       <c r="O4" s="2" t="n"/>
     </row>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="18" t="inlineStr">
+      <c r="A5" s="26" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="B5" s="19" t="n"/>
-      <c r="C5" s="19" t="n"/>
-      <c r="D5" s="19" t="n"/>
-      <c r="E5" s="19" t="n"/>
-      <c r="F5" s="19" t="n"/>
-      <c r="G5" s="19" t="n"/>
+      <c r="B5" s="27" t="n"/>
+      <c r="C5" s="27" t="n"/>
+      <c r="D5" s="27" t="n"/>
+      <c r="E5" s="27" t="n"/>
+      <c r="F5" s="27" t="n"/>
+      <c r="G5" s="27" t="n"/>
       <c r="H5" s="2" t="n"/>
       <c r="I5" s="2" t="n"/>
       <c r="J5" s="2" t="n"/>
@@ -1187,17 +1814,17 @@
       <c r="O5" s="2" t="n"/>
     </row>
     <row r="6" ht="83.25" customHeight="1">
-      <c r="A6" s="20" t="inlineStr">
+      <c r="A6" s="28" t="inlineStr">
         <is>
           <t>INVOICE</t>
         </is>
       </c>
-      <c r="B6" s="21" t="n"/>
-      <c r="C6" s="21" t="n"/>
-      <c r="D6" s="21" t="n"/>
-      <c r="E6" s="21" t="n"/>
-      <c r="F6" s="21" t="n"/>
-      <c r="G6" s="21" t="n"/>
+      <c r="B6" s="29" t="n"/>
+      <c r="C6" s="29" t="n"/>
+      <c r="D6" s="29" t="n"/>
+      <c r="E6" s="29" t="n"/>
+      <c r="F6" s="29" t="n"/>
+      <c r="G6" s="29" t="n"/>
       <c r="H6" s="2" t="n"/>
       <c r="I6" s="2" t="n"/>
       <c r="J6" s="2" t="n"/>
@@ -1208,17 +1835,17 @@
       <c r="O6" s="2" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="22" t="n"/>
-      <c r="B7" s="22" t="n"/>
-      <c r="C7" s="22" t="n"/>
-      <c r="D7" s="22" t="n"/>
-      <c r="E7" s="22" t="n"/>
-      <c r="F7" s="23" t="inlineStr">
+      <c r="A7" s="30" t="n"/>
+      <c r="B7" s="30" t="n"/>
+      <c r="C7" s="30" t="n"/>
+      <c r="D7" s="30" t="n"/>
+      <c r="E7" s="30" t="n"/>
+      <c r="F7" s="31" t="inlineStr">
         <is>
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="32">
         <f>'Packing list'!I7</f>
         <v/>
       </c>
@@ -1232,25 +1859,25 @@
       <c r="O7" s="2" t="n"/>
     </row>
     <row r="8" ht="30" customHeight="1">
-      <c r="A8" s="25" t="inlineStr">
+      <c r="A8" s="33" t="inlineStr">
         <is>
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="26" t="inlineStr">
+      <c r="B8" s="34" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
       <c r="C8" s="2" t="n"/>
       <c r="D8" s="2" t="n"/>
-      <c r="E8" s="26" t="n"/>
-      <c r="F8" s="27" t="inlineStr">
+      <c r="E8" s="34" t="n"/>
+      <c r="F8" s="35" t="inlineStr">
         <is>
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="36">
         <f>'Packing list'!I8</f>
         <v/>
       </c>
@@ -1264,21 +1891,21 @@
       <c r="O8" s="2" t="n"/>
     </row>
     <row r="9" ht="21" customHeight="1">
-      <c r="A9" s="22" t="n"/>
-      <c r="B9" s="22" t="inlineStr">
+      <c r="A9" s="30" t="n"/>
+      <c r="B9" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, </t>
         </is>
       </c>
       <c r="C9" s="2" t="n"/>
       <c r="D9" s="2" t="n"/>
-      <c r="E9" s="22" t="n"/>
-      <c r="F9" s="27" t="inlineStr">
+      <c r="E9" s="30" t="n"/>
+      <c r="F9" s="35" t="inlineStr">
         <is>
           <t>Date:</t>
         </is>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="37">
         <f>'Packing list'!I9</f>
         <v/>
       </c>
@@ -1292,21 +1919,21 @@
       <c r="O9" s="2" t="n"/>
     </row>
     <row r="10" ht="22.5" customHeight="1">
-      <c r="A10" s="22" t="n"/>
-      <c r="B10" s="22" t="inlineStr">
+      <c r="A10" s="30" t="n"/>
+      <c r="B10" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia </t>
         </is>
       </c>
       <c r="C10" s="2" t="n"/>
       <c r="D10" s="2" t="n"/>
-      <c r="E10" s="22" t="n"/>
-      <c r="F10" s="30" t="inlineStr">
+      <c r="E10" s="30" t="n"/>
+      <c r="F10" s="38" t="inlineStr">
         <is>
           <t>FCA :</t>
         </is>
       </c>
-      <c r="G10" s="31" t="inlineStr">
+      <c r="G10" s="39" t="inlineStr">
         <is>
           <t>BAVET, SVAYRIENG</t>
         </is>
@@ -1321,17 +1948,17 @@
       <c r="O10" s="2" t="n"/>
     </row>
     <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="22" t="n"/>
-      <c r="B11" s="22" t="inlineStr">
+      <c r="A11" s="30" t="n"/>
+      <c r="B11" s="30" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
       <c r="C11" s="2" t="n"/>
       <c r="D11" s="2" t="n"/>
-      <c r="E11" s="22" t="n"/>
-      <c r="F11" s="22" t="n"/>
-      <c r="G11" s="16" t="n"/>
+      <c r="E11" s="30" t="n"/>
+      <c r="F11" s="30" t="n"/>
+      <c r="G11" s="24" t="n"/>
       <c r="H11" s="2" t="n"/>
       <c r="I11" s="2" t="n"/>
       <c r="J11" s="2" t="n"/>
@@ -1342,13 +1969,13 @@
       <c r="O11" s="2" t="n"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="22" t="n"/>
-      <c r="B12" s="22" t="n"/>
-      <c r="C12" s="22" t="n"/>
-      <c r="D12" s="22" t="n"/>
-      <c r="E12" s="22" t="n"/>
-      <c r="F12" s="22" t="n"/>
-      <c r="G12" s="16" t="n"/>
+      <c r="A12" s="30" t="n"/>
+      <c r="B12" s="30" t="n"/>
+      <c r="C12" s="30" t="n"/>
+      <c r="D12" s="30" t="n"/>
+      <c r="E12" s="30" t="n"/>
+      <c r="F12" s="30" t="n"/>
+      <c r="G12" s="24" t="n"/>
       <c r="H12" s="2" t="n"/>
       <c r="I12" s="2" t="n"/>
       <c r="J12" s="2" t="n"/>
@@ -1359,21 +1986,21 @@
       <c r="O12" s="2" t="n"/>
     </row>
     <row r="13" ht="25.5" customHeight="1">
-      <c r="A13" s="32" t="inlineStr">
+      <c r="A13" s="40" t="inlineStr">
         <is>
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="33" t="inlineStr">
+      <c r="B13" s="41" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
       </c>
       <c r="C13" s="2" t="n"/>
       <c r="D13" s="2" t="n"/>
-      <c r="E13" s="34" t="n"/>
-      <c r="F13" s="34" t="n"/>
-      <c r="G13" s="35" t="n"/>
+      <c r="E13" s="42" t="n"/>
+      <c r="F13" s="42" t="n"/>
+      <c r="G13" s="43" t="n"/>
       <c r="H13" s="2" t="n"/>
       <c r="I13" s="2" t="n"/>
       <c r="J13" s="2" t="n"/>
@@ -1384,16 +2011,16 @@
       <c r="O13" s="2" t="n"/>
     </row>
     <row r="14" ht="25.5" customHeight="1">
-      <c r="A14" s="22" t="n"/>
-      <c r="B14" s="36" t="inlineStr">
+      <c r="A14" s="30" t="n"/>
+      <c r="B14" s="44" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
-      <c r="C14" s="37" t="n"/>
-      <c r="D14" s="37" t="n"/>
-      <c r="E14" s="37" t="n"/>
-      <c r="F14" s="37" t="n"/>
+      <c r="C14" s="45" t="n"/>
+      <c r="D14" s="45" t="n"/>
+      <c r="E14" s="45" t="n"/>
+      <c r="F14" s="45" t="n"/>
       <c r="G14" s="2" t="n"/>
       <c r="H14" s="2" t="n"/>
       <c r="I14" s="2" t="n"/>
@@ -1405,16 +2032,16 @@
       <c r="O14" s="2" t="n"/>
     </row>
     <row r="15" ht="25.5" customHeight="1">
-      <c r="A15" s="22" t="n"/>
-      <c r="B15" s="38" t="inlineStr">
+      <c r="A15" s="30" t="n"/>
+      <c r="B15" s="46" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
         </is>
       </c>
-      <c r="C15" s="39" t="n"/>
-      <c r="D15" s="39" t="n"/>
-      <c r="E15" s="39" t="n"/>
-      <c r="F15" s="35" t="n"/>
+      <c r="C15" s="47" t="n"/>
+      <c r="D15" s="47" t="n"/>
+      <c r="E15" s="47" t="n"/>
+      <c r="F15" s="43" t="n"/>
       <c r="G15" s="2" t="n"/>
       <c r="H15" s="2" t="n"/>
       <c r="I15" s="2" t="n"/>
@@ -1426,16 +2053,16 @@
       <c r="O15" s="2" t="n"/>
     </row>
     <row r="16" ht="25.5" customHeight="1">
-      <c r="A16" s="22" t="n"/>
-      <c r="B16" s="40" t="inlineStr">
+      <c r="A16" s="30" t="n"/>
+      <c r="B16" s="48" t="inlineStr">
         <is>
           <t>Contact Person : Mr. Thuy   TEl: 0379367084</t>
         </is>
       </c>
-      <c r="C16" s="39" t="n"/>
-      <c r="D16" s="39" t="n"/>
-      <c r="E16" s="39" t="n"/>
-      <c r="F16" s="39" t="n"/>
+      <c r="C16" s="47" t="n"/>
+      <c r="D16" s="47" t="n"/>
+      <c r="E16" s="47" t="n"/>
+      <c r="F16" s="47" t="n"/>
       <c r="G16" s="2" t="n"/>
       <c r="H16" s="2" t="n"/>
       <c r="I16" s="2" t="n"/>
@@ -1447,16 +2074,16 @@
       <c r="O16" s="2" t="n"/>
     </row>
     <row r="17" ht="25.5" customHeight="1">
-      <c r="A17" s="22" t="n"/>
-      <c r="B17" s="40" t="inlineStr">
+      <c r="A17" s="30" t="n"/>
+      <c r="B17" s="48" t="inlineStr">
         <is>
           <t xml:space="preserve">EMAlL:jyangbin4720@dingtalk.com jialy@kukahome.com </t>
         </is>
       </c>
-      <c r="C17" s="39" t="n"/>
-      <c r="D17" s="39" t="n"/>
-      <c r="E17" s="39" t="n"/>
-      <c r="F17" s="35" t="n"/>
+      <c r="C17" s="47" t="n"/>
+      <c r="D17" s="47" t="n"/>
+      <c r="E17" s="47" t="n"/>
+      <c r="F17" s="43" t="n"/>
       <c r="G17" s="2" t="n"/>
       <c r="H17" s="2" t="n"/>
       <c r="I17" s="2" t="n"/>
@@ -1468,16 +2095,16 @@
       <c r="O17" s="2" t="n"/>
     </row>
     <row r="18" ht="25.5" customHeight="1">
-      <c r="A18" s="22" t="n"/>
-      <c r="B18" s="40" t="inlineStr">
+      <c r="A18" s="30" t="n"/>
+      <c r="B18" s="48" t="inlineStr">
         <is>
           <t>dailin@kukahome.com huanggf@kukahome.com zhangzp@kukahome.com</t>
         </is>
       </c>
-      <c r="C18" s="22" t="n"/>
-      <c r="D18" s="22" t="n"/>
-      <c r="E18" s="22" t="n"/>
-      <c r="F18" s="16" t="n"/>
+      <c r="C18" s="30" t="n"/>
+      <c r="D18" s="30" t="n"/>
+      <c r="E18" s="30" t="n"/>
+      <c r="F18" s="24" t="n"/>
       <c r="G18" s="2" t="n"/>
       <c r="H18" s="2" t="n"/>
       <c r="I18" s="2" t="n"/>
@@ -1489,12 +2116,12 @@
       <c r="O18" s="2" t="n"/>
     </row>
     <row r="19" ht="27.75" customHeight="1">
-      <c r="A19" s="41" t="inlineStr">
+      <c r="A19" s="49" t="inlineStr">
         <is>
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B19" s="22" t="inlineStr">
+      <c r="B19" s="30" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
         </is>
@@ -1502,7 +2129,7 @@
       <c r="C19" s="2" t="n"/>
       <c r="D19" s="2" t="n"/>
       <c r="E19" s="2" t="n"/>
-      <c r="F19" s="42" t="n"/>
+      <c r="F19" s="50" t="n"/>
       <c r="G19" s="2" t="n"/>
       <c r="H19" s="2" t="n"/>
       <c r="I19" s="2" t="n"/>
@@ -1514,8 +2141,8 @@
       <c r="O19" s="2" t="n"/>
     </row>
     <row r="20" ht="27.75" customHeight="1">
-      <c r="A20" s="43" t="n"/>
-      <c r="B20" s="43" t="n"/>
+      <c r="A20" s="51" t="n"/>
+      <c r="B20" s="51" t="n"/>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
@@ -1530,32 +2157,626 @@
       <c r="N20" s="2" t="n"/>
       <c r="O20" s="2" t="n"/>
     </row>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
+    <row r="21">
+      <c r="A21" s="52" t="inlineStr">
+        <is>
+          <t>Mark &amp; Nº</t>
+        </is>
+      </c>
+      <c r="B21" s="52" t="inlineStr">
+        <is>
+          <t>P.O. Nº</t>
+        </is>
+      </c>
+      <c r="C21" s="52" t="inlineStr">
+        <is>
+          <t>ITEM Nº</t>
+        </is>
+      </c>
+      <c r="D21" s="52" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E21" s="52" t="inlineStr">
+        <is>
+          <t>Quantity(SF)</t>
+        </is>
+      </c>
+      <c r="F21" s="52" t="inlineStr">
+        <is>
+          <t>Unit price (USD)</t>
+        </is>
+      </c>
+      <c r="G21" s="52" t="inlineStr">
+        <is>
+          <t>Amount (USD)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>VENDOR#:</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>9000675121</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>01.10.W653191</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>6461.7</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G22">
+        <f>F22*E22</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Des: LEATHER</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>9000675121</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>01.10.W653191</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>77.90000000000001</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="G23">
+        <f>F23*E23</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>9000678762</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>01.10.U756071</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>20949.5</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G24">
+        <f>F24*E24</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>9000678762</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>01.10.U756071</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>241.9</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="G25">
+        <f>F25*E25</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="n">
+        <v>9000697761</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>28156.8</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="G26">
+        <f>F26*E26</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n">
+        <v>9000697761</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>711.1</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="G27">
+        <f>F27*E27</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>1301.4</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="G28">
+        <f>F28*E28</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>18717.9</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="G29">
+        <f>F29*E29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>106711.7</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G30">
+        <f>F30*E30</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>1320.6</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="G31">
+        <f>F31*E31</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>367.3</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="G32">
+        <f>F32*E32</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>101424.8</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G33">
+        <f>F33*E33</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>1205.1</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="G34">
+        <f>F34*E34</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>9000678672</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>01.10.L2924</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>5345</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G35">
+        <f>F35*E35</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>9000678672</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>01.10.L2924</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>121</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="G36">
+        <f>F36*E36</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" ht="35" customHeight="1">
+      <c r="A37" s="53" t="n"/>
+      <c r="B37" s="16" t="n"/>
+      <c r="C37" s="16" t="n"/>
+      <c r="D37" s="53" t="n"/>
+      <c r="E37" s="16" t="n"/>
+      <c r="F37" s="16" t="n"/>
+      <c r="G37" s="16" t="n"/>
+    </row>
+    <row r="38" ht="61.5" customHeight="1">
+      <c r="A38" s="54" t="inlineStr">
+        <is>
+          <t>Manufacture:</t>
+        </is>
+      </c>
+      <c r="B38" s="55" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
+XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="D38" s="55" t="n"/>
+      <c r="E38" s="55" t="n"/>
+      <c r="F38" s="30" t="n"/>
+      <c r="G38" s="24" t="n"/>
+      <c r="H38" s="2" t="n"/>
+      <c r="I38" s="2" t="n"/>
+      <c r="J38" s="2" t="n"/>
+      <c r="K38" s="2" t="n"/>
+      <c r="L38" s="56" t="n"/>
+      <c r="M38" s="57" t="n"/>
+      <c r="N38" s="58" t="n"/>
+      <c r="O38" s="58" t="n"/>
+    </row>
+    <row r="39" ht="42" customHeight="1">
+      <c r="A39" s="59" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="D39" s="59" t="n"/>
+      <c r="E39" s="59" t="n"/>
+      <c r="F39" s="59" t="n"/>
+      <c r="G39" s="24" t="n"/>
+      <c r="H39" s="2" t="n"/>
+      <c r="I39" s="2" t="n"/>
+      <c r="J39" s="2" t="n"/>
+      <c r="K39" s="2" t="n"/>
+      <c r="L39" s="56" t="n"/>
+      <c r="M39" s="57" t="n"/>
+      <c r="N39" s="58" t="n"/>
+      <c r="O39" s="58" t="n"/>
+    </row>
+    <row r="40" ht="24.75" customHeight="1">
+      <c r="A40" s="60" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+      <c r="H40" s="2" t="n"/>
+      <c r="I40" s="2" t="n"/>
+      <c r="J40" s="2" t="n"/>
+      <c r="K40" s="2" t="n"/>
+      <c r="L40" s="56" t="n"/>
+      <c r="M40" s="57" t="n"/>
+      <c r="N40" s="58" t="n"/>
+      <c r="O40" s="58" t="n"/>
+    </row>
+    <row r="41" ht="27" customHeight="1">
+      <c r="A41" s="60" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="H41" s="2" t="n"/>
+      <c r="I41" s="2" t="n"/>
+      <c r="J41" s="2" t="n"/>
+      <c r="K41" s="2" t="n"/>
+      <c r="L41" s="56" t="n"/>
+      <c r="M41" s="57" t="n"/>
+      <c r="N41" s="58" t="n"/>
+      <c r="O41" s="58" t="n"/>
+    </row>
+    <row r="42" ht="61.5" customHeight="1">
+      <c r="A42" s="2" t="n"/>
+      <c r="B42" s="2" t="n"/>
+      <c r="C42" s="2" t="n"/>
+      <c r="D42" s="2" t="n"/>
+      <c r="E42" s="61" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="F42" s="61" t="n"/>
+      <c r="G42" s="61" t="n"/>
+      <c r="H42" s="61" t="n"/>
+      <c r="I42" s="2" t="n"/>
+      <c r="J42" s="2" t="n"/>
+      <c r="K42" s="2" t="n"/>
+      <c r="L42" s="56" t="n"/>
+      <c r="M42" s="57" t="n"/>
+      <c r="N42" s="58" t="n"/>
+      <c r="O42" s="58" t="n"/>
+    </row>
+    <row r="43" ht="42" customHeight="1">
+      <c r="A43" s="2" t="n"/>
+      <c r="B43" s="2" t="n"/>
+      <c r="C43" s="2" t="n"/>
+      <c r="D43" s="62" t="n"/>
+      <c r="E43" s="63" t="n"/>
+      <c r="F43" s="64" t="inlineStr">
+        <is>
+          <t>Sign &amp; Stamp</t>
+        </is>
+      </c>
+      <c r="G43" s="65" t="n"/>
+      <c r="H43" s="2" t="n"/>
+      <c r="I43" s="2" t="n"/>
+      <c r="J43" s="2" t="n"/>
+      <c r="K43" s="2" t="n"/>
+      <c r="L43" s="56" t="n"/>
+      <c r="M43" s="57" t="n"/>
+      <c r="N43" s="58" t="n"/>
+      <c r="O43" s="58" t="n"/>
+    </row>
+    <row r="44" ht="24.75" customHeight="1">
+      <c r="A44" s="2" t="n"/>
+      <c r="B44" s="2" t="n"/>
+      <c r="C44" s="2" t="n"/>
+      <c r="D44" s="62" t="n"/>
+      <c r="E44" s="63" t="n"/>
+      <c r="F44" s="63" t="n"/>
+      <c r="G44" s="65" t="n"/>
+      <c r="H44" s="2" t="n"/>
+      <c r="I44" s="2" t="n"/>
+      <c r="J44" s="2" t="n"/>
+      <c r="K44" s="2" t="n"/>
+      <c r="L44" s="56" t="n"/>
+      <c r="M44" s="57" t="n"/>
+      <c r="N44" s="58" t="n"/>
+      <c r="O44" s="58" t="n"/>
+    </row>
+    <row r="45" ht="27" customHeight="1">
+      <c r="A45" s="2" t="n"/>
+      <c r="B45" s="2" t="n"/>
+      <c r="C45" s="2" t="n"/>
+      <c r="D45" s="62" t="n"/>
+      <c r="E45" s="63" t="n"/>
+      <c r="F45" s="63" t="n"/>
+      <c r="G45" s="65" t="n"/>
+      <c r="H45" s="2" t="n"/>
+      <c r="I45" s="2" t="n"/>
+      <c r="J45" s="2" t="n"/>
+      <c r="K45" s="2" t="n"/>
+      <c r="L45" s="56" t="n"/>
+      <c r="M45" s="57" t="n"/>
+      <c r="N45" s="58" t="n"/>
+      <c r="O45" s="58" t="n"/>
+    </row>
+    <row r="46" ht="21" customHeight="1">
+      <c r="A46" s="2" t="n"/>
+      <c r="B46" s="2" t="n"/>
+      <c r="C46" s="2" t="n"/>
+      <c r="D46" s="62" t="n"/>
+      <c r="E46" s="63" t="n"/>
+      <c r="F46" s="66" t="inlineStr">
+        <is>
+          <t>ZENG XUELI</t>
+        </is>
+      </c>
+      <c r="G46" s="66" t="n"/>
+      <c r="H46" s="2" t="n"/>
+      <c r="I46" s="2" t="n"/>
+      <c r="J46" s="2" t="n"/>
+      <c r="K46" s="2" t="n"/>
+      <c r="L46" s="56" t="n"/>
+      <c r="M46" s="57" t="n"/>
+      <c r="N46" s="58" t="n"/>
+      <c r="O46" s="58" t="n"/>
+    </row>
     <row r="47"/>
     <row r="48"/>
     <row r="49"/>
@@ -1711,12 +2932,16 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A40:G40"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A41:G41"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1729,7 +2954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P200"/>
+  <dimension ref="A1:T200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1746,92 +2971,180 @@
     <col width="13.6640625" customWidth="1" min="7" max="7"/>
     <col width="15.5546875" customWidth="1" min="8" max="8"/>
     <col width="23.6640625" customWidth="1" min="9" max="9"/>
+    <col width="12.44140625" customWidth="1" min="10" max="10"/>
+    <col width="12.88671875" customWidth="1" min="11" max="11"/>
+    <col width="12.5546875" customWidth="1" min="12" max="12"/>
+    <col width="13" customWidth="1" min="13" max="13"/>
+    <col width="12.5546875" customWidth="1" min="14" max="14"/>
+    <col width="13" customWidth="1" min="15" max="15"/>
+    <col width="12.5546875" customWidth="1" min="16" max="16"/>
+    <col width="13" customWidth="1" min="17" max="17"/>
+    <col width="13" customWidth="1" min="18" max="18"/>
+    <col width="13" customWidth="1" min="19" max="19"/>
+    <col width="13" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1" ht="38.25" customHeight="1">
-      <c r="A1" s="15" t="inlineStr">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
     </row>
     <row r="2" ht="24" customHeight="1">
-      <c r="A2" s="16" t="inlineStr">
+      <c r="A2" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
         </is>
       </c>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="2" t="n"/>
+      <c r="P2" s="2" t="n"/>
+      <c r="Q2" s="2" t="n"/>
+      <c r="R2" s="2" t="n"/>
+      <c r="S2" s="2" t="n"/>
+      <c r="T2" s="2" t="n"/>
     </row>
     <row r="3" ht="25.5" customHeight="1">
-      <c r="A3" s="17" t="inlineStr">
+      <c r="A3" s="25" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
       </c>
+      <c r="J3" s="2" t="n"/>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="n"/>
+      <c r="O3" s="2" t="n"/>
+      <c r="P3" s="2" t="n"/>
+      <c r="Q3" s="2" t="n"/>
+      <c r="R3" s="2" t="n"/>
+      <c r="S3" s="2" t="n"/>
+      <c r="T3" s="2" t="n"/>
     </row>
     <row r="4" ht="25.5" customHeight="1">
-      <c r="A4" s="16" t="inlineStr">
+      <c r="A4" s="24" t="inlineStr">
         <is>
           <t>VAT:L001-901903209</t>
         </is>
       </c>
+      <c r="J4" s="2" t="n"/>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+      <c r="M4" s="2" t="n"/>
+      <c r="N4" s="2" t="n"/>
+      <c r="O4" s="2" t="n"/>
+      <c r="P4" s="2" t="n"/>
+      <c r="Q4" s="2" t="n"/>
+      <c r="R4" s="2" t="n"/>
+      <c r="S4" s="2" t="n"/>
+      <c r="T4" s="2" t="n"/>
     </row>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="18" t="inlineStr">
+      <c r="A5" s="26" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="B5" s="19" t="n"/>
-      <c r="C5" s="19" t="n"/>
-      <c r="D5" s="19" t="n"/>
-      <c r="E5" s="19" t="n"/>
-      <c r="F5" s="19" t="n"/>
-      <c r="G5" s="19" t="n"/>
-      <c r="H5" s="19" t="n"/>
-      <c r="I5" s="19" t="n"/>
+      <c r="B5" s="27" t="n"/>
+      <c r="C5" s="27" t="n"/>
+      <c r="D5" s="27" t="n"/>
+      <c r="E5" s="27" t="n"/>
+      <c r="F5" s="27" t="n"/>
+      <c r="G5" s="27" t="n"/>
+      <c r="H5" s="27" t="n"/>
+      <c r="I5" s="27" t="n"/>
+      <c r="J5" s="2" t="n"/>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+      <c r="M5" s="2" t="n"/>
+      <c r="N5" s="2" t="n"/>
+      <c r="O5" s="2" t="n"/>
+      <c r="P5" s="2" t="n"/>
+      <c r="Q5" s="2" t="n"/>
+      <c r="R5" s="2" t="n"/>
+      <c r="S5" s="2" t="n"/>
+      <c r="T5" s="2" t="n"/>
     </row>
     <row r="6" ht="54" customHeight="1">
-      <c r="A6" s="20" t="inlineStr">
+      <c r="A6" s="28" t="inlineStr">
         <is>
           <t>PACKING LIST</t>
         </is>
       </c>
-      <c r="B6" s="21" t="n"/>
-      <c r="C6" s="21" t="n"/>
-      <c r="D6" s="21" t="n"/>
-      <c r="E6" s="21" t="n"/>
-      <c r="F6" s="21" t="n"/>
-      <c r="G6" s="21" t="n"/>
-      <c r="H6" s="21" t="n"/>
-      <c r="I6" s="21" t="n"/>
+      <c r="B6" s="29" t="n"/>
+      <c r="C6" s="29" t="n"/>
+      <c r="D6" s="29" t="n"/>
+      <c r="E6" s="29" t="n"/>
+      <c r="F6" s="29" t="n"/>
+      <c r="G6" s="29" t="n"/>
+      <c r="H6" s="29" t="n"/>
+      <c r="I6" s="29" t="n"/>
+      <c r="J6" s="2" t="n"/>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
+      <c r="N6" s="2" t="n"/>
+      <c r="O6" s="2" t="n"/>
+      <c r="P6" s="2" t="n"/>
+      <c r="Q6" s="2" t="n"/>
+      <c r="R6" s="2" t="n"/>
+      <c r="S6" s="2" t="n"/>
+      <c r="T6" s="2" t="n"/>
     </row>
     <row r="7" ht="18" customHeight="1">
-      <c r="A7" s="22" t="n"/>
-      <c r="B7" s="44" t="n"/>
-      <c r="C7" s="22" t="n"/>
-      <c r="D7" s="22" t="n"/>
-      <c r="E7" s="16" t="n"/>
-      <c r="F7" s="16" t="n"/>
-      <c r="G7" s="16" t="n"/>
-      <c r="H7" s="23" t="inlineStr">
+      <c r="A7" s="30" t="n"/>
+      <c r="B7" s="67" t="n"/>
+      <c r="C7" s="30" t="n"/>
+      <c r="D7" s="30" t="n"/>
+      <c r="E7" s="24" t="n"/>
+      <c r="F7" s="24" t="n"/>
+      <c r="G7" s="24" t="n"/>
+      <c r="H7" s="31" t="inlineStr">
         <is>
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="I7" s="45" t="inlineStr">
+      <c r="I7" s="68" t="inlineStr">
         <is>
           <t>JFREF</t>
         </is>
       </c>
+      <c r="J7" s="2" t="n"/>
+      <c r="K7" s="2" t="n"/>
+      <c r="L7" s="2" t="n"/>
+      <c r="M7" s="2" t="n"/>
+      <c r="N7" s="2" t="n"/>
+      <c r="O7" s="2" t="n"/>
+      <c r="P7" s="2" t="n"/>
+      <c r="Q7" s="2" t="n"/>
+      <c r="R7" s="2" t="n"/>
+      <c r="S7" s="2" t="n"/>
+      <c r="T7" s="2" t="n"/>
     </row>
     <row r="8" ht="30" customHeight="1">
-      <c r="A8" s="25" t="inlineStr">
+      <c r="A8" s="33" t="inlineStr">
         <is>
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="46" t="inlineStr">
+      <c r="B8" s="69" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
@@ -1839,22 +3152,33 @@
       <c r="C8" s="2" t="n"/>
       <c r="D8" s="2" t="n"/>
       <c r="E8" s="2" t="n"/>
-      <c r="F8" s="27" t="n"/>
-      <c r="G8" s="27" t="n"/>
-      <c r="H8" s="27" t="inlineStr">
+      <c r="F8" s="35" t="n"/>
+      <c r="G8" s="35" t="n"/>
+      <c r="H8" s="35" t="inlineStr">
         <is>
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="I8" s="47" t="inlineStr">
+      <c r="I8" s="70" t="inlineStr">
         <is>
           <t>JFINV</t>
         </is>
       </c>
+      <c r="J8" s="2" t="n"/>
+      <c r="K8" s="2" t="n"/>
+      <c r="L8" s="2" t="n"/>
+      <c r="M8" s="2" t="n"/>
+      <c r="N8" s="2" t="n"/>
+      <c r="O8" s="2" t="n"/>
+      <c r="P8" s="2" t="n"/>
+      <c r="Q8" s="2" t="n"/>
+      <c r="R8" s="2" t="n"/>
+      <c r="S8" s="2" t="n"/>
+      <c r="T8" s="2" t="n"/>
     </row>
     <row r="9" ht="21" customHeight="1">
-      <c r="A9" s="22" t="n"/>
-      <c r="B9" s="44" t="inlineStr">
+      <c r="A9" s="30" t="n"/>
+      <c r="B9" s="67" t="inlineStr">
         <is>
           <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages,</t>
         </is>
@@ -1862,22 +3186,33 @@
       <c r="C9" s="2" t="n"/>
       <c r="D9" s="2" t="n"/>
       <c r="E9" s="2" t="n"/>
-      <c r="F9" s="16" t="n"/>
-      <c r="G9" s="16" t="n"/>
-      <c r="H9" s="27" t="inlineStr">
+      <c r="F9" s="24" t="n"/>
+      <c r="G9" s="24" t="n"/>
+      <c r="H9" s="35" t="inlineStr">
         <is>
           <t>Date:</t>
         </is>
       </c>
-      <c r="I9" s="29" t="inlineStr">
+      <c r="I9" s="37" t="inlineStr">
         <is>
           <t>JFTIME</t>
         </is>
       </c>
+      <c r="J9" s="2" t="n"/>
+      <c r="K9" s="2" t="n"/>
+      <c r="L9" s="2" t="n"/>
+      <c r="M9" s="2" t="n"/>
+      <c r="N9" s="2" t="n"/>
+      <c r="O9" s="2" t="n"/>
+      <c r="P9" s="2" t="n"/>
+      <c r="Q9" s="2" t="n"/>
+      <c r="R9" s="2" t="n"/>
+      <c r="S9" s="2" t="n"/>
+      <c r="T9" s="2" t="n"/>
     </row>
     <row r="10" ht="22.5" customHeight="1">
-      <c r="A10" s="22" t="n"/>
-      <c r="B10" s="44" t="inlineStr">
+      <c r="A10" s="30" t="n"/>
+      <c r="B10" s="67" t="inlineStr">
         <is>
           <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
         </is>
@@ -1885,22 +3220,33 @@
       <c r="C10" s="2" t="n"/>
       <c r="D10" s="2" t="n"/>
       <c r="E10" s="2" t="n"/>
-      <c r="F10" s="16" t="n"/>
-      <c r="G10" s="16" t="n"/>
-      <c r="H10" s="30" t="inlineStr">
+      <c r="F10" s="24" t="n"/>
+      <c r="G10" s="24" t="n"/>
+      <c r="H10" s="38" t="inlineStr">
         <is>
           <t>FCA :</t>
         </is>
       </c>
-      <c r="I10" s="48" t="inlineStr">
+      <c r="I10" s="71" t="inlineStr">
         <is>
           <t>BAVET, SVAY RIENG</t>
         </is>
       </c>
+      <c r="J10" s="2" t="n"/>
+      <c r="K10" s="2" t="n"/>
+      <c r="L10" s="2" t="n"/>
+      <c r="M10" s="2" t="n"/>
+      <c r="N10" s="2" t="n"/>
+      <c r="O10" s="2" t="n"/>
+      <c r="P10" s="2" t="n"/>
+      <c r="Q10" s="2" t="n"/>
+      <c r="R10" s="2" t="n"/>
+      <c r="S10" s="2" t="n"/>
+      <c r="T10" s="2" t="n"/>
     </row>
     <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="22" t="n"/>
-      <c r="B11" s="44" t="inlineStr">
+      <c r="A11" s="30" t="n"/>
+      <c r="B11" s="67" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
@@ -1908,29 +3254,51 @@
       <c r="C11" s="2" t="n"/>
       <c r="D11" s="2" t="n"/>
       <c r="E11" s="2" t="n"/>
-      <c r="F11" s="16" t="n"/>
-      <c r="G11" s="16" t="n"/>
-      <c r="H11" s="16" t="n"/>
-      <c r="I11" s="16" t="n"/>
+      <c r="F11" s="24" t="n"/>
+      <c r="G11" s="24" t="n"/>
+      <c r="H11" s="24" t="n"/>
+      <c r="I11" s="24" t="n"/>
+      <c r="J11" s="2" t="n"/>
+      <c r="K11" s="2" t="n"/>
+      <c r="L11" s="2" t="n"/>
+      <c r="M11" s="2" t="n"/>
+      <c r="N11" s="2" t="n"/>
+      <c r="O11" s="2" t="n"/>
+      <c r="P11" s="2" t="n"/>
+      <c r="Q11" s="2" t="n"/>
+      <c r="R11" s="2" t="n"/>
+      <c r="S11" s="2" t="n"/>
+      <c r="T11" s="2" t="n"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="22" t="n"/>
-      <c r="B12" s="44" t="n"/>
-      <c r="C12" s="22" t="n"/>
-      <c r="D12" s="22" t="n"/>
-      <c r="E12" s="16" t="n"/>
-      <c r="F12" s="16" t="n"/>
-      <c r="G12" s="16" t="n"/>
-      <c r="H12" s="16" t="n"/>
-      <c r="I12" s="16" t="n"/>
+      <c r="A12" s="30" t="n"/>
+      <c r="B12" s="67" t="n"/>
+      <c r="C12" s="30" t="n"/>
+      <c r="D12" s="30" t="n"/>
+      <c r="E12" s="24" t="n"/>
+      <c r="F12" s="24" t="n"/>
+      <c r="G12" s="24" t="n"/>
+      <c r="H12" s="24" t="n"/>
+      <c r="I12" s="24" t="n"/>
+      <c r="J12" s="2" t="n"/>
+      <c r="K12" s="2" t="n"/>
+      <c r="L12" s="2" t="n"/>
+      <c r="M12" s="2" t="n"/>
+      <c r="N12" s="2" t="n"/>
+      <c r="O12" s="2" t="n"/>
+      <c r="P12" s="2" t="n"/>
+      <c r="Q12" s="2" t="n"/>
+      <c r="R12" s="2" t="n"/>
+      <c r="S12" s="2" t="n"/>
+      <c r="T12" s="2" t="n"/>
     </row>
     <row r="13" ht="25.5" customHeight="1">
-      <c r="A13" s="32" t="inlineStr">
+      <c r="A13" s="40" t="inlineStr">
         <is>
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="49" t="inlineStr">
+      <c r="B13" s="72" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
@@ -1938,93 +3306,159 @@
       <c r="C13" s="2" t="n"/>
       <c r="D13" s="2" t="n"/>
       <c r="E13" s="2" t="n"/>
-      <c r="F13" s="50" t="n"/>
-      <c r="G13" s="50" t="n"/>
-      <c r="H13" s="50" t="n"/>
-      <c r="I13" s="35" t="n"/>
+      <c r="F13" s="73" t="n"/>
+      <c r="G13" s="73" t="n"/>
+      <c r="H13" s="73" t="n"/>
+      <c r="I13" s="43" t="n"/>
+      <c r="J13" s="2" t="n"/>
+      <c r="K13" s="2" t="n"/>
+      <c r="L13" s="2" t="n"/>
+      <c r="M13" s="2" t="n"/>
+      <c r="N13" s="2" t="n"/>
+      <c r="O13" s="2" t="n"/>
+      <c r="P13" s="2" t="n"/>
+      <c r="Q13" s="2" t="n"/>
+      <c r="R13" s="2" t="n"/>
+      <c r="S13" s="2" t="n"/>
+      <c r="T13" s="2" t="n"/>
     </row>
     <row r="14" ht="25.5" customHeight="1">
-      <c r="A14" s="22" t="n"/>
-      <c r="B14" s="51" t="inlineStr">
+      <c r="A14" s="30" t="n"/>
+      <c r="B14" s="74" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
-      <c r="C14" s="37" t="n"/>
-      <c r="D14" s="37" t="n"/>
-      <c r="E14" s="52" t="n"/>
-      <c r="F14" s="52" t="n"/>
-      <c r="G14" s="52" t="n"/>
-      <c r="H14" s="52" t="n"/>
+      <c r="C14" s="45" t="n"/>
+      <c r="D14" s="45" t="n"/>
+      <c r="E14" s="75" t="n"/>
+      <c r="F14" s="75" t="n"/>
+      <c r="G14" s="75" t="n"/>
+      <c r="H14" s="75" t="n"/>
       <c r="I14" s="2" t="n"/>
+      <c r="J14" s="2" t="n"/>
+      <c r="K14" s="2" t="n"/>
+      <c r="L14" s="2" t="n"/>
+      <c r="M14" s="2" t="n"/>
+      <c r="N14" s="2" t="n"/>
+      <c r="O14" s="2" t="n"/>
+      <c r="P14" s="2" t="n"/>
+      <c r="Q14" s="2" t="n"/>
+      <c r="R14" s="2" t="n"/>
+      <c r="S14" s="2" t="n"/>
+      <c r="T14" s="2" t="n"/>
     </row>
     <row r="15" ht="21" customHeight="1">
-      <c r="A15" s="22" t="n"/>
-      <c r="B15" s="53" t="inlineStr">
+      <c r="A15" s="30" t="n"/>
+      <c r="B15" s="76" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
         </is>
       </c>
-      <c r="C15" s="39" t="n"/>
-      <c r="D15" s="39" t="n"/>
-      <c r="E15" s="35" t="n"/>
-      <c r="F15" s="35" t="n"/>
-      <c r="G15" s="35" t="n"/>
-      <c r="H15" s="35" t="n"/>
+      <c r="C15" s="47" t="n"/>
+      <c r="D15" s="47" t="n"/>
+      <c r="E15" s="43" t="n"/>
+      <c r="F15" s="43" t="n"/>
+      <c r="G15" s="43" t="n"/>
+      <c r="H15" s="43" t="n"/>
       <c r="I15" s="2" t="n"/>
+      <c r="J15" s="2" t="n"/>
+      <c r="K15" s="2" t="n"/>
+      <c r="L15" s="2" t="n"/>
+      <c r="M15" s="2" t="n"/>
+      <c r="N15" s="2" t="n"/>
+      <c r="O15" s="2" t="n"/>
+      <c r="P15" s="2" t="n"/>
+      <c r="Q15" s="2" t="n"/>
+      <c r="R15" s="2" t="n"/>
+      <c r="S15" s="2" t="n"/>
+      <c r="T15" s="2" t="n"/>
     </row>
     <row r="16" ht="21" customHeight="1">
-      <c r="A16" s="22" t="n"/>
-      <c r="B16" s="38" t="inlineStr">
+      <c r="A16" s="30" t="n"/>
+      <c r="B16" s="46" t="inlineStr">
         <is>
           <t>Contact Person : Mr. Thuy   TEl: 0379367084</t>
         </is>
       </c>
-      <c r="C16" s="39" t="n"/>
-      <c r="D16" s="39" t="n"/>
-      <c r="E16" s="35" t="n"/>
-      <c r="F16" s="35" t="n"/>
-      <c r="G16" s="35" t="n"/>
-      <c r="H16" s="35" t="n"/>
+      <c r="C16" s="47" t="n"/>
+      <c r="D16" s="47" t="n"/>
+      <c r="E16" s="43" t="n"/>
+      <c r="F16" s="43" t="n"/>
+      <c r="G16" s="43" t="n"/>
+      <c r="H16" s="43" t="n"/>
       <c r="I16" s="2" t="n"/>
+      <c r="J16" s="2" t="n"/>
+      <c r="K16" s="2" t="n"/>
+      <c r="L16" s="2" t="n"/>
+      <c r="M16" s="2" t="n"/>
+      <c r="N16" s="2" t="n"/>
+      <c r="O16" s="2" t="n"/>
+      <c r="P16" s="2" t="n"/>
+      <c r="Q16" s="2" t="n"/>
+      <c r="R16" s="2" t="n"/>
+      <c r="S16" s="2" t="n"/>
+      <c r="T16" s="2" t="n"/>
     </row>
     <row r="17" ht="21" customHeight="1">
-      <c r="A17" s="22" t="n"/>
-      <c r="B17" s="38" t="inlineStr">
+      <c r="A17" s="30" t="n"/>
+      <c r="B17" s="46" t="inlineStr">
         <is>
           <t>EMAlL:jyangbin4720@dingtalk.com jialy@kukahome.com</t>
         </is>
       </c>
-      <c r="C17" s="39" t="n"/>
-      <c r="D17" s="39" t="n"/>
-      <c r="E17" s="35" t="n"/>
-      <c r="F17" s="35" t="n"/>
-      <c r="G17" s="35" t="n"/>
-      <c r="H17" s="35" t="n"/>
+      <c r="C17" s="47" t="n"/>
+      <c r="D17" s="47" t="n"/>
+      <c r="E17" s="43" t="n"/>
+      <c r="F17" s="43" t="n"/>
+      <c r="G17" s="43" t="n"/>
+      <c r="H17" s="43" t="n"/>
       <c r="I17" s="2" t="n"/>
+      <c r="J17" s="2" t="n"/>
+      <c r="K17" s="2" t="n"/>
+      <c r="L17" s="2" t="n"/>
+      <c r="M17" s="2" t="n"/>
+      <c r="N17" s="2" t="n"/>
+      <c r="O17" s="2" t="n"/>
+      <c r="P17" s="2" t="n"/>
+      <c r="Q17" s="2" t="n"/>
+      <c r="R17" s="2" t="n"/>
+      <c r="S17" s="2" t="n"/>
+      <c r="T17" s="2" t="n"/>
     </row>
     <row r="18" ht="21" customHeight="1">
-      <c r="A18" s="22" t="n"/>
-      <c r="B18" s="38" t="inlineStr">
+      <c r="A18" s="30" t="n"/>
+      <c r="B18" s="46" t="inlineStr">
         <is>
           <t>dailin@kukahome.com huanggf@kukahome.com zhangzp@kukahome.com</t>
         </is>
       </c>
-      <c r="C18" s="22" t="n"/>
-      <c r="D18" s="22" t="n"/>
-      <c r="E18" s="16" t="n"/>
-      <c r="F18" s="16" t="n"/>
-      <c r="G18" s="16" t="n"/>
-      <c r="H18" s="16" t="n"/>
+      <c r="C18" s="30" t="n"/>
+      <c r="D18" s="30" t="n"/>
+      <c r="E18" s="24" t="n"/>
+      <c r="F18" s="24" t="n"/>
+      <c r="G18" s="24" t="n"/>
+      <c r="H18" s="24" t="n"/>
       <c r="I18" s="2" t="n"/>
+      <c r="J18" s="2" t="n"/>
+      <c r="K18" s="2" t="n"/>
+      <c r="L18" s="2" t="n"/>
+      <c r="M18" s="2" t="n"/>
+      <c r="N18" s="2" t="n"/>
+      <c r="O18" s="2" t="n"/>
+      <c r="P18" s="2" t="n"/>
+      <c r="Q18" s="2" t="n"/>
+      <c r="R18" s="2" t="n"/>
+      <c r="S18" s="2" t="n"/>
+      <c r="T18" s="2" t="n"/>
     </row>
     <row r="19" ht="27.75" customHeight="1">
-      <c r="A19" s="41" t="inlineStr">
+      <c r="A19" s="49" t="inlineStr">
         <is>
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B19" s="44" t="inlineStr">
+      <c r="B19" s="67" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
         </is>
@@ -2036,10 +3470,21 @@
       <c r="G19" s="2" t="n"/>
       <c r="H19" s="2" t="n"/>
       <c r="I19" s="2" t="n"/>
+      <c r="J19" s="2" t="n"/>
+      <c r="K19" s="2" t="n"/>
+      <c r="L19" s="2" t="n"/>
+      <c r="M19" s="2" t="n"/>
+      <c r="N19" s="2" t="n"/>
+      <c r="O19" s="2" t="n"/>
+      <c r="P19" s="2" t="n"/>
+      <c r="Q19" s="2" t="n"/>
+      <c r="R19" s="2" t="n"/>
+      <c r="S19" s="2" t="n"/>
+      <c r="T19" s="2" t="n"/>
     </row>
     <row r="20" ht="27.75" customHeight="1">
-      <c r="A20" s="43" t="n"/>
-      <c r="B20" s="54" t="n"/>
+      <c r="A20" s="51" t="n"/>
+      <c r="B20" s="77" t="n"/>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
@@ -2047,41 +3492,1093 @@
       <c r="G20" s="2" t="n"/>
       <c r="H20" s="2" t="n"/>
       <c r="I20" s="2" t="n"/>
-    </row>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
+      <c r="J20" s="2" t="n"/>
+      <c r="K20" s="2" t="n"/>
+      <c r="L20" s="2" t="n"/>
+      <c r="M20" s="2" t="n"/>
+      <c r="N20" s="2" t="n"/>
+      <c r="O20" s="2" t="n"/>
+      <c r="P20" s="2" t="n"/>
+      <c r="Q20" s="2" t="n"/>
+      <c r="R20" s="2" t="n"/>
+      <c r="S20" s="2" t="n"/>
+      <c r="T20" s="2" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="52" t="inlineStr">
+        <is>
+          <t>Mark &amp; Nº</t>
+        </is>
+      </c>
+      <c r="B21" s="52" t="inlineStr">
+        <is>
+          <t>P.O Nº</t>
+        </is>
+      </c>
+      <c r="C21" s="52" t="inlineStr">
+        <is>
+          <t>ITEM Nº</t>
+        </is>
+      </c>
+      <c r="D21" s="52" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E21" s="52" t="inlineStr">
+        <is>
+          <t>Quantity(SF)</t>
+        </is>
+      </c>
+      <c r="F21" s="78" t="n"/>
+      <c r="G21" s="52" t="inlineStr">
+        <is>
+          <t>N.W (kgs)</t>
+        </is>
+      </c>
+      <c r="H21" s="52" t="inlineStr">
+        <is>
+          <t>G.W (kgs)</t>
+        </is>
+      </c>
+      <c r="I21" s="52" t="inlineStr">
+        <is>
+          <t>CBM</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="79" t="n"/>
+      <c r="B22" s="79" t="n"/>
+      <c r="C22" s="79" t="n"/>
+      <c r="D22" s="79" t="n"/>
+      <c r="E22" s="52" t="inlineStr">
+        <is>
+          <t>PCS</t>
+        </is>
+      </c>
+      <c r="F22" s="52" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="G22" s="79" t="n"/>
+      <c r="H22" s="79" t="n"/>
+      <c r="I22" s="79" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>VENDOR#:</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>195</v>
+      </c>
+      <c r="F23" t="n">
+        <v>10187.1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>842.5</v>
+      </c>
+      <c r="H23" t="n">
+        <v>887.5</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2.6532</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Des: LEATHER</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>195</v>
+      </c>
+      <c r="F24" t="n">
+        <v>10219.2</v>
+      </c>
+      <c r="G24" t="n">
+        <v>846</v>
+      </c>
+      <c r="H24" t="n">
+        <v>891</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2.4948</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Case Qty:</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>207</v>
+      </c>
+      <c r="F25" t="n">
+        <v>10773.3</v>
+      </c>
+      <c r="G25" t="n">
+        <v>883.7671</v>
+      </c>
+      <c r="H25" t="n">
+        <v>926.3013999999999</v>
+      </c>
+      <c r="I25" t="n">
+        <v>2.8447</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>12</v>
+      </c>
+      <c r="F26" t="n">
+        <v>479.1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>51.2329</v>
+      </c>
+      <c r="H26" t="n">
+        <v>53.6986</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.1649</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>195</v>
+      </c>
+      <c r="F27" t="n">
+        <v>10215.8</v>
+      </c>
+      <c r="G27" t="n">
+        <v>840</v>
+      </c>
+      <c r="H27" t="n">
+        <v>885</v>
+      </c>
+      <c r="I27" t="n">
+        <v>2.6136</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>195</v>
+      </c>
+      <c r="F28" t="n">
+        <v>10237.5</v>
+      </c>
+      <c r="G28" t="n">
+        <v>863.5</v>
+      </c>
+      <c r="H28" t="n">
+        <v>908.5</v>
+      </c>
+      <c r="I28" t="n">
+        <v>2.6928</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>195</v>
+      </c>
+      <c r="F29" t="n">
+        <v>10196.1</v>
+      </c>
+      <c r="G29" t="n">
+        <v>849</v>
+      </c>
+      <c r="H29" t="n">
+        <v>894</v>
+      </c>
+      <c r="I29" t="n">
+        <v>2.6136</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>175</v>
+      </c>
+      <c r="F30" t="n">
+        <v>9097.6</v>
+      </c>
+      <c r="G30" t="n">
+        <v>739.443</v>
+      </c>
+      <c r="H30" t="n">
+        <v>780.2461</v>
+      </c>
+      <c r="I30" t="n">
+        <v>2.3339</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>18</v>
+      </c>
+      <c r="F31" t="n">
+        <v>726</v>
+      </c>
+      <c r="G31" t="n">
+        <v>76.057</v>
+      </c>
+      <c r="H31" t="n">
+        <v>80.2539</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.2401</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>195</v>
+      </c>
+      <c r="F32" t="n">
+        <v>10110.4</v>
+      </c>
+      <c r="G32" t="n">
+        <v>840</v>
+      </c>
+      <c r="H32" t="n">
+        <v>885</v>
+      </c>
+      <c r="I32" t="n">
+        <v>2.574</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>195</v>
+      </c>
+      <c r="F33" t="n">
+        <v>10165.7</v>
+      </c>
+      <c r="G33" t="n">
+        <v>844.5</v>
+      </c>
+      <c r="H33" t="n">
+        <v>889.5</v>
+      </c>
+      <c r="I33" t="n">
+        <v>2.772</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>195</v>
+      </c>
+      <c r="F34" t="n">
+        <v>10222.1</v>
+      </c>
+      <c r="G34" t="n">
+        <v>843</v>
+      </c>
+      <c r="H34" t="n">
+        <v>888</v>
+      </c>
+      <c r="I34" t="n">
+        <v>2.6136</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>9000678672</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>01.10.L2924</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>106</v>
+      </c>
+      <c r="F35" t="n">
+        <v>5345</v>
+      </c>
+      <c r="G35" t="n">
+        <v>381.211</v>
+      </c>
+      <c r="H35" t="n">
+        <v>424.9725</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2.0795</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>9000678672</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>01.10.L2924</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>3</v>
+      </c>
+      <c r="F36" t="n">
+        <v>121</v>
+      </c>
+      <c r="G36" t="n">
+        <v>10.789</v>
+      </c>
+      <c r="H36" t="n">
+        <v>12.0275</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.0589</v>
+      </c>
+    </row>
+    <row r="37" ht="27" customHeight="1">
+      <c r="B37" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>215</v>
+      </c>
+      <c r="F37" t="n">
+        <v>11117</v>
+      </c>
+      <c r="G37" t="n">
+        <v>901.5</v>
+      </c>
+      <c r="H37" t="n">
+        <v>946.5</v>
+      </c>
+      <c r="I37" t="n">
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="38" ht="27" customHeight="1">
+      <c r="A38" s="80" t="n"/>
+      <c r="B38" s="16" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C38" s="16" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D38" s="16" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E38" s="16" t="n">
+        <v>215</v>
+      </c>
+      <c r="F38" s="16" t="n">
+        <v>11227</v>
+      </c>
+      <c r="G38" s="16" t="n">
+        <v>918</v>
+      </c>
+      <c r="H38" s="16" t="n">
+        <v>963</v>
+      </c>
+      <c r="I38" s="16" t="n">
+        <v>2.6136</v>
+      </c>
+    </row>
+    <row r="39" ht="27" customHeight="1">
+      <c r="A39" s="80" t="n"/>
+      <c r="B39" s="16" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C39" s="16" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D39" s="16" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E39" s="16" t="n">
+        <v>192</v>
+      </c>
+      <c r="F39" s="16" t="n">
+        <v>9879.4</v>
+      </c>
+      <c r="G39" s="16" t="n">
+        <v>795.0291</v>
+      </c>
+      <c r="H39" s="16" t="n">
+        <v>836.9709</v>
+      </c>
+      <c r="I39" s="16" t="n">
+        <v>2.4729</v>
+      </c>
+    </row>
+    <row r="40" ht="27" customHeight="1">
+      <c r="A40" s="81" t="inlineStr">
+        <is>
+          <t>Country of Original Cambodia</t>
+        </is>
+      </c>
+      <c r="B40" s="81" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C40" s="81" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D40" s="82" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E40" s="83" t="n">
+        <v>14</v>
+      </c>
+      <c r="F40" s="24" t="n">
+        <v>561</v>
+      </c>
+      <c r="G40" s="24" t="n">
+        <v>57.9709</v>
+      </c>
+      <c r="H40" s="24" t="n">
+        <v>61.0291</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>0.1803</v>
+      </c>
+      <c r="J40" s="2" t="n"/>
+      <c r="K40" s="2" t="n"/>
+      <c r="L40" s="2" t="n"/>
+      <c r="M40" s="2" t="n"/>
+      <c r="N40" s="2" t="n"/>
+      <c r="O40" s="2" t="n"/>
+      <c r="P40" s="2" t="n"/>
+      <c r="Q40" s="2" t="n"/>
+      <c r="R40" s="2" t="n"/>
+      <c r="S40" s="2" t="n"/>
+      <c r="T40" s="2" t="n"/>
+    </row>
+    <row r="41" ht="65.25" customHeight="1">
+      <c r="A41" s="54" t="inlineStr">
+        <is>
+          <t>Manufacture:</t>
+        </is>
+      </c>
+      <c r="B41" s="84" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
+XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="E41" s="85" t="n">
+        <v>97</v>
+      </c>
+      <c r="F41" s="85" t="n">
+        <v>5016.1</v>
+      </c>
+      <c r="G41" s="85" t="n">
+        <v>408</v>
+      </c>
+      <c r="H41" s="24" t="n">
+        <v>453</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>1.782</v>
+      </c>
+      <c r="J41" s="2" t="n"/>
+      <c r="K41" s="2" t="n"/>
+      <c r="L41" s="2" t="n"/>
+      <c r="M41" s="2" t="n"/>
+      <c r="N41" s="2" t="n"/>
+      <c r="O41" s="2" t="n"/>
+      <c r="P41" s="2" t="n"/>
+      <c r="Q41" s="2" t="n"/>
+      <c r="R41" s="2" t="n"/>
+      <c r="S41" s="2" t="n"/>
+      <c r="T41" s="2" t="n"/>
+    </row>
+    <row r="42" ht="51.75" customHeight="1">
+      <c r="A42" s="84" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
+                                          /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="E42" s="85" t="n">
+        <v>97</v>
+      </c>
+      <c r="F42" s="85" t="n">
+        <v>5022.5</v>
+      </c>
+      <c r="G42" s="85" t="n">
+        <v>407</v>
+      </c>
+      <c r="H42" s="85" t="n">
+        <v>452</v>
+      </c>
+      <c r="I42" s="2" t="n">
+        <v>1.8216</v>
+      </c>
+      <c r="J42" s="2" t="n"/>
+      <c r="K42" s="2" t="n"/>
+      <c r="L42" s="2" t="n"/>
+      <c r="M42" s="2" t="n"/>
+      <c r="N42" s="2" t="n"/>
+      <c r="O42" s="2" t="n"/>
+      <c r="P42" s="2" t="n"/>
+      <c r="Q42" s="2" t="n"/>
+      <c r="R42" s="2" t="n"/>
+      <c r="S42" s="2" t="n"/>
+      <c r="T42" s="2" t="n"/>
+    </row>
+    <row r="43" ht="27" customHeight="1">
+      <c r="A43" s="60" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+      <c r="B43" s="60" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C43" s="60" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D43" s="60" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E43" s="48" t="n">
+        <v>184</v>
+      </c>
+      <c r="F43" s="48" t="n">
+        <v>9583.5</v>
+      </c>
+      <c r="G43" s="48" t="n">
+        <v>773.7684</v>
+      </c>
+      <c r="H43" s="48" t="n">
+        <v>817.3474</v>
+      </c>
+      <c r="I43" s="2" t="n">
+        <v>2.6461</v>
+      </c>
+      <c r="J43" s="2" t="n"/>
+      <c r="K43" s="2" t="n"/>
+      <c r="L43" s="2" t="n"/>
+      <c r="M43" s="2" t="n"/>
+      <c r="N43" s="2" t="n"/>
+      <c r="O43" s="2" t="n"/>
+      <c r="P43" s="2" t="n"/>
+      <c r="Q43" s="2" t="n"/>
+      <c r="R43" s="2" t="n"/>
+      <c r="S43" s="2" t="n"/>
+      <c r="T43" s="2" t="n"/>
+    </row>
+    <row r="44" ht="27" customHeight="1">
+      <c r="A44" s="60" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="B44" s="60" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C44" s="60" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D44" s="60" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E44" s="48" t="n">
+        <v>6</v>
+      </c>
+      <c r="F44" s="48" t="n">
+        <v>237.8</v>
+      </c>
+      <c r="G44" s="48" t="n">
+        <v>25.2316</v>
+      </c>
+      <c r="H44" s="48" t="n">
+        <v>26.6526</v>
+      </c>
+      <c r="I44" s="2" t="n">
+        <v>0.0863</v>
+      </c>
+      <c r="J44" s="2" t="n"/>
+      <c r="K44" s="2" t="n"/>
+      <c r="L44" s="2" t="n"/>
+      <c r="M44" s="2" t="n"/>
+      <c r="N44" s="2" t="n"/>
+      <c r="O44" s="2" t="n"/>
+      <c r="P44" s="2" t="n"/>
+      <c r="Q44" s="2" t="n"/>
+      <c r="R44" s="2" t="n"/>
+      <c r="S44" s="2" t="n"/>
+      <c r="T44" s="2" t="n"/>
+    </row>
+    <row r="45" ht="27" customHeight="1">
+      <c r="A45" s="2" t="n"/>
+      <c r="B45" s="86" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C45" s="2" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E45" s="50" t="n">
+        <v>185</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>9782.9</v>
+      </c>
+      <c r="G45" s="24" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="H45" s="50" t="n">
+        <v>830.0658</v>
+      </c>
+      <c r="I45" s="2" t="n">
+        <v>2.5063</v>
+      </c>
+      <c r="J45" s="2" t="n"/>
+      <c r="K45" s="2" t="n"/>
+      <c r="L45" s="2" t="n"/>
+      <c r="M45" s="2" t="n"/>
+      <c r="N45" s="2" t="n"/>
+      <c r="O45" s="2" t="n"/>
+      <c r="P45" s="2" t="n"/>
+      <c r="Q45" s="2" t="n"/>
+      <c r="R45" s="2" t="n"/>
+      <c r="S45" s="2" t="n"/>
+      <c r="T45" s="2" t="n"/>
+    </row>
+    <row r="46">
+      <c r="B46" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>5</v>
+      </c>
+      <c r="F46" t="n">
+        <v>199</v>
+      </c>
+      <c r="G46" t="n">
+        <v>21.25</v>
+      </c>
+      <c r="H46" t="n">
+        <v>22.4342</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.0677</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>190</v>
+      </c>
+      <c r="F47" t="n">
+        <v>10009.4</v>
+      </c>
+      <c r="G47" t="n">
+        <v>824</v>
+      </c>
+      <c r="H47" t="n">
+        <v>869</v>
+      </c>
+      <c r="I47" t="n">
+        <v>2.574</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>195</v>
+      </c>
+      <c r="F48" t="n">
+        <v>10072.6</v>
+      </c>
+      <c r="G48" t="n">
+        <v>821</v>
+      </c>
+      <c r="H48" t="n">
+        <v>866</v>
+      </c>
+      <c r="I48" t="n">
+        <v>2.574</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>195</v>
+      </c>
+      <c r="F49" t="n">
+        <v>10117.1</v>
+      </c>
+      <c r="G49" t="n">
+        <v>825.5</v>
+      </c>
+      <c r="H49" t="n">
+        <v>870.5</v>
+      </c>
+      <c r="I49" t="n">
+        <v>2.4948</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>89</v>
+      </c>
+      <c r="F50" t="n">
+        <v>4707.4</v>
+      </c>
+      <c r="G50" t="n">
+        <v>376.5385</v>
+      </c>
+      <c r="H50" t="n">
+        <v>415.0481</v>
+      </c>
+      <c r="I50" t="n">
+        <v>1.4572</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>8</v>
+      </c>
+      <c r="F51" t="n">
+        <v>322.8</v>
+      </c>
+      <c r="G51" t="n">
+        <v>33.8462</v>
+      </c>
+      <c r="H51" t="n">
+        <v>37.3077</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.131</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>7</v>
+      </c>
+      <c r="F52" t="n">
+        <v>367.3</v>
+      </c>
+      <c r="G52" t="n">
+        <v>29.6154</v>
+      </c>
+      <c r="H52" t="n">
+        <v>32.6442</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.1146</v>
+      </c>
+    </row>
+    <row r="53" ht="27" customHeight="1"/>
+    <row r="54" ht="27" customHeight="1">
+      <c r="A54" s="80" t="n"/>
+      <c r="B54" s="16" t="n"/>
+      <c r="C54" s="16" t="n"/>
+      <c r="D54" s="16" t="n"/>
+      <c r="E54" s="16" t="n"/>
+      <c r="F54" s="16" t="n"/>
+      <c r="G54" s="16" t="n"/>
+      <c r="H54" s="16" t="n"/>
+      <c r="I54" s="16" t="n"/>
+    </row>
     <row r="55"/>
     <row r="56"/>
     <row r="57"/>
@@ -2229,13 +4726,23 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="16">
     <mergeCell ref="A2:I2"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A42:D42"/>
     <mergeCell ref="A5:I5"/>
+    <mergeCell ref="B41:D41"/>
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="I21:I22"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A6:I6"/>
+    <mergeCell ref="H21:H22"/>
     <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
adding the static row before the footer into the footer add on but still has border at static row issue
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -1439,11 +1439,25 @@
       </c>
     </row>
     <row r="31" ht="36" customHeight="1">
-      <c r="A31" s="15" t="n"/>
-      <c r="B31" s="15" t="n"/>
-      <c r="C31" s="16" t="n"/>
+      <c r="A31" s="15" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="B31" s="15" t="inlineStr">
+        <is>
+          <t>31 PALLETS</t>
+        </is>
+      </c>
+      <c r="C31" s="16">
+        <f>SUM(C16:C30)</f>
+        <v/>
+      </c>
       <c r="D31" s="16" t="n"/>
-      <c r="E31" s="16" t="n"/>
+      <c r="E31" s="16">
+        <f>SUM(E16:E30)</f>
+        <v/>
+      </c>
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="A32" s="8" t="inlineStr">
@@ -2597,47 +2611,54 @@
     <row r="37" ht="35" customHeight="1">
       <c r="A37" s="54" t="n"/>
       <c r="B37" s="54" t="n"/>
-      <c r="C37" s="54" t="n"/>
+      <c r="C37" s="54" t="inlineStr">
+        <is>
+          <t>HS.CODE: 4107.12.00</t>
+        </is>
+      </c>
       <c r="D37" s="55" t="n"/>
       <c r="E37" s="56" t="n"/>
       <c r="F37" s="56" t="n"/>
       <c r="G37" s="56" t="n"/>
     </row>
-    <row r="38" ht="61.5" customHeight="1">
-      <c r="A38" s="60" t="inlineStr">
+    <row r="38" ht="35" customHeight="1">
+      <c r="A38" s="54" t="n"/>
+      <c r="B38" s="54" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="C38" s="54" t="inlineStr">
+        <is>
+          <t>31 PALLETS</t>
+        </is>
+      </c>
+      <c r="D38" s="55" t="n"/>
+      <c r="E38" s="56">
+        <f>SUM(E22:E36)</f>
+        <v/>
+      </c>
+      <c r="F38" s="56" t="n"/>
+      <c r="G38" s="56">
+        <f>SUM(G22:G36)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" ht="61.5" customHeight="1">
+      <c r="A39" s="60" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B38" s="61" t="inlineStr">
+      <c r="B39" s="61" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D38" s="61" t="n"/>
-      <c r="E38" s="61" t="n"/>
-      <c r="F38" s="32" t="n"/>
-      <c r="G38" s="26" t="n"/>
-      <c r="H38" s="2" t="n"/>
-      <c r="I38" s="2" t="n"/>
-      <c r="J38" s="2" t="n"/>
-      <c r="K38" s="2" t="n"/>
-      <c r="L38" s="62" t="n"/>
-      <c r="M38" s="63" t="n"/>
-      <c r="N38" s="64" t="n"/>
-      <c r="O38" s="64" t="n"/>
-    </row>
-    <row r="39" ht="42" customHeight="1">
-      <c r="A39" s="65" t="inlineStr">
-        <is>
-          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
-                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-      <c r="D39" s="65" t="n"/>
-      <c r="E39" s="65" t="n"/>
-      <c r="F39" s="65" t="n"/>
+      <c r="D39" s="61" t="n"/>
+      <c r="E39" s="61" t="n"/>
+      <c r="F39" s="32" t="n"/>
       <c r="G39" s="26" t="n"/>
       <c r="H39" s="2" t="n"/>
       <c r="I39" s="2" t="n"/>
@@ -2648,12 +2669,17 @@
       <c r="N39" s="64" t="n"/>
       <c r="O39" s="64" t="n"/>
     </row>
-    <row r="40" ht="24.75" customHeight="1">
-      <c r="A40" s="66" t="inlineStr">
-        <is>
-          <t>A/C NO:100001100764430</t>
-        </is>
-      </c>
+    <row r="40" ht="42" customHeight="1">
+      <c r="A40" s="65" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="D40" s="65" t="n"/>
+      <c r="E40" s="65" t="n"/>
+      <c r="F40" s="65" t="n"/>
+      <c r="G40" s="26" t="n"/>
       <c r="H40" s="2" t="n"/>
       <c r="I40" s="2" t="n"/>
       <c r="J40" s="2" t="n"/>
@@ -2663,10 +2689,10 @@
       <c r="N40" s="64" t="n"/>
       <c r="O40" s="64" t="n"/>
     </row>
-    <row r="41" ht="27" customHeight="1">
+    <row r="41" ht="24.75" customHeight="1">
       <c r="A41" s="66" t="inlineStr">
         <is>
-          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+          <t>A/C NO:100001100764430</t>
         </is>
       </c>
       <c r="H41" s="2" t="n"/>
@@ -2678,19 +2704,13 @@
       <c r="N41" s="64" t="n"/>
       <c r="O41" s="64" t="n"/>
     </row>
-    <row r="42" ht="61.5" customHeight="1">
-      <c r="A42" s="2" t="n"/>
-      <c r="B42" s="2" t="n"/>
-      <c r="C42" s="2" t="n"/>
-      <c r="D42" s="2" t="n"/>
-      <c r="E42" s="67" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
-      <c r="F42" s="67" t="n"/>
-      <c r="G42" s="67" t="n"/>
-      <c r="H42" s="67" t="n"/>
+    <row r="42" ht="27" customHeight="1">
+      <c r="A42" s="66" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="H42" s="2" t="n"/>
       <c r="I42" s="2" t="n"/>
       <c r="J42" s="2" t="n"/>
       <c r="K42" s="2" t="n"/>
@@ -2699,19 +2719,19 @@
       <c r="N42" s="64" t="n"/>
       <c r="O42" s="64" t="n"/>
     </row>
-    <row r="43" ht="42" customHeight="1">
+    <row r="43" ht="61.5" customHeight="1">
       <c r="A43" s="2" t="n"/>
       <c r="B43" s="2" t="n"/>
       <c r="C43" s="2" t="n"/>
-      <c r="D43" s="68" t="n"/>
-      <c r="E43" s="69" t="n"/>
-      <c r="F43" s="70" t="inlineStr">
-        <is>
-          <t>Sign &amp; Stamp</t>
-        </is>
-      </c>
-      <c r="G43" s="71" t="n"/>
-      <c r="H43" s="2" t="n"/>
+      <c r="D43" s="2" t="n"/>
+      <c r="E43" s="67" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="F43" s="67" t="n"/>
+      <c r="G43" s="67" t="n"/>
+      <c r="H43" s="67" t="n"/>
       <c r="I43" s="2" t="n"/>
       <c r="J43" s="2" t="n"/>
       <c r="K43" s="2" t="n"/>
@@ -2720,13 +2740,17 @@
       <c r="N43" s="64" t="n"/>
       <c r="O43" s="64" t="n"/>
     </row>
-    <row r="44" ht="24.75" customHeight="1">
+    <row r="44" ht="42" customHeight="1">
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="2" t="n"/>
       <c r="C44" s="2" t="n"/>
       <c r="D44" s="68" t="n"/>
       <c r="E44" s="69" t="n"/>
-      <c r="F44" s="69" t="n"/>
+      <c r="F44" s="70" t="inlineStr">
+        <is>
+          <t>Sign &amp; Stamp</t>
+        </is>
+      </c>
       <c r="G44" s="71" t="n"/>
       <c r="H44" s="2" t="n"/>
       <c r="I44" s="2" t="n"/>
@@ -2737,7 +2761,7 @@
       <c r="N44" s="64" t="n"/>
       <c r="O44" s="64" t="n"/>
     </row>
-    <row r="45" ht="27" customHeight="1">
+    <row r="45" ht="24.75" customHeight="1">
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="n"/>
       <c r="C45" s="2" t="n"/>
@@ -2754,18 +2778,14 @@
       <c r="N45" s="64" t="n"/>
       <c r="O45" s="64" t="n"/>
     </row>
-    <row r="46" ht="21" customHeight="1">
+    <row r="46" ht="27" customHeight="1">
       <c r="A46" s="2" t="n"/>
       <c r="B46" s="2" t="n"/>
       <c r="C46" s="2" t="n"/>
       <c r="D46" s="68" t="n"/>
       <c r="E46" s="69" t="n"/>
-      <c r="F46" s="72" t="inlineStr">
-        <is>
-          <t>ZENG XUELI</t>
-        </is>
-      </c>
-      <c r="G46" s="72" t="n"/>
+      <c r="F46" s="69" t="n"/>
+      <c r="G46" s="71" t="n"/>
       <c r="H46" s="2" t="n"/>
       <c r="I46" s="2" t="n"/>
       <c r="J46" s="2" t="n"/>
@@ -2775,7 +2795,27 @@
       <c r="N46" s="64" t="n"/>
       <c r="O46" s="64" t="n"/>
     </row>
-    <row r="47"/>
+    <row r="47" ht="21" customHeight="1">
+      <c r="A47" s="2" t="n"/>
+      <c r="B47" s="2" t="n"/>
+      <c r="C47" s="2" t="n"/>
+      <c r="D47" s="68" t="n"/>
+      <c r="E47" s="69" t="n"/>
+      <c r="F47" s="72" t="inlineStr">
+        <is>
+          <t>ZENG XUELI</t>
+        </is>
+      </c>
+      <c r="G47" s="72" t="n"/>
+      <c r="H47" s="2" t="n"/>
+      <c r="I47" s="2" t="n"/>
+      <c r="J47" s="2" t="n"/>
+      <c r="K47" s="2" t="n"/>
+      <c r="L47" s="62" t="n"/>
+      <c r="M47" s="63" t="n"/>
+      <c r="N47" s="64" t="n"/>
+      <c r="O47" s="64" t="n"/>
+    </row>
     <row r="48"/>
     <row r="49"/>
     <row r="50"/>
@@ -2931,14 +2971,14 @@
     <row r="200"/>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A40:G40"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A42:G42"/>
     <mergeCell ref="A41:G41"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
@@ -4385,17 +4425,54 @@
         <v>0.1146</v>
       </c>
     </row>
-    <row r="53" ht="27" customHeight="1"/>
+    <row r="53" ht="27" customHeight="1">
+      <c r="A53" s="55" t="n"/>
+      <c r="B53" s="55" t="inlineStr">
+        <is>
+          <t>LEATHER (HS.CODE: 4107.12.00)</t>
+        </is>
+      </c>
+      <c r="C53" s="55" t="n"/>
+      <c r="D53" s="55" t="n"/>
+      <c r="E53" s="87" t="n"/>
+      <c r="F53" s="56" t="n"/>
+      <c r="G53" s="56" t="n"/>
+      <c r="H53" s="56" t="n"/>
+      <c r="I53" s="85" t="n"/>
+    </row>
     <row r="54" ht="27" customHeight="1">
       <c r="A54" s="55" t="n"/>
-      <c r="B54" s="55" t="n"/>
-      <c r="C54" s="55" t="n"/>
+      <c r="B54" s="55" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="C54" s="55" t="inlineStr">
+        <is>
+          <t>20 PALLETS</t>
+        </is>
+      </c>
       <c r="D54" s="55" t="n"/>
-      <c r="E54" s="87" t="n"/>
-      <c r="F54" s="56" t="n"/>
-      <c r="G54" s="56" t="n"/>
-      <c r="H54" s="56" t="n"/>
-      <c r="I54" s="85" t="n"/>
+      <c r="E54" s="87">
+        <f>SUM(E23:E52)</f>
+        <v/>
+      </c>
+      <c r="F54" s="56">
+        <f>SUM(F23:F52)</f>
+        <v/>
+      </c>
+      <c r="G54" s="56">
+        <f>SUM(G23:G52)</f>
+        <v/>
+      </c>
+      <c r="H54" s="56">
+        <f>SUM(H23:H52)</f>
+        <v/>
+      </c>
+      <c r="I54" s="85">
+        <f>SUM(I23:I52)</f>
+        <v/>
+      </c>
     </row>
     <row r="55"/>
     <row r="56" ht="27" customHeight="1">
@@ -4848,28 +4925,88 @@
         <v>0.0589</v>
       </c>
     </row>
-    <row r="72" ht="27" customHeight="1"/>
+    <row r="72" ht="27" customHeight="1">
+      <c r="A72" s="55" t="n"/>
+      <c r="B72" s="55" t="inlineStr">
+        <is>
+          <t>LEATHER (HS.CODE: 4107.12.00)</t>
+        </is>
+      </c>
+      <c r="C72" s="55" t="n"/>
+      <c r="D72" s="55" t="n"/>
+      <c r="E72" s="87" t="n"/>
+      <c r="F72" s="56" t="n"/>
+      <c r="G72" s="56" t="n"/>
+      <c r="H72" s="56" t="n"/>
+      <c r="I72" s="85" t="n"/>
+    </row>
     <row r="73" ht="27" customHeight="1">
       <c r="A73" s="55" t="n"/>
-      <c r="B73" s="55" t="n"/>
-      <c r="C73" s="55" t="n"/>
+      <c r="B73" s="55" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="C73" s="55" t="inlineStr">
+        <is>
+          <t>11 PALLETS</t>
+        </is>
+      </c>
       <c r="D73" s="55" t="n"/>
-      <c r="E73" s="87" t="n"/>
-      <c r="F73" s="56" t="n"/>
-      <c r="G73" s="56" t="n"/>
-      <c r="H73" s="56" t="n"/>
-      <c r="I73" s="85" t="n"/>
+      <c r="E73" s="87">
+        <f>SUM(E58:E71)</f>
+        <v/>
+      </c>
+      <c r="F73" s="56">
+        <f>SUM(F58:F71)</f>
+        <v/>
+      </c>
+      <c r="G73" s="56">
+        <f>SUM(G58:G71)</f>
+        <v/>
+      </c>
+      <c r="H73" s="56">
+        <f>SUM(H58:H71)</f>
+        <v/>
+      </c>
+      <c r="I73" s="85">
+        <f>SUM(I58:I71)</f>
+        <v/>
+      </c>
     </row>
     <row r="74" ht="27" customHeight="1">
       <c r="A74" s="55" t="n"/>
-      <c r="B74" s="55" t="n"/>
-      <c r="C74" s="55" t="n"/>
+      <c r="B74" s="55" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C74" s="55" t="inlineStr">
+        <is>
+          <t>31 PALLETS</t>
+        </is>
+      </c>
       <c r="D74" s="55" t="n"/>
-      <c r="E74" s="87" t="n"/>
-      <c r="F74" s="56" t="n"/>
-      <c r="G74" s="56" t="n"/>
-      <c r="H74" s="56" t="n"/>
-      <c r="I74" s="85" t="n"/>
+      <c r="E74" s="87">
+        <f>SUM(E23:E52,E58:E71)</f>
+        <v/>
+      </c>
+      <c r="F74" s="56">
+        <f>SUM(F23:F52,F58:F71)</f>
+        <v/>
+      </c>
+      <c r="G74" s="56">
+        <f>SUM(G23:G52,G58:G71)</f>
+        <v/>
+      </c>
+      <c r="H74" s="56">
+        <f>SUM(H23:H52,H58:H71)</f>
+        <v/>
+      </c>
+      <c r="I74" s="85">
+        <f>SUM(I23:I52,I58:I71)</f>
+        <v/>
+      </c>
     </row>
     <row r="75" ht="27" customHeight="1">
       <c r="A75" s="2" t="n"/>
@@ -5019,7 +5156,9 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="27">
+    <mergeCell ref="B74"/>
+    <mergeCell ref="B72:C72"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="A3:I3"/>
@@ -5032,8 +5171,11 @@
     <mergeCell ref="D56:D57"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="I21:I22"/>
+    <mergeCell ref="B54"/>
     <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B53:C53"/>
     <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B73"/>
     <mergeCell ref="G56:G57"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B56:B57"/>

</xml_diff>

<commit_message>
fixing the border issue on static row
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -219,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -258,6 +258,14 @@
       <bottom style="thin">
         <color rgb="00000000"/>
       </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
     </border>
     <border>
       <left style="thin">
@@ -329,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -490,6 +498,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -552,11 +563,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,6 +575,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2609,13 +2635,13 @@
       </c>
     </row>
     <row r="37" ht="35" customHeight="1">
-      <c r="A37" s="54" t="n"/>
-      <c r="B37" s="54" t="n"/>
-      <c r="C37" s="54" t="inlineStr">
+      <c r="A37" s="60" t="n"/>
+      <c r="B37" s="54" t="inlineStr">
         <is>
           <t>HS.CODE: 4107.12.00</t>
         </is>
       </c>
+      <c r="C37" s="54" t="n"/>
       <c r="D37" s="55" t="n"/>
       <c r="E37" s="56" t="n"/>
       <c r="F37" s="56" t="n"/>
@@ -2645,52 +2671,52 @@
       </c>
     </row>
     <row r="39" ht="61.5" customHeight="1">
-      <c r="A39" s="60" t="inlineStr">
+      <c r="A39" s="61" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B39" s="61" t="inlineStr">
+      <c r="B39" s="62" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D39" s="61" t="n"/>
-      <c r="E39" s="61" t="n"/>
+      <c r="D39" s="62" t="n"/>
+      <c r="E39" s="62" t="n"/>
       <c r="F39" s="32" t="n"/>
       <c r="G39" s="26" t="n"/>
       <c r="H39" s="2" t="n"/>
       <c r="I39" s="2" t="n"/>
       <c r="J39" s="2" t="n"/>
       <c r="K39" s="2" t="n"/>
-      <c r="L39" s="62" t="n"/>
-      <c r="M39" s="63" t="n"/>
-      <c r="N39" s="64" t="n"/>
-      <c r="O39" s="64" t="n"/>
+      <c r="L39" s="63" t="n"/>
+      <c r="M39" s="64" t="n"/>
+      <c r="N39" s="65" t="n"/>
+      <c r="O39" s="65" t="n"/>
     </row>
     <row r="40" ht="42" customHeight="1">
-      <c r="A40" s="65" t="inlineStr">
+      <c r="A40" s="66" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                                   /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="D40" s="65" t="n"/>
-      <c r="E40" s="65" t="n"/>
-      <c r="F40" s="65" t="n"/>
+      <c r="D40" s="66" t="n"/>
+      <c r="E40" s="66" t="n"/>
+      <c r="F40" s="66" t="n"/>
       <c r="G40" s="26" t="n"/>
       <c r="H40" s="2" t="n"/>
       <c r="I40" s="2" t="n"/>
       <c r="J40" s="2" t="n"/>
       <c r="K40" s="2" t="n"/>
-      <c r="L40" s="62" t="n"/>
-      <c r="M40" s="63" t="n"/>
-      <c r="N40" s="64" t="n"/>
-      <c r="O40" s="64" t="n"/>
+      <c r="L40" s="63" t="n"/>
+      <c r="M40" s="64" t="n"/>
+      <c r="N40" s="65" t="n"/>
+      <c r="O40" s="65" t="n"/>
     </row>
     <row r="41" ht="24.75" customHeight="1">
-      <c r="A41" s="66" t="inlineStr">
+      <c r="A41" s="67" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
@@ -2699,13 +2725,13 @@
       <c r="I41" s="2" t="n"/>
       <c r="J41" s="2" t="n"/>
       <c r="K41" s="2" t="n"/>
-      <c r="L41" s="62" t="n"/>
-      <c r="M41" s="63" t="n"/>
-      <c r="N41" s="64" t="n"/>
-      <c r="O41" s="64" t="n"/>
+      <c r="L41" s="63" t="n"/>
+      <c r="M41" s="64" t="n"/>
+      <c r="N41" s="65" t="n"/>
+      <c r="O41" s="65" t="n"/>
     </row>
     <row r="42" ht="27" customHeight="1">
-      <c r="A42" s="66" t="inlineStr">
+      <c r="A42" s="67" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
@@ -2714,107 +2740,107 @@
       <c r="I42" s="2" t="n"/>
       <c r="J42" s="2" t="n"/>
       <c r="K42" s="2" t="n"/>
-      <c r="L42" s="62" t="n"/>
-      <c r="M42" s="63" t="n"/>
-      <c r="N42" s="64" t="n"/>
-      <c r="O42" s="64" t="n"/>
+      <c r="L42" s="63" t="n"/>
+      <c r="M42" s="64" t="n"/>
+      <c r="N42" s="65" t="n"/>
+      <c r="O42" s="65" t="n"/>
     </row>
     <row r="43" ht="61.5" customHeight="1">
       <c r="A43" s="2" t="n"/>
       <c r="B43" s="2" t="n"/>
       <c r="C43" s="2" t="n"/>
       <c r="D43" s="2" t="n"/>
-      <c r="E43" s="67" t="inlineStr">
+      <c r="E43" s="68" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="F43" s="67" t="n"/>
-      <c r="G43" s="67" t="n"/>
-      <c r="H43" s="67" t="n"/>
+      <c r="F43" s="68" t="n"/>
+      <c r="G43" s="68" t="n"/>
+      <c r="H43" s="68" t="n"/>
       <c r="I43" s="2" t="n"/>
       <c r="J43" s="2" t="n"/>
       <c r="K43" s="2" t="n"/>
-      <c r="L43" s="62" t="n"/>
-      <c r="M43" s="63" t="n"/>
-      <c r="N43" s="64" t="n"/>
-      <c r="O43" s="64" t="n"/>
+      <c r="L43" s="63" t="n"/>
+      <c r="M43" s="64" t="n"/>
+      <c r="N43" s="65" t="n"/>
+      <c r="O43" s="65" t="n"/>
     </row>
     <row r="44" ht="42" customHeight="1">
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="2" t="n"/>
       <c r="C44" s="2" t="n"/>
-      <c r="D44" s="68" t="n"/>
-      <c r="E44" s="69" t="n"/>
-      <c r="F44" s="70" t="inlineStr">
+      <c r="D44" s="69" t="n"/>
+      <c r="E44" s="70" t="n"/>
+      <c r="F44" s="71" t="inlineStr">
         <is>
           <t>Sign &amp; Stamp</t>
         </is>
       </c>
-      <c r="G44" s="71" t="n"/>
+      <c r="G44" s="72" t="n"/>
       <c r="H44" s="2" t="n"/>
       <c r="I44" s="2" t="n"/>
       <c r="J44" s="2" t="n"/>
       <c r="K44" s="2" t="n"/>
-      <c r="L44" s="62" t="n"/>
-      <c r="M44" s="63" t="n"/>
-      <c r="N44" s="64" t="n"/>
-      <c r="O44" s="64" t="n"/>
+      <c r="L44" s="63" t="n"/>
+      <c r="M44" s="64" t="n"/>
+      <c r="N44" s="65" t="n"/>
+      <c r="O44" s="65" t="n"/>
     </row>
     <row r="45" ht="24.75" customHeight="1">
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="n"/>
       <c r="C45" s="2" t="n"/>
-      <c r="D45" s="68" t="n"/>
-      <c r="E45" s="69" t="n"/>
-      <c r="F45" s="69" t="n"/>
-      <c r="G45" s="71" t="n"/>
+      <c r="D45" s="69" t="n"/>
+      <c r="E45" s="70" t="n"/>
+      <c r="F45" s="70" t="n"/>
+      <c r="G45" s="72" t="n"/>
       <c r="H45" s="2" t="n"/>
       <c r="I45" s="2" t="n"/>
       <c r="J45" s="2" t="n"/>
       <c r="K45" s="2" t="n"/>
-      <c r="L45" s="62" t="n"/>
-      <c r="M45" s="63" t="n"/>
-      <c r="N45" s="64" t="n"/>
-      <c r="O45" s="64" t="n"/>
+      <c r="L45" s="63" t="n"/>
+      <c r="M45" s="64" t="n"/>
+      <c r="N45" s="65" t="n"/>
+      <c r="O45" s="65" t="n"/>
     </row>
     <row r="46" ht="27" customHeight="1">
       <c r="A46" s="2" t="n"/>
       <c r="B46" s="2" t="n"/>
       <c r="C46" s="2" t="n"/>
-      <c r="D46" s="68" t="n"/>
-      <c r="E46" s="69" t="n"/>
-      <c r="F46" s="69" t="n"/>
-      <c r="G46" s="71" t="n"/>
+      <c r="D46" s="69" t="n"/>
+      <c r="E46" s="70" t="n"/>
+      <c r="F46" s="70" t="n"/>
+      <c r="G46" s="72" t="n"/>
       <c r="H46" s="2" t="n"/>
       <c r="I46" s="2" t="n"/>
       <c r="J46" s="2" t="n"/>
       <c r="K46" s="2" t="n"/>
-      <c r="L46" s="62" t="n"/>
-      <c r="M46" s="63" t="n"/>
-      <c r="N46" s="64" t="n"/>
-      <c r="O46" s="64" t="n"/>
+      <c r="L46" s="63" t="n"/>
+      <c r="M46" s="64" t="n"/>
+      <c r="N46" s="65" t="n"/>
+      <c r="O46" s="65" t="n"/>
     </row>
     <row r="47" ht="21" customHeight="1">
       <c r="A47" s="2" t="n"/>
       <c r="B47" s="2" t="n"/>
       <c r="C47" s="2" t="n"/>
-      <c r="D47" s="68" t="n"/>
-      <c r="E47" s="69" t="n"/>
-      <c r="F47" s="72" t="inlineStr">
+      <c r="D47" s="69" t="n"/>
+      <c r="E47" s="70" t="n"/>
+      <c r="F47" s="73" t="inlineStr">
         <is>
           <t>ZENG XUELI</t>
         </is>
       </c>
-      <c r="G47" s="72" t="n"/>
+      <c r="G47" s="73" t="n"/>
       <c r="H47" s="2" t="n"/>
       <c r="I47" s="2" t="n"/>
       <c r="J47" s="2" t="n"/>
       <c r="K47" s="2" t="n"/>
-      <c r="L47" s="62" t="n"/>
-      <c r="M47" s="63" t="n"/>
-      <c r="N47" s="64" t="n"/>
-      <c r="O47" s="64" t="n"/>
+      <c r="L47" s="63" t="n"/>
+      <c r="M47" s="64" t="n"/>
+      <c r="N47" s="65" t="n"/>
+      <c r="O47" s="65" t="n"/>
     </row>
     <row r="48"/>
     <row r="49"/>
@@ -3148,7 +3174,7 @@
     </row>
     <row r="7" ht="18" customHeight="1">
       <c r="A7" s="32" t="n"/>
-      <c r="B7" s="73" t="n"/>
+      <c r="B7" s="74" t="n"/>
       <c r="C7" s="32" t="n"/>
       <c r="D7" s="32" t="n"/>
       <c r="E7" s="26" t="n"/>
@@ -3159,7 +3185,7 @@
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="I7" s="74" t="inlineStr">
+      <c r="I7" s="75" t="inlineStr">
         <is>
           <t>JFREF</t>
         </is>
@@ -3182,7 +3208,7 @@
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="75" t="inlineStr">
+      <c r="B8" s="76" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
@@ -3197,7 +3223,7 @@
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="I8" s="76" t="inlineStr">
+      <c r="I8" s="77" t="inlineStr">
         <is>
           <t>JFINV</t>
         </is>
@@ -3216,7 +3242,7 @@
     </row>
     <row r="9" ht="21" customHeight="1">
       <c r="A9" s="32" t="n"/>
-      <c r="B9" s="73" t="inlineStr">
+      <c r="B9" s="74" t="inlineStr">
         <is>
           <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages,</t>
         </is>
@@ -3250,7 +3276,7 @@
     </row>
     <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="32" t="n"/>
-      <c r="B10" s="73" t="inlineStr">
+      <c r="B10" s="74" t="inlineStr">
         <is>
           <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
         </is>
@@ -3265,7 +3291,7 @@
           <t>FCA :</t>
         </is>
       </c>
-      <c r="I10" s="77" t="inlineStr">
+      <c r="I10" s="78" t="inlineStr">
         <is>
           <t>BAVET, SVAY RIENG</t>
         </is>
@@ -3284,7 +3310,7 @@
     </row>
     <row r="11" ht="20.25" customHeight="1">
       <c r="A11" s="32" t="n"/>
-      <c r="B11" s="73" t="inlineStr">
+      <c r="B11" s="74" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
@@ -3310,7 +3336,7 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="n"/>
-      <c r="B12" s="73" t="n"/>
+      <c r="B12" s="74" t="n"/>
       <c r="C12" s="32" t="n"/>
       <c r="D12" s="32" t="n"/>
       <c r="E12" s="26" t="n"/>
@@ -3336,7 +3362,7 @@
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="78" t="inlineStr">
+      <c r="B13" s="79" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
@@ -3344,9 +3370,9 @@
       <c r="C13" s="2" t="n"/>
       <c r="D13" s="2" t="n"/>
       <c r="E13" s="2" t="n"/>
-      <c r="F13" s="79" t="n"/>
-      <c r="G13" s="79" t="n"/>
-      <c r="H13" s="79" t="n"/>
+      <c r="F13" s="80" t="n"/>
+      <c r="G13" s="80" t="n"/>
+      <c r="H13" s="80" t="n"/>
       <c r="I13" s="45" t="n"/>
       <c r="J13" s="2" t="n"/>
       <c r="K13" s="2" t="n"/>
@@ -3362,17 +3388,17 @@
     </row>
     <row r="14" ht="25.5" customHeight="1">
       <c r="A14" s="32" t="n"/>
-      <c r="B14" s="80" t="inlineStr">
+      <c r="B14" s="81" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
       <c r="C14" s="47" t="n"/>
       <c r="D14" s="47" t="n"/>
-      <c r="E14" s="81" t="n"/>
-      <c r="F14" s="81" t="n"/>
-      <c r="G14" s="81" t="n"/>
-      <c r="H14" s="81" t="n"/>
+      <c r="E14" s="82" t="n"/>
+      <c r="F14" s="82" t="n"/>
+      <c r="G14" s="82" t="n"/>
+      <c r="H14" s="82" t="n"/>
       <c r="I14" s="2" t="n"/>
       <c r="J14" s="2" t="n"/>
       <c r="K14" s="2" t="n"/>
@@ -3388,7 +3414,7 @@
     </row>
     <row r="15" ht="21" customHeight="1">
       <c r="A15" s="32" t="n"/>
-      <c r="B15" s="82" t="inlineStr">
+      <c r="B15" s="83" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
         </is>
@@ -3496,7 +3522,7 @@
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B19" s="73" t="inlineStr">
+      <c r="B19" s="74" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
         </is>
@@ -3522,7 +3548,7 @@
     </row>
     <row r="20" ht="27.75" customHeight="1">
       <c r="A20" s="53" t="n"/>
-      <c r="B20" s="83" t="n"/>
+      <c r="B20" s="84" t="n"/>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
@@ -3568,7 +3594,7 @@
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F21" s="84" t="n"/>
+      <c r="F21" s="85" t="n"/>
       <c r="G21" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -3579,7 +3605,7 @@
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I21" s="85" t="inlineStr">
+      <c r="I21" s="86" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
@@ -3597,11 +3623,11 @@
       <c r="T21" s="2" t="n"/>
     </row>
     <row r="22" ht="27" customHeight="1">
-      <c r="A22" s="86" t="n"/>
-      <c r="B22" s="86" t="n"/>
-      <c r="C22" s="86" t="n"/>
-      <c r="D22" s="86" t="n"/>
-      <c r="E22" s="87" t="inlineStr">
+      <c r="A22" s="87" t="n"/>
+      <c r="B22" s="87" t="n"/>
+      <c r="C22" s="87" t="n"/>
+      <c r="D22" s="87" t="n"/>
+      <c r="E22" s="88" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
@@ -3611,9 +3637,9 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="G22" s="86" t="n"/>
-      <c r="H22" s="86" t="n"/>
-      <c r="I22" s="86" t="n"/>
+      <c r="G22" s="87" t="n"/>
+      <c r="H22" s="87" t="n"/>
+      <c r="I22" s="87" t="n"/>
     </row>
     <row r="23" ht="27" customHeight="1">
       <c r="A23" s="58" t="inlineStr">
@@ -3632,7 +3658,7 @@
         </is>
       </c>
       <c r="D23" s="58" t="n"/>
-      <c r="E23" s="88" t="n">
+      <c r="E23" s="89" t="n">
         <v>122</v>
       </c>
       <c r="F23" s="59" t="n">
@@ -3644,7 +3670,7 @@
       <c r="H23" s="59" t="n">
         <v>512.1048</v>
       </c>
-      <c r="I23" s="89" t="n">
+      <c r="I23" s="90" t="n">
         <v>1.8312</v>
       </c>
     </row>
@@ -3665,7 +3691,7 @@
         </is>
       </c>
       <c r="D24" s="58" t="n"/>
-      <c r="E24" s="88" t="n">
+      <c r="E24" s="89" t="n">
         <v>2</v>
       </c>
       <c r="F24" s="59" t="n">
@@ -3677,7 +3703,7 @@
       <c r="H24" s="59" t="n">
         <v>8.395200000000001</v>
       </c>
-      <c r="I24" s="89" t="n">
+      <c r="I24" s="90" t="n">
         <v>0.03</v>
       </c>
     </row>
@@ -3698,7 +3724,7 @@
         </is>
       </c>
       <c r="D25" s="58" t="n"/>
-      <c r="E25" s="88" t="n">
+      <c r="E25" s="89" t="n">
         <v>190</v>
       </c>
       <c r="F25" s="59" t="n">
@@ -3710,7 +3736,7 @@
       <c r="H25" s="59" t="n">
         <v>802</v>
       </c>
-      <c r="I25" s="89" t="n">
+      <c r="I25" s="90" t="n">
         <v>2.4552</v>
       </c>
     </row>
@@ -3731,7 +3757,7 @@
         </is>
       </c>
       <c r="D26" s="58" t="n"/>
-      <c r="E26" s="88" t="n">
+      <c r="E26" s="89" t="n">
         <v>208</v>
       </c>
       <c r="F26" s="59" t="n">
@@ -3743,7 +3769,7 @@
       <c r="H26" s="59" t="n">
         <v>885.9439</v>
       </c>
-      <c r="I26" s="89" t="n">
+      <c r="I26" s="90" t="n">
         <v>2.6943</v>
       </c>
     </row>
@@ -3759,7 +3785,7 @@
         </is>
       </c>
       <c r="D27" s="58" t="n"/>
-      <c r="E27" s="88" t="n">
+      <c r="E27" s="89" t="n">
         <v>6</v>
       </c>
       <c r="F27" s="59" t="n">
@@ -3771,7 +3797,7 @@
       <c r="H27" s="59" t="n">
         <v>25.5561</v>
       </c>
-      <c r="I27" s="89" t="n">
+      <c r="I27" s="90" t="n">
         <v>0.07770000000000001</v>
       </c>
     </row>
@@ -3785,7 +3811,7 @@
         </is>
       </c>
       <c r="D28" s="58" t="n"/>
-      <c r="E28" s="88" t="n">
+      <c r="E28" s="89" t="n">
         <v>154</v>
       </c>
       <c r="F28" s="59" t="n">
@@ -3797,7 +3823,7 @@
       <c r="H28" s="59" t="n">
         <v>658.0814</v>
       </c>
-      <c r="I28" s="89" t="n">
+      <c r="I28" s="90" t="n">
         <v>2.0564</v>
       </c>
     </row>
@@ -3811,7 +3837,7 @@
         </is>
       </c>
       <c r="D29" s="58" t="n"/>
-      <c r="E29" s="88" t="n">
+      <c r="E29" s="89" t="n">
         <v>18</v>
       </c>
       <c r="F29" s="59" t="n">
@@ -3823,7 +3849,7 @@
       <c r="H29" s="59" t="n">
         <v>76.9186</v>
       </c>
-      <c r="I29" s="89" t="n">
+      <c r="I29" s="90" t="n">
         <v>0.2404</v>
       </c>
     </row>
@@ -3837,7 +3863,7 @@
         </is>
       </c>
       <c r="D30" s="58" t="n"/>
-      <c r="E30" s="88" t="n">
+      <c r="E30" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F30" s="59" t="n">
@@ -3849,7 +3875,7 @@
       <c r="H30" s="59" t="n">
         <v>859.5</v>
       </c>
-      <c r="I30" s="89" t="n">
+      <c r="I30" s="90" t="n">
         <v>2.376</v>
       </c>
     </row>
@@ -3863,7 +3889,7 @@
         </is>
       </c>
       <c r="D31" s="58" t="n"/>
-      <c r="E31" s="88" t="n">
+      <c r="E31" s="89" t="n">
         <v>200</v>
       </c>
       <c r="F31" s="59" t="n">
@@ -3875,7 +3901,7 @@
       <c r="H31" s="59" t="n">
         <v>780.1762</v>
       </c>
-      <c r="I31" s="89" t="n">
+      <c r="I31" s="90" t="n">
         <v>2.2678</v>
       </c>
     </row>
@@ -3889,7 +3915,7 @@
         </is>
       </c>
       <c r="D32" s="58" t="n"/>
-      <c r="E32" s="88" t="n">
+      <c r="E32" s="89" t="n">
         <v>27</v>
       </c>
       <c r="F32" s="59" t="n">
@@ -3901,7 +3927,7 @@
       <c r="H32" s="59" t="n">
         <v>105.3238</v>
       </c>
-      <c r="I32" s="89" t="n">
+      <c r="I32" s="90" t="n">
         <v>0.3062</v>
       </c>
     </row>
@@ -3915,7 +3941,7 @@
         </is>
       </c>
       <c r="D33" s="58" t="n"/>
-      <c r="E33" s="88" t="n">
+      <c r="E33" s="89" t="n">
         <v>169</v>
       </c>
       <c r="F33" s="59" t="n">
@@ -3927,7 +3953,7 @@
       <c r="H33" s="59" t="n">
         <v>736.84</v>
       </c>
-      <c r="I33" s="89" t="n">
+      <c r="I33" s="90" t="n">
         <v>2.2181</v>
       </c>
     </row>
@@ -3941,7 +3967,7 @@
         </is>
       </c>
       <c r="D34" s="58" t="n"/>
-      <c r="E34" s="88" t="n">
+      <c r="E34" s="89" t="n">
         <v>6</v>
       </c>
       <c r="F34" s="59" t="n">
@@ -3953,7 +3979,7 @@
       <c r="H34" s="59" t="n">
         <v>26.16</v>
       </c>
-      <c r="I34" s="89" t="n">
+      <c r="I34" s="90" t="n">
         <v>0.07870000000000001</v>
       </c>
     </row>
@@ -3967,7 +3993,7 @@
         </is>
       </c>
       <c r="D35" s="58" t="n"/>
-      <c r="E35" s="88" t="n">
+      <c r="E35" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F35" s="59" t="n">
@@ -3979,7 +4005,7 @@
       <c r="H35" s="59" t="n">
         <v>859.5</v>
       </c>
-      <c r="I35" s="89" t="n">
+      <c r="I35" s="90" t="n">
         <v>2.376</v>
       </c>
     </row>
@@ -3993,7 +4019,7 @@
         </is>
       </c>
       <c r="D36" s="58" t="n"/>
-      <c r="E36" s="88" t="n">
+      <c r="E36" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F36" s="59" t="n">
@@ -4005,7 +4031,7 @@
       <c r="H36" s="59" t="n">
         <v>875.5</v>
       </c>
-      <c r="I36" s="89" t="n">
+      <c r="I36" s="90" t="n">
         <v>2.6136</v>
       </c>
     </row>
@@ -4019,7 +4045,7 @@
         </is>
       </c>
       <c r="D37" s="58" t="n"/>
-      <c r="E37" s="88" t="n">
+      <c r="E37" s="89" t="n">
         <v>215</v>
       </c>
       <c r="F37" s="59" t="n">
@@ -4031,7 +4057,7 @@
       <c r="H37" s="59" t="n">
         <v>946.5</v>
       </c>
-      <c r="I37" s="89" t="n">
+      <c r="I37" s="90" t="n">
         <v>2.97</v>
       </c>
     </row>
@@ -4045,7 +4071,7 @@
         </is>
       </c>
       <c r="D38" s="58" t="n"/>
-      <c r="E38" s="88" t="n">
+      <c r="E38" s="89" t="n">
         <v>215</v>
       </c>
       <c r="F38" s="59" t="n">
@@ -4057,7 +4083,7 @@
       <c r="H38" s="59" t="n">
         <v>963</v>
       </c>
-      <c r="I38" s="89" t="n">
+      <c r="I38" s="90" t="n">
         <v>2.6136</v>
       </c>
     </row>
@@ -4071,7 +4097,7 @@
         </is>
       </c>
       <c r="D39" s="58" t="n"/>
-      <c r="E39" s="88" t="n">
+      <c r="E39" s="89" t="n">
         <v>192</v>
       </c>
       <c r="F39" s="59" t="n">
@@ -4083,7 +4109,7 @@
       <c r="H39" s="59" t="n">
         <v>836.9709</v>
       </c>
-      <c r="I39" s="89" t="n">
+      <c r="I39" s="90" t="n">
         <v>2.4729</v>
       </c>
     </row>
@@ -4097,7 +4123,7 @@
         </is>
       </c>
       <c r="D40" s="58" t="n"/>
-      <c r="E40" s="88" t="n">
+      <c r="E40" s="89" t="n">
         <v>14</v>
       </c>
       <c r="F40" s="59" t="n">
@@ -4109,7 +4135,7 @@
       <c r="H40" s="59" t="n">
         <v>61.0291</v>
       </c>
-      <c r="I40" s="89" t="n">
+      <c r="I40" s="90" t="n">
         <v>0.1803</v>
       </c>
     </row>
@@ -4123,7 +4149,7 @@
         </is>
       </c>
       <c r="D41" s="58" t="n"/>
-      <c r="E41" s="88" t="n">
+      <c r="E41" s="89" t="n">
         <v>97</v>
       </c>
       <c r="F41" s="59" t="n">
@@ -4135,7 +4161,7 @@
       <c r="H41" s="59" t="n">
         <v>453</v>
       </c>
-      <c r="I41" s="89" t="n">
+      <c r="I41" s="90" t="n">
         <v>1.782</v>
       </c>
     </row>
@@ -4149,7 +4175,7 @@
         </is>
       </c>
       <c r="D42" s="58" t="n"/>
-      <c r="E42" s="88" t="n">
+      <c r="E42" s="89" t="n">
         <v>97</v>
       </c>
       <c r="F42" s="59" t="n">
@@ -4161,7 +4187,7 @@
       <c r="H42" s="59" t="n">
         <v>452</v>
       </c>
-      <c r="I42" s="89" t="n">
+      <c r="I42" s="90" t="n">
         <v>1.8216</v>
       </c>
     </row>
@@ -4175,7 +4201,7 @@
         </is>
       </c>
       <c r="D43" s="58" t="n"/>
-      <c r="E43" s="88" t="n">
+      <c r="E43" s="89" t="n">
         <v>184</v>
       </c>
       <c r="F43" s="59" t="n">
@@ -4187,7 +4213,7 @@
       <c r="H43" s="59" t="n">
         <v>817.3474</v>
       </c>
-      <c r="I43" s="89" t="n">
+      <c r="I43" s="90" t="n">
         <v>2.6461</v>
       </c>
     </row>
@@ -4201,7 +4227,7 @@
         </is>
       </c>
       <c r="D44" s="58" t="n"/>
-      <c r="E44" s="88" t="n">
+      <c r="E44" s="89" t="n">
         <v>6</v>
       </c>
       <c r="F44" s="59" t="n">
@@ -4213,7 +4239,7 @@
       <c r="H44" s="59" t="n">
         <v>26.6526</v>
       </c>
-      <c r="I44" s="89" t="n">
+      <c r="I44" s="90" t="n">
         <v>0.0863</v>
       </c>
     </row>
@@ -4227,7 +4253,7 @@
         </is>
       </c>
       <c r="D45" s="58" t="n"/>
-      <c r="E45" s="88" t="n">
+      <c r="E45" s="89" t="n">
         <v>185</v>
       </c>
       <c r="F45" s="59" t="n">
@@ -4239,7 +4265,7 @@
       <c r="H45" s="59" t="n">
         <v>830.0658</v>
       </c>
-      <c r="I45" s="89" t="n">
+      <c r="I45" s="90" t="n">
         <v>2.5063</v>
       </c>
     </row>
@@ -4253,7 +4279,7 @@
         </is>
       </c>
       <c r="D46" s="58" t="n"/>
-      <c r="E46" s="88" t="n">
+      <c r="E46" s="89" t="n">
         <v>5</v>
       </c>
       <c r="F46" s="59" t="n">
@@ -4265,7 +4291,7 @@
       <c r="H46" s="59" t="n">
         <v>22.4342</v>
       </c>
-      <c r="I46" s="89" t="n">
+      <c r="I46" s="90" t="n">
         <v>0.0677</v>
       </c>
     </row>
@@ -4279,7 +4305,7 @@
         </is>
       </c>
       <c r="D47" s="58" t="n"/>
-      <c r="E47" s="88" t="n">
+      <c r="E47" s="89" t="n">
         <v>190</v>
       </c>
       <c r="F47" s="59" t="n">
@@ -4291,7 +4317,7 @@
       <c r="H47" s="59" t="n">
         <v>869</v>
       </c>
-      <c r="I47" s="89" t="n">
+      <c r="I47" s="90" t="n">
         <v>2.574</v>
       </c>
     </row>
@@ -4305,7 +4331,7 @@
         </is>
       </c>
       <c r="D48" s="58" t="n"/>
-      <c r="E48" s="88" t="n">
+      <c r="E48" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F48" s="59" t="n">
@@ -4317,7 +4343,7 @@
       <c r="H48" s="59" t="n">
         <v>866</v>
       </c>
-      <c r="I48" s="89" t="n">
+      <c r="I48" s="90" t="n">
         <v>2.574</v>
       </c>
     </row>
@@ -4331,7 +4357,7 @@
         </is>
       </c>
       <c r="D49" s="58" t="n"/>
-      <c r="E49" s="88" t="n">
+      <c r="E49" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F49" s="59" t="n">
@@ -4343,7 +4369,7 @@
       <c r="H49" s="59" t="n">
         <v>870.5</v>
       </c>
-      <c r="I49" s="89" t="n">
+      <c r="I49" s="90" t="n">
         <v>2.4948</v>
       </c>
     </row>
@@ -4357,7 +4383,7 @@
         </is>
       </c>
       <c r="D50" s="58" t="n"/>
-      <c r="E50" s="88" t="n">
+      <c r="E50" s="89" t="n">
         <v>89</v>
       </c>
       <c r="F50" s="59" t="n">
@@ -4369,7 +4395,7 @@
       <c r="H50" s="59" t="n">
         <v>415.0481</v>
       </c>
-      <c r="I50" s="89" t="n">
+      <c r="I50" s="90" t="n">
         <v>1.4572</v>
       </c>
     </row>
@@ -4383,7 +4409,7 @@
         </is>
       </c>
       <c r="D51" s="58" t="n"/>
-      <c r="E51" s="88" t="n">
+      <c r="E51" s="89" t="n">
         <v>8</v>
       </c>
       <c r="F51" s="59" t="n">
@@ -4395,7 +4421,7 @@
       <c r="H51" s="59" t="n">
         <v>37.3077</v>
       </c>
-      <c r="I51" s="89" t="n">
+      <c r="I51" s="90" t="n">
         <v>0.131</v>
       </c>
     </row>
@@ -4409,7 +4435,7 @@
         </is>
       </c>
       <c r="D52" s="58" t="n"/>
-      <c r="E52" s="88" t="n">
+      <c r="E52" s="89" t="n">
         <v>7</v>
       </c>
       <c r="F52" s="59" t="n">
@@ -4421,12 +4447,12 @@
       <c r="H52" s="59" t="n">
         <v>32.6442</v>
       </c>
-      <c r="I52" s="89" t="n">
+      <c r="I52" s="90" t="n">
         <v>0.1146</v>
       </c>
     </row>
     <row r="53" ht="27" customHeight="1">
-      <c r="A53" s="55" t="n"/>
+      <c r="A53" s="91" t="n"/>
       <c r="B53" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
@@ -4434,11 +4460,11 @@
       </c>
       <c r="C53" s="55" t="n"/>
       <c r="D53" s="55" t="n"/>
-      <c r="E53" s="87" t="n"/>
+      <c r="E53" s="88" t="n"/>
       <c r="F53" s="56" t="n"/>
       <c r="G53" s="56" t="n"/>
       <c r="H53" s="56" t="n"/>
-      <c r="I53" s="85" t="n"/>
+      <c r="I53" s="86" t="n"/>
     </row>
     <row r="54" ht="27" customHeight="1">
       <c r="A54" s="55" t="n"/>
@@ -4453,7 +4479,7 @@
         </is>
       </c>
       <c r="D54" s="55" t="n"/>
-      <c r="E54" s="87">
+      <c r="E54" s="88">
         <f>SUM(E23:E52)</f>
         <v/>
       </c>
@@ -4469,7 +4495,7 @@
         <f>SUM(H23:H52)</f>
         <v/>
       </c>
-      <c r="I54" s="85">
+      <c r="I54" s="86">
         <f>SUM(I23:I52)</f>
         <v/>
       </c>
@@ -4501,7 +4527,7 @@
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F56" s="84" t="n"/>
+      <c r="F56" s="85" t="n"/>
       <c r="G56" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -4512,18 +4538,18 @@
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I56" s="85" t="inlineStr">
+      <c r="I56" s="86" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
     <row r="57" ht="27" customHeight="1">
-      <c r="A57" s="86" t="n"/>
-      <c r="B57" s="86" t="n"/>
-      <c r="C57" s="86" t="n"/>
-      <c r="D57" s="86" t="n"/>
-      <c r="E57" s="87" t="inlineStr">
+      <c r="A57" s="87" t="n"/>
+      <c r="B57" s="87" t="n"/>
+      <c r="C57" s="87" t="n"/>
+      <c r="D57" s="87" t="n"/>
+      <c r="E57" s="88" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
@@ -4533,9 +4559,9 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="G57" s="86" t="n"/>
-      <c r="H57" s="86" t="n"/>
-      <c r="I57" s="86" t="n"/>
+      <c r="G57" s="87" t="n"/>
+      <c r="H57" s="87" t="n"/>
+      <c r="I57" s="87" t="n"/>
     </row>
     <row r="58" ht="27" customHeight="1">
       <c r="A58" s="58" t="inlineStr">
@@ -4552,7 +4578,7 @@
         </is>
       </c>
       <c r="D58" s="58" t="n"/>
-      <c r="E58" s="88" t="n">
+      <c r="E58" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F58" s="59" t="n">
@@ -4564,7 +4590,7 @@
       <c r="H58" s="59" t="n">
         <v>887.5</v>
       </c>
-      <c r="I58" s="89" t="n">
+      <c r="I58" s="90" t="n">
         <v>2.6532</v>
       </c>
     </row>
@@ -4583,7 +4609,7 @@
         </is>
       </c>
       <c r="D59" s="58" t="n"/>
-      <c r="E59" s="88" t="n">
+      <c r="E59" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F59" s="59" t="n">
@@ -4595,7 +4621,7 @@
       <c r="H59" s="59" t="n">
         <v>891</v>
       </c>
-      <c r="I59" s="89" t="n">
+      <c r="I59" s="90" t="n">
         <v>2.4948</v>
       </c>
     </row>
@@ -4614,7 +4640,7 @@
         </is>
       </c>
       <c r="D60" s="58" t="n"/>
-      <c r="E60" s="88" t="n">
+      <c r="E60" s="89" t="n">
         <v>207</v>
       </c>
       <c r="F60" s="59" t="n">
@@ -4626,7 +4652,7 @@
       <c r="H60" s="59" t="n">
         <v>926.3013999999999</v>
       </c>
-      <c r="I60" s="89" t="n">
+      <c r="I60" s="90" t="n">
         <v>2.8447</v>
       </c>
     </row>
@@ -4645,7 +4671,7 @@
         </is>
       </c>
       <c r="D61" s="58" t="n"/>
-      <c r="E61" s="88" t="n">
+      <c r="E61" s="89" t="n">
         <v>12</v>
       </c>
       <c r="F61" s="59" t="n">
@@ -4657,7 +4683,7 @@
       <c r="H61" s="59" t="n">
         <v>53.6986</v>
       </c>
-      <c r="I61" s="89" t="n">
+      <c r="I61" s="90" t="n">
         <v>0.1649</v>
       </c>
     </row>
@@ -4671,7 +4697,7 @@
         </is>
       </c>
       <c r="D62" s="58" t="n"/>
-      <c r="E62" s="88" t="n">
+      <c r="E62" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F62" s="59" t="n">
@@ -4683,7 +4709,7 @@
       <c r="H62" s="59" t="n">
         <v>885</v>
       </c>
-      <c r="I62" s="89" t="n">
+      <c r="I62" s="90" t="n">
         <v>2.6136</v>
       </c>
     </row>
@@ -4697,7 +4723,7 @@
         </is>
       </c>
       <c r="D63" s="58" t="n"/>
-      <c r="E63" s="88" t="n">
+      <c r="E63" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F63" s="59" t="n">
@@ -4709,7 +4735,7 @@
       <c r="H63" s="59" t="n">
         <v>908.5</v>
       </c>
-      <c r="I63" s="89" t="n">
+      <c r="I63" s="90" t="n">
         <v>2.6928</v>
       </c>
     </row>
@@ -4723,7 +4749,7 @@
         </is>
       </c>
       <c r="D64" s="58" t="n"/>
-      <c r="E64" s="88" t="n">
+      <c r="E64" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F64" s="59" t="n">
@@ -4735,7 +4761,7 @@
       <c r="H64" s="59" t="n">
         <v>894</v>
       </c>
-      <c r="I64" s="89" t="n">
+      <c r="I64" s="90" t="n">
         <v>2.6136</v>
       </c>
     </row>
@@ -4749,7 +4775,7 @@
         </is>
       </c>
       <c r="D65" s="58" t="n"/>
-      <c r="E65" s="88" t="n">
+      <c r="E65" s="89" t="n">
         <v>175</v>
       </c>
       <c r="F65" s="59" t="n">
@@ -4761,7 +4787,7 @@
       <c r="H65" s="59" t="n">
         <v>780.2461</v>
       </c>
-      <c r="I65" s="89" t="n">
+      <c r="I65" s="90" t="n">
         <v>2.3339</v>
       </c>
     </row>
@@ -4775,7 +4801,7 @@
         </is>
       </c>
       <c r="D66" s="58" t="n"/>
-      <c r="E66" s="88" t="n">
+      <c r="E66" s="89" t="n">
         <v>18</v>
       </c>
       <c r="F66" s="59" t="n">
@@ -4787,7 +4813,7 @@
       <c r="H66" s="59" t="n">
         <v>80.2539</v>
       </c>
-      <c r="I66" s="89" t="n">
+      <c r="I66" s="90" t="n">
         <v>0.2401</v>
       </c>
     </row>
@@ -4801,7 +4827,7 @@
         </is>
       </c>
       <c r="D67" s="58" t="n"/>
-      <c r="E67" s="88" t="n">
+      <c r="E67" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F67" s="59" t="n">
@@ -4813,7 +4839,7 @@
       <c r="H67" s="59" t="n">
         <v>885</v>
       </c>
-      <c r="I67" s="89" t="n">
+      <c r="I67" s="90" t="n">
         <v>2.574</v>
       </c>
     </row>
@@ -4827,7 +4853,7 @@
         </is>
       </c>
       <c r="D68" s="58" t="n"/>
-      <c r="E68" s="88" t="n">
+      <c r="E68" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F68" s="59" t="n">
@@ -4839,7 +4865,7 @@
       <c r="H68" s="59" t="n">
         <v>889.5</v>
       </c>
-      <c r="I68" s="89" t="n">
+      <c r="I68" s="90" t="n">
         <v>2.772</v>
       </c>
     </row>
@@ -4853,7 +4879,7 @@
         </is>
       </c>
       <c r="D69" s="58" t="n"/>
-      <c r="E69" s="88" t="n">
+      <c r="E69" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F69" s="59" t="n">
@@ -4865,7 +4891,7 @@
       <c r="H69" s="59" t="n">
         <v>888</v>
       </c>
-      <c r="I69" s="89" t="n">
+      <c r="I69" s="90" t="n">
         <v>2.6136</v>
       </c>
     </row>
@@ -4881,7 +4907,7 @@
         </is>
       </c>
       <c r="D70" s="58" t="n"/>
-      <c r="E70" s="88" t="n">
+      <c r="E70" s="89" t="n">
         <v>106</v>
       </c>
       <c r="F70" s="59" t="n">
@@ -4893,7 +4919,7 @@
       <c r="H70" s="59" t="n">
         <v>424.9725</v>
       </c>
-      <c r="I70" s="89" t="n">
+      <c r="I70" s="90" t="n">
         <v>2.0795</v>
       </c>
     </row>
@@ -4909,7 +4935,7 @@
         </is>
       </c>
       <c r="D71" s="58" t="n"/>
-      <c r="E71" s="88" t="n">
+      <c r="E71" s="89" t="n">
         <v>3</v>
       </c>
       <c r="F71" s="59" t="n">
@@ -4921,12 +4947,12 @@
       <c r="H71" s="59" t="n">
         <v>12.0275</v>
       </c>
-      <c r="I71" s="89" t="n">
+      <c r="I71" s="90" t="n">
         <v>0.0589</v>
       </c>
     </row>
     <row r="72" ht="27" customHeight="1">
-      <c r="A72" s="55" t="n"/>
+      <c r="A72" s="91" t="n"/>
       <c r="B72" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
@@ -4934,11 +4960,11 @@
       </c>
       <c r="C72" s="55" t="n"/>
       <c r="D72" s="55" t="n"/>
-      <c r="E72" s="87" t="n"/>
+      <c r="E72" s="88" t="n"/>
       <c r="F72" s="56" t="n"/>
       <c r="G72" s="56" t="n"/>
       <c r="H72" s="56" t="n"/>
-      <c r="I72" s="85" t="n"/>
+      <c r="I72" s="86" t="n"/>
     </row>
     <row r="73" ht="27" customHeight="1">
       <c r="A73" s="55" t="n"/>
@@ -4953,7 +4979,7 @@
         </is>
       </c>
       <c r="D73" s="55" t="n"/>
-      <c r="E73" s="87">
+      <c r="E73" s="88">
         <f>SUM(E58:E71)</f>
         <v/>
       </c>
@@ -4969,41 +4995,41 @@
         <f>SUM(H58:H71)</f>
         <v/>
       </c>
-      <c r="I73" s="85">
+      <c r="I73" s="86">
         <f>SUM(I58:I71)</f>
         <v/>
       </c>
     </row>
     <row r="74" ht="27" customHeight="1">
-      <c r="A74" s="55" t="n"/>
-      <c r="B74" s="55" t="inlineStr">
+      <c r="A74" s="92" t="n"/>
+      <c r="B74" s="92" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="C74" s="55" t="inlineStr">
+      <c r="C74" s="92" t="inlineStr">
         <is>
           <t>31 PALLETS</t>
         </is>
       </c>
-      <c r="D74" s="55" t="n"/>
-      <c r="E74" s="87">
+      <c r="D74" s="92" t="n"/>
+      <c r="E74" s="93">
         <f>SUM(E23:E52,E58:E71)</f>
         <v/>
       </c>
-      <c r="F74" s="56">
+      <c r="F74" s="94">
         <f>SUM(F23:F52,F58:F71)</f>
         <v/>
       </c>
-      <c r="G74" s="56">
+      <c r="G74" s="94">
         <f>SUM(G23:G52,G58:G71)</f>
         <v/>
       </c>
-      <c r="H74" s="56">
+      <c r="H74" s="94">
         <f>SUM(H23:H52,H58:H71)</f>
         <v/>
       </c>
-      <c r="I74" s="85">
+      <c r="I74" s="95">
         <f>SUM(I23:I52,I58:I71)</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
fix the tempalte footer crash and add veritcle merge
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -263,14 +263,6 @@
       <left style="thin">
         <color rgb="00000000"/>
       </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -299,6 +291,14 @@
         <color rgb="00000000"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
     </border>
     <border>
       <left/>
@@ -337,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -495,12 +495,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -567,17 +569,19 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -592,6 +596,22 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -2308,7 +2328,11 @@
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="D22" s="58" t="n"/>
+      <c r="D22" s="58" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
       <c r="E22" s="59" t="n">
         <v>6461.7</v>
       </c>
@@ -2336,7 +2360,7 @@
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="D23" s="58" t="n"/>
+      <c r="D23" s="60" t="n"/>
       <c r="E23" s="59" t="n">
         <v>77.90000000000001</v>
       </c>
@@ -2364,7 +2388,7 @@
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D24" s="58" t="n"/>
+      <c r="D24" s="60" t="n"/>
       <c r="E24" s="59" t="n">
         <v>20949.5</v>
       </c>
@@ -2387,7 +2411,7 @@
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D25" s="58" t="n"/>
+      <c r="D25" s="60" t="n"/>
       <c r="E25" s="59" t="n">
         <v>241.9</v>
       </c>
@@ -2408,7 +2432,7 @@
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D26" s="58" t="n"/>
+      <c r="D26" s="60" t="n"/>
       <c r="E26" s="59" t="n">
         <v>28156.8</v>
       </c>
@@ -2429,7 +2453,7 @@
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D27" s="58" t="n"/>
+      <c r="D27" s="60" t="n"/>
       <c r="E27" s="59" t="n">
         <v>711.1</v>
       </c>
@@ -2450,7 +2474,7 @@
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D28" s="58" t="n"/>
+      <c r="D28" s="60" t="n"/>
       <c r="E28" s="59" t="n">
         <v>1301.4</v>
       </c>
@@ -2471,7 +2495,7 @@
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D29" s="58" t="n"/>
+      <c r="D29" s="60" t="n"/>
       <c r="E29" s="59" t="n">
         <v>18717.9</v>
       </c>
@@ -2492,7 +2516,7 @@
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D30" s="58" t="n"/>
+      <c r="D30" s="60" t="n"/>
       <c r="E30" s="59" t="n">
         <v>106711.7</v>
       </c>
@@ -2513,7 +2537,7 @@
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D31" s="58" t="n"/>
+      <c r="D31" s="60" t="n"/>
       <c r="E31" s="59" t="n">
         <v>1320.6</v>
       </c>
@@ -2534,7 +2558,7 @@
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D32" s="58" t="n"/>
+      <c r="D32" s="60" t="n"/>
       <c r="E32" s="59" t="n">
         <v>367.3</v>
       </c>
@@ -2555,7 +2579,7 @@
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D33" s="58" t="n"/>
+      <c r="D33" s="60" t="n"/>
       <c r="E33" s="59" t="n">
         <v>101424.8</v>
       </c>
@@ -2576,7 +2600,7 @@
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D34" s="58" t="n"/>
+      <c r="D34" s="60" t="n"/>
       <c r="E34" s="59" t="n">
         <v>1205.1</v>
       </c>
@@ -2599,7 +2623,7 @@
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="D35" s="58" t="n"/>
+      <c r="D35" s="60" t="n"/>
       <c r="E35" s="59" t="n">
         <v>5345</v>
       </c>
@@ -2622,7 +2646,7 @@
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="D36" s="58" t="n"/>
+      <c r="D36" s="61" t="n"/>
       <c r="E36" s="59" t="n">
         <v>121</v>
       </c>
@@ -2635,7 +2659,7 @@
       </c>
     </row>
     <row r="37" ht="35" customHeight="1">
-      <c r="A37" s="60" t="n"/>
+      <c r="A37" s="62" t="n"/>
       <c r="B37" s="54" t="inlineStr">
         <is>
           <t>HS.CODE: 4107.12.00</t>
@@ -2671,52 +2695,52 @@
       </c>
     </row>
     <row r="39" ht="61.5" customHeight="1">
-      <c r="A39" s="61" t="inlineStr">
+      <c r="A39" s="63" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B39" s="62" t="inlineStr">
+      <c r="B39" s="64" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D39" s="62" t="n"/>
-      <c r="E39" s="62" t="n"/>
+      <c r="D39" s="64" t="n"/>
+      <c r="E39" s="64" t="n"/>
       <c r="F39" s="32" t="n"/>
       <c r="G39" s="26" t="n"/>
       <c r="H39" s="2" t="n"/>
       <c r="I39" s="2" t="n"/>
       <c r="J39" s="2" t="n"/>
       <c r="K39" s="2" t="n"/>
-      <c r="L39" s="63" t="n"/>
-      <c r="M39" s="64" t="n"/>
-      <c r="N39" s="65" t="n"/>
-      <c r="O39" s="65" t="n"/>
+      <c r="L39" s="65" t="n"/>
+      <c r="M39" s="66" t="n"/>
+      <c r="N39" s="67" t="n"/>
+      <c r="O39" s="67" t="n"/>
     </row>
     <row r="40" ht="42" customHeight="1">
-      <c r="A40" s="66" t="inlineStr">
+      <c r="A40" s="68" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                                   /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="D40" s="66" t="n"/>
-      <c r="E40" s="66" t="n"/>
-      <c r="F40" s="66" t="n"/>
+      <c r="D40" s="68" t="n"/>
+      <c r="E40" s="68" t="n"/>
+      <c r="F40" s="68" t="n"/>
       <c r="G40" s="26" t="n"/>
       <c r="H40" s="2" t="n"/>
       <c r="I40" s="2" t="n"/>
       <c r="J40" s="2" t="n"/>
       <c r="K40" s="2" t="n"/>
-      <c r="L40" s="63" t="n"/>
-      <c r="M40" s="64" t="n"/>
-      <c r="N40" s="65" t="n"/>
-      <c r="O40" s="65" t="n"/>
+      <c r="L40" s="65" t="n"/>
+      <c r="M40" s="66" t="n"/>
+      <c r="N40" s="67" t="n"/>
+      <c r="O40" s="67" t="n"/>
     </row>
     <row r="41" ht="24.75" customHeight="1">
-      <c r="A41" s="67" t="inlineStr">
+      <c r="A41" s="69" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
@@ -2725,13 +2749,13 @@
       <c r="I41" s="2" t="n"/>
       <c r="J41" s="2" t="n"/>
       <c r="K41" s="2" t="n"/>
-      <c r="L41" s="63" t="n"/>
-      <c r="M41" s="64" t="n"/>
-      <c r="N41" s="65" t="n"/>
-      <c r="O41" s="65" t="n"/>
+      <c r="L41" s="65" t="n"/>
+      <c r="M41" s="66" t="n"/>
+      <c r="N41" s="67" t="n"/>
+      <c r="O41" s="67" t="n"/>
     </row>
     <row r="42" ht="27" customHeight="1">
-      <c r="A42" s="67" t="inlineStr">
+      <c r="A42" s="69" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
@@ -2740,107 +2764,107 @@
       <c r="I42" s="2" t="n"/>
       <c r="J42" s="2" t="n"/>
       <c r="K42" s="2" t="n"/>
-      <c r="L42" s="63" t="n"/>
-      <c r="M42" s="64" t="n"/>
-      <c r="N42" s="65" t="n"/>
-      <c r="O42" s="65" t="n"/>
+      <c r="L42" s="65" t="n"/>
+      <c r="M42" s="66" t="n"/>
+      <c r="N42" s="67" t="n"/>
+      <c r="O42" s="67" t="n"/>
     </row>
     <row r="43" ht="61.5" customHeight="1">
       <c r="A43" s="2" t="n"/>
       <c r="B43" s="2" t="n"/>
       <c r="C43" s="2" t="n"/>
       <c r="D43" s="2" t="n"/>
-      <c r="E43" s="68" t="inlineStr">
+      <c r="E43" s="70" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="F43" s="68" t="n"/>
-      <c r="G43" s="68" t="n"/>
-      <c r="H43" s="68" t="n"/>
+      <c r="F43" s="70" t="n"/>
+      <c r="G43" s="70" t="n"/>
+      <c r="H43" s="70" t="n"/>
       <c r="I43" s="2" t="n"/>
       <c r="J43" s="2" t="n"/>
       <c r="K43" s="2" t="n"/>
-      <c r="L43" s="63" t="n"/>
-      <c r="M43" s="64" t="n"/>
-      <c r="N43" s="65" t="n"/>
-      <c r="O43" s="65" t="n"/>
+      <c r="L43" s="65" t="n"/>
+      <c r="M43" s="66" t="n"/>
+      <c r="N43" s="67" t="n"/>
+      <c r="O43" s="67" t="n"/>
     </row>
     <row r="44" ht="42" customHeight="1">
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="2" t="n"/>
       <c r="C44" s="2" t="n"/>
-      <c r="D44" s="69" t="n"/>
-      <c r="E44" s="70" t="n"/>
-      <c r="F44" s="71" t="inlineStr">
+      <c r="D44" s="71" t="n"/>
+      <c r="E44" s="72" t="n"/>
+      <c r="F44" s="73" t="inlineStr">
         <is>
           <t>Sign &amp; Stamp</t>
         </is>
       </c>
-      <c r="G44" s="72" t="n"/>
+      <c r="G44" s="74" t="n"/>
       <c r="H44" s="2" t="n"/>
       <c r="I44" s="2" t="n"/>
       <c r="J44" s="2" t="n"/>
       <c r="K44" s="2" t="n"/>
-      <c r="L44" s="63" t="n"/>
-      <c r="M44" s="64" t="n"/>
-      <c r="N44" s="65" t="n"/>
-      <c r="O44" s="65" t="n"/>
+      <c r="L44" s="65" t="n"/>
+      <c r="M44" s="66" t="n"/>
+      <c r="N44" s="67" t="n"/>
+      <c r="O44" s="67" t="n"/>
     </row>
     <row r="45" ht="24.75" customHeight="1">
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="n"/>
       <c r="C45" s="2" t="n"/>
-      <c r="D45" s="69" t="n"/>
-      <c r="E45" s="70" t="n"/>
-      <c r="F45" s="70" t="n"/>
-      <c r="G45" s="72" t="n"/>
+      <c r="D45" s="71" t="n"/>
+      <c r="E45" s="72" t="n"/>
+      <c r="F45" s="72" t="n"/>
+      <c r="G45" s="74" t="n"/>
       <c r="H45" s="2" t="n"/>
       <c r="I45" s="2" t="n"/>
       <c r="J45" s="2" t="n"/>
       <c r="K45" s="2" t="n"/>
-      <c r="L45" s="63" t="n"/>
-      <c r="M45" s="64" t="n"/>
-      <c r="N45" s="65" t="n"/>
-      <c r="O45" s="65" t="n"/>
+      <c r="L45" s="65" t="n"/>
+      <c r="M45" s="66" t="n"/>
+      <c r="N45" s="67" t="n"/>
+      <c r="O45" s="67" t="n"/>
     </row>
     <row r="46" ht="27" customHeight="1">
       <c r="A46" s="2" t="n"/>
       <c r="B46" s="2" t="n"/>
       <c r="C46" s="2" t="n"/>
-      <c r="D46" s="69" t="n"/>
-      <c r="E46" s="70" t="n"/>
-      <c r="F46" s="70" t="n"/>
-      <c r="G46" s="72" t="n"/>
+      <c r="D46" s="71" t="n"/>
+      <c r="E46" s="72" t="n"/>
+      <c r="F46" s="72" t="n"/>
+      <c r="G46" s="74" t="n"/>
       <c r="H46" s="2" t="n"/>
       <c r="I46" s="2" t="n"/>
       <c r="J46" s="2" t="n"/>
       <c r="K46" s="2" t="n"/>
-      <c r="L46" s="63" t="n"/>
-      <c r="M46" s="64" t="n"/>
-      <c r="N46" s="65" t="n"/>
-      <c r="O46" s="65" t="n"/>
+      <c r="L46" s="65" t="n"/>
+      <c r="M46" s="66" t="n"/>
+      <c r="N46" s="67" t="n"/>
+      <c r="O46" s="67" t="n"/>
     </row>
     <row r="47" ht="21" customHeight="1">
       <c r="A47" s="2" t="n"/>
       <c r="B47" s="2" t="n"/>
       <c r="C47" s="2" t="n"/>
-      <c r="D47" s="69" t="n"/>
-      <c r="E47" s="70" t="n"/>
-      <c r="F47" s="73" t="inlineStr">
+      <c r="D47" s="71" t="n"/>
+      <c r="E47" s="72" t="n"/>
+      <c r="F47" s="75" t="inlineStr">
         <is>
           <t>ZENG XUELI</t>
         </is>
       </c>
-      <c r="G47" s="73" t="n"/>
+      <c r="G47" s="75" t="n"/>
       <c r="H47" s="2" t="n"/>
       <c r="I47" s="2" t="n"/>
       <c r="J47" s="2" t="n"/>
       <c r="K47" s="2" t="n"/>
-      <c r="L47" s="63" t="n"/>
-      <c r="M47" s="64" t="n"/>
-      <c r="N47" s="65" t="n"/>
-      <c r="O47" s="65" t="n"/>
+      <c r="L47" s="65" t="n"/>
+      <c r="M47" s="66" t="n"/>
+      <c r="N47" s="67" t="n"/>
+      <c r="O47" s="67" t="n"/>
     </row>
     <row r="48"/>
     <row r="49"/>
@@ -2996,8 +3020,9 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D22:D36"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
@@ -3174,7 +3199,7 @@
     </row>
     <row r="7" ht="18" customHeight="1">
       <c r="A7" s="32" t="n"/>
-      <c r="B7" s="74" t="n"/>
+      <c r="B7" s="76" t="n"/>
       <c r="C7" s="32" t="n"/>
       <c r="D7" s="32" t="n"/>
       <c r="E7" s="26" t="n"/>
@@ -3185,7 +3210,7 @@
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="I7" s="75" t="inlineStr">
+      <c r="I7" s="77" t="inlineStr">
         <is>
           <t>JFREF</t>
         </is>
@@ -3208,7 +3233,7 @@
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="76" t="inlineStr">
+      <c r="B8" s="78" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
@@ -3223,7 +3248,7 @@
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="I8" s="77" t="inlineStr">
+      <c r="I8" s="79" t="inlineStr">
         <is>
           <t>JFINV</t>
         </is>
@@ -3242,7 +3267,7 @@
     </row>
     <row r="9" ht="21" customHeight="1">
       <c r="A9" s="32" t="n"/>
-      <c r="B9" s="74" t="inlineStr">
+      <c r="B9" s="76" t="inlineStr">
         <is>
           <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages,</t>
         </is>
@@ -3276,7 +3301,7 @@
     </row>
     <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="32" t="n"/>
-      <c r="B10" s="74" t="inlineStr">
+      <c r="B10" s="76" t="inlineStr">
         <is>
           <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
         </is>
@@ -3291,7 +3316,7 @@
           <t>FCA :</t>
         </is>
       </c>
-      <c r="I10" s="78" t="inlineStr">
+      <c r="I10" s="80" t="inlineStr">
         <is>
           <t>BAVET, SVAY RIENG</t>
         </is>
@@ -3310,7 +3335,7 @@
     </row>
     <row r="11" ht="20.25" customHeight="1">
       <c r="A11" s="32" t="n"/>
-      <c r="B11" s="74" t="inlineStr">
+      <c r="B11" s="76" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
@@ -3336,7 +3361,7 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="n"/>
-      <c r="B12" s="74" t="n"/>
+      <c r="B12" s="76" t="n"/>
       <c r="C12" s="32" t="n"/>
       <c r="D12" s="32" t="n"/>
       <c r="E12" s="26" t="n"/>
@@ -3362,7 +3387,7 @@
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="79" t="inlineStr">
+      <c r="B13" s="81" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
@@ -3370,9 +3395,9 @@
       <c r="C13" s="2" t="n"/>
       <c r="D13" s="2" t="n"/>
       <c r="E13" s="2" t="n"/>
-      <c r="F13" s="80" t="n"/>
-      <c r="G13" s="80" t="n"/>
-      <c r="H13" s="80" t="n"/>
+      <c r="F13" s="82" t="n"/>
+      <c r="G13" s="82" t="n"/>
+      <c r="H13" s="82" t="n"/>
       <c r="I13" s="45" t="n"/>
       <c r="J13" s="2" t="n"/>
       <c r="K13" s="2" t="n"/>
@@ -3388,17 +3413,17 @@
     </row>
     <row r="14" ht="25.5" customHeight="1">
       <c r="A14" s="32" t="n"/>
-      <c r="B14" s="81" t="inlineStr">
+      <c r="B14" s="83" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
       <c r="C14" s="47" t="n"/>
       <c r="D14" s="47" t="n"/>
-      <c r="E14" s="82" t="n"/>
-      <c r="F14" s="82" t="n"/>
-      <c r="G14" s="82" t="n"/>
-      <c r="H14" s="82" t="n"/>
+      <c r="E14" s="84" t="n"/>
+      <c r="F14" s="84" t="n"/>
+      <c r="G14" s="84" t="n"/>
+      <c r="H14" s="84" t="n"/>
       <c r="I14" s="2" t="n"/>
       <c r="J14" s="2" t="n"/>
       <c r="K14" s="2" t="n"/>
@@ -3414,7 +3439,7 @@
     </row>
     <row r="15" ht="21" customHeight="1">
       <c r="A15" s="32" t="n"/>
-      <c r="B15" s="83" t="inlineStr">
+      <c r="B15" s="85" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
         </is>
@@ -3522,7 +3547,7 @@
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B19" s="74" t="inlineStr">
+      <c r="B19" s="76" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
         </is>
@@ -3548,7 +3573,7 @@
     </row>
     <row r="20" ht="27.75" customHeight="1">
       <c r="A20" s="53" t="n"/>
-      <c r="B20" s="84" t="n"/>
+      <c r="B20" s="86" t="n"/>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
@@ -3594,7 +3619,7 @@
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F21" s="85" t="n"/>
+      <c r="F21" s="87" t="n"/>
       <c r="G21" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -3605,7 +3630,7 @@
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I21" s="86" t="inlineStr">
+      <c r="I21" s="88" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
@@ -3623,11 +3648,11 @@
       <c r="T21" s="2" t="n"/>
     </row>
     <row r="22" ht="27" customHeight="1">
-      <c r="A22" s="87" t="n"/>
-      <c r="B22" s="87" t="n"/>
-      <c r="C22" s="87" t="n"/>
-      <c r="D22" s="87" t="n"/>
-      <c r="E22" s="88" t="inlineStr">
+      <c r="A22" s="61" t="n"/>
+      <c r="B22" s="61" t="n"/>
+      <c r="C22" s="61" t="n"/>
+      <c r="D22" s="61" t="n"/>
+      <c r="E22" s="89" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
@@ -3637,28 +3662,32 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="G22" s="87" t="n"/>
-      <c r="H22" s="87" t="n"/>
-      <c r="I22" s="87" t="n"/>
+      <c r="G22" s="61" t="n"/>
+      <c r="H22" s="61" t="n"/>
+      <c r="I22" s="61" t="n"/>
     </row>
     <row r="23" ht="27" customHeight="1">
-      <c r="A23" s="58" t="inlineStr">
+      <c r="A23" s="90" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B23" s="58" t="inlineStr">
+      <c r="B23" s="90" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="C23" s="58" t="inlineStr">
+      <c r="C23" s="90" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="D23" s="58" t="n"/>
-      <c r="E23" s="89" t="n">
+      <c r="D23" s="58" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E23" s="91" t="n">
         <v>122</v>
       </c>
       <c r="F23" s="59" t="n">
@@ -3670,28 +3699,28 @@
       <c r="H23" s="59" t="n">
         <v>512.1048</v>
       </c>
-      <c r="I23" s="90" t="n">
+      <c r="I23" s="92" t="n">
         <v>1.8312</v>
       </c>
     </row>
     <row r="24" ht="27" customHeight="1">
-      <c r="A24" s="58" t="inlineStr">
+      <c r="A24" s="90" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B24" s="58" t="inlineStr">
+      <c r="B24" s="90" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="C24" s="58" t="inlineStr">
+      <c r="C24" s="90" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="D24" s="58" t="n"/>
-      <c r="E24" s="89" t="n">
+      <c r="D24" s="60" t="n"/>
+      <c r="E24" s="91" t="n">
         <v>2</v>
       </c>
       <c r="F24" s="59" t="n">
@@ -3703,28 +3732,28 @@
       <c r="H24" s="59" t="n">
         <v>8.395200000000001</v>
       </c>
-      <c r="I24" s="90" t="n">
+      <c r="I24" s="92" t="n">
         <v>0.03</v>
       </c>
     </row>
     <row r="25" ht="27" customHeight="1">
-      <c r="A25" s="58" t="inlineStr">
+      <c r="A25" s="90" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B25" s="58" t="inlineStr">
+      <c r="B25" s="90" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C25" s="58" t="inlineStr">
+      <c r="C25" s="90" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D25" s="58" t="n"/>
-      <c r="E25" s="89" t="n">
+      <c r="D25" s="60" t="n"/>
+      <c r="E25" s="91" t="n">
         <v>190</v>
       </c>
       <c r="F25" s="59" t="n">
@@ -3736,28 +3765,28 @@
       <c r="H25" s="59" t="n">
         <v>802</v>
       </c>
-      <c r="I25" s="90" t="n">
+      <c r="I25" s="92" t="n">
         <v>2.4552</v>
       </c>
     </row>
     <row r="26" ht="27" customHeight="1">
-      <c r="A26" s="58" t="inlineStr">
+      <c r="A26" s="90" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B26" s="58" t="inlineStr">
+      <c r="B26" s="90" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C26" s="58" t="inlineStr">
+      <c r="C26" s="90" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D26" s="58" t="n"/>
-      <c r="E26" s="89" t="n">
+      <c r="D26" s="60" t="n"/>
+      <c r="E26" s="91" t="n">
         <v>208</v>
       </c>
       <c r="F26" s="59" t="n">
@@ -3769,23 +3798,23 @@
       <c r="H26" s="59" t="n">
         <v>885.9439</v>
       </c>
-      <c r="I26" s="90" t="n">
+      <c r="I26" s="92" t="n">
         <v>2.6943</v>
       </c>
     </row>
     <row r="27" ht="27" customHeight="1">
-      <c r="B27" s="58" t="inlineStr">
+      <c r="B27" s="90" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C27" s="58" t="inlineStr">
+      <c r="C27" s="90" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D27" s="58" t="n"/>
-      <c r="E27" s="89" t="n">
+      <c r="D27" s="60" t="n"/>
+      <c r="E27" s="91" t="n">
         <v>6</v>
       </c>
       <c r="F27" s="59" t="n">
@@ -3797,21 +3826,21 @@
       <c r="H27" s="59" t="n">
         <v>25.5561</v>
       </c>
-      <c r="I27" s="90" t="n">
+      <c r="I27" s="92" t="n">
         <v>0.07770000000000001</v>
       </c>
     </row>
     <row r="28" ht="27" customHeight="1">
-      <c r="B28" s="58" t="n">
+      <c r="B28" s="90" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C28" s="58" t="inlineStr">
+      <c r="C28" s="90" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D28" s="58" t="n"/>
-      <c r="E28" s="89" t="n">
+      <c r="D28" s="60" t="n"/>
+      <c r="E28" s="91" t="n">
         <v>154</v>
       </c>
       <c r="F28" s="59" t="n">
@@ -3823,21 +3852,21 @@
       <c r="H28" s="59" t="n">
         <v>658.0814</v>
       </c>
-      <c r="I28" s="90" t="n">
+      <c r="I28" s="92" t="n">
         <v>2.0564</v>
       </c>
     </row>
     <row r="29" ht="27" customHeight="1">
-      <c r="B29" s="58" t="n">
+      <c r="B29" s="90" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C29" s="58" t="inlineStr">
+      <c r="C29" s="90" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D29" s="58" t="n"/>
-      <c r="E29" s="89" t="n">
+      <c r="D29" s="60" t="n"/>
+      <c r="E29" s="91" t="n">
         <v>18</v>
       </c>
       <c r="F29" s="59" t="n">
@@ -3849,21 +3878,21 @@
       <c r="H29" s="59" t="n">
         <v>76.9186</v>
       </c>
-      <c r="I29" s="90" t="n">
+      <c r="I29" s="92" t="n">
         <v>0.2404</v>
       </c>
     </row>
     <row r="30" ht="27" customHeight="1">
-      <c r="B30" s="58" t="n">
+      <c r="B30" s="90" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C30" s="58" t="inlineStr">
+      <c r="C30" s="90" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D30" s="58" t="n"/>
-      <c r="E30" s="89" t="n">
+      <c r="D30" s="60" t="n"/>
+      <c r="E30" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F30" s="59" t="n">
@@ -3875,21 +3904,21 @@
       <c r="H30" s="59" t="n">
         <v>859.5</v>
       </c>
-      <c r="I30" s="90" t="n">
+      <c r="I30" s="92" t="n">
         <v>2.376</v>
       </c>
     </row>
     <row r="31" ht="27" customHeight="1">
-      <c r="B31" s="58" t="n">
+      <c r="B31" s="90" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C31" s="58" t="inlineStr">
+      <c r="C31" s="90" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D31" s="58" t="n"/>
-      <c r="E31" s="89" t="n">
+      <c r="D31" s="60" t="n"/>
+      <c r="E31" s="91" t="n">
         <v>200</v>
       </c>
       <c r="F31" s="59" t="n">
@@ -3901,21 +3930,21 @@
       <c r="H31" s="59" t="n">
         <v>780.1762</v>
       </c>
-      <c r="I31" s="90" t="n">
+      <c r="I31" s="92" t="n">
         <v>2.2678</v>
       </c>
     </row>
     <row r="32" ht="27" customHeight="1">
-      <c r="B32" s="58" t="n">
+      <c r="B32" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C32" s="58" t="inlineStr">
+      <c r="C32" s="90" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D32" s="58" t="n"/>
-      <c r="E32" s="89" t="n">
+      <c r="D32" s="60" t="n"/>
+      <c r="E32" s="91" t="n">
         <v>27</v>
       </c>
       <c r="F32" s="59" t="n">
@@ -3927,21 +3956,21 @@
       <c r="H32" s="59" t="n">
         <v>105.3238</v>
       </c>
-      <c r="I32" s="90" t="n">
+      <c r="I32" s="92" t="n">
         <v>0.3062</v>
       </c>
     </row>
     <row r="33" ht="27" customHeight="1">
-      <c r="B33" s="58" t="n">
+      <c r="B33" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C33" s="58" t="inlineStr">
+      <c r="C33" s="90" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D33" s="58" t="n"/>
-      <c r="E33" s="89" t="n">
+      <c r="D33" s="60" t="n"/>
+      <c r="E33" s="91" t="n">
         <v>169</v>
       </c>
       <c r="F33" s="59" t="n">
@@ -3953,21 +3982,21 @@
       <c r="H33" s="59" t="n">
         <v>736.84</v>
       </c>
-      <c r="I33" s="90" t="n">
+      <c r="I33" s="92" t="n">
         <v>2.2181</v>
       </c>
     </row>
     <row r="34" ht="27" customHeight="1">
-      <c r="B34" s="58" t="n">
+      <c r="B34" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C34" s="58" t="inlineStr">
+      <c r="C34" s="90" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D34" s="58" t="n"/>
-      <c r="E34" s="89" t="n">
+      <c r="D34" s="60" t="n"/>
+      <c r="E34" s="91" t="n">
         <v>6</v>
       </c>
       <c r="F34" s="59" t="n">
@@ -3979,21 +4008,21 @@
       <c r="H34" s="59" t="n">
         <v>26.16</v>
       </c>
-      <c r="I34" s="90" t="n">
+      <c r="I34" s="92" t="n">
         <v>0.07870000000000001</v>
       </c>
     </row>
     <row r="35" ht="27" customHeight="1">
-      <c r="B35" s="58" t="n">
+      <c r="B35" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C35" s="58" t="inlineStr">
+      <c r="C35" s="90" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D35" s="58" t="n"/>
-      <c r="E35" s="89" t="n">
+      <c r="D35" s="60" t="n"/>
+      <c r="E35" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F35" s="59" t="n">
@@ -4005,21 +4034,21 @@
       <c r="H35" s="59" t="n">
         <v>859.5</v>
       </c>
-      <c r="I35" s="90" t="n">
+      <c r="I35" s="92" t="n">
         <v>2.376</v>
       </c>
     </row>
     <row r="36" ht="27" customHeight="1">
-      <c r="B36" s="58" t="n">
+      <c r="B36" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C36" s="58" t="inlineStr">
+      <c r="C36" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D36" s="58" t="n"/>
-      <c r="E36" s="89" t="n">
+      <c r="D36" s="60" t="n"/>
+      <c r="E36" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F36" s="59" t="n">
@@ -4031,21 +4060,21 @@
       <c r="H36" s="59" t="n">
         <v>875.5</v>
       </c>
-      <c r="I36" s="90" t="n">
+      <c r="I36" s="92" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="37" ht="27" customHeight="1">
-      <c r="B37" s="58" t="n">
+      <c r="B37" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C37" s="58" t="inlineStr">
+      <c r="C37" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D37" s="58" t="n"/>
-      <c r="E37" s="89" t="n">
+      <c r="D37" s="60" t="n"/>
+      <c r="E37" s="91" t="n">
         <v>215</v>
       </c>
       <c r="F37" s="59" t="n">
@@ -4057,21 +4086,21 @@
       <c r="H37" s="59" t="n">
         <v>946.5</v>
       </c>
-      <c r="I37" s="90" t="n">
+      <c r="I37" s="92" t="n">
         <v>2.97</v>
       </c>
     </row>
     <row r="38" ht="27" customHeight="1">
-      <c r="B38" s="58" t="n">
+      <c r="B38" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C38" s="58" t="inlineStr">
+      <c r="C38" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D38" s="58" t="n"/>
-      <c r="E38" s="89" t="n">
+      <c r="D38" s="60" t="n"/>
+      <c r="E38" s="91" t="n">
         <v>215</v>
       </c>
       <c r="F38" s="59" t="n">
@@ -4083,21 +4112,21 @@
       <c r="H38" s="59" t="n">
         <v>963</v>
       </c>
-      <c r="I38" s="90" t="n">
+      <c r="I38" s="92" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="39" ht="27" customHeight="1">
-      <c r="B39" s="58" t="n">
+      <c r="B39" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C39" s="58" t="inlineStr">
+      <c r="C39" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D39" s="58" t="n"/>
-      <c r="E39" s="89" t="n">
+      <c r="D39" s="60" t="n"/>
+      <c r="E39" s="91" t="n">
         <v>192</v>
       </c>
       <c r="F39" s="59" t="n">
@@ -4109,21 +4138,21 @@
       <c r="H39" s="59" t="n">
         <v>836.9709</v>
       </c>
-      <c r="I39" s="90" t="n">
+      <c r="I39" s="92" t="n">
         <v>2.4729</v>
       </c>
     </row>
     <row r="40" ht="27" customHeight="1">
-      <c r="B40" s="58" t="n">
+      <c r="B40" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C40" s="58" t="inlineStr">
+      <c r="C40" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D40" s="58" t="n"/>
-      <c r="E40" s="89" t="n">
+      <c r="D40" s="60" t="n"/>
+      <c r="E40" s="91" t="n">
         <v>14</v>
       </c>
       <c r="F40" s="59" t="n">
@@ -4135,21 +4164,21 @@
       <c r="H40" s="59" t="n">
         <v>61.0291</v>
       </c>
-      <c r="I40" s="90" t="n">
+      <c r="I40" s="92" t="n">
         <v>0.1803</v>
       </c>
     </row>
     <row r="41" ht="27" customHeight="1">
-      <c r="B41" s="58" t="n">
+      <c r="B41" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C41" s="58" t="inlineStr">
+      <c r="C41" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D41" s="58" t="n"/>
-      <c r="E41" s="89" t="n">
+      <c r="D41" s="60" t="n"/>
+      <c r="E41" s="91" t="n">
         <v>97</v>
       </c>
       <c r="F41" s="59" t="n">
@@ -4161,21 +4190,21 @@
       <c r="H41" s="59" t="n">
         <v>453</v>
       </c>
-      <c r="I41" s="90" t="n">
+      <c r="I41" s="92" t="n">
         <v>1.782</v>
       </c>
     </row>
     <row r="42" ht="27" customHeight="1">
-      <c r="B42" s="58" t="n">
+      <c r="B42" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C42" s="58" t="inlineStr">
+      <c r="C42" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D42" s="58" t="n"/>
-      <c r="E42" s="89" t="n">
+      <c r="D42" s="60" t="n"/>
+      <c r="E42" s="91" t="n">
         <v>97</v>
       </c>
       <c r="F42" s="59" t="n">
@@ -4187,21 +4216,21 @@
       <c r="H42" s="59" t="n">
         <v>452</v>
       </c>
-      <c r="I42" s="90" t="n">
+      <c r="I42" s="92" t="n">
         <v>1.8216</v>
       </c>
     </row>
     <row r="43" ht="27" customHeight="1">
-      <c r="B43" s="58" t="n">
+      <c r="B43" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C43" s="58" t="inlineStr">
+      <c r="C43" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D43" s="58" t="n"/>
-      <c r="E43" s="89" t="n">
+      <c r="D43" s="60" t="n"/>
+      <c r="E43" s="91" t="n">
         <v>184</v>
       </c>
       <c r="F43" s="59" t="n">
@@ -4213,21 +4242,21 @@
       <c r="H43" s="59" t="n">
         <v>817.3474</v>
       </c>
-      <c r="I43" s="90" t="n">
+      <c r="I43" s="92" t="n">
         <v>2.6461</v>
       </c>
     </row>
     <row r="44" ht="27" customHeight="1">
-      <c r="B44" s="58" t="n">
+      <c r="B44" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C44" s="58" t="inlineStr">
+      <c r="C44" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D44" s="58" t="n"/>
-      <c r="E44" s="89" t="n">
+      <c r="D44" s="60" t="n"/>
+      <c r="E44" s="91" t="n">
         <v>6</v>
       </c>
       <c r="F44" s="59" t="n">
@@ -4239,21 +4268,21 @@
       <c r="H44" s="59" t="n">
         <v>26.6526</v>
       </c>
-      <c r="I44" s="90" t="n">
+      <c r="I44" s="92" t="n">
         <v>0.0863</v>
       </c>
     </row>
     <row r="45" ht="27" customHeight="1">
-      <c r="B45" s="58" t="n">
+      <c r="B45" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C45" s="58" t="inlineStr">
+      <c r="C45" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D45" s="58" t="n"/>
-      <c r="E45" s="89" t="n">
+      <c r="D45" s="60" t="n"/>
+      <c r="E45" s="91" t="n">
         <v>185</v>
       </c>
       <c r="F45" s="59" t="n">
@@ -4265,21 +4294,21 @@
       <c r="H45" s="59" t="n">
         <v>830.0658</v>
       </c>
-      <c r="I45" s="90" t="n">
+      <c r="I45" s="92" t="n">
         <v>2.5063</v>
       </c>
     </row>
     <row r="46" ht="27" customHeight="1">
-      <c r="B46" s="58" t="n">
+      <c r="B46" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C46" s="58" t="inlineStr">
+      <c r="C46" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D46" s="58" t="n"/>
-      <c r="E46" s="89" t="n">
+      <c r="D46" s="60" t="n"/>
+      <c r="E46" s="91" t="n">
         <v>5</v>
       </c>
       <c r="F46" s="59" t="n">
@@ -4291,21 +4320,21 @@
       <c r="H46" s="59" t="n">
         <v>22.4342</v>
       </c>
-      <c r="I46" s="90" t="n">
+      <c r="I46" s="92" t="n">
         <v>0.0677</v>
       </c>
     </row>
     <row r="47" ht="27" customHeight="1">
-      <c r="B47" s="58" t="n">
+      <c r="B47" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C47" s="58" t="inlineStr">
+      <c r="C47" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D47" s="58" t="n"/>
-      <c r="E47" s="89" t="n">
+      <c r="D47" s="60" t="n"/>
+      <c r="E47" s="91" t="n">
         <v>190</v>
       </c>
       <c r="F47" s="59" t="n">
@@ -4317,21 +4346,21 @@
       <c r="H47" s="59" t="n">
         <v>869</v>
       </c>
-      <c r="I47" s="90" t="n">
+      <c r="I47" s="92" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="48" ht="27" customHeight="1">
-      <c r="B48" s="58" t="n">
+      <c r="B48" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C48" s="58" t="inlineStr">
+      <c r="C48" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D48" s="58" t="n"/>
-      <c r="E48" s="89" t="n">
+      <c r="D48" s="60" t="n"/>
+      <c r="E48" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F48" s="59" t="n">
@@ -4343,21 +4372,21 @@
       <c r="H48" s="59" t="n">
         <v>866</v>
       </c>
-      <c r="I48" s="90" t="n">
+      <c r="I48" s="92" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="49" ht="27" customHeight="1">
-      <c r="B49" s="58" t="n">
+      <c r="B49" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C49" s="58" t="inlineStr">
+      <c r="C49" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D49" s="58" t="n"/>
-      <c r="E49" s="89" t="n">
+      <c r="D49" s="60" t="n"/>
+      <c r="E49" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F49" s="59" t="n">
@@ -4369,21 +4398,21 @@
       <c r="H49" s="59" t="n">
         <v>870.5</v>
       </c>
-      <c r="I49" s="90" t="n">
+      <c r="I49" s="92" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="50" ht="27" customHeight="1">
-      <c r="B50" s="58" t="n">
+      <c r="B50" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C50" s="58" t="inlineStr">
+      <c r="C50" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D50" s="58" t="n"/>
-      <c r="E50" s="89" t="n">
+      <c r="D50" s="60" t="n"/>
+      <c r="E50" s="91" t="n">
         <v>89</v>
       </c>
       <c r="F50" s="59" t="n">
@@ -4395,21 +4424,21 @@
       <c r="H50" s="59" t="n">
         <v>415.0481</v>
       </c>
-      <c r="I50" s="90" t="n">
+      <c r="I50" s="92" t="n">
         <v>1.4572</v>
       </c>
     </row>
     <row r="51" ht="27" customHeight="1">
-      <c r="B51" s="58" t="n">
+      <c r="B51" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C51" s="58" t="inlineStr">
+      <c r="C51" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D51" s="58" t="n"/>
-      <c r="E51" s="89" t="n">
+      <c r="D51" s="60" t="n"/>
+      <c r="E51" s="91" t="n">
         <v>8</v>
       </c>
       <c r="F51" s="59" t="n">
@@ -4421,21 +4450,21 @@
       <c r="H51" s="59" t="n">
         <v>37.3077</v>
       </c>
-      <c r="I51" s="90" t="n">
+      <c r="I51" s="92" t="n">
         <v>0.131</v>
       </c>
     </row>
     <row r="52" ht="27" customHeight="1">
-      <c r="B52" s="58" t="n">
+      <c r="B52" s="90" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C52" s="58" t="inlineStr">
+      <c r="C52" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D52" s="58" t="n"/>
-      <c r="E52" s="89" t="n">
+      <c r="D52" s="61" t="n"/>
+      <c r="E52" s="91" t="n">
         <v>7</v>
       </c>
       <c r="F52" s="59" t="n">
@@ -4447,12 +4476,12 @@
       <c r="H52" s="59" t="n">
         <v>32.6442</v>
       </c>
-      <c r="I52" s="90" t="n">
+      <c r="I52" s="92" t="n">
         <v>0.1146</v>
       </c>
     </row>
     <row r="53" ht="27" customHeight="1">
-      <c r="A53" s="91" t="n"/>
+      <c r="A53" s="93" t="n"/>
       <c r="B53" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
@@ -4460,11 +4489,11 @@
       </c>
       <c r="C53" s="55" t="n"/>
       <c r="D53" s="55" t="n"/>
-      <c r="E53" s="88" t="n"/>
+      <c r="E53" s="89" t="n"/>
       <c r="F53" s="56" t="n"/>
       <c r="G53" s="56" t="n"/>
       <c r="H53" s="56" t="n"/>
-      <c r="I53" s="86" t="n"/>
+      <c r="I53" s="88" t="n"/>
     </row>
     <row r="54" ht="27" customHeight="1">
       <c r="A54" s="55" t="n"/>
@@ -4479,7 +4508,7 @@
         </is>
       </c>
       <c r="D54" s="55" t="n"/>
-      <c r="E54" s="88">
+      <c r="E54" s="89">
         <f>SUM(E23:E52)</f>
         <v/>
       </c>
@@ -4495,7 +4524,7 @@
         <f>SUM(H23:H52)</f>
         <v/>
       </c>
-      <c r="I54" s="86">
+      <c r="I54" s="88">
         <f>SUM(I23:I52)</f>
         <v/>
       </c>
@@ -4527,7 +4556,7 @@
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F56" s="85" t="n"/>
+      <c r="F56" s="87" t="n"/>
       <c r="G56" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -4538,18 +4567,18 @@
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I56" s="86" t="inlineStr">
+      <c r="I56" s="88" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
     <row r="57" ht="27" customHeight="1">
-      <c r="A57" s="87" t="n"/>
-      <c r="B57" s="87" t="n"/>
-      <c r="C57" s="87" t="n"/>
-      <c r="D57" s="87" t="n"/>
-      <c r="E57" s="88" t="inlineStr">
+      <c r="A57" s="61" t="n"/>
+      <c r="B57" s="61" t="n"/>
+      <c r="C57" s="61" t="n"/>
+      <c r="D57" s="61" t="n"/>
+      <c r="E57" s="89" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
@@ -4559,26 +4588,30 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="G57" s="87" t="n"/>
-      <c r="H57" s="87" t="n"/>
-      <c r="I57" s="87" t="n"/>
+      <c r="G57" s="61" t="n"/>
+      <c r="H57" s="61" t="n"/>
+      <c r="I57" s="61" t="n"/>
     </row>
     <row r="58" ht="27" customHeight="1">
-      <c r="A58" s="58" t="inlineStr">
+      <c r="A58" s="90" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B58" s="58" t="n">
+      <c r="B58" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C58" s="58" t="inlineStr">
+      <c r="C58" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D58" s="58" t="n"/>
-      <c r="E58" s="89" t="n">
+      <c r="D58" s="58" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="E58" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F58" s="59" t="n">
@@ -4590,26 +4623,26 @@
       <c r="H58" s="59" t="n">
         <v>887.5</v>
       </c>
-      <c r="I58" s="90" t="n">
+      <c r="I58" s="92" t="n">
         <v>2.6532</v>
       </c>
     </row>
     <row r="59" ht="27" customHeight="1">
-      <c r="A59" s="58" t="inlineStr">
+      <c r="A59" s="90" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B59" s="58" t="n">
+      <c r="B59" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C59" s="58" t="inlineStr">
+      <c r="C59" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D59" s="58" t="n"/>
-      <c r="E59" s="89" t="n">
+      <c r="D59" s="60" t="n"/>
+      <c r="E59" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F59" s="59" t="n">
@@ -4621,26 +4654,26 @@
       <c r="H59" s="59" t="n">
         <v>891</v>
       </c>
-      <c r="I59" s="90" t="n">
+      <c r="I59" s="92" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="60" ht="27" customHeight="1">
-      <c r="A60" s="58" t="inlineStr">
+      <c r="A60" s="90" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B60" s="58" t="n">
+      <c r="B60" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C60" s="58" t="inlineStr">
+      <c r="C60" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D60" s="58" t="n"/>
-      <c r="E60" s="89" t="n">
+      <c r="D60" s="60" t="n"/>
+      <c r="E60" s="91" t="n">
         <v>207</v>
       </c>
       <c r="F60" s="59" t="n">
@@ -4652,26 +4685,26 @@
       <c r="H60" s="59" t="n">
         <v>926.3013999999999</v>
       </c>
-      <c r="I60" s="90" t="n">
+      <c r="I60" s="92" t="n">
         <v>2.8447</v>
       </c>
     </row>
     <row r="61" ht="27" customHeight="1">
-      <c r="A61" s="58" t="inlineStr">
+      <c r="A61" s="90" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B61" s="58" t="n">
+      <c r="B61" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C61" s="58" t="inlineStr">
+      <c r="C61" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D61" s="58" t="n"/>
-      <c r="E61" s="89" t="n">
+      <c r="D61" s="60" t="n"/>
+      <c r="E61" s="91" t="n">
         <v>12</v>
       </c>
       <c r="F61" s="59" t="n">
@@ -4683,21 +4716,21 @@
       <c r="H61" s="59" t="n">
         <v>53.6986</v>
       </c>
-      <c r="I61" s="90" t="n">
+      <c r="I61" s="92" t="n">
         <v>0.1649</v>
       </c>
     </row>
     <row r="62" ht="27" customHeight="1">
-      <c r="B62" s="58" t="n">
+      <c r="B62" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C62" s="58" t="inlineStr">
+      <c r="C62" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D62" s="58" t="n"/>
-      <c r="E62" s="89" t="n">
+      <c r="D62" s="60" t="n"/>
+      <c r="E62" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F62" s="59" t="n">
@@ -4709,21 +4742,21 @@
       <c r="H62" s="59" t="n">
         <v>885</v>
       </c>
-      <c r="I62" s="90" t="n">
+      <c r="I62" s="92" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="63" ht="27" customHeight="1">
-      <c r="B63" s="58" t="n">
+      <c r="B63" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C63" s="58" t="inlineStr">
+      <c r="C63" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D63" s="58" t="n"/>
-      <c r="E63" s="89" t="n">
+      <c r="D63" s="60" t="n"/>
+      <c r="E63" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F63" s="59" t="n">
@@ -4735,21 +4768,21 @@
       <c r="H63" s="59" t="n">
         <v>908.5</v>
       </c>
-      <c r="I63" s="90" t="n">
+      <c r="I63" s="92" t="n">
         <v>2.6928</v>
       </c>
     </row>
     <row r="64" ht="27" customHeight="1">
-      <c r="B64" s="58" t="n">
+      <c r="B64" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C64" s="58" t="inlineStr">
+      <c r="C64" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D64" s="58" t="n"/>
-      <c r="E64" s="89" t="n">
+      <c r="D64" s="60" t="n"/>
+      <c r="E64" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F64" s="59" t="n">
@@ -4761,21 +4794,21 @@
       <c r="H64" s="59" t="n">
         <v>894</v>
       </c>
-      <c r="I64" s="90" t="n">
+      <c r="I64" s="92" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="65" ht="27" customHeight="1">
-      <c r="B65" s="58" t="n">
+      <c r="B65" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C65" s="58" t="inlineStr">
+      <c r="C65" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D65" s="58" t="n"/>
-      <c r="E65" s="89" t="n">
+      <c r="D65" s="60" t="n"/>
+      <c r="E65" s="91" t="n">
         <v>175</v>
       </c>
       <c r="F65" s="59" t="n">
@@ -4787,21 +4820,21 @@
       <c r="H65" s="59" t="n">
         <v>780.2461</v>
       </c>
-      <c r="I65" s="90" t="n">
+      <c r="I65" s="92" t="n">
         <v>2.3339</v>
       </c>
     </row>
     <row r="66" ht="27" customHeight="1">
-      <c r="B66" s="58" t="n">
+      <c r="B66" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C66" s="58" t="inlineStr">
+      <c r="C66" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D66" s="58" t="n"/>
-      <c r="E66" s="89" t="n">
+      <c r="D66" s="60" t="n"/>
+      <c r="E66" s="91" t="n">
         <v>18</v>
       </c>
       <c r="F66" s="59" t="n">
@@ -4813,21 +4846,21 @@
       <c r="H66" s="59" t="n">
         <v>80.2539</v>
       </c>
-      <c r="I66" s="90" t="n">
+      <c r="I66" s="92" t="n">
         <v>0.2401</v>
       </c>
     </row>
     <row r="67" ht="27" customHeight="1">
-      <c r="B67" s="58" t="n">
+      <c r="B67" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C67" s="58" t="inlineStr">
+      <c r="C67" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D67" s="58" t="n"/>
-      <c r="E67" s="89" t="n">
+      <c r="D67" s="60" t="n"/>
+      <c r="E67" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F67" s="59" t="n">
@@ -4839,21 +4872,21 @@
       <c r="H67" s="59" t="n">
         <v>885</v>
       </c>
-      <c r="I67" s="90" t="n">
+      <c r="I67" s="92" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="68" ht="27" customHeight="1">
-      <c r="B68" s="58" t="n">
+      <c r="B68" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C68" s="58" t="inlineStr">
+      <c r="C68" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D68" s="58" t="n"/>
-      <c r="E68" s="89" t="n">
+      <c r="D68" s="60" t="n"/>
+      <c r="E68" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F68" s="59" t="n">
@@ -4865,21 +4898,21 @@
       <c r="H68" s="59" t="n">
         <v>889.5</v>
       </c>
-      <c r="I68" s="90" t="n">
+      <c r="I68" s="92" t="n">
         <v>2.772</v>
       </c>
     </row>
     <row r="69" ht="27" customHeight="1">
-      <c r="B69" s="58" t="n">
+      <c r="B69" s="90" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C69" s="58" t="inlineStr">
+      <c r="C69" s="90" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D69" s="58" t="n"/>
-      <c r="E69" s="89" t="n">
+      <c r="D69" s="60" t="n"/>
+      <c r="E69" s="91" t="n">
         <v>195</v>
       </c>
       <c r="F69" s="59" t="n">
@@ -4891,23 +4924,23 @@
       <c r="H69" s="59" t="n">
         <v>888</v>
       </c>
-      <c r="I69" s="90" t="n">
+      <c r="I69" s="92" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="70" ht="27" customHeight="1">
-      <c r="B70" s="58" t="inlineStr">
+      <c r="B70" s="90" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="C70" s="58" t="inlineStr">
+      <c r="C70" s="90" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="D70" s="58" t="n"/>
-      <c r="E70" s="89" t="n">
+      <c r="D70" s="60" t="n"/>
+      <c r="E70" s="91" t="n">
         <v>106</v>
       </c>
       <c r="F70" s="59" t="n">
@@ -4919,23 +4952,23 @@
       <c r="H70" s="59" t="n">
         <v>424.9725</v>
       </c>
-      <c r="I70" s="90" t="n">
+      <c r="I70" s="92" t="n">
         <v>2.0795</v>
       </c>
     </row>
     <row r="71" ht="27" customHeight="1">
-      <c r="B71" s="58" t="inlineStr">
+      <c r="B71" s="90" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="C71" s="58" t="inlineStr">
+      <c r="C71" s="90" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="D71" s="58" t="n"/>
-      <c r="E71" s="89" t="n">
+      <c r="D71" s="61" t="n"/>
+      <c r="E71" s="91" t="n">
         <v>3</v>
       </c>
       <c r="F71" s="59" t="n">
@@ -4947,12 +4980,12 @@
       <c r="H71" s="59" t="n">
         <v>12.0275</v>
       </c>
-      <c r="I71" s="90" t="n">
+      <c r="I71" s="92" t="n">
         <v>0.0589</v>
       </c>
     </row>
     <row r="72" ht="27" customHeight="1">
-      <c r="A72" s="91" t="n"/>
+      <c r="A72" s="93" t="n"/>
       <c r="B72" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
@@ -4960,11 +4993,11 @@
       </c>
       <c r="C72" s="55" t="n"/>
       <c r="D72" s="55" t="n"/>
-      <c r="E72" s="88" t="n"/>
+      <c r="E72" s="89" t="n"/>
       <c r="F72" s="56" t="n"/>
       <c r="G72" s="56" t="n"/>
       <c r="H72" s="56" t="n"/>
-      <c r="I72" s="86" t="n"/>
+      <c r="I72" s="88" t="n"/>
     </row>
     <row r="73" ht="27" customHeight="1">
       <c r="A73" s="55" t="n"/>
@@ -4979,7 +5012,7 @@
         </is>
       </c>
       <c r="D73" s="55" t="n"/>
-      <c r="E73" s="88">
+      <c r="E73" s="89">
         <f>SUM(E58:E71)</f>
         <v/>
       </c>
@@ -4995,54 +5028,58 @@
         <f>SUM(H58:H71)</f>
         <v/>
       </c>
-      <c r="I73" s="86">
+      <c r="I73" s="88">
         <f>SUM(I58:I71)</f>
         <v/>
       </c>
     </row>
     <row r="74" ht="27" customHeight="1">
-      <c r="A74" s="92" t="n"/>
-      <c r="B74" s="92" t="inlineStr">
+      <c r="A74" s="94" t="n"/>
+      <c r="B74" s="94" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="C74" s="92" t="inlineStr">
+      <c r="C74" s="94" t="inlineStr">
         <is>
           <t>31 PALLETS</t>
         </is>
       </c>
-      <c r="D74" s="92" t="n"/>
-      <c r="E74" s="93">
+      <c r="D74" s="94" t="n"/>
+      <c r="E74" s="95">
         <f>SUM(E23:E52,E58:E71)</f>
         <v/>
       </c>
-      <c r="F74" s="94">
+      <c r="F74" s="96">
         <f>SUM(F23:F52,F58:F71)</f>
         <v/>
       </c>
-      <c r="G74" s="94">
+      <c r="G74" s="96">
         <f>SUM(G23:G52,G58:G71)</f>
         <v/>
       </c>
-      <c r="H74" s="94">
+      <c r="H74" s="96">
         <f>SUM(H23:H52,H58:H71)</f>
         <v/>
       </c>
-      <c r="I74" s="95">
+      <c r="I74" s="97">
         <f>SUM(I23:I52,I58:I71)</f>
         <v/>
       </c>
     </row>
     <row r="75" ht="27" customHeight="1">
-      <c r="A75" s="2" t="n"/>
-      <c r="B75" s="2" t="n"/>
-      <c r="C75" s="2" t="n"/>
-      <c r="D75" s="2" t="n"/>
-      <c r="E75" s="2" t="n"/>
-      <c r="F75" s="2" t="n"/>
-      <c r="G75" s="2" t="n"/>
-      <c r="H75" s="2" t="n"/>
+      <c r="A75" s="98" t="inlineStr">
+        <is>
+          <t>Country of Original Cambodia</t>
+        </is>
+      </c>
+      <c r="B75" s="98" t="n"/>
+      <c r="C75" s="98" t="n"/>
+      <c r="D75" s="99" t="n"/>
+      <c r="E75" s="100" t="n"/>
+      <c r="F75" s="26" t="n"/>
+      <c r="G75" s="26" t="n"/>
+      <c r="H75" s="26" t="n"/>
       <c r="I75" s="2" t="n"/>
       <c r="J75" s="2" t="n"/>
       <c r="K75" s="2" t="n"/>
@@ -5056,11 +5093,137 @@
       <c r="S75" s="2" t="n"/>
       <c r="T75" s="2" t="n"/>
     </row>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
+    <row r="76" ht="65.25" customHeight="1">
+      <c r="A76" s="63" t="inlineStr">
+        <is>
+          <t>Manufacture:</t>
+        </is>
+      </c>
+      <c r="B76" s="101" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
+XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="E76" s="102" t="n"/>
+      <c r="F76" s="102" t="n"/>
+      <c r="G76" s="102" t="n"/>
+      <c r="H76" s="26" t="n"/>
+      <c r="I76" s="2" t="n"/>
+      <c r="J76" s="2" t="n"/>
+      <c r="K76" s="2" t="n"/>
+      <c r="L76" s="2" t="n"/>
+      <c r="M76" s="2" t="n"/>
+      <c r="N76" s="2" t="n"/>
+      <c r="O76" s="2" t="n"/>
+      <c r="P76" s="2" t="n"/>
+      <c r="Q76" s="2" t="n"/>
+      <c r="R76" s="2" t="n"/>
+      <c r="S76" s="2" t="n"/>
+      <c r="T76" s="2" t="n"/>
+    </row>
+    <row r="77" ht="51.75" customHeight="1">
+      <c r="A77" s="101" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
+                                          /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="E77" s="102" t="n"/>
+      <c r="F77" s="102" t="n"/>
+      <c r="G77" s="102" t="n"/>
+      <c r="H77" s="102" t="n"/>
+      <c r="I77" s="2" t="n"/>
+      <c r="J77" s="2" t="n"/>
+      <c r="K77" s="2" t="n"/>
+      <c r="L77" s="2" t="n"/>
+      <c r="M77" s="2" t="n"/>
+      <c r="N77" s="2" t="n"/>
+      <c r="O77" s="2" t="n"/>
+      <c r="P77" s="2" t="n"/>
+      <c r="Q77" s="2" t="n"/>
+      <c r="R77" s="2" t="n"/>
+      <c r="S77" s="2" t="n"/>
+      <c r="T77" s="2" t="n"/>
+    </row>
+    <row r="78" ht="27" customHeight="1">
+      <c r="A78" s="69" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+      <c r="B78" s="69" t="n"/>
+      <c r="C78" s="69" t="n"/>
+      <c r="D78" s="69" t="n"/>
+      <c r="E78" s="50" t="n"/>
+      <c r="F78" s="50" t="n"/>
+      <c r="G78" s="50" t="n"/>
+      <c r="H78" s="50" t="n"/>
+      <c r="I78" s="2" t="n"/>
+      <c r="J78" s="2" t="n"/>
+      <c r="K78" s="2" t="n"/>
+      <c r="L78" s="2" t="n"/>
+      <c r="M78" s="2" t="n"/>
+      <c r="N78" s="2" t="n"/>
+      <c r="O78" s="2" t="n"/>
+      <c r="P78" s="2" t="n"/>
+      <c r="Q78" s="2" t="n"/>
+      <c r="R78" s="2" t="n"/>
+      <c r="S78" s="2" t="n"/>
+      <c r="T78" s="2" t="n"/>
+    </row>
+    <row r="79" ht="27" customHeight="1">
+      <c r="A79" s="69" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="B79" s="69" t="n"/>
+      <c r="C79" s="69" t="n"/>
+      <c r="D79" s="69" t="n"/>
+      <c r="E79" s="50" t="n"/>
+      <c r="F79" s="50" t="n"/>
+      <c r="G79" s="50" t="n"/>
+      <c r="H79" s="50" t="n"/>
+      <c r="I79" s="2" t="n"/>
+      <c r="J79" s="2" t="n"/>
+      <c r="K79" s="2" t="n"/>
+      <c r="L79" s="2" t="n"/>
+      <c r="M79" s="2" t="n"/>
+      <c r="N79" s="2" t="n"/>
+      <c r="O79" s="2" t="n"/>
+      <c r="P79" s="2" t="n"/>
+      <c r="Q79" s="2" t="n"/>
+      <c r="R79" s="2" t="n"/>
+      <c r="S79" s="2" t="n"/>
+      <c r="T79" s="2" t="n"/>
+    </row>
+    <row r="80" ht="27" customHeight="1">
+      <c r="A80" s="2" t="n"/>
+      <c r="B80" s="103" t="n"/>
+      <c r="C80" s="2" t="n"/>
+      <c r="D80" s="2" t="n"/>
+      <c r="E80" s="52" t="n"/>
+      <c r="F80" s="2" t="n"/>
+      <c r="G80" s="26" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="H80" s="52" t="n"/>
+      <c r="I80" s="2" t="n"/>
+      <c r="J80" s="2" t="n"/>
+      <c r="K80" s="2" t="n"/>
+      <c r="L80" s="2" t="n"/>
+      <c r="M80" s="2" t="n"/>
+      <c r="N80" s="2" t="n"/>
+      <c r="O80" s="2" t="n"/>
+      <c r="P80" s="2" t="n"/>
+      <c r="Q80" s="2" t="n"/>
+      <c r="R80" s="2" t="n"/>
+      <c r="S80" s="2" t="n"/>
+      <c r="T80" s="2" t="n"/>
+    </row>
     <row r="81"/>
     <row r="82"/>
     <row r="83"/>
@@ -5182,15 +5345,18 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="31">
+    <mergeCell ref="D23:D52"/>
     <mergeCell ref="B74"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="H21:H22"/>
+    <mergeCell ref="D58:D71"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="I56:I57"/>
+    <mergeCell ref="A77:D77"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="A56:A57"/>
     <mergeCell ref="C56:C57"/>
@@ -5201,6 +5367,7 @@
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B76:D76"/>
     <mergeCell ref="B73"/>
     <mergeCell ref="G56:G57"/>
     <mergeCell ref="A1:I1"/>

</xml_diff>

<commit_message>
adding border side only to the col_static rows
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -219,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -258,6 +258,16 @@
       <bottom style="thin">
         <color rgb="00000000"/>
       </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
     </border>
     <border>
       <left style="thin">
@@ -337,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -491,6 +501,9 @@
     <xf numFmtId="4" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -500,9 +513,9 @@
     <xf numFmtId="4" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -565,13 +578,16 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -581,7 +597,7 @@
     <xf numFmtId="2" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -2318,28 +2334,28 @@
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B22" s="57" t="inlineStr">
+      <c r="B22" s="58" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="C22" s="57" t="inlineStr">
+      <c r="C22" s="58" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="D22" s="58" t="inlineStr">
+      <c r="D22" s="59" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E22" s="59" t="n">
+      <c r="E22" s="60" t="n">
         <v>6461.7</v>
       </c>
-      <c r="F22" s="59" t="n">
+      <c r="F22" s="60" t="n">
         <v>1.3</v>
       </c>
-      <c r="G22" s="59">
+      <c r="G22" s="60">
         <f>F22*E22</f>
         <v/>
       </c>
@@ -2350,24 +2366,24 @@
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B23" s="57" t="inlineStr">
+      <c r="B23" s="58" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="C23" s="57" t="inlineStr">
+      <c r="C23" s="58" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="D23" s="60" t="n"/>
-      <c r="E23" s="59" t="n">
+      <c r="D23" s="61" t="n"/>
+      <c r="E23" s="60" t="n">
         <v>77.90000000000001</v>
       </c>
-      <c r="F23" s="59" t="n">
+      <c r="F23" s="60" t="n">
         <v>1.17</v>
       </c>
-      <c r="G23" s="59">
+      <c r="G23" s="60">
         <f>F23*E23</f>
         <v/>
       </c>
@@ -2378,288 +2394,288 @@
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B24" s="57" t="inlineStr">
+      <c r="B24" s="58" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C24" s="57" t="inlineStr">
+      <c r="C24" s="58" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D24" s="60" t="n"/>
-      <c r="E24" s="59" t="n">
+      <c r="D24" s="61" t="n"/>
+      <c r="E24" s="60" t="n">
         <v>20949.5</v>
       </c>
-      <c r="F24" s="59" t="n">
+      <c r="F24" s="60" t="n">
         <v>1.25</v>
       </c>
-      <c r="G24" s="59">
+      <c r="G24" s="60">
         <f>F24*E24</f>
         <v/>
       </c>
     </row>
     <row r="25" ht="35" customHeight="1">
-      <c r="B25" s="57" t="inlineStr">
+      <c r="B25" s="58" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C25" s="57" t="inlineStr">
+      <c r="C25" s="58" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D25" s="60" t="n"/>
-      <c r="E25" s="59" t="n">
+      <c r="D25" s="61" t="n"/>
+      <c r="E25" s="60" t="n">
         <v>241.9</v>
       </c>
-      <c r="F25" s="59" t="n">
+      <c r="F25" s="60" t="n">
         <v>1.13</v>
       </c>
-      <c r="G25" s="59">
+      <c r="G25" s="60">
         <f>F25*E25</f>
         <v/>
       </c>
     </row>
     <row r="26" ht="35" customHeight="1">
-      <c r="B26" s="57" t="n">
+      <c r="B26" s="58" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C26" s="57" t="inlineStr">
+      <c r="C26" s="58" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D26" s="60" t="n"/>
-      <c r="E26" s="59" t="n">
+      <c r="D26" s="61" t="n"/>
+      <c r="E26" s="60" t="n">
         <v>28156.8</v>
       </c>
-      <c r="F26" s="59" t="n">
+      <c r="F26" s="60" t="n">
         <v>1.27</v>
       </c>
-      <c r="G26" s="59">
+      <c r="G26" s="60">
         <f>F26*E26</f>
         <v/>
       </c>
     </row>
     <row r="27" ht="35" customHeight="1">
-      <c r="B27" s="57" t="n">
+      <c r="B27" s="58" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C27" s="57" t="inlineStr">
+      <c r="C27" s="58" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D27" s="60" t="n"/>
-      <c r="E27" s="59" t="n">
+      <c r="D27" s="61" t="n"/>
+      <c r="E27" s="60" t="n">
         <v>711.1</v>
       </c>
-      <c r="F27" s="59" t="n">
+      <c r="F27" s="60" t="n">
         <v>1.14</v>
       </c>
-      <c r="G27" s="59">
+      <c r="G27" s="60">
         <f>F27*E27</f>
         <v/>
       </c>
     </row>
     <row r="28" ht="35" customHeight="1">
-      <c r="B28" s="57" t="n">
+      <c r="B28" s="58" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C28" s="57" t="inlineStr">
+      <c r="C28" s="58" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D28" s="60" t="n"/>
-      <c r="E28" s="59" t="n">
+      <c r="D28" s="61" t="n"/>
+      <c r="E28" s="60" t="n">
         <v>1301.4</v>
       </c>
-      <c r="F28" s="59" t="n">
+      <c r="F28" s="60" t="n">
         <v>1.14</v>
       </c>
-      <c r="G28" s="59">
+      <c r="G28" s="60">
         <f>F28*E28</f>
         <v/>
       </c>
     </row>
     <row r="29" ht="35" customHeight="1">
-      <c r="B29" s="57" t="n">
+      <c r="B29" s="58" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C29" s="57" t="inlineStr">
+      <c r="C29" s="58" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D29" s="60" t="n"/>
-      <c r="E29" s="59" t="n">
+      <c r="D29" s="61" t="n"/>
+      <c r="E29" s="60" t="n">
         <v>18717.9</v>
       </c>
-      <c r="F29" s="59" t="n">
+      <c r="F29" s="60" t="n">
         <v>1.27</v>
       </c>
-      <c r="G29" s="59">
+      <c r="G29" s="60">
         <f>F29*E29</f>
         <v/>
       </c>
     </row>
     <row r="30" ht="35" customHeight="1">
-      <c r="B30" s="57" t="n">
+      <c r="B30" s="58" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C30" s="57" t="inlineStr">
+      <c r="C30" s="58" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D30" s="60" t="n"/>
-      <c r="E30" s="59" t="n">
+      <c r="D30" s="61" t="n"/>
+      <c r="E30" s="60" t="n">
         <v>106711.7</v>
       </c>
-      <c r="F30" s="59" t="n">
+      <c r="F30" s="60" t="n">
         <v>1.25</v>
       </c>
-      <c r="G30" s="59">
+      <c r="G30" s="60">
         <f>F30*E30</f>
         <v/>
       </c>
     </row>
     <row r="31" ht="35" customHeight="1">
-      <c r="B31" s="57" t="n">
+      <c r="B31" s="58" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C31" s="57" t="inlineStr">
+      <c r="C31" s="58" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D31" s="60" t="n"/>
-      <c r="E31" s="59" t="n">
+      <c r="D31" s="61" t="n"/>
+      <c r="E31" s="60" t="n">
         <v>1320.6</v>
       </c>
-      <c r="F31" s="59" t="n">
+      <c r="F31" s="60" t="n">
         <v>1.13</v>
       </c>
-      <c r="G31" s="59">
+      <c r="G31" s="60">
         <f>F31*E31</f>
         <v/>
       </c>
     </row>
     <row r="32" ht="35" customHeight="1">
-      <c r="B32" s="57" t="n">
+      <c r="B32" s="58" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C32" s="57" t="inlineStr">
+      <c r="C32" s="58" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D32" s="60" t="n"/>
-      <c r="E32" s="59" t="n">
+      <c r="D32" s="61" t="n"/>
+      <c r="E32" s="60" t="n">
         <v>367.3</v>
       </c>
-      <c r="F32" s="59" t="n">
+      <c r="F32" s="60" t="n">
         <v>1.06</v>
       </c>
-      <c r="G32" s="59">
+      <c r="G32" s="60">
         <f>F32*E32</f>
         <v/>
       </c>
     </row>
     <row r="33" ht="35" customHeight="1">
-      <c r="B33" s="57" t="n">
+      <c r="B33" s="58" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C33" s="57" t="inlineStr">
+      <c r="C33" s="58" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D33" s="60" t="n"/>
-      <c r="E33" s="59" t="n">
+      <c r="D33" s="61" t="n"/>
+      <c r="E33" s="60" t="n">
         <v>101424.8</v>
       </c>
-      <c r="F33" s="59" t="n">
+      <c r="F33" s="60" t="n">
         <v>1.25</v>
       </c>
-      <c r="G33" s="59">
+      <c r="G33" s="60">
         <f>F33*E33</f>
         <v/>
       </c>
     </row>
     <row r="34" ht="35" customHeight="1">
-      <c r="B34" s="57" t="n">
+      <c r="B34" s="58" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C34" s="57" t="inlineStr">
+      <c r="C34" s="58" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D34" s="60" t="n"/>
-      <c r="E34" s="59" t="n">
+      <c r="D34" s="61" t="n"/>
+      <c r="E34" s="60" t="n">
         <v>1205.1</v>
       </c>
-      <c r="F34" s="59" t="n">
+      <c r="F34" s="60" t="n">
         <v>1.13</v>
       </c>
-      <c r="G34" s="59">
+      <c r="G34" s="60">
         <f>F34*E34</f>
         <v/>
       </c>
     </row>
     <row r="35" ht="35" customHeight="1">
-      <c r="B35" s="57" t="inlineStr">
+      <c r="B35" s="58" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="C35" s="57" t="inlineStr">
+      <c r="C35" s="58" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="D35" s="60" t="n"/>
-      <c r="E35" s="59" t="n">
+      <c r="D35" s="61" t="n"/>
+      <c r="E35" s="60" t="n">
         <v>5345</v>
       </c>
-      <c r="F35" s="59" t="n">
+      <c r="F35" s="60" t="n">
         <v>1.3</v>
       </c>
-      <c r="G35" s="59">
+      <c r="G35" s="60">
         <f>F35*E35</f>
         <v/>
       </c>
     </row>
     <row r="36" ht="35" customHeight="1">
-      <c r="B36" s="57" t="inlineStr">
+      <c r="B36" s="58" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="C36" s="57" t="inlineStr">
+      <c r="C36" s="58" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="D36" s="61" t="n"/>
-      <c r="E36" s="59" t="n">
+      <c r="D36" s="62" t="n"/>
+      <c r="E36" s="60" t="n">
         <v>121</v>
       </c>
-      <c r="F36" s="59" t="n">
+      <c r="F36" s="60" t="n">
         <v>1.17</v>
       </c>
-      <c r="G36" s="59">
+      <c r="G36" s="60">
         <f>F36*E36</f>
         <v/>
       </c>
     </row>
     <row r="37" ht="35" customHeight="1">
-      <c r="A37" s="62" t="n"/>
+      <c r="A37" s="63" t="n"/>
       <c r="B37" s="54" t="inlineStr">
         <is>
           <t>HS.CODE: 4107.12.00</t>
@@ -2695,52 +2711,52 @@
       </c>
     </row>
     <row r="39" ht="61.5" customHeight="1">
-      <c r="A39" s="63" t="inlineStr">
+      <c r="A39" s="64" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B39" s="64" t="inlineStr">
+      <c r="B39" s="65" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D39" s="64" t="n"/>
-      <c r="E39" s="64" t="n"/>
+      <c r="D39" s="65" t="n"/>
+      <c r="E39" s="65" t="n"/>
       <c r="F39" s="32" t="n"/>
       <c r="G39" s="26" t="n"/>
       <c r="H39" s="2" t="n"/>
       <c r="I39" s="2" t="n"/>
       <c r="J39" s="2" t="n"/>
       <c r="K39" s="2" t="n"/>
-      <c r="L39" s="65" t="n"/>
-      <c r="M39" s="66" t="n"/>
-      <c r="N39" s="67" t="n"/>
-      <c r="O39" s="67" t="n"/>
+      <c r="L39" s="66" t="n"/>
+      <c r="M39" s="67" t="n"/>
+      <c r="N39" s="68" t="n"/>
+      <c r="O39" s="68" t="n"/>
     </row>
     <row r="40" ht="42" customHeight="1">
-      <c r="A40" s="68" t="inlineStr">
+      <c r="A40" s="69" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                                   /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="D40" s="68" t="n"/>
-      <c r="E40" s="68" t="n"/>
-      <c r="F40" s="68" t="n"/>
+      <c r="D40" s="69" t="n"/>
+      <c r="E40" s="69" t="n"/>
+      <c r="F40" s="69" t="n"/>
       <c r="G40" s="26" t="n"/>
       <c r="H40" s="2" t="n"/>
       <c r="I40" s="2" t="n"/>
       <c r="J40" s="2" t="n"/>
       <c r="K40" s="2" t="n"/>
-      <c r="L40" s="65" t="n"/>
-      <c r="M40" s="66" t="n"/>
-      <c r="N40" s="67" t="n"/>
-      <c r="O40" s="67" t="n"/>
+      <c r="L40" s="66" t="n"/>
+      <c r="M40" s="67" t="n"/>
+      <c r="N40" s="68" t="n"/>
+      <c r="O40" s="68" t="n"/>
     </row>
     <row r="41" ht="24.75" customHeight="1">
-      <c r="A41" s="69" t="inlineStr">
+      <c r="A41" s="70" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
@@ -2749,13 +2765,13 @@
       <c r="I41" s="2" t="n"/>
       <c r="J41" s="2" t="n"/>
       <c r="K41" s="2" t="n"/>
-      <c r="L41" s="65" t="n"/>
-      <c r="M41" s="66" t="n"/>
-      <c r="N41" s="67" t="n"/>
-      <c r="O41" s="67" t="n"/>
+      <c r="L41" s="66" t="n"/>
+      <c r="M41" s="67" t="n"/>
+      <c r="N41" s="68" t="n"/>
+      <c r="O41" s="68" t="n"/>
     </row>
     <row r="42" ht="27" customHeight="1">
-      <c r="A42" s="69" t="inlineStr">
+      <c r="A42" s="70" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
@@ -2764,107 +2780,107 @@
       <c r="I42" s="2" t="n"/>
       <c r="J42" s="2" t="n"/>
       <c r="K42" s="2" t="n"/>
-      <c r="L42" s="65" t="n"/>
-      <c r="M42" s="66" t="n"/>
-      <c r="N42" s="67" t="n"/>
-      <c r="O42" s="67" t="n"/>
+      <c r="L42" s="66" t="n"/>
+      <c r="M42" s="67" t="n"/>
+      <c r="N42" s="68" t="n"/>
+      <c r="O42" s="68" t="n"/>
     </row>
     <row r="43" ht="61.5" customHeight="1">
       <c r="A43" s="2" t="n"/>
       <c r="B43" s="2" t="n"/>
       <c r="C43" s="2" t="n"/>
       <c r="D43" s="2" t="n"/>
-      <c r="E43" s="70" t="inlineStr">
+      <c r="E43" s="71" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="F43" s="70" t="n"/>
-      <c r="G43" s="70" t="n"/>
-      <c r="H43" s="70" t="n"/>
+      <c r="F43" s="71" t="n"/>
+      <c r="G43" s="71" t="n"/>
+      <c r="H43" s="71" t="n"/>
       <c r="I43" s="2" t="n"/>
       <c r="J43" s="2" t="n"/>
       <c r="K43" s="2" t="n"/>
-      <c r="L43" s="65" t="n"/>
-      <c r="M43" s="66" t="n"/>
-      <c r="N43" s="67" t="n"/>
-      <c r="O43" s="67" t="n"/>
+      <c r="L43" s="66" t="n"/>
+      <c r="M43" s="67" t="n"/>
+      <c r="N43" s="68" t="n"/>
+      <c r="O43" s="68" t="n"/>
     </row>
     <row r="44" ht="42" customHeight="1">
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="2" t="n"/>
       <c r="C44" s="2" t="n"/>
-      <c r="D44" s="71" t="n"/>
-      <c r="E44" s="72" t="n"/>
-      <c r="F44" s="73" t="inlineStr">
+      <c r="D44" s="72" t="n"/>
+      <c r="E44" s="73" t="n"/>
+      <c r="F44" s="74" t="inlineStr">
         <is>
           <t>Sign &amp; Stamp</t>
         </is>
       </c>
-      <c r="G44" s="74" t="n"/>
+      <c r="G44" s="75" t="n"/>
       <c r="H44" s="2" t="n"/>
       <c r="I44" s="2" t="n"/>
       <c r="J44" s="2" t="n"/>
       <c r="K44" s="2" t="n"/>
-      <c r="L44" s="65" t="n"/>
-      <c r="M44" s="66" t="n"/>
-      <c r="N44" s="67" t="n"/>
-      <c r="O44" s="67" t="n"/>
+      <c r="L44" s="66" t="n"/>
+      <c r="M44" s="67" t="n"/>
+      <c r="N44" s="68" t="n"/>
+      <c r="O44" s="68" t="n"/>
     </row>
     <row r="45" ht="24.75" customHeight="1">
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="n"/>
       <c r="C45" s="2" t="n"/>
-      <c r="D45" s="71" t="n"/>
-      <c r="E45" s="72" t="n"/>
-      <c r="F45" s="72" t="n"/>
-      <c r="G45" s="74" t="n"/>
+      <c r="D45" s="72" t="n"/>
+      <c r="E45" s="73" t="n"/>
+      <c r="F45" s="73" t="n"/>
+      <c r="G45" s="75" t="n"/>
       <c r="H45" s="2" t="n"/>
       <c r="I45" s="2" t="n"/>
       <c r="J45" s="2" t="n"/>
       <c r="K45" s="2" t="n"/>
-      <c r="L45" s="65" t="n"/>
-      <c r="M45" s="66" t="n"/>
-      <c r="N45" s="67" t="n"/>
-      <c r="O45" s="67" t="n"/>
+      <c r="L45" s="66" t="n"/>
+      <c r="M45" s="67" t="n"/>
+      <c r="N45" s="68" t="n"/>
+      <c r="O45" s="68" t="n"/>
     </row>
     <row r="46" ht="27" customHeight="1">
       <c r="A46" s="2" t="n"/>
       <c r="B46" s="2" t="n"/>
       <c r="C46" s="2" t="n"/>
-      <c r="D46" s="71" t="n"/>
-      <c r="E46" s="72" t="n"/>
-      <c r="F46" s="72" t="n"/>
-      <c r="G46" s="74" t="n"/>
+      <c r="D46" s="72" t="n"/>
+      <c r="E46" s="73" t="n"/>
+      <c r="F46" s="73" t="n"/>
+      <c r="G46" s="75" t="n"/>
       <c r="H46" s="2" t="n"/>
       <c r="I46" s="2" t="n"/>
       <c r="J46" s="2" t="n"/>
       <c r="K46" s="2" t="n"/>
-      <c r="L46" s="65" t="n"/>
-      <c r="M46" s="66" t="n"/>
-      <c r="N46" s="67" t="n"/>
-      <c r="O46" s="67" t="n"/>
+      <c r="L46" s="66" t="n"/>
+      <c r="M46" s="67" t="n"/>
+      <c r="N46" s="68" t="n"/>
+      <c r="O46" s="68" t="n"/>
     </row>
     <row r="47" ht="21" customHeight="1">
       <c r="A47" s="2" t="n"/>
       <c r="B47" s="2" t="n"/>
       <c r="C47" s="2" t="n"/>
-      <c r="D47" s="71" t="n"/>
-      <c r="E47" s="72" t="n"/>
-      <c r="F47" s="75" t="inlineStr">
+      <c r="D47" s="72" t="n"/>
+      <c r="E47" s="73" t="n"/>
+      <c r="F47" s="76" t="inlineStr">
         <is>
           <t>ZENG XUELI</t>
         </is>
       </c>
-      <c r="G47" s="75" t="n"/>
+      <c r="G47" s="76" t="n"/>
       <c r="H47" s="2" t="n"/>
       <c r="I47" s="2" t="n"/>
       <c r="J47" s="2" t="n"/>
       <c r="K47" s="2" t="n"/>
-      <c r="L47" s="65" t="n"/>
-      <c r="M47" s="66" t="n"/>
-      <c r="N47" s="67" t="n"/>
-      <c r="O47" s="67" t="n"/>
+      <c r="L47" s="66" t="n"/>
+      <c r="M47" s="67" t="n"/>
+      <c r="N47" s="68" t="n"/>
+      <c r="O47" s="68" t="n"/>
     </row>
     <row r="48"/>
     <row r="49"/>
@@ -3199,7 +3215,7 @@
     </row>
     <row r="7" ht="18" customHeight="1">
       <c r="A7" s="32" t="n"/>
-      <c r="B7" s="76" t="n"/>
+      <c r="B7" s="77" t="n"/>
       <c r="C7" s="32" t="n"/>
       <c r="D7" s="32" t="n"/>
       <c r="E7" s="26" t="n"/>
@@ -3210,7 +3226,7 @@
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="I7" s="77" t="inlineStr">
+      <c r="I7" s="78" t="inlineStr">
         <is>
           <t>JFREF</t>
         </is>
@@ -3233,7 +3249,7 @@
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="78" t="inlineStr">
+      <c r="B8" s="79" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
@@ -3248,7 +3264,7 @@
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="I8" s="79" t="inlineStr">
+      <c r="I8" s="80" t="inlineStr">
         <is>
           <t>JFINV</t>
         </is>
@@ -3267,7 +3283,7 @@
     </row>
     <row r="9" ht="21" customHeight="1">
       <c r="A9" s="32" t="n"/>
-      <c r="B9" s="76" t="inlineStr">
+      <c r="B9" s="77" t="inlineStr">
         <is>
           <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages,</t>
         </is>
@@ -3301,7 +3317,7 @@
     </row>
     <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="32" t="n"/>
-      <c r="B10" s="76" t="inlineStr">
+      <c r="B10" s="77" t="inlineStr">
         <is>
           <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
         </is>
@@ -3316,7 +3332,7 @@
           <t>FCA :</t>
         </is>
       </c>
-      <c r="I10" s="80" t="inlineStr">
+      <c r="I10" s="81" t="inlineStr">
         <is>
           <t>BAVET, SVAY RIENG</t>
         </is>
@@ -3335,7 +3351,7 @@
     </row>
     <row r="11" ht="20.25" customHeight="1">
       <c r="A11" s="32" t="n"/>
-      <c r="B11" s="76" t="inlineStr">
+      <c r="B11" s="77" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
@@ -3361,7 +3377,7 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="n"/>
-      <c r="B12" s="76" t="n"/>
+      <c r="B12" s="77" t="n"/>
       <c r="C12" s="32" t="n"/>
       <c r="D12" s="32" t="n"/>
       <c r="E12" s="26" t="n"/>
@@ -3387,7 +3403,7 @@
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="81" t="inlineStr">
+      <c r="B13" s="82" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
@@ -3395,9 +3411,9 @@
       <c r="C13" s="2" t="n"/>
       <c r="D13" s="2" t="n"/>
       <c r="E13" s="2" t="n"/>
-      <c r="F13" s="82" t="n"/>
-      <c r="G13" s="82" t="n"/>
-      <c r="H13" s="82" t="n"/>
+      <c r="F13" s="83" t="n"/>
+      <c r="G13" s="83" t="n"/>
+      <c r="H13" s="83" t="n"/>
       <c r="I13" s="45" t="n"/>
       <c r="J13" s="2" t="n"/>
       <c r="K13" s="2" t="n"/>
@@ -3413,17 +3429,17 @@
     </row>
     <row r="14" ht="25.5" customHeight="1">
       <c r="A14" s="32" t="n"/>
-      <c r="B14" s="83" t="inlineStr">
+      <c r="B14" s="84" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
       <c r="C14" s="47" t="n"/>
       <c r="D14" s="47" t="n"/>
-      <c r="E14" s="84" t="n"/>
-      <c r="F14" s="84" t="n"/>
-      <c r="G14" s="84" t="n"/>
-      <c r="H14" s="84" t="n"/>
+      <c r="E14" s="85" t="n"/>
+      <c r="F14" s="85" t="n"/>
+      <c r="G14" s="85" t="n"/>
+      <c r="H14" s="85" t="n"/>
       <c r="I14" s="2" t="n"/>
       <c r="J14" s="2" t="n"/>
       <c r="K14" s="2" t="n"/>
@@ -3439,7 +3455,7 @@
     </row>
     <row r="15" ht="21" customHeight="1">
       <c r="A15" s="32" t="n"/>
-      <c r="B15" s="85" t="inlineStr">
+      <c r="B15" s="86" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
         </is>
@@ -3547,7 +3563,7 @@
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B19" s="76" t="inlineStr">
+      <c r="B19" s="77" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
         </is>
@@ -3573,7 +3589,7 @@
     </row>
     <row r="20" ht="27.75" customHeight="1">
       <c r="A20" s="53" t="n"/>
-      <c r="B20" s="86" t="n"/>
+      <c r="B20" s="87" t="n"/>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
@@ -3619,7 +3635,7 @@
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F21" s="87" t="n"/>
+      <c r="F21" s="88" t="n"/>
       <c r="G21" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -3630,7 +3646,7 @@
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I21" s="88" t="inlineStr">
+      <c r="I21" s="89" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
@@ -3648,11 +3664,11 @@
       <c r="T21" s="2" t="n"/>
     </row>
     <row r="22" ht="27" customHeight="1">
-      <c r="A22" s="61" t="n"/>
-      <c r="B22" s="61" t="n"/>
-      <c r="C22" s="61" t="n"/>
-      <c r="D22" s="61" t="n"/>
-      <c r="E22" s="89" t="inlineStr">
+      <c r="A22" s="62" t="n"/>
+      <c r="B22" s="62" t="n"/>
+      <c r="C22" s="62" t="n"/>
+      <c r="D22" s="62" t="n"/>
+      <c r="E22" s="90" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
@@ -3662,826 +3678,826 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="G22" s="61" t="n"/>
-      <c r="H22" s="61" t="n"/>
-      <c r="I22" s="61" t="n"/>
+      <c r="G22" s="62" t="n"/>
+      <c r="H22" s="62" t="n"/>
+      <c r="I22" s="62" t="n"/>
     </row>
     <row r="23" ht="27" customHeight="1">
-      <c r="A23" s="90" t="inlineStr">
+      <c r="A23" s="91" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B23" s="90" t="inlineStr">
+      <c r="B23" s="92" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="C23" s="90" t="inlineStr">
+      <c r="C23" s="92" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="D23" s="58" t="inlineStr">
+      <c r="D23" s="59" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E23" s="91" t="n">
+      <c r="E23" s="93" t="n">
         <v>122</v>
       </c>
-      <c r="F23" s="59" t="n">
+      <c r="F23" s="60" t="n">
         <v>6461.7</v>
       </c>
-      <c r="G23" s="59" t="n">
+      <c r="G23" s="60" t="n">
         <v>467.8306</v>
       </c>
-      <c r="H23" s="59" t="n">
+      <c r="H23" s="60" t="n">
         <v>512.1048</v>
       </c>
-      <c r="I23" s="92" t="n">
+      <c r="I23" s="94" t="n">
         <v>1.8312</v>
       </c>
     </row>
     <row r="24" ht="27" customHeight="1">
-      <c r="A24" s="90" t="inlineStr">
+      <c r="A24" s="91" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B24" s="90" t="inlineStr">
+      <c r="B24" s="92" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="C24" s="90" t="inlineStr">
+      <c r="C24" s="92" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="D24" s="60" t="n"/>
-      <c r="E24" s="91" t="n">
+      <c r="D24" s="61" t="n"/>
+      <c r="E24" s="93" t="n">
         <v>2</v>
       </c>
-      <c r="F24" s="59" t="n">
+      <c r="F24" s="60" t="n">
         <v>77.90000000000001</v>
       </c>
-      <c r="G24" s="59" t="n">
+      <c r="G24" s="60" t="n">
         <v>7.6694</v>
       </c>
-      <c r="H24" s="59" t="n">
+      <c r="H24" s="60" t="n">
         <v>8.395200000000001</v>
       </c>
-      <c r="I24" s="92" t="n">
+      <c r="I24" s="94" t="n">
         <v>0.03</v>
       </c>
     </row>
     <row r="25" ht="27" customHeight="1">
-      <c r="A25" s="90" t="inlineStr">
+      <c r="A25" s="91" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B25" s="90" t="inlineStr">
+      <c r="B25" s="92" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C25" s="90" t="inlineStr">
+      <c r="C25" s="92" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D25" s="60" t="n"/>
-      <c r="E25" s="91" t="n">
+      <c r="D25" s="61" t="n"/>
+      <c r="E25" s="93" t="n">
         <v>190</v>
       </c>
-      <c r="F25" s="59" t="n">
+      <c r="F25" s="60" t="n">
         <v>10009.4</v>
       </c>
-      <c r="G25" s="59" t="n">
+      <c r="G25" s="60" t="n">
         <v>757</v>
       </c>
-      <c r="H25" s="59" t="n">
+      <c r="H25" s="60" t="n">
         <v>802</v>
       </c>
-      <c r="I25" s="92" t="n">
+      <c r="I25" s="94" t="n">
         <v>2.4552</v>
       </c>
     </row>
     <row r="26" ht="27" customHeight="1">
-      <c r="A26" s="90" t="inlineStr">
+      <c r="A26" s="91" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B26" s="90" t="inlineStr">
+      <c r="B26" s="92" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C26" s="90" t="inlineStr">
+      <c r="C26" s="92" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D26" s="60" t="n"/>
-      <c r="E26" s="91" t="n">
+      <c r="D26" s="61" t="n"/>
+      <c r="E26" s="93" t="n">
         <v>208</v>
       </c>
-      <c r="F26" s="59" t="n">
+      <c r="F26" s="60" t="n">
         <v>10940.1</v>
       </c>
-      <c r="G26" s="59" t="n">
+      <c r="G26" s="60" t="n">
         <v>842.2056</v>
       </c>
-      <c r="H26" s="59" t="n">
+      <c r="H26" s="60" t="n">
         <v>885.9439</v>
       </c>
-      <c r="I26" s="92" t="n">
+      <c r="I26" s="94" t="n">
         <v>2.6943</v>
       </c>
     </row>
     <row r="27" ht="27" customHeight="1">
-      <c r="B27" s="90" t="inlineStr">
+      <c r="B27" s="92" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C27" s="90" t="inlineStr">
+      <c r="C27" s="92" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D27" s="60" t="n"/>
-      <c r="E27" s="91" t="n">
+      <c r="D27" s="61" t="n"/>
+      <c r="E27" s="93" t="n">
         <v>6</v>
       </c>
-      <c r="F27" s="59" t="n">
+      <c r="F27" s="60" t="n">
         <v>241.9</v>
       </c>
-      <c r="G27" s="59" t="n">
+      <c r="G27" s="60" t="n">
         <v>24.2944</v>
       </c>
-      <c r="H27" s="59" t="n">
+      <c r="H27" s="60" t="n">
         <v>25.5561</v>
       </c>
-      <c r="I27" s="92" t="n">
+      <c r="I27" s="94" t="n">
         <v>0.07770000000000001</v>
       </c>
     </row>
     <row r="28" ht="27" customHeight="1">
-      <c r="B28" s="90" t="n">
+      <c r="B28" s="92" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C28" s="90" t="inlineStr">
+      <c r="C28" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D28" s="60" t="n"/>
-      <c r="E28" s="91" t="n">
+      <c r="D28" s="61" t="n"/>
+      <c r="E28" s="93" t="n">
         <v>154</v>
       </c>
-      <c r="F28" s="59" t="n">
+      <c r="F28" s="60" t="n">
         <v>7788.7</v>
       </c>
-      <c r="G28" s="59" t="n">
+      <c r="G28" s="60" t="n">
         <v>617.7907</v>
       </c>
-      <c r="H28" s="59" t="n">
+      <c r="H28" s="60" t="n">
         <v>658.0814</v>
       </c>
-      <c r="I28" s="92" t="n">
+      <c r="I28" s="94" t="n">
         <v>2.0564</v>
       </c>
     </row>
     <row r="29" ht="27" customHeight="1">
-      <c r="B29" s="90" t="n">
+      <c r="B29" s="92" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C29" s="90" t="inlineStr">
+      <c r="C29" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D29" s="60" t="n"/>
-      <c r="E29" s="91" t="n">
+      <c r="D29" s="61" t="n"/>
+      <c r="E29" s="93" t="n">
         <v>18</v>
       </c>
-      <c r="F29" s="59" t="n">
+      <c r="F29" s="60" t="n">
         <v>711.1</v>
       </c>
-      <c r="G29" s="59" t="n">
+      <c r="G29" s="60" t="n">
         <v>72.2093</v>
       </c>
-      <c r="H29" s="59" t="n">
+      <c r="H29" s="60" t="n">
         <v>76.9186</v>
       </c>
-      <c r="I29" s="92" t="n">
+      <c r="I29" s="94" t="n">
         <v>0.2404</v>
       </c>
     </row>
     <row r="30" ht="27" customHeight="1">
-      <c r="B30" s="90" t="n">
+      <c r="B30" s="92" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C30" s="90" t="inlineStr">
+      <c r="C30" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D30" s="60" t="n"/>
-      <c r="E30" s="91" t="n">
+      <c r="D30" s="61" t="n"/>
+      <c r="E30" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F30" s="59" t="n">
+      <c r="F30" s="60" t="n">
         <v>10033.3</v>
       </c>
-      <c r="G30" s="59" t="n">
+      <c r="G30" s="60" t="n">
         <v>814.5</v>
       </c>
-      <c r="H30" s="59" t="n">
+      <c r="H30" s="60" t="n">
         <v>859.5</v>
       </c>
-      <c r="I30" s="92" t="n">
+      <c r="I30" s="94" t="n">
         <v>2.376</v>
       </c>
     </row>
     <row r="31" ht="27" customHeight="1">
-      <c r="B31" s="90" t="n">
+      <c r="B31" s="92" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C31" s="90" t="inlineStr">
+      <c r="C31" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D31" s="60" t="n"/>
-      <c r="E31" s="91" t="n">
+      <c r="D31" s="61" t="n"/>
+      <c r="E31" s="93" t="n">
         <v>200</v>
       </c>
-      <c r="F31" s="59" t="n">
+      <c r="F31" s="60" t="n">
         <v>10334.8</v>
       </c>
-      <c r="G31" s="59" t="n">
+      <c r="G31" s="60" t="n">
         <v>740.5286</v>
       </c>
-      <c r="H31" s="59" t="n">
+      <c r="H31" s="60" t="n">
         <v>780.1762</v>
       </c>
-      <c r="I31" s="92" t="n">
+      <c r="I31" s="94" t="n">
         <v>2.2678</v>
       </c>
     </row>
     <row r="32" ht="27" customHeight="1">
-      <c r="B32" s="90" t="n">
+      <c r="B32" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C32" s="90" t="inlineStr">
+      <c r="C32" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D32" s="60" t="n"/>
-      <c r="E32" s="91" t="n">
+      <c r="D32" s="61" t="n"/>
+      <c r="E32" s="93" t="n">
         <v>27</v>
       </c>
-      <c r="F32" s="59" t="n">
+      <c r="F32" s="60" t="n">
         <v>1065.4</v>
       </c>
-      <c r="G32" s="59" t="n">
+      <c r="G32" s="60" t="n">
         <v>99.9714</v>
       </c>
-      <c r="H32" s="59" t="n">
+      <c r="H32" s="60" t="n">
         <v>105.3238</v>
       </c>
-      <c r="I32" s="92" t="n">
+      <c r="I32" s="94" t="n">
         <v>0.3062</v>
       </c>
     </row>
     <row r="33" ht="27" customHeight="1">
-      <c r="B33" s="90" t="n">
+      <c r="B33" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C33" s="90" t="inlineStr">
+      <c r="C33" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D33" s="60" t="n"/>
-      <c r="E33" s="91" t="n">
+      <c r="D33" s="61" t="n"/>
+      <c r="E33" s="93" t="n">
         <v>169</v>
       </c>
-      <c r="F33" s="59" t="n">
+      <c r="F33" s="60" t="n">
         <v>8660.5</v>
       </c>
-      <c r="G33" s="59" t="n">
+      <c r="G33" s="60" t="n">
         <v>693.3828999999999</v>
       </c>
-      <c r="H33" s="59" t="n">
+      <c r="H33" s="60" t="n">
         <v>736.84</v>
       </c>
-      <c r="I33" s="92" t="n">
+      <c r="I33" s="94" t="n">
         <v>2.2181</v>
       </c>
     </row>
     <row r="34" ht="27" customHeight="1">
-      <c r="B34" s="90" t="n">
+      <c r="B34" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C34" s="90" t="inlineStr">
+      <c r="C34" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D34" s="60" t="n"/>
-      <c r="E34" s="91" t="n">
+      <c r="D34" s="61" t="n"/>
+      <c r="E34" s="93" t="n">
         <v>6</v>
       </c>
-      <c r="F34" s="59" t="n">
+      <c r="F34" s="60" t="n">
         <v>236</v>
       </c>
-      <c r="G34" s="59" t="n">
+      <c r="G34" s="60" t="n">
         <v>24.6171</v>
       </c>
-      <c r="H34" s="59" t="n">
+      <c r="H34" s="60" t="n">
         <v>26.16</v>
       </c>
-      <c r="I34" s="92" t="n">
+      <c r="I34" s="94" t="n">
         <v>0.07870000000000001</v>
       </c>
     </row>
     <row r="35" ht="27" customHeight="1">
-      <c r="B35" s="90" t="n">
+      <c r="B35" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C35" s="90" t="inlineStr">
+      <c r="C35" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D35" s="60" t="n"/>
-      <c r="E35" s="91" t="n">
+      <c r="D35" s="61" t="n"/>
+      <c r="E35" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F35" s="59" t="n">
+      <c r="F35" s="60" t="n">
         <v>10057.4</v>
       </c>
-      <c r="G35" s="59" t="n">
+      <c r="G35" s="60" t="n">
         <v>814.5</v>
       </c>
-      <c r="H35" s="59" t="n">
+      <c r="H35" s="60" t="n">
         <v>859.5</v>
       </c>
-      <c r="I35" s="92" t="n">
+      <c r="I35" s="94" t="n">
         <v>2.376</v>
       </c>
     </row>
     <row r="36" ht="27" customHeight="1">
-      <c r="B36" s="90" t="n">
+      <c r="B36" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C36" s="90" t="inlineStr">
+      <c r="C36" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D36" s="60" t="n"/>
-      <c r="E36" s="91" t="n">
+      <c r="D36" s="61" t="n"/>
+      <c r="E36" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F36" s="59" t="n">
+      <c r="F36" s="60" t="n">
         <v>10176.8</v>
       </c>
-      <c r="G36" s="59" t="n">
+      <c r="G36" s="60" t="n">
         <v>830.5</v>
       </c>
-      <c r="H36" s="59" t="n">
+      <c r="H36" s="60" t="n">
         <v>875.5</v>
       </c>
-      <c r="I36" s="92" t="n">
+      <c r="I36" s="94" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="37" ht="27" customHeight="1">
-      <c r="B37" s="90" t="n">
+      <c r="B37" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C37" s="90" t="inlineStr">
+      <c r="C37" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D37" s="60" t="n"/>
-      <c r="E37" s="91" t="n">
+      <c r="D37" s="61" t="n"/>
+      <c r="E37" s="93" t="n">
         <v>215</v>
       </c>
-      <c r="F37" s="59" t="n">
+      <c r="F37" s="60" t="n">
         <v>11117</v>
       </c>
-      <c r="G37" s="59" t="n">
+      <c r="G37" s="60" t="n">
         <v>901.5</v>
       </c>
-      <c r="H37" s="59" t="n">
+      <c r="H37" s="60" t="n">
         <v>946.5</v>
       </c>
-      <c r="I37" s="92" t="n">
+      <c r="I37" s="94" t="n">
         <v>2.97</v>
       </c>
     </row>
     <row r="38" ht="27" customHeight="1">
-      <c r="B38" s="90" t="n">
+      <c r="B38" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C38" s="90" t="inlineStr">
+      <c r="C38" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D38" s="60" t="n"/>
-      <c r="E38" s="91" t="n">
+      <c r="D38" s="61" t="n"/>
+      <c r="E38" s="93" t="n">
         <v>215</v>
       </c>
-      <c r="F38" s="59" t="n">
+      <c r="F38" s="60" t="n">
         <v>11227</v>
       </c>
-      <c r="G38" s="59" t="n">
+      <c r="G38" s="60" t="n">
         <v>918</v>
       </c>
-      <c r="H38" s="59" t="n">
+      <c r="H38" s="60" t="n">
         <v>963</v>
       </c>
-      <c r="I38" s="92" t="n">
+      <c r="I38" s="94" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="39" ht="27" customHeight="1">
-      <c r="B39" s="90" t="n">
+      <c r="B39" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C39" s="90" t="inlineStr">
+      <c r="C39" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D39" s="60" t="n"/>
-      <c r="E39" s="91" t="n">
+      <c r="D39" s="61" t="n"/>
+      <c r="E39" s="93" t="n">
         <v>192</v>
       </c>
-      <c r="F39" s="59" t="n">
+      <c r="F39" s="60" t="n">
         <v>9879.4</v>
       </c>
-      <c r="G39" s="59" t="n">
+      <c r="G39" s="60" t="n">
         <v>795.0291</v>
       </c>
-      <c r="H39" s="59" t="n">
+      <c r="H39" s="60" t="n">
         <v>836.9709</v>
       </c>
-      <c r="I39" s="92" t="n">
+      <c r="I39" s="94" t="n">
         <v>2.4729</v>
       </c>
     </row>
     <row r="40" ht="27" customHeight="1">
-      <c r="B40" s="90" t="n">
+      <c r="B40" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C40" s="90" t="inlineStr">
+      <c r="C40" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D40" s="60" t="n"/>
-      <c r="E40" s="91" t="n">
+      <c r="D40" s="61" t="n"/>
+      <c r="E40" s="93" t="n">
         <v>14</v>
       </c>
-      <c r="F40" s="59" t="n">
+      <c r="F40" s="60" t="n">
         <v>561</v>
       </c>
-      <c r="G40" s="59" t="n">
+      <c r="G40" s="60" t="n">
         <v>57.9709</v>
       </c>
-      <c r="H40" s="59" t="n">
+      <c r="H40" s="60" t="n">
         <v>61.0291</v>
       </c>
-      <c r="I40" s="92" t="n">
+      <c r="I40" s="94" t="n">
         <v>0.1803</v>
       </c>
     </row>
     <row r="41" ht="27" customHeight="1">
-      <c r="B41" s="90" t="n">
+      <c r="B41" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C41" s="90" t="inlineStr">
+      <c r="C41" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D41" s="60" t="n"/>
-      <c r="E41" s="91" t="n">
+      <c r="D41" s="61" t="n"/>
+      <c r="E41" s="93" t="n">
         <v>97</v>
       </c>
-      <c r="F41" s="59" t="n">
+      <c r="F41" s="60" t="n">
         <v>5016.1</v>
       </c>
-      <c r="G41" s="59" t="n">
+      <c r="G41" s="60" t="n">
         <v>408</v>
       </c>
-      <c r="H41" s="59" t="n">
+      <c r="H41" s="60" t="n">
         <v>453</v>
       </c>
-      <c r="I41" s="92" t="n">
+      <c r="I41" s="94" t="n">
         <v>1.782</v>
       </c>
     </row>
     <row r="42" ht="27" customHeight="1">
-      <c r="B42" s="90" t="n">
+      <c r="B42" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C42" s="90" t="inlineStr">
+      <c r="C42" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D42" s="60" t="n"/>
-      <c r="E42" s="91" t="n">
+      <c r="D42" s="61" t="n"/>
+      <c r="E42" s="93" t="n">
         <v>97</v>
       </c>
-      <c r="F42" s="59" t="n">
+      <c r="F42" s="60" t="n">
         <v>5022.5</v>
       </c>
-      <c r="G42" s="59" t="n">
+      <c r="G42" s="60" t="n">
         <v>407</v>
       </c>
-      <c r="H42" s="59" t="n">
+      <c r="H42" s="60" t="n">
         <v>452</v>
       </c>
-      <c r="I42" s="92" t="n">
+      <c r="I42" s="94" t="n">
         <v>1.8216</v>
       </c>
     </row>
     <row r="43" ht="27" customHeight="1">
-      <c r="B43" s="90" t="n">
+      <c r="B43" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C43" s="90" t="inlineStr">
+      <c r="C43" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D43" s="60" t="n"/>
-      <c r="E43" s="91" t="n">
+      <c r="D43" s="61" t="n"/>
+      <c r="E43" s="93" t="n">
         <v>184</v>
       </c>
-      <c r="F43" s="59" t="n">
+      <c r="F43" s="60" t="n">
         <v>9583.5</v>
       </c>
-      <c r="G43" s="59" t="n">
+      <c r="G43" s="60" t="n">
         <v>773.7684</v>
       </c>
-      <c r="H43" s="59" t="n">
+      <c r="H43" s="60" t="n">
         <v>817.3474</v>
       </c>
-      <c r="I43" s="92" t="n">
+      <c r="I43" s="94" t="n">
         <v>2.6461</v>
       </c>
     </row>
     <row r="44" ht="27" customHeight="1">
-      <c r="B44" s="90" t="n">
+      <c r="B44" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C44" s="90" t="inlineStr">
+      <c r="C44" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D44" s="60" t="n"/>
-      <c r="E44" s="91" t="n">
+      <c r="D44" s="61" t="n"/>
+      <c r="E44" s="93" t="n">
         <v>6</v>
       </c>
-      <c r="F44" s="59" t="n">
+      <c r="F44" s="60" t="n">
         <v>237.8</v>
       </c>
-      <c r="G44" s="59" t="n">
+      <c r="G44" s="60" t="n">
         <v>25.2316</v>
       </c>
-      <c r="H44" s="59" t="n">
+      <c r="H44" s="60" t="n">
         <v>26.6526</v>
       </c>
-      <c r="I44" s="92" t="n">
+      <c r="I44" s="94" t="n">
         <v>0.0863</v>
       </c>
     </row>
     <row r="45" ht="27" customHeight="1">
-      <c r="B45" s="90" t="n">
+      <c r="B45" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C45" s="90" t="inlineStr">
+      <c r="C45" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D45" s="60" t="n"/>
-      <c r="E45" s="91" t="n">
+      <c r="D45" s="61" t="n"/>
+      <c r="E45" s="93" t="n">
         <v>185</v>
       </c>
-      <c r="F45" s="59" t="n">
+      <c r="F45" s="60" t="n">
         <v>9782.9</v>
       </c>
-      <c r="G45" s="59" t="n">
+      <c r="G45" s="60" t="n">
         <v>786.25</v>
       </c>
-      <c r="H45" s="59" t="n">
+      <c r="H45" s="60" t="n">
         <v>830.0658</v>
       </c>
-      <c r="I45" s="92" t="n">
+      <c r="I45" s="94" t="n">
         <v>2.5063</v>
       </c>
     </row>
     <row r="46" ht="27" customHeight="1">
-      <c r="B46" s="90" t="n">
+      <c r="B46" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C46" s="90" t="inlineStr">
+      <c r="C46" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D46" s="60" t="n"/>
-      <c r="E46" s="91" t="n">
+      <c r="D46" s="61" t="n"/>
+      <c r="E46" s="93" t="n">
         <v>5</v>
       </c>
-      <c r="F46" s="59" t="n">
+      <c r="F46" s="60" t="n">
         <v>199</v>
       </c>
-      <c r="G46" s="59" t="n">
+      <c r="G46" s="60" t="n">
         <v>21.25</v>
       </c>
-      <c r="H46" s="59" t="n">
+      <c r="H46" s="60" t="n">
         <v>22.4342</v>
       </c>
-      <c r="I46" s="92" t="n">
+      <c r="I46" s="94" t="n">
         <v>0.0677</v>
       </c>
     </row>
     <row r="47" ht="27" customHeight="1">
-      <c r="B47" s="90" t="n">
+      <c r="B47" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C47" s="90" t="inlineStr">
+      <c r="C47" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D47" s="60" t="n"/>
-      <c r="E47" s="91" t="n">
+      <c r="D47" s="61" t="n"/>
+      <c r="E47" s="93" t="n">
         <v>190</v>
       </c>
-      <c r="F47" s="59" t="n">
+      <c r="F47" s="60" t="n">
         <v>10009.4</v>
       </c>
-      <c r="G47" s="59" t="n">
+      <c r="G47" s="60" t="n">
         <v>824</v>
       </c>
-      <c r="H47" s="59" t="n">
+      <c r="H47" s="60" t="n">
         <v>869</v>
       </c>
-      <c r="I47" s="92" t="n">
+      <c r="I47" s="94" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="48" ht="27" customHeight="1">
-      <c r="B48" s="90" t="n">
+      <c r="B48" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C48" s="90" t="inlineStr">
+      <c r="C48" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D48" s="60" t="n"/>
-      <c r="E48" s="91" t="n">
+      <c r="D48" s="61" t="n"/>
+      <c r="E48" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F48" s="59" t="n">
+      <c r="F48" s="60" t="n">
         <v>10072.6</v>
       </c>
-      <c r="G48" s="59" t="n">
+      <c r="G48" s="60" t="n">
         <v>821</v>
       </c>
-      <c r="H48" s="59" t="n">
+      <c r="H48" s="60" t="n">
         <v>866</v>
       </c>
-      <c r="I48" s="92" t="n">
+      <c r="I48" s="94" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="49" ht="27" customHeight="1">
-      <c r="B49" s="90" t="n">
+      <c r="B49" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C49" s="90" t="inlineStr">
+      <c r="C49" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D49" s="60" t="n"/>
-      <c r="E49" s="91" t="n">
+      <c r="D49" s="61" t="n"/>
+      <c r="E49" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F49" s="59" t="n">
+      <c r="F49" s="60" t="n">
         <v>10117.1</v>
       </c>
-      <c r="G49" s="59" t="n">
+      <c r="G49" s="60" t="n">
         <v>825.5</v>
       </c>
-      <c r="H49" s="59" t="n">
+      <c r="H49" s="60" t="n">
         <v>870.5</v>
       </c>
-      <c r="I49" s="92" t="n">
+      <c r="I49" s="94" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="50" ht="27" customHeight="1">
-      <c r="B50" s="90" t="n">
+      <c r="B50" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C50" s="90" t="inlineStr">
+      <c r="C50" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D50" s="60" t="n"/>
-      <c r="E50" s="91" t="n">
+      <c r="D50" s="61" t="n"/>
+      <c r="E50" s="93" t="n">
         <v>89</v>
       </c>
-      <c r="F50" s="59" t="n">
+      <c r="F50" s="60" t="n">
         <v>4707.4</v>
       </c>
-      <c r="G50" s="59" t="n">
+      <c r="G50" s="60" t="n">
         <v>376.5385</v>
       </c>
-      <c r="H50" s="59" t="n">
+      <c r="H50" s="60" t="n">
         <v>415.0481</v>
       </c>
-      <c r="I50" s="92" t="n">
+      <c r="I50" s="94" t="n">
         <v>1.4572</v>
       </c>
     </row>
     <row r="51" ht="27" customHeight="1">
-      <c r="B51" s="90" t="n">
+      <c r="B51" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C51" s="90" t="inlineStr">
+      <c r="C51" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D51" s="60" t="n"/>
-      <c r="E51" s="91" t="n">
+      <c r="D51" s="61" t="n"/>
+      <c r="E51" s="93" t="n">
         <v>8</v>
       </c>
-      <c r="F51" s="59" t="n">
+      <c r="F51" s="60" t="n">
         <v>322.8</v>
       </c>
-      <c r="G51" s="59" t="n">
+      <c r="G51" s="60" t="n">
         <v>33.8462</v>
       </c>
-      <c r="H51" s="59" t="n">
+      <c r="H51" s="60" t="n">
         <v>37.3077</v>
       </c>
-      <c r="I51" s="92" t="n">
+      <c r="I51" s="94" t="n">
         <v>0.131</v>
       </c>
     </row>
     <row r="52" ht="27" customHeight="1">
-      <c r="B52" s="90" t="n">
+      <c r="B52" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C52" s="90" t="inlineStr">
+      <c r="C52" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D52" s="61" t="n"/>
-      <c r="E52" s="91" t="n">
+      <c r="D52" s="62" t="n"/>
+      <c r="E52" s="93" t="n">
         <v>7</v>
       </c>
-      <c r="F52" s="59" t="n">
+      <c r="F52" s="60" t="n">
         <v>367.3</v>
       </c>
-      <c r="G52" s="59" t="n">
+      <c r="G52" s="60" t="n">
         <v>29.6154</v>
       </c>
-      <c r="H52" s="59" t="n">
+      <c r="H52" s="60" t="n">
         <v>32.6442</v>
       </c>
-      <c r="I52" s="92" t="n">
+      <c r="I52" s="94" t="n">
         <v>0.1146</v>
       </c>
     </row>
     <row r="53" ht="27" customHeight="1">
-      <c r="A53" s="93" t="n"/>
+      <c r="A53" s="95" t="n"/>
       <c r="B53" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
@@ -4489,11 +4505,11 @@
       </c>
       <c r="C53" s="55" t="n"/>
       <c r="D53" s="55" t="n"/>
-      <c r="E53" s="89" t="n"/>
+      <c r="E53" s="90" t="n"/>
       <c r="F53" s="56" t="n"/>
       <c r="G53" s="56" t="n"/>
       <c r="H53" s="56" t="n"/>
-      <c r="I53" s="88" t="n"/>
+      <c r="I53" s="89" t="n"/>
     </row>
     <row r="54" ht="27" customHeight="1">
       <c r="A54" s="55" t="n"/>
@@ -4508,7 +4524,7 @@
         </is>
       </c>
       <c r="D54" s="55" t="n"/>
-      <c r="E54" s="89">
+      <c r="E54" s="90">
         <f>SUM(E23:E52)</f>
         <v/>
       </c>
@@ -4524,7 +4540,7 @@
         <f>SUM(H23:H52)</f>
         <v/>
       </c>
-      <c r="I54" s="88">
+      <c r="I54" s="89">
         <f>SUM(I23:I52)</f>
         <v/>
       </c>
@@ -4556,7 +4572,7 @@
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F56" s="87" t="n"/>
+      <c r="F56" s="88" t="n"/>
       <c r="G56" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -4567,18 +4583,18 @@
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I56" s="88" t="inlineStr">
+      <c r="I56" s="89" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
     <row r="57" ht="27" customHeight="1">
-      <c r="A57" s="61" t="n"/>
-      <c r="B57" s="61" t="n"/>
-      <c r="C57" s="61" t="n"/>
-      <c r="D57" s="61" t="n"/>
-      <c r="E57" s="89" t="inlineStr">
+      <c r="A57" s="62" t="n"/>
+      <c r="B57" s="62" t="n"/>
+      <c r="C57" s="62" t="n"/>
+      <c r="D57" s="62" t="n"/>
+      <c r="E57" s="90" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
@@ -4588,404 +4604,404 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="G57" s="61" t="n"/>
-      <c r="H57" s="61" t="n"/>
-      <c r="I57" s="61" t="n"/>
+      <c r="G57" s="62" t="n"/>
+      <c r="H57" s="62" t="n"/>
+      <c r="I57" s="62" t="n"/>
     </row>
     <row r="58" ht="27" customHeight="1">
-      <c r="A58" s="90" t="inlineStr">
+      <c r="A58" s="91" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B58" s="90" t="n">
+      <c r="B58" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C58" s="90" t="inlineStr">
+      <c r="C58" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D58" s="58" t="inlineStr">
+      <c r="D58" s="59" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E58" s="91" t="n">
+      <c r="E58" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F58" s="59" t="n">
+      <c r="F58" s="60" t="n">
         <v>10187.1</v>
       </c>
-      <c r="G58" s="59" t="n">
+      <c r="G58" s="60" t="n">
         <v>842.5</v>
       </c>
-      <c r="H58" s="59" t="n">
+      <c r="H58" s="60" t="n">
         <v>887.5</v>
       </c>
-      <c r="I58" s="92" t="n">
+      <c r="I58" s="94" t="n">
         <v>2.6532</v>
       </c>
     </row>
     <row r="59" ht="27" customHeight="1">
-      <c r="A59" s="90" t="inlineStr">
+      <c r="A59" s="91" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B59" s="90" t="n">
+      <c r="B59" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C59" s="90" t="inlineStr">
+      <c r="C59" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D59" s="60" t="n"/>
-      <c r="E59" s="91" t="n">
+      <c r="D59" s="61" t="n"/>
+      <c r="E59" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F59" s="59" t="n">
+      <c r="F59" s="60" t="n">
         <v>10219.2</v>
       </c>
-      <c r="G59" s="59" t="n">
+      <c r="G59" s="60" t="n">
         <v>846</v>
       </c>
-      <c r="H59" s="59" t="n">
+      <c r="H59" s="60" t="n">
         <v>891</v>
       </c>
-      <c r="I59" s="92" t="n">
+      <c r="I59" s="94" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="60" ht="27" customHeight="1">
-      <c r="A60" s="90" t="inlineStr">
+      <c r="A60" s="91" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B60" s="90" t="n">
+      <c r="B60" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C60" s="90" t="inlineStr">
+      <c r="C60" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D60" s="60" t="n"/>
-      <c r="E60" s="91" t="n">
+      <c r="D60" s="61" t="n"/>
+      <c r="E60" s="93" t="n">
         <v>207</v>
       </c>
-      <c r="F60" s="59" t="n">
+      <c r="F60" s="60" t="n">
         <v>10773.3</v>
       </c>
-      <c r="G60" s="59" t="n">
+      <c r="G60" s="60" t="n">
         <v>883.7671</v>
       </c>
-      <c r="H60" s="59" t="n">
+      <c r="H60" s="60" t="n">
         <v>926.3013999999999</v>
       </c>
-      <c r="I60" s="92" t="n">
+      <c r="I60" s="94" t="n">
         <v>2.8447</v>
       </c>
     </row>
     <row r="61" ht="27" customHeight="1">
-      <c r="A61" s="90" t="inlineStr">
+      <c r="A61" s="91" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B61" s="90" t="n">
+      <c r="B61" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C61" s="90" t="inlineStr">
+      <c r="C61" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D61" s="60" t="n"/>
-      <c r="E61" s="91" t="n">
+      <c r="D61" s="61" t="n"/>
+      <c r="E61" s="93" t="n">
         <v>12</v>
       </c>
-      <c r="F61" s="59" t="n">
+      <c r="F61" s="60" t="n">
         <v>479.1</v>
       </c>
-      <c r="G61" s="59" t="n">
+      <c r="G61" s="60" t="n">
         <v>51.2329</v>
       </c>
-      <c r="H61" s="59" t="n">
+      <c r="H61" s="60" t="n">
         <v>53.6986</v>
       </c>
-      <c r="I61" s="92" t="n">
+      <c r="I61" s="94" t="n">
         <v>0.1649</v>
       </c>
     </row>
     <row r="62" ht="27" customHeight="1">
-      <c r="B62" s="90" t="n">
+      <c r="B62" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C62" s="90" t="inlineStr">
+      <c r="C62" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D62" s="60" t="n"/>
-      <c r="E62" s="91" t="n">
+      <c r="D62" s="61" t="n"/>
+      <c r="E62" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F62" s="59" t="n">
+      <c r="F62" s="60" t="n">
         <v>10215.8</v>
       </c>
-      <c r="G62" s="59" t="n">
+      <c r="G62" s="60" t="n">
         <v>840</v>
       </c>
-      <c r="H62" s="59" t="n">
+      <c r="H62" s="60" t="n">
         <v>885</v>
       </c>
-      <c r="I62" s="92" t="n">
+      <c r="I62" s="94" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="63" ht="27" customHeight="1">
-      <c r="B63" s="90" t="n">
+      <c r="B63" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C63" s="90" t="inlineStr">
+      <c r="C63" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D63" s="60" t="n"/>
-      <c r="E63" s="91" t="n">
+      <c r="D63" s="61" t="n"/>
+      <c r="E63" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F63" s="59" t="n">
+      <c r="F63" s="60" t="n">
         <v>10237.5</v>
       </c>
-      <c r="G63" s="59" t="n">
+      <c r="G63" s="60" t="n">
         <v>863.5</v>
       </c>
-      <c r="H63" s="59" t="n">
+      <c r="H63" s="60" t="n">
         <v>908.5</v>
       </c>
-      <c r="I63" s="92" t="n">
+      <c r="I63" s="94" t="n">
         <v>2.6928</v>
       </c>
     </row>
     <row r="64" ht="27" customHeight="1">
-      <c r="B64" s="90" t="n">
+      <c r="B64" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C64" s="90" t="inlineStr">
+      <c r="C64" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D64" s="60" t="n"/>
-      <c r="E64" s="91" t="n">
+      <c r="D64" s="61" t="n"/>
+      <c r="E64" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F64" s="59" t="n">
+      <c r="F64" s="60" t="n">
         <v>10196.1</v>
       </c>
-      <c r="G64" s="59" t="n">
+      <c r="G64" s="60" t="n">
         <v>849</v>
       </c>
-      <c r="H64" s="59" t="n">
+      <c r="H64" s="60" t="n">
         <v>894</v>
       </c>
-      <c r="I64" s="92" t="n">
+      <c r="I64" s="94" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="65" ht="27" customHeight="1">
-      <c r="B65" s="90" t="n">
+      <c r="B65" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C65" s="90" t="inlineStr">
+      <c r="C65" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D65" s="60" t="n"/>
-      <c r="E65" s="91" t="n">
+      <c r="D65" s="61" t="n"/>
+      <c r="E65" s="93" t="n">
         <v>175</v>
       </c>
-      <c r="F65" s="59" t="n">
+      <c r="F65" s="60" t="n">
         <v>9097.6</v>
       </c>
-      <c r="G65" s="59" t="n">
+      <c r="G65" s="60" t="n">
         <v>739.443</v>
       </c>
-      <c r="H65" s="59" t="n">
+      <c r="H65" s="60" t="n">
         <v>780.2461</v>
       </c>
-      <c r="I65" s="92" t="n">
+      <c r="I65" s="94" t="n">
         <v>2.3339</v>
       </c>
     </row>
     <row r="66" ht="27" customHeight="1">
-      <c r="B66" s="90" t="n">
+      <c r="B66" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C66" s="90" t="inlineStr">
+      <c r="C66" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D66" s="60" t="n"/>
-      <c r="E66" s="91" t="n">
+      <c r="D66" s="61" t="n"/>
+      <c r="E66" s="93" t="n">
         <v>18</v>
       </c>
-      <c r="F66" s="59" t="n">
+      <c r="F66" s="60" t="n">
         <v>726</v>
       </c>
-      <c r="G66" s="59" t="n">
+      <c r="G66" s="60" t="n">
         <v>76.057</v>
       </c>
-      <c r="H66" s="59" t="n">
+      <c r="H66" s="60" t="n">
         <v>80.2539</v>
       </c>
-      <c r="I66" s="92" t="n">
+      <c r="I66" s="94" t="n">
         <v>0.2401</v>
       </c>
     </row>
     <row r="67" ht="27" customHeight="1">
-      <c r="B67" s="90" t="n">
+      <c r="B67" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C67" s="90" t="inlineStr">
+      <c r="C67" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D67" s="60" t="n"/>
-      <c r="E67" s="91" t="n">
+      <c r="D67" s="61" t="n"/>
+      <c r="E67" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F67" s="59" t="n">
+      <c r="F67" s="60" t="n">
         <v>10110.4</v>
       </c>
-      <c r="G67" s="59" t="n">
+      <c r="G67" s="60" t="n">
         <v>840</v>
       </c>
-      <c r="H67" s="59" t="n">
+      <c r="H67" s="60" t="n">
         <v>885</v>
       </c>
-      <c r="I67" s="92" t="n">
+      <c r="I67" s="94" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="68" ht="27" customHeight="1">
-      <c r="B68" s="90" t="n">
+      <c r="B68" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C68" s="90" t="inlineStr">
+      <c r="C68" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D68" s="60" t="n"/>
-      <c r="E68" s="91" t="n">
+      <c r="D68" s="61" t="n"/>
+      <c r="E68" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F68" s="59" t="n">
+      <c r="F68" s="60" t="n">
         <v>10165.7</v>
       </c>
-      <c r="G68" s="59" t="n">
+      <c r="G68" s="60" t="n">
         <v>844.5</v>
       </c>
-      <c r="H68" s="59" t="n">
+      <c r="H68" s="60" t="n">
         <v>889.5</v>
       </c>
-      <c r="I68" s="92" t="n">
+      <c r="I68" s="94" t="n">
         <v>2.772</v>
       </c>
     </row>
     <row r="69" ht="27" customHeight="1">
-      <c r="B69" s="90" t="n">
+      <c r="B69" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C69" s="90" t="inlineStr">
+      <c r="C69" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D69" s="60" t="n"/>
-      <c r="E69" s="91" t="n">
+      <c r="D69" s="61" t="n"/>
+      <c r="E69" s="93" t="n">
         <v>195</v>
       </c>
-      <c r="F69" s="59" t="n">
+      <c r="F69" s="60" t="n">
         <v>10222.1</v>
       </c>
-      <c r="G69" s="59" t="n">
+      <c r="G69" s="60" t="n">
         <v>843</v>
       </c>
-      <c r="H69" s="59" t="n">
+      <c r="H69" s="60" t="n">
         <v>888</v>
       </c>
-      <c r="I69" s="92" t="n">
+      <c r="I69" s="94" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="70" ht="27" customHeight="1">
-      <c r="B70" s="90" t="inlineStr">
+      <c r="B70" s="92" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="C70" s="90" t="inlineStr">
+      <c r="C70" s="92" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="D70" s="60" t="n"/>
-      <c r="E70" s="91" t="n">
+      <c r="D70" s="61" t="n"/>
+      <c r="E70" s="93" t="n">
         <v>106</v>
       </c>
-      <c r="F70" s="59" t="n">
+      <c r="F70" s="60" t="n">
         <v>5345</v>
       </c>
-      <c r="G70" s="59" t="n">
+      <c r="G70" s="60" t="n">
         <v>381.211</v>
       </c>
-      <c r="H70" s="59" t="n">
+      <c r="H70" s="60" t="n">
         <v>424.9725</v>
       </c>
-      <c r="I70" s="92" t="n">
+      <c r="I70" s="94" t="n">
         <v>2.0795</v>
       </c>
     </row>
     <row r="71" ht="27" customHeight="1">
-      <c r="B71" s="90" t="inlineStr">
+      <c r="B71" s="92" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="C71" s="90" t="inlineStr">
+      <c r="C71" s="92" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="D71" s="61" t="n"/>
-      <c r="E71" s="91" t="n">
+      <c r="D71" s="62" t="n"/>
+      <c r="E71" s="93" t="n">
         <v>3</v>
       </c>
-      <c r="F71" s="59" t="n">
+      <c r="F71" s="60" t="n">
         <v>121</v>
       </c>
-      <c r="G71" s="59" t="n">
+      <c r="G71" s="60" t="n">
         <v>10.789</v>
       </c>
-      <c r="H71" s="59" t="n">
+      <c r="H71" s="60" t="n">
         <v>12.0275</v>
       </c>
-      <c r="I71" s="92" t="n">
+      <c r="I71" s="94" t="n">
         <v>0.0589</v>
       </c>
     </row>
     <row r="72" ht="27" customHeight="1">
-      <c r="A72" s="93" t="n"/>
+      <c r="A72" s="95" t="n"/>
       <c r="B72" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
@@ -4993,11 +5009,11 @@
       </c>
       <c r="C72" s="55" t="n"/>
       <c r="D72" s="55" t="n"/>
-      <c r="E72" s="89" t="n"/>
+      <c r="E72" s="90" t="n"/>
       <c r="F72" s="56" t="n"/>
       <c r="G72" s="56" t="n"/>
       <c r="H72" s="56" t="n"/>
-      <c r="I72" s="88" t="n"/>
+      <c r="I72" s="89" t="n"/>
     </row>
     <row r="73" ht="27" customHeight="1">
       <c r="A73" s="55" t="n"/>
@@ -5012,7 +5028,7 @@
         </is>
       </c>
       <c r="D73" s="55" t="n"/>
-      <c r="E73" s="89">
+      <c r="E73" s="90">
         <f>SUM(E58:E71)</f>
         <v/>
       </c>
@@ -5028,55 +5044,55 @@
         <f>SUM(H58:H71)</f>
         <v/>
       </c>
-      <c r="I73" s="88">
+      <c r="I73" s="89">
         <f>SUM(I58:I71)</f>
         <v/>
       </c>
     </row>
     <row r="74" ht="27" customHeight="1">
-      <c r="A74" s="94" t="n"/>
-      <c r="B74" s="94" t="inlineStr">
+      <c r="A74" s="96" t="n"/>
+      <c r="B74" s="96" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="C74" s="94" t="inlineStr">
+      <c r="C74" s="96" t="inlineStr">
         <is>
           <t>31 PALLETS</t>
         </is>
       </c>
-      <c r="D74" s="94" t="n"/>
-      <c r="E74" s="95">
+      <c r="D74" s="96" t="n"/>
+      <c r="E74" s="97">
         <f>SUM(E23:E52,E58:E71)</f>
         <v/>
       </c>
-      <c r="F74" s="96">
+      <c r="F74" s="98">
         <f>SUM(F23:F52,F58:F71)</f>
         <v/>
       </c>
-      <c r="G74" s="96">
+      <c r="G74" s="98">
         <f>SUM(G23:G52,G58:G71)</f>
         <v/>
       </c>
-      <c r="H74" s="96">
+      <c r="H74" s="98">
         <f>SUM(H23:H52,H58:H71)</f>
         <v/>
       </c>
-      <c r="I74" s="97">
+      <c r="I74" s="99">
         <f>SUM(I23:I52,I58:I71)</f>
         <v/>
       </c>
     </row>
     <row r="75" ht="27" customHeight="1">
-      <c r="A75" s="98" t="inlineStr">
+      <c r="A75" s="100" t="inlineStr">
         <is>
           <t>Country of Original Cambodia</t>
         </is>
       </c>
-      <c r="B75" s="98" t="n"/>
-      <c r="C75" s="98" t="n"/>
-      <c r="D75" s="99" t="n"/>
-      <c r="E75" s="100" t="n"/>
+      <c r="B75" s="100" t="n"/>
+      <c r="C75" s="100" t="n"/>
+      <c r="D75" s="101" t="n"/>
+      <c r="E75" s="102" t="n"/>
       <c r="F75" s="26" t="n"/>
       <c r="G75" s="26" t="n"/>
       <c r="H75" s="26" t="n"/>
@@ -5094,20 +5110,20 @@
       <c r="T75" s="2" t="n"/>
     </row>
     <row r="76" ht="65.25" customHeight="1">
-      <c r="A76" s="63" t="inlineStr">
+      <c r="A76" s="64" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B76" s="101" t="inlineStr">
+      <c r="B76" s="103" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="E76" s="102" t="n"/>
-      <c r="F76" s="102" t="n"/>
-      <c r="G76" s="102" t="n"/>
+      <c r="E76" s="104" t="n"/>
+      <c r="F76" s="104" t="n"/>
+      <c r="G76" s="104" t="n"/>
       <c r="H76" s="26" t="n"/>
       <c r="I76" s="2" t="n"/>
       <c r="J76" s="2" t="n"/>
@@ -5123,16 +5139,16 @@
       <c r="T76" s="2" t="n"/>
     </row>
     <row r="77" ht="51.75" customHeight="1">
-      <c r="A77" s="101" t="inlineStr">
+      <c r="A77" s="103" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
                                           /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="E77" s="102" t="n"/>
-      <c r="F77" s="102" t="n"/>
-      <c r="G77" s="102" t="n"/>
-      <c r="H77" s="102" t="n"/>
+      <c r="E77" s="104" t="n"/>
+      <c r="F77" s="104" t="n"/>
+      <c r="G77" s="104" t="n"/>
+      <c r="H77" s="104" t="n"/>
       <c r="I77" s="2" t="n"/>
       <c r="J77" s="2" t="n"/>
       <c r="K77" s="2" t="n"/>
@@ -5147,14 +5163,14 @@
       <c r="T77" s="2" t="n"/>
     </row>
     <row r="78" ht="27" customHeight="1">
-      <c r="A78" s="69" t="inlineStr">
+      <c r="A78" s="70" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
-      <c r="B78" s="69" t="n"/>
-      <c r="C78" s="69" t="n"/>
-      <c r="D78" s="69" t="n"/>
+      <c r="B78" s="70" t="n"/>
+      <c r="C78" s="70" t="n"/>
+      <c r="D78" s="70" t="n"/>
       <c r="E78" s="50" t="n"/>
       <c r="F78" s="50" t="n"/>
       <c r="G78" s="50" t="n"/>
@@ -5173,14 +5189,14 @@
       <c r="T78" s="2" t="n"/>
     </row>
     <row r="79" ht="27" customHeight="1">
-      <c r="A79" s="69" t="inlineStr">
+      <c r="A79" s="70" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
       </c>
-      <c r="B79" s="69" t="n"/>
-      <c r="C79" s="69" t="n"/>
-      <c r="D79" s="69" t="n"/>
+      <c r="B79" s="70" t="n"/>
+      <c r="C79" s="70" t="n"/>
+      <c r="D79" s="70" t="n"/>
       <c r="E79" s="50" t="n"/>
       <c r="F79" s="50" t="n"/>
       <c r="G79" s="50" t="n"/>
@@ -5200,7 +5216,7 @@
     </row>
     <row r="80" ht="27" customHeight="1">
       <c r="A80" s="2" t="n"/>
-      <c r="B80" s="103" t="n"/>
+      <c r="B80" s="105" t="n"/>
       <c r="C80" s="2" t="n"/>
       <c r="D80" s="2" t="n"/>
       <c r="E80" s="52" t="n"/>

</xml_diff>

<commit_message>
adding the orderly header col system wherer it depend on runtime index
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -219,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -335,6 +335,37 @@
       <right style="thin">
         <color rgb="00000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
       <top style="thin">
         <color rgb="00000000"/>
       </top>
@@ -347,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -578,16 +609,20 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3615,43 +3650,43 @@
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B21" s="55" t="inlineStr">
+      <c r="B21" s="88" t="n"/>
+      <c r="C21" s="55" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="C21" s="55" t="inlineStr">
+      <c r="D21" s="55" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="D21" s="55" t="inlineStr">
+      <c r="E21" s="55" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E21" s="55" t="inlineStr">
+      <c r="F21" s="55" t="inlineStr">
         <is>
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F21" s="88" t="n"/>
-      <c r="G21" s="56" t="inlineStr">
+      <c r="G21" s="89" t="n"/>
+      <c r="H21" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="H21" s="56" t="inlineStr">
+      <c r="I21" s="56" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I21" s="89" t="inlineStr">
+      <c r="J21" s="90" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
-      <c r="J21" s="2" t="n"/>
       <c r="K21" s="2" t="n"/>
       <c r="L21" s="2" t="n"/>
       <c r="M21" s="2" t="n"/>
@@ -3664,871 +3699,873 @@
       <c r="T21" s="2" t="n"/>
     </row>
     <row r="22" ht="27" customHeight="1">
-      <c r="A22" s="62" t="n"/>
-      <c r="B22" s="62" t="n"/>
+      <c r="A22" s="91" t="n"/>
+      <c r="B22" s="92" t="n"/>
       <c r="C22" s="62" t="n"/>
       <c r="D22" s="62" t="n"/>
-      <c r="E22" s="90" t="inlineStr">
+      <c r="E22" s="62" t="n"/>
+      <c r="F22" s="93" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="F22" s="56" t="inlineStr">
+      <c r="G22" s="56" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="G22" s="62" t="n"/>
       <c r="H22" s="62" t="n"/>
       <c r="I22" s="62" t="n"/>
+      <c r="J22" s="62" t="n"/>
     </row>
     <row r="23" ht="27" customHeight="1">
-      <c r="A23" s="91" t="inlineStr">
+      <c r="A23" s="94" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B23" s="92" t="inlineStr">
+      <c r="B23" s="95" t="n"/>
+      <c r="C23" s="96" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="C23" s="92" t="inlineStr">
+      <c r="D23" s="96" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="D23" s="59" t="inlineStr">
+      <c r="E23" s="59" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E23" s="93" t="n">
+      <c r="F23" s="97" t="n">
         <v>122</v>
       </c>
-      <c r="F23" s="60" t="n">
+      <c r="G23" s="60" t="n">
         <v>6461.7</v>
       </c>
-      <c r="G23" s="60" t="n">
+      <c r="H23" s="60" t="n">
         <v>467.8306</v>
       </c>
-      <c r="H23" s="60" t="n">
+      <c r="I23" s="60" t="n">
         <v>512.1048</v>
       </c>
-      <c r="I23" s="94" t="n">
+      <c r="J23" s="98" t="n">
         <v>1.8312</v>
       </c>
     </row>
     <row r="24" ht="27" customHeight="1">
-      <c r="A24" s="91" t="inlineStr">
+      <c r="A24" s="94" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B24" s="92" t="inlineStr">
+      <c r="B24" s="95" t="n"/>
+      <c r="C24" s="96" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="C24" s="92" t="inlineStr">
+      <c r="D24" s="96" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="D24" s="61" t="n"/>
-      <c r="E24" s="93" t="n">
+      <c r="E24" s="61" t="n"/>
+      <c r="F24" s="97" t="n">
         <v>2</v>
       </c>
-      <c r="F24" s="60" t="n">
+      <c r="G24" s="60" t="n">
         <v>77.90000000000001</v>
       </c>
-      <c r="G24" s="60" t="n">
+      <c r="H24" s="60" t="n">
         <v>7.6694</v>
       </c>
-      <c r="H24" s="60" t="n">
+      <c r="I24" s="60" t="n">
         <v>8.395200000000001</v>
       </c>
-      <c r="I24" s="94" t="n">
+      <c r="J24" s="98" t="n">
         <v>0.03</v>
       </c>
     </row>
     <row r="25" ht="27" customHeight="1">
-      <c r="A25" s="91" t="inlineStr">
+      <c r="A25" s="94" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B25" s="92" t="inlineStr">
+      <c r="B25" s="95" t="n"/>
+      <c r="C25" s="96" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C25" s="92" t="inlineStr">
+      <c r="D25" s="96" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D25" s="61" t="n"/>
-      <c r="E25" s="93" t="n">
+      <c r="E25" s="61" t="n"/>
+      <c r="F25" s="97" t="n">
         <v>190</v>
       </c>
-      <c r="F25" s="60" t="n">
+      <c r="G25" s="60" t="n">
         <v>10009.4</v>
       </c>
-      <c r="G25" s="60" t="n">
+      <c r="H25" s="60" t="n">
         <v>757</v>
       </c>
-      <c r="H25" s="60" t="n">
+      <c r="I25" s="60" t="n">
         <v>802</v>
       </c>
-      <c r="I25" s="94" t="n">
+      <c r="J25" s="98" t="n">
         <v>2.4552</v>
       </c>
     </row>
     <row r="26" ht="27" customHeight="1">
-      <c r="A26" s="91" t="inlineStr">
+      <c r="A26" s="94" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B26" s="92" t="inlineStr">
+      <c r="B26" s="95" t="n"/>
+      <c r="C26" s="96" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C26" s="92" t="inlineStr">
+      <c r="D26" s="96" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D26" s="61" t="n"/>
-      <c r="E26" s="93" t="n">
+      <c r="E26" s="61" t="n"/>
+      <c r="F26" s="97" t="n">
         <v>208</v>
       </c>
-      <c r="F26" s="60" t="n">
+      <c r="G26" s="60" t="n">
         <v>10940.1</v>
       </c>
-      <c r="G26" s="60" t="n">
+      <c r="H26" s="60" t="n">
         <v>842.2056</v>
       </c>
-      <c r="H26" s="60" t="n">
+      <c r="I26" s="60" t="n">
         <v>885.9439</v>
       </c>
-      <c r="I26" s="94" t="n">
+      <c r="J26" s="98" t="n">
         <v>2.6943</v>
       </c>
     </row>
     <row r="27" ht="27" customHeight="1">
-      <c r="B27" s="92" t="inlineStr">
+      <c r="C27" s="96" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C27" s="92" t="inlineStr">
+      <c r="D27" s="96" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="D27" s="61" t="n"/>
-      <c r="E27" s="93" t="n">
+      <c r="E27" s="61" t="n"/>
+      <c r="F27" s="97" t="n">
         <v>6</v>
       </c>
-      <c r="F27" s="60" t="n">
+      <c r="G27" s="60" t="n">
         <v>241.9</v>
       </c>
-      <c r="G27" s="60" t="n">
+      <c r="H27" s="60" t="n">
         <v>24.2944</v>
       </c>
-      <c r="H27" s="60" t="n">
+      <c r="I27" s="60" t="n">
         <v>25.5561</v>
       </c>
-      <c r="I27" s="94" t="n">
+      <c r="J27" s="98" t="n">
         <v>0.07770000000000001</v>
       </c>
     </row>
     <row r="28" ht="27" customHeight="1">
-      <c r="B28" s="92" t="n">
+      <c r="C28" s="96" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C28" s="92" t="inlineStr">
+      <c r="D28" s="96" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D28" s="61" t="n"/>
-      <c r="E28" s="93" t="n">
+      <c r="E28" s="61" t="n"/>
+      <c r="F28" s="97" t="n">
         <v>154</v>
       </c>
-      <c r="F28" s="60" t="n">
+      <c r="G28" s="60" t="n">
         <v>7788.7</v>
       </c>
-      <c r="G28" s="60" t="n">
+      <c r="H28" s="60" t="n">
         <v>617.7907</v>
       </c>
-      <c r="H28" s="60" t="n">
+      <c r="I28" s="60" t="n">
         <v>658.0814</v>
       </c>
-      <c r="I28" s="94" t="n">
+      <c r="J28" s="98" t="n">
         <v>2.0564</v>
       </c>
     </row>
     <row r="29" ht="27" customHeight="1">
-      <c r="B29" s="92" t="n">
+      <c r="C29" s="96" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C29" s="92" t="inlineStr">
+      <c r="D29" s="96" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D29" s="61" t="n"/>
-      <c r="E29" s="93" t="n">
+      <c r="E29" s="61" t="n"/>
+      <c r="F29" s="97" t="n">
         <v>18</v>
       </c>
-      <c r="F29" s="60" t="n">
+      <c r="G29" s="60" t="n">
         <v>711.1</v>
       </c>
-      <c r="G29" s="60" t="n">
+      <c r="H29" s="60" t="n">
         <v>72.2093</v>
       </c>
-      <c r="H29" s="60" t="n">
+      <c r="I29" s="60" t="n">
         <v>76.9186</v>
       </c>
-      <c r="I29" s="94" t="n">
+      <c r="J29" s="98" t="n">
         <v>0.2404</v>
       </c>
     </row>
     <row r="30" ht="27" customHeight="1">
-      <c r="B30" s="92" t="n">
+      <c r="C30" s="96" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C30" s="92" t="inlineStr">
+      <c r="D30" s="96" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D30" s="61" t="n"/>
-      <c r="E30" s="93" t="n">
+      <c r="E30" s="61" t="n"/>
+      <c r="F30" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F30" s="60" t="n">
+      <c r="G30" s="60" t="n">
         <v>10033.3</v>
       </c>
-      <c r="G30" s="60" t="n">
+      <c r="H30" s="60" t="n">
         <v>814.5</v>
       </c>
-      <c r="H30" s="60" t="n">
+      <c r="I30" s="60" t="n">
         <v>859.5</v>
       </c>
-      <c r="I30" s="94" t="n">
+      <c r="J30" s="98" t="n">
         <v>2.376</v>
       </c>
     </row>
     <row r="31" ht="27" customHeight="1">
-      <c r="B31" s="92" t="n">
+      <c r="C31" s="96" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C31" s="92" t="inlineStr">
+      <c r="D31" s="96" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D31" s="61" t="n"/>
-      <c r="E31" s="93" t="n">
+      <c r="E31" s="61" t="n"/>
+      <c r="F31" s="97" t="n">
         <v>200</v>
       </c>
-      <c r="F31" s="60" t="n">
+      <c r="G31" s="60" t="n">
         <v>10334.8</v>
       </c>
-      <c r="G31" s="60" t="n">
+      <c r="H31" s="60" t="n">
         <v>740.5286</v>
       </c>
-      <c r="H31" s="60" t="n">
+      <c r="I31" s="60" t="n">
         <v>780.1762</v>
       </c>
-      <c r="I31" s="94" t="n">
+      <c r="J31" s="98" t="n">
         <v>2.2678</v>
       </c>
     </row>
     <row r="32" ht="27" customHeight="1">
-      <c r="B32" s="92" t="n">
+      <c r="C32" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C32" s="92" t="inlineStr">
+      <c r="D32" s="96" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D32" s="61" t="n"/>
-      <c r="E32" s="93" t="n">
+      <c r="E32" s="61" t="n"/>
+      <c r="F32" s="97" t="n">
         <v>27</v>
       </c>
-      <c r="F32" s="60" t="n">
+      <c r="G32" s="60" t="n">
         <v>1065.4</v>
       </c>
-      <c r="G32" s="60" t="n">
+      <c r="H32" s="60" t="n">
         <v>99.9714</v>
       </c>
-      <c r="H32" s="60" t="n">
+      <c r="I32" s="60" t="n">
         <v>105.3238</v>
       </c>
-      <c r="I32" s="94" t="n">
+      <c r="J32" s="98" t="n">
         <v>0.3062</v>
       </c>
     </row>
     <row r="33" ht="27" customHeight="1">
-      <c r="B33" s="92" t="n">
+      <c r="C33" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C33" s="92" t="inlineStr">
+      <c r="D33" s="96" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D33" s="61" t="n"/>
-      <c r="E33" s="93" t="n">
+      <c r="E33" s="61" t="n"/>
+      <c r="F33" s="97" t="n">
         <v>169</v>
       </c>
-      <c r="F33" s="60" t="n">
+      <c r="G33" s="60" t="n">
         <v>8660.5</v>
       </c>
-      <c r="G33" s="60" t="n">
+      <c r="H33" s="60" t="n">
         <v>693.3828999999999</v>
       </c>
-      <c r="H33" s="60" t="n">
+      <c r="I33" s="60" t="n">
         <v>736.84</v>
       </c>
-      <c r="I33" s="94" t="n">
+      <c r="J33" s="98" t="n">
         <v>2.2181</v>
       </c>
     </row>
     <row r="34" ht="27" customHeight="1">
-      <c r="B34" s="92" t="n">
+      <c r="C34" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C34" s="92" t="inlineStr">
+      <c r="D34" s="96" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D34" s="61" t="n"/>
-      <c r="E34" s="93" t="n">
+      <c r="E34" s="61" t="n"/>
+      <c r="F34" s="97" t="n">
         <v>6</v>
       </c>
-      <c r="F34" s="60" t="n">
+      <c r="G34" s="60" t="n">
         <v>236</v>
       </c>
-      <c r="G34" s="60" t="n">
+      <c r="H34" s="60" t="n">
         <v>24.6171</v>
       </c>
-      <c r="H34" s="60" t="n">
+      <c r="I34" s="60" t="n">
         <v>26.16</v>
       </c>
-      <c r="I34" s="94" t="n">
+      <c r="J34" s="98" t="n">
         <v>0.07870000000000001</v>
       </c>
     </row>
     <row r="35" ht="27" customHeight="1">
-      <c r="B35" s="92" t="n">
+      <c r="C35" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C35" s="92" t="inlineStr">
+      <c r="D35" s="96" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
-      <c r="D35" s="61" t="n"/>
-      <c r="E35" s="93" t="n">
+      <c r="E35" s="61" t="n"/>
+      <c r="F35" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F35" s="60" t="n">
+      <c r="G35" s="60" t="n">
         <v>10057.4</v>
       </c>
-      <c r="G35" s="60" t="n">
+      <c r="H35" s="60" t="n">
         <v>814.5</v>
       </c>
-      <c r="H35" s="60" t="n">
+      <c r="I35" s="60" t="n">
         <v>859.5</v>
       </c>
-      <c r="I35" s="94" t="n">
+      <c r="J35" s="98" t="n">
         <v>2.376</v>
       </c>
     </row>
     <row r="36" ht="27" customHeight="1">
-      <c r="B36" s="92" t="n">
+      <c r="C36" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C36" s="92" t="inlineStr">
+      <c r="D36" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D36" s="61" t="n"/>
-      <c r="E36" s="93" t="n">
+      <c r="E36" s="61" t="n"/>
+      <c r="F36" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F36" s="60" t="n">
+      <c r="G36" s="60" t="n">
         <v>10176.8</v>
       </c>
-      <c r="G36" s="60" t="n">
+      <c r="H36" s="60" t="n">
         <v>830.5</v>
       </c>
-      <c r="H36" s="60" t="n">
+      <c r="I36" s="60" t="n">
         <v>875.5</v>
       </c>
-      <c r="I36" s="94" t="n">
+      <c r="J36" s="98" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="37" ht="27" customHeight="1">
-      <c r="B37" s="92" t="n">
+      <c r="C37" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C37" s="92" t="inlineStr">
+      <c r="D37" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D37" s="61" t="n"/>
-      <c r="E37" s="93" t="n">
+      <c r="E37" s="61" t="n"/>
+      <c r="F37" s="97" t="n">
         <v>215</v>
       </c>
-      <c r="F37" s="60" t="n">
+      <c r="G37" s="60" t="n">
         <v>11117</v>
       </c>
-      <c r="G37" s="60" t="n">
+      <c r="H37" s="60" t="n">
         <v>901.5</v>
       </c>
-      <c r="H37" s="60" t="n">
+      <c r="I37" s="60" t="n">
         <v>946.5</v>
       </c>
-      <c r="I37" s="94" t="n">
+      <c r="J37" s="98" t="n">
         <v>2.97</v>
       </c>
     </row>
     <row r="38" ht="27" customHeight="1">
-      <c r="B38" s="92" t="n">
+      <c r="C38" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C38" s="92" t="inlineStr">
+      <c r="D38" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D38" s="61" t="n"/>
-      <c r="E38" s="93" t="n">
+      <c r="E38" s="61" t="n"/>
+      <c r="F38" s="97" t="n">
         <v>215</v>
       </c>
-      <c r="F38" s="60" t="n">
+      <c r="G38" s="60" t="n">
         <v>11227</v>
       </c>
-      <c r="G38" s="60" t="n">
+      <c r="H38" s="60" t="n">
         <v>918</v>
       </c>
-      <c r="H38" s="60" t="n">
+      <c r="I38" s="60" t="n">
         <v>963</v>
       </c>
-      <c r="I38" s="94" t="n">
+      <c r="J38" s="98" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="39" ht="27" customHeight="1">
-      <c r="B39" s="92" t="n">
+      <c r="C39" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C39" s="92" t="inlineStr">
+      <c r="D39" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D39" s="61" t="n"/>
-      <c r="E39" s="93" t="n">
+      <c r="E39" s="61" t="n"/>
+      <c r="F39" s="97" t="n">
         <v>192</v>
       </c>
-      <c r="F39" s="60" t="n">
+      <c r="G39" s="60" t="n">
         <v>9879.4</v>
       </c>
-      <c r="G39" s="60" t="n">
+      <c r="H39" s="60" t="n">
         <v>795.0291</v>
       </c>
-      <c r="H39" s="60" t="n">
+      <c r="I39" s="60" t="n">
         <v>836.9709</v>
       </c>
-      <c r="I39" s="94" t="n">
+      <c r="J39" s="98" t="n">
         <v>2.4729</v>
       </c>
     </row>
     <row r="40" ht="27" customHeight="1">
-      <c r="B40" s="92" t="n">
+      <c r="C40" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C40" s="92" t="inlineStr">
+      <c r="D40" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D40" s="61" t="n"/>
-      <c r="E40" s="93" t="n">
+      <c r="E40" s="61" t="n"/>
+      <c r="F40" s="97" t="n">
         <v>14</v>
       </c>
-      <c r="F40" s="60" t="n">
+      <c r="G40" s="60" t="n">
         <v>561</v>
       </c>
-      <c r="G40" s="60" t="n">
+      <c r="H40" s="60" t="n">
         <v>57.9709</v>
       </c>
-      <c r="H40" s="60" t="n">
+      <c r="I40" s="60" t="n">
         <v>61.0291</v>
       </c>
-      <c r="I40" s="94" t="n">
+      <c r="J40" s="98" t="n">
         <v>0.1803</v>
       </c>
     </row>
     <row r="41" ht="27" customHeight="1">
-      <c r="B41" s="92" t="n">
+      <c r="C41" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C41" s="92" t="inlineStr">
+      <c r="D41" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D41" s="61" t="n"/>
-      <c r="E41" s="93" t="n">
+      <c r="E41" s="61" t="n"/>
+      <c r="F41" s="97" t="n">
         <v>97</v>
       </c>
-      <c r="F41" s="60" t="n">
+      <c r="G41" s="60" t="n">
         <v>5016.1</v>
       </c>
-      <c r="G41" s="60" t="n">
+      <c r="H41" s="60" t="n">
         <v>408</v>
       </c>
-      <c r="H41" s="60" t="n">
+      <c r="I41" s="60" t="n">
         <v>453</v>
       </c>
-      <c r="I41" s="94" t="n">
+      <c r="J41" s="98" t="n">
         <v>1.782</v>
       </c>
     </row>
     <row r="42" ht="27" customHeight="1">
-      <c r="B42" s="92" t="n">
+      <c r="C42" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C42" s="92" t="inlineStr">
+      <c r="D42" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D42" s="61" t="n"/>
-      <c r="E42" s="93" t="n">
+      <c r="E42" s="61" t="n"/>
+      <c r="F42" s="97" t="n">
         <v>97</v>
       </c>
-      <c r="F42" s="60" t="n">
+      <c r="G42" s="60" t="n">
         <v>5022.5</v>
       </c>
-      <c r="G42" s="60" t="n">
+      <c r="H42" s="60" t="n">
         <v>407</v>
       </c>
-      <c r="H42" s="60" t="n">
+      <c r="I42" s="60" t="n">
         <v>452</v>
       </c>
-      <c r="I42" s="94" t="n">
+      <c r="J42" s="98" t="n">
         <v>1.8216</v>
       </c>
     </row>
     <row r="43" ht="27" customHeight="1">
-      <c r="B43" s="92" t="n">
+      <c r="C43" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C43" s="92" t="inlineStr">
+      <c r="D43" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D43" s="61" t="n"/>
-      <c r="E43" s="93" t="n">
+      <c r="E43" s="61" t="n"/>
+      <c r="F43" s="97" t="n">
         <v>184</v>
       </c>
-      <c r="F43" s="60" t="n">
+      <c r="G43" s="60" t="n">
         <v>9583.5</v>
       </c>
-      <c r="G43" s="60" t="n">
+      <c r="H43" s="60" t="n">
         <v>773.7684</v>
       </c>
-      <c r="H43" s="60" t="n">
+      <c r="I43" s="60" t="n">
         <v>817.3474</v>
       </c>
-      <c r="I43" s="94" t="n">
+      <c r="J43" s="98" t="n">
         <v>2.6461</v>
       </c>
     </row>
     <row r="44" ht="27" customHeight="1">
-      <c r="B44" s="92" t="n">
+      <c r="C44" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C44" s="92" t="inlineStr">
+      <c r="D44" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D44" s="61" t="n"/>
-      <c r="E44" s="93" t="n">
+      <c r="E44" s="61" t="n"/>
+      <c r="F44" s="97" t="n">
         <v>6</v>
       </c>
-      <c r="F44" s="60" t="n">
+      <c r="G44" s="60" t="n">
         <v>237.8</v>
       </c>
-      <c r="G44" s="60" t="n">
+      <c r="H44" s="60" t="n">
         <v>25.2316</v>
       </c>
-      <c r="H44" s="60" t="n">
+      <c r="I44" s="60" t="n">
         <v>26.6526</v>
       </c>
-      <c r="I44" s="94" t="n">
+      <c r="J44" s="98" t="n">
         <v>0.0863</v>
       </c>
     </row>
     <row r="45" ht="27" customHeight="1">
-      <c r="B45" s="92" t="n">
+      <c r="C45" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C45" s="92" t="inlineStr">
+      <c r="D45" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D45" s="61" t="n"/>
-      <c r="E45" s="93" t="n">
+      <c r="E45" s="61" t="n"/>
+      <c r="F45" s="97" t="n">
         <v>185</v>
       </c>
-      <c r="F45" s="60" t="n">
+      <c r="G45" s="60" t="n">
         <v>9782.9</v>
       </c>
-      <c r="G45" s="60" t="n">
+      <c r="H45" s="60" t="n">
         <v>786.25</v>
       </c>
-      <c r="H45" s="60" t="n">
+      <c r="I45" s="60" t="n">
         <v>830.0658</v>
       </c>
-      <c r="I45" s="94" t="n">
+      <c r="J45" s="98" t="n">
         <v>2.5063</v>
       </c>
     </row>
     <row r="46" ht="27" customHeight="1">
-      <c r="B46" s="92" t="n">
+      <c r="C46" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C46" s="92" t="inlineStr">
+      <c r="D46" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D46" s="61" t="n"/>
-      <c r="E46" s="93" t="n">
+      <c r="E46" s="61" t="n"/>
+      <c r="F46" s="97" t="n">
         <v>5</v>
       </c>
-      <c r="F46" s="60" t="n">
+      <c r="G46" s="60" t="n">
         <v>199</v>
       </c>
-      <c r="G46" s="60" t="n">
+      <c r="H46" s="60" t="n">
         <v>21.25</v>
       </c>
-      <c r="H46" s="60" t="n">
+      <c r="I46" s="60" t="n">
         <v>22.4342</v>
       </c>
-      <c r="I46" s="94" t="n">
+      <c r="J46" s="98" t="n">
         <v>0.0677</v>
       </c>
     </row>
     <row r="47" ht="27" customHeight="1">
-      <c r="B47" s="92" t="n">
+      <c r="C47" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C47" s="92" t="inlineStr">
+      <c r="D47" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D47" s="61" t="n"/>
-      <c r="E47" s="93" t="n">
+      <c r="E47" s="61" t="n"/>
+      <c r="F47" s="97" t="n">
         <v>190</v>
       </c>
-      <c r="F47" s="60" t="n">
+      <c r="G47" s="60" t="n">
         <v>10009.4</v>
       </c>
-      <c r="G47" s="60" t="n">
+      <c r="H47" s="60" t="n">
         <v>824</v>
       </c>
-      <c r="H47" s="60" t="n">
+      <c r="I47" s="60" t="n">
         <v>869</v>
       </c>
-      <c r="I47" s="94" t="n">
+      <c r="J47" s="98" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="48" ht="27" customHeight="1">
-      <c r="B48" s="92" t="n">
+      <c r="C48" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C48" s="92" t="inlineStr">
+      <c r="D48" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D48" s="61" t="n"/>
-      <c r="E48" s="93" t="n">
+      <c r="E48" s="61" t="n"/>
+      <c r="F48" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F48" s="60" t="n">
+      <c r="G48" s="60" t="n">
         <v>10072.6</v>
       </c>
-      <c r="G48" s="60" t="n">
+      <c r="H48" s="60" t="n">
         <v>821</v>
       </c>
-      <c r="H48" s="60" t="n">
+      <c r="I48" s="60" t="n">
         <v>866</v>
       </c>
-      <c r="I48" s="94" t="n">
+      <c r="J48" s="98" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="49" ht="27" customHeight="1">
-      <c r="B49" s="92" t="n">
+      <c r="C49" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C49" s="92" t="inlineStr">
+      <c r="D49" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D49" s="61" t="n"/>
-      <c r="E49" s="93" t="n">
+      <c r="E49" s="61" t="n"/>
+      <c r="F49" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F49" s="60" t="n">
+      <c r="G49" s="60" t="n">
         <v>10117.1</v>
       </c>
-      <c r="G49" s="60" t="n">
+      <c r="H49" s="60" t="n">
         <v>825.5</v>
       </c>
-      <c r="H49" s="60" t="n">
+      <c r="I49" s="60" t="n">
         <v>870.5</v>
       </c>
-      <c r="I49" s="94" t="n">
+      <c r="J49" s="98" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="50" ht="27" customHeight="1">
-      <c r="B50" s="92" t="n">
+      <c r="C50" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C50" s="92" t="inlineStr">
+      <c r="D50" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D50" s="61" t="n"/>
-      <c r="E50" s="93" t="n">
+      <c r="E50" s="61" t="n"/>
+      <c r="F50" s="97" t="n">
         <v>89</v>
       </c>
-      <c r="F50" s="60" t="n">
+      <c r="G50" s="60" t="n">
         <v>4707.4</v>
       </c>
-      <c r="G50" s="60" t="n">
+      <c r="H50" s="60" t="n">
         <v>376.5385</v>
       </c>
-      <c r="H50" s="60" t="n">
+      <c r="I50" s="60" t="n">
         <v>415.0481</v>
       </c>
-      <c r="I50" s="94" t="n">
+      <c r="J50" s="98" t="n">
         <v>1.4572</v>
       </c>
     </row>
     <row r="51" ht="27" customHeight="1">
-      <c r="B51" s="92" t="n">
+      <c r="C51" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C51" s="92" t="inlineStr">
+      <c r="D51" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D51" s="61" t="n"/>
-      <c r="E51" s="93" t="n">
+      <c r="E51" s="61" t="n"/>
+      <c r="F51" s="97" t="n">
         <v>8</v>
       </c>
-      <c r="F51" s="60" t="n">
+      <c r="G51" s="60" t="n">
         <v>322.8</v>
       </c>
-      <c r="G51" s="60" t="n">
+      <c r="H51" s="60" t="n">
         <v>33.8462</v>
       </c>
-      <c r="H51" s="60" t="n">
+      <c r="I51" s="60" t="n">
         <v>37.3077</v>
       </c>
-      <c r="I51" s="94" t="n">
+      <c r="J51" s="98" t="n">
         <v>0.131</v>
       </c>
     </row>
     <row r="52" ht="27" customHeight="1">
-      <c r="B52" s="92" t="n">
+      <c r="C52" s="96" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C52" s="92" t="inlineStr">
+      <c r="D52" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D52" s="62" t="n"/>
-      <c r="E52" s="93" t="n">
+      <c r="E52" s="62" t="n"/>
+      <c r="F52" s="97" t="n">
         <v>7</v>
       </c>
-      <c r="F52" s="60" t="n">
+      <c r="G52" s="60" t="n">
         <v>367.3</v>
       </c>
-      <c r="G52" s="60" t="n">
+      <c r="H52" s="60" t="n">
         <v>29.6154</v>
       </c>
-      <c r="H52" s="60" t="n">
+      <c r="I52" s="60" t="n">
         <v>32.6442</v>
       </c>
-      <c r="I52" s="94" t="n">
+      <c r="J52" s="98" t="n">
         <v>0.1146</v>
       </c>
     </row>
     <row r="53" ht="27" customHeight="1">
-      <c r="A53" s="95" t="n"/>
-      <c r="B53" s="55" t="inlineStr">
+      <c r="A53" s="99" t="n"/>
+      <c r="C53" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
         </is>
       </c>
-      <c r="C53" s="55" t="n"/>
       <c r="D53" s="55" t="n"/>
-      <c r="E53" s="90" t="n"/>
-      <c r="F53" s="56" t="n"/>
+      <c r="E53" s="55" t="n"/>
+      <c r="F53" s="93" t="n"/>
       <c r="G53" s="56" t="n"/>
       <c r="H53" s="56" t="n"/>
-      <c r="I53" s="89" t="n"/>
+      <c r="I53" s="56" t="n"/>
+      <c r="J53" s="90" t="n"/>
     </row>
     <row r="54" ht="27" customHeight="1">
       <c r="A54" s="55" t="n"/>
-      <c r="B54" s="55" t="inlineStr">
+      <c r="B54" s="89" t="n"/>
+      <c r="C54" s="55" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="C54" s="55" t="inlineStr">
+      <c r="D54" s="55" t="inlineStr">
         <is>
           <t>20 PALLETS</t>
         </is>
       </c>
-      <c r="D54" s="55" t="n"/>
-      <c r="E54" s="90">
-        <f>SUM(E23:E52)</f>
-        <v/>
-      </c>
-      <c r="F54" s="56">
+      <c r="E54" s="55" t="n"/>
+      <c r="F54" s="93">
         <f>SUM(F23:F52)</f>
         <v/>
       </c>
@@ -4540,8 +4577,12 @@
         <f>SUM(H23:H52)</f>
         <v/>
       </c>
-      <c r="I54" s="89">
+      <c r="I54" s="56">
         <f>SUM(I23:I52)</f>
+        <v/>
+      </c>
+      <c r="J54" s="90">
+        <f>SUM(J23:J52)</f>
         <v/>
       </c>
     </row>
@@ -4552,487 +4593,490 @@
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B56" s="55" t="inlineStr">
+      <c r="B56" s="88" t="n"/>
+      <c r="C56" s="55" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="C56" s="55" t="inlineStr">
+      <c r="D56" s="55" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="D56" s="55" t="inlineStr">
+      <c r="E56" s="55" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E56" s="55" t="inlineStr">
+      <c r="F56" s="55" t="inlineStr">
         <is>
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F56" s="88" t="n"/>
-      <c r="G56" s="56" t="inlineStr">
+      <c r="G56" s="89" t="n"/>
+      <c r="H56" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="H56" s="56" t="inlineStr">
+      <c r="I56" s="56" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I56" s="89" t="inlineStr">
+      <c r="J56" s="90" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
     <row r="57" ht="27" customHeight="1">
-      <c r="A57" s="62" t="n"/>
-      <c r="B57" s="62" t="n"/>
+      <c r="A57" s="91" t="n"/>
+      <c r="B57" s="92" t="n"/>
       <c r="C57" s="62" t="n"/>
       <c r="D57" s="62" t="n"/>
-      <c r="E57" s="90" t="inlineStr">
+      <c r="E57" s="62" t="n"/>
+      <c r="F57" s="93" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="F57" s="56" t="inlineStr">
+      <c r="G57" s="56" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="G57" s="62" t="n"/>
       <c r="H57" s="62" t="n"/>
       <c r="I57" s="62" t="n"/>
+      <c r="J57" s="62" t="n"/>
     </row>
     <row r="58" ht="27" customHeight="1">
-      <c r="A58" s="91" t="inlineStr">
+      <c r="A58" s="94" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B58" s="92" t="n">
+      <c r="B58" s="95" t="n"/>
+      <c r="C58" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C58" s="92" t="inlineStr">
+      <c r="D58" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D58" s="59" t="inlineStr">
+      <c r="E58" s="59" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E58" s="93" t="n">
+      <c r="F58" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F58" s="60" t="n">
+      <c r="G58" s="60" t="n">
         <v>10187.1</v>
       </c>
-      <c r="G58" s="60" t="n">
+      <c r="H58" s="60" t="n">
         <v>842.5</v>
       </c>
-      <c r="H58" s="60" t="n">
+      <c r="I58" s="60" t="n">
         <v>887.5</v>
       </c>
-      <c r="I58" s="94" t="n">
+      <c r="J58" s="98" t="n">
         <v>2.6532</v>
       </c>
     </row>
     <row r="59" ht="27" customHeight="1">
-      <c r="A59" s="91" t="inlineStr">
+      <c r="A59" s="94" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B59" s="92" t="n">
+      <c r="B59" s="95" t="n"/>
+      <c r="C59" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C59" s="92" t="inlineStr">
+      <c r="D59" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D59" s="61" t="n"/>
-      <c r="E59" s="93" t="n">
+      <c r="E59" s="61" t="n"/>
+      <c r="F59" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F59" s="60" t="n">
+      <c r="G59" s="60" t="n">
         <v>10219.2</v>
       </c>
-      <c r="G59" s="60" t="n">
+      <c r="H59" s="60" t="n">
         <v>846</v>
       </c>
-      <c r="H59" s="60" t="n">
+      <c r="I59" s="60" t="n">
         <v>891</v>
       </c>
-      <c r="I59" s="94" t="n">
+      <c r="J59" s="98" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="60" ht="27" customHeight="1">
-      <c r="A60" s="91" t="inlineStr">
+      <c r="A60" s="94" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B60" s="92" t="n">
+      <c r="B60" s="95" t="n"/>
+      <c r="C60" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C60" s="92" t="inlineStr">
+      <c r="D60" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D60" s="61" t="n"/>
-      <c r="E60" s="93" t="n">
+      <c r="E60" s="61" t="n"/>
+      <c r="F60" s="97" t="n">
         <v>207</v>
       </c>
-      <c r="F60" s="60" t="n">
+      <c r="G60" s="60" t="n">
         <v>10773.3</v>
       </c>
-      <c r="G60" s="60" t="n">
+      <c r="H60" s="60" t="n">
         <v>883.7671</v>
       </c>
-      <c r="H60" s="60" t="n">
+      <c r="I60" s="60" t="n">
         <v>926.3013999999999</v>
       </c>
-      <c r="I60" s="94" t="n">
+      <c r="J60" s="98" t="n">
         <v>2.8447</v>
       </c>
     </row>
     <row r="61" ht="27" customHeight="1">
-      <c r="A61" s="91" t="inlineStr">
+      <c r="A61" s="94" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B61" s="92" t="n">
+      <c r="B61" s="95" t="n"/>
+      <c r="C61" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C61" s="92" t="inlineStr">
+      <c r="D61" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D61" s="61" t="n"/>
-      <c r="E61" s="93" t="n">
+      <c r="E61" s="61" t="n"/>
+      <c r="F61" s="97" t="n">
         <v>12</v>
       </c>
-      <c r="F61" s="60" t="n">
+      <c r="G61" s="60" t="n">
         <v>479.1</v>
       </c>
-      <c r="G61" s="60" t="n">
+      <c r="H61" s="60" t="n">
         <v>51.2329</v>
       </c>
-      <c r="H61" s="60" t="n">
+      <c r="I61" s="60" t="n">
         <v>53.6986</v>
       </c>
-      <c r="I61" s="94" t="n">
+      <c r="J61" s="98" t="n">
         <v>0.1649</v>
       </c>
     </row>
     <row r="62" ht="27" customHeight="1">
-      <c r="B62" s="92" t="n">
+      <c r="C62" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C62" s="92" t="inlineStr">
+      <c r="D62" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D62" s="61" t="n"/>
-      <c r="E62" s="93" t="n">
+      <c r="E62" s="61" t="n"/>
+      <c r="F62" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F62" s="60" t="n">
+      <c r="G62" s="60" t="n">
         <v>10215.8</v>
       </c>
-      <c r="G62" s="60" t="n">
+      <c r="H62" s="60" t="n">
         <v>840</v>
       </c>
-      <c r="H62" s="60" t="n">
+      <c r="I62" s="60" t="n">
         <v>885</v>
       </c>
-      <c r="I62" s="94" t="n">
+      <c r="J62" s="98" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="63" ht="27" customHeight="1">
-      <c r="B63" s="92" t="n">
+      <c r="C63" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C63" s="92" t="inlineStr">
+      <c r="D63" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D63" s="61" t="n"/>
-      <c r="E63" s="93" t="n">
+      <c r="E63" s="61" t="n"/>
+      <c r="F63" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F63" s="60" t="n">
+      <c r="G63" s="60" t="n">
         <v>10237.5</v>
       </c>
-      <c r="G63" s="60" t="n">
+      <c r="H63" s="60" t="n">
         <v>863.5</v>
       </c>
-      <c r="H63" s="60" t="n">
+      <c r="I63" s="60" t="n">
         <v>908.5</v>
       </c>
-      <c r="I63" s="94" t="n">
+      <c r="J63" s="98" t="n">
         <v>2.6928</v>
       </c>
     </row>
     <row r="64" ht="27" customHeight="1">
-      <c r="B64" s="92" t="n">
+      <c r="C64" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C64" s="92" t="inlineStr">
+      <c r="D64" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D64" s="61" t="n"/>
-      <c r="E64" s="93" t="n">
+      <c r="E64" s="61" t="n"/>
+      <c r="F64" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F64" s="60" t="n">
+      <c r="G64" s="60" t="n">
         <v>10196.1</v>
       </c>
-      <c r="G64" s="60" t="n">
+      <c r="H64" s="60" t="n">
         <v>849</v>
       </c>
-      <c r="H64" s="60" t="n">
+      <c r="I64" s="60" t="n">
         <v>894</v>
       </c>
-      <c r="I64" s="94" t="n">
+      <c r="J64" s="98" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="65" ht="27" customHeight="1">
-      <c r="B65" s="92" t="n">
+      <c r="C65" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C65" s="92" t="inlineStr">
+      <c r="D65" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D65" s="61" t="n"/>
-      <c r="E65" s="93" t="n">
+      <c r="E65" s="61" t="n"/>
+      <c r="F65" s="97" t="n">
         <v>175</v>
       </c>
-      <c r="F65" s="60" t="n">
+      <c r="G65" s="60" t="n">
         <v>9097.6</v>
       </c>
-      <c r="G65" s="60" t="n">
+      <c r="H65" s="60" t="n">
         <v>739.443</v>
       </c>
-      <c r="H65" s="60" t="n">
+      <c r="I65" s="60" t="n">
         <v>780.2461</v>
       </c>
-      <c r="I65" s="94" t="n">
+      <c r="J65" s="98" t="n">
         <v>2.3339</v>
       </c>
     </row>
     <row r="66" ht="27" customHeight="1">
-      <c r="B66" s="92" t="n">
+      <c r="C66" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C66" s="92" t="inlineStr">
+      <c r="D66" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D66" s="61" t="n"/>
-      <c r="E66" s="93" t="n">
+      <c r="E66" s="61" t="n"/>
+      <c r="F66" s="97" t="n">
         <v>18</v>
       </c>
-      <c r="F66" s="60" t="n">
+      <c r="G66" s="60" t="n">
         <v>726</v>
       </c>
-      <c r="G66" s="60" t="n">
+      <c r="H66" s="60" t="n">
         <v>76.057</v>
       </c>
-      <c r="H66" s="60" t="n">
+      <c r="I66" s="60" t="n">
         <v>80.2539</v>
       </c>
-      <c r="I66" s="94" t="n">
+      <c r="J66" s="98" t="n">
         <v>0.2401</v>
       </c>
     </row>
     <row r="67" ht="27" customHeight="1">
-      <c r="B67" s="92" t="n">
+      <c r="C67" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C67" s="92" t="inlineStr">
+      <c r="D67" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D67" s="61" t="n"/>
-      <c r="E67" s="93" t="n">
+      <c r="E67" s="61" t="n"/>
+      <c r="F67" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F67" s="60" t="n">
+      <c r="G67" s="60" t="n">
         <v>10110.4</v>
       </c>
-      <c r="G67" s="60" t="n">
+      <c r="H67" s="60" t="n">
         <v>840</v>
       </c>
-      <c r="H67" s="60" t="n">
+      <c r="I67" s="60" t="n">
         <v>885</v>
       </c>
-      <c r="I67" s="94" t="n">
+      <c r="J67" s="98" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="68" ht="27" customHeight="1">
-      <c r="B68" s="92" t="n">
+      <c r="C68" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C68" s="92" t="inlineStr">
+      <c r="D68" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D68" s="61" t="n"/>
-      <c r="E68" s="93" t="n">
+      <c r="E68" s="61" t="n"/>
+      <c r="F68" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F68" s="60" t="n">
+      <c r="G68" s="60" t="n">
         <v>10165.7</v>
       </c>
-      <c r="G68" s="60" t="n">
+      <c r="H68" s="60" t="n">
         <v>844.5</v>
       </c>
-      <c r="H68" s="60" t="n">
+      <c r="I68" s="60" t="n">
         <v>889.5</v>
       </c>
-      <c r="I68" s="94" t="n">
+      <c r="J68" s="98" t="n">
         <v>2.772</v>
       </c>
     </row>
     <row r="69" ht="27" customHeight="1">
-      <c r="B69" s="92" t="n">
+      <c r="C69" s="96" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C69" s="92" t="inlineStr">
+      <c r="D69" s="96" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="D69" s="61" t="n"/>
-      <c r="E69" s="93" t="n">
+      <c r="E69" s="61" t="n"/>
+      <c r="F69" s="97" t="n">
         <v>195</v>
       </c>
-      <c r="F69" s="60" t="n">
+      <c r="G69" s="60" t="n">
         <v>10222.1</v>
       </c>
-      <c r="G69" s="60" t="n">
+      <c r="H69" s="60" t="n">
         <v>843</v>
       </c>
-      <c r="H69" s="60" t="n">
+      <c r="I69" s="60" t="n">
         <v>888</v>
       </c>
-      <c r="I69" s="94" t="n">
+      <c r="J69" s="98" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="70" ht="27" customHeight="1">
-      <c r="B70" s="92" t="inlineStr">
+      <c r="C70" s="96" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="C70" s="92" t="inlineStr">
+      <c r="D70" s="96" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="D70" s="61" t="n"/>
-      <c r="E70" s="93" t="n">
+      <c r="E70" s="61" t="n"/>
+      <c r="F70" s="97" t="n">
         <v>106</v>
       </c>
-      <c r="F70" s="60" t="n">
+      <c r="G70" s="60" t="n">
         <v>5345</v>
       </c>
-      <c r="G70" s="60" t="n">
+      <c r="H70" s="60" t="n">
         <v>381.211</v>
       </c>
-      <c r="H70" s="60" t="n">
+      <c r="I70" s="60" t="n">
         <v>424.9725</v>
       </c>
-      <c r="I70" s="94" t="n">
+      <c r="J70" s="98" t="n">
         <v>2.0795</v>
       </c>
     </row>
     <row r="71" ht="27" customHeight="1">
-      <c r="B71" s="92" t="inlineStr">
+      <c r="C71" s="96" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="C71" s="92" t="inlineStr">
+      <c r="D71" s="96" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="D71" s="62" t="n"/>
-      <c r="E71" s="93" t="n">
+      <c r="E71" s="62" t="n"/>
+      <c r="F71" s="97" t="n">
         <v>3</v>
       </c>
-      <c r="F71" s="60" t="n">
+      <c r="G71" s="60" t="n">
         <v>121</v>
       </c>
-      <c r="G71" s="60" t="n">
+      <c r="H71" s="60" t="n">
         <v>10.789</v>
       </c>
-      <c r="H71" s="60" t="n">
+      <c r="I71" s="60" t="n">
         <v>12.0275</v>
       </c>
-      <c r="I71" s="94" t="n">
+      <c r="J71" s="98" t="n">
         <v>0.0589</v>
       </c>
     </row>
     <row r="72" ht="27" customHeight="1">
-      <c r="A72" s="95" t="n"/>
-      <c r="B72" s="55" t="inlineStr">
+      <c r="A72" s="99" t="n"/>
+      <c r="C72" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
         </is>
       </c>
-      <c r="C72" s="55" t="n"/>
       <c r="D72" s="55" t="n"/>
-      <c r="E72" s="90" t="n"/>
-      <c r="F72" s="56" t="n"/>
+      <c r="E72" s="55" t="n"/>
+      <c r="F72" s="93" t="n"/>
       <c r="G72" s="56" t="n"/>
       <c r="H72" s="56" t="n"/>
-      <c r="I72" s="89" t="n"/>
+      <c r="I72" s="56" t="n"/>
+      <c r="J72" s="90" t="n"/>
     </row>
     <row r="73" ht="27" customHeight="1">
       <c r="A73" s="55" t="n"/>
-      <c r="B73" s="55" t="inlineStr">
+      <c r="B73" s="89" t="n"/>
+      <c r="C73" s="55" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="C73" s="55" t="inlineStr">
+      <c r="D73" s="55" t="inlineStr">
         <is>
           <t>11 PALLETS</t>
         </is>
       </c>
-      <c r="D73" s="55" t="n"/>
-      <c r="E73" s="90">
-        <f>SUM(E58:E71)</f>
-        <v/>
-      </c>
-      <c r="F73" s="56">
+      <c r="E73" s="55" t="n"/>
+      <c r="F73" s="93">
         <f>SUM(F58:F71)</f>
         <v/>
       </c>
@@ -5044,58 +5088,58 @@
         <f>SUM(H58:H71)</f>
         <v/>
       </c>
-      <c r="I73" s="89">
+      <c r="I73" s="56">
         <f>SUM(I58:I71)</f>
         <v/>
       </c>
+      <c r="J73" s="90">
+        <f>SUM(J58:J71)</f>
+        <v/>
+      </c>
     </row>
     <row r="74" ht="27" customHeight="1">
-      <c r="A74" s="96" t="n"/>
-      <c r="B74" s="96" t="inlineStr">
+      <c r="A74" s="100" t="n"/>
+      <c r="C74" s="100" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="C74" s="96" t="inlineStr">
+      <c r="D74" s="100" t="inlineStr">
         <is>
           <t>31 PALLETS</t>
         </is>
       </c>
-      <c r="D74" s="96" t="n"/>
-      <c r="E74" s="97">
-        <f>SUM(E23:E52,E58:E71)</f>
-        <v/>
-      </c>
-      <c r="F74" s="98">
+      <c r="E74" s="100" t="n"/>
+      <c r="F74" s="101">
         <f>SUM(F23:F52,F58:F71)</f>
         <v/>
       </c>
-      <c r="G74" s="98">
+      <c r="G74" s="102">
         <f>SUM(G23:G52,G58:G71)</f>
         <v/>
       </c>
-      <c r="H74" s="98">
+      <c r="H74" s="102">
         <f>SUM(H23:H52,H58:H71)</f>
         <v/>
       </c>
-      <c r="I74" s="99">
+      <c r="I74" s="102">
         <f>SUM(I23:I52,I58:I71)</f>
         <v/>
       </c>
+      <c r="J74" s="103">
+        <f>SUM(J23:J52,J58:J71)</f>
+        <v/>
+      </c>
     </row>
     <row r="75" ht="27" customHeight="1">
-      <c r="A75" s="100" t="inlineStr">
-        <is>
-          <t>Country of Original Cambodia</t>
-        </is>
-      </c>
-      <c r="B75" s="100" t="n"/>
-      <c r="C75" s="100" t="n"/>
-      <c r="D75" s="101" t="n"/>
-      <c r="E75" s="102" t="n"/>
-      <c r="F75" s="26" t="n"/>
-      <c r="G75" s="26" t="n"/>
-      <c r="H75" s="26" t="n"/>
+      <c r="A75" s="2" t="n"/>
+      <c r="B75" s="2" t="n"/>
+      <c r="C75" s="2" t="n"/>
+      <c r="D75" s="2" t="n"/>
+      <c r="E75" s="2" t="n"/>
+      <c r="F75" s="2" t="n"/>
+      <c r="G75" s="2" t="n"/>
+      <c r="H75" s="2" t="n"/>
       <c r="I75" s="2" t="n"/>
       <c r="J75" s="2" t="n"/>
       <c r="K75" s="2" t="n"/>
@@ -5109,22 +5153,15 @@
       <c r="S75" s="2" t="n"/>
       <c r="T75" s="2" t="n"/>
     </row>
-    <row r="76" ht="65.25" customHeight="1">
-      <c r="A76" s="64" t="inlineStr">
-        <is>
-          <t>Manufacture:</t>
-        </is>
-      </c>
-      <c r="B76" s="103" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
-XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
-        </is>
-      </c>
-      <c r="E76" s="104" t="n"/>
-      <c r="F76" s="104" t="n"/>
-      <c r="G76" s="104" t="n"/>
-      <c r="H76" s="26" t="n"/>
+    <row r="76" ht="27" customHeight="1">
+      <c r="A76" s="2" t="n"/>
+      <c r="B76" s="2" t="n"/>
+      <c r="C76" s="2" t="n"/>
+      <c r="D76" s="2" t="n"/>
+      <c r="E76" s="2" t="n"/>
+      <c r="F76" s="2" t="n"/>
+      <c r="G76" s="2" t="n"/>
+      <c r="H76" s="2" t="n"/>
       <c r="I76" s="2" t="n"/>
       <c r="J76" s="2" t="n"/>
       <c r="K76" s="2" t="n"/>
@@ -5138,17 +5175,15 @@
       <c r="S76" s="2" t="n"/>
       <c r="T76" s="2" t="n"/>
     </row>
-    <row r="77" ht="51.75" customHeight="1">
-      <c r="A77" s="103" t="inlineStr">
-        <is>
-          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
-                                          /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-      <c r="E77" s="104" t="n"/>
-      <c r="F77" s="104" t="n"/>
-      <c r="G77" s="104" t="n"/>
-      <c r="H77" s="104" t="n"/>
+    <row r="77" ht="27" customHeight="1">
+      <c r="A77" s="53" t="n"/>
+      <c r="B77" s="87" t="n"/>
+      <c r="C77" s="2" t="n"/>
+      <c r="D77" s="2" t="n"/>
+      <c r="E77" s="2" t="n"/>
+      <c r="F77" s="2" t="n"/>
+      <c r="G77" s="2" t="n"/>
+      <c r="H77" s="2" t="n"/>
       <c r="I77" s="2" t="n"/>
       <c r="J77" s="2" t="n"/>
       <c r="K77" s="2" t="n"/>
@@ -5163,18 +5198,18 @@
       <c r="T77" s="2" t="n"/>
     </row>
     <row r="78" ht="27" customHeight="1">
-      <c r="A78" s="70" t="inlineStr">
-        <is>
-          <t>A/C NO:100001100764430</t>
-        </is>
-      </c>
-      <c r="B78" s="70" t="n"/>
-      <c r="C78" s="70" t="n"/>
-      <c r="D78" s="70" t="n"/>
-      <c r="E78" s="50" t="n"/>
-      <c r="F78" s="50" t="n"/>
-      <c r="G78" s="50" t="n"/>
-      <c r="H78" s="50" t="n"/>
+      <c r="A78" s="104" t="inlineStr">
+        <is>
+          <t>Country of Original Cambodia</t>
+        </is>
+      </c>
+      <c r="B78" s="104" t="n"/>
+      <c r="C78" s="104" t="n"/>
+      <c r="D78" s="105" t="n"/>
+      <c r="E78" s="106" t="n"/>
+      <c r="F78" s="26" t="n"/>
+      <c r="G78" s="26" t="n"/>
+      <c r="H78" s="26" t="n"/>
       <c r="I78" s="2" t="n"/>
       <c r="J78" s="2" t="n"/>
       <c r="K78" s="2" t="n"/>
@@ -5188,19 +5223,22 @@
       <c r="S78" s="2" t="n"/>
       <c r="T78" s="2" t="n"/>
     </row>
-    <row r="79" ht="27" customHeight="1">
-      <c r="A79" s="70" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
-        </is>
-      </c>
-      <c r="B79" s="70" t="n"/>
-      <c r="C79" s="70" t="n"/>
-      <c r="D79" s="70" t="n"/>
-      <c r="E79" s="50" t="n"/>
-      <c r="F79" s="50" t="n"/>
-      <c r="G79" s="50" t="n"/>
-      <c r="H79" s="50" t="n"/>
+    <row r="79" ht="65.25" customHeight="1">
+      <c r="A79" s="64" t="inlineStr">
+        <is>
+          <t>Manufacture:</t>
+        </is>
+      </c>
+      <c r="B79" s="107" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
+XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="E79" s="108" t="n"/>
+      <c r="F79" s="108" t="n"/>
+      <c r="G79" s="108" t="n"/>
+      <c r="H79" s="26" t="n"/>
       <c r="I79" s="2" t="n"/>
       <c r="J79" s="2" t="n"/>
       <c r="K79" s="2" t="n"/>
@@ -5214,19 +5252,17 @@
       <c r="S79" s="2" t="n"/>
       <c r="T79" s="2" t="n"/>
     </row>
-    <row r="80" ht="27" customHeight="1">
-      <c r="A80" s="2" t="n"/>
-      <c r="B80" s="105" t="n"/>
-      <c r="C80" s="2" t="n"/>
-      <c r="D80" s="2" t="n"/>
-      <c r="E80" s="52" t="n"/>
-      <c r="F80" s="2" t="n"/>
-      <c r="G80" s="26" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
-      <c r="H80" s="52" t="n"/>
+    <row r="80" ht="51.75" customHeight="1">
+      <c r="A80" s="107" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
+                                          /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="E80" s="108" t="n"/>
+      <c r="F80" s="108" t="n"/>
+      <c r="G80" s="108" t="n"/>
+      <c r="H80" s="108" t="n"/>
       <c r="I80" s="2" t="n"/>
       <c r="J80" s="2" t="n"/>
       <c r="K80" s="2" t="n"/>
@@ -5240,9 +5276,84 @@
       <c r="S80" s="2" t="n"/>
       <c r="T80" s="2" t="n"/>
     </row>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
+    <row r="81" ht="27" customHeight="1">
+      <c r="A81" s="70" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+      <c r="B81" s="70" t="n"/>
+      <c r="C81" s="70" t="n"/>
+      <c r="D81" s="70" t="n"/>
+      <c r="E81" s="50" t="n"/>
+      <c r="F81" s="50" t="n"/>
+      <c r="G81" s="50" t="n"/>
+      <c r="H81" s="50" t="n"/>
+      <c r="I81" s="2" t="n"/>
+      <c r="J81" s="2" t="n"/>
+      <c r="K81" s="2" t="n"/>
+      <c r="L81" s="2" t="n"/>
+      <c r="M81" s="2" t="n"/>
+      <c r="N81" s="2" t="n"/>
+      <c r="O81" s="2" t="n"/>
+      <c r="P81" s="2" t="n"/>
+      <c r="Q81" s="2" t="n"/>
+      <c r="R81" s="2" t="n"/>
+      <c r="S81" s="2" t="n"/>
+      <c r="T81" s="2" t="n"/>
+    </row>
+    <row r="82" ht="27" customHeight="1">
+      <c r="A82" s="70" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="B82" s="70" t="n"/>
+      <c r="C82" s="70" t="n"/>
+      <c r="D82" s="70" t="n"/>
+      <c r="E82" s="50" t="n"/>
+      <c r="F82" s="50" t="n"/>
+      <c r="G82" s="50" t="n"/>
+      <c r="H82" s="50" t="n"/>
+      <c r="I82" s="2" t="n"/>
+      <c r="J82" s="2" t="n"/>
+      <c r="K82" s="2" t="n"/>
+      <c r="L82" s="2" t="n"/>
+      <c r="M82" s="2" t="n"/>
+      <c r="N82" s="2" t="n"/>
+      <c r="O82" s="2" t="n"/>
+      <c r="P82" s="2" t="n"/>
+      <c r="Q82" s="2" t="n"/>
+      <c r="R82" s="2" t="n"/>
+      <c r="S82" s="2" t="n"/>
+      <c r="T82" s="2" t="n"/>
+    </row>
+    <row r="83" ht="27" customHeight="1">
+      <c r="A83" s="2" t="n"/>
+      <c r="B83" s="109" t="n"/>
+      <c r="C83" s="2" t="n"/>
+      <c r="D83" s="2" t="n"/>
+      <c r="E83" s="52" t="n"/>
+      <c r="F83" s="2" t="n"/>
+      <c r="G83" s="26" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="H83" s="52" t="n"/>
+      <c r="I83" s="2" t="n"/>
+      <c r="J83" s="2" t="n"/>
+      <c r="K83" s="2" t="n"/>
+      <c r="L83" s="2" t="n"/>
+      <c r="M83" s="2" t="n"/>
+      <c r="N83" s="2" t="n"/>
+      <c r="O83" s="2" t="n"/>
+      <c r="P83" s="2" t="n"/>
+      <c r="Q83" s="2" t="n"/>
+      <c r="R83" s="2" t="n"/>
+      <c r="S83" s="2" t="n"/>
+      <c r="T83" s="2" t="n"/>
+    </row>
     <row r="84"/>
     <row r="85"/>
     <row r="86"/>
@@ -5361,38 +5472,87 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="D23:D52"/>
-    <mergeCell ref="B74"/>
-    <mergeCell ref="B72:C72"/>
+  <mergeCells count="80">
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A51:B51"/>
     <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C74"/>
+    <mergeCell ref="E58:E71"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="E23:E52"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A49:B49"/>
     <mergeCell ref="H56:H57"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C54"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A60:B60"/>
     <mergeCell ref="H21:H22"/>
-    <mergeCell ref="D58:D71"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="D56:D57"/>
-    <mergeCell ref="C21:C22"/>
     <mergeCell ref="I21:I22"/>
-    <mergeCell ref="B54"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B73"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="J56:J57"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A58:B58"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
adding the template state restore perfect suit to packing list, replacement work now
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -378,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -488,7 +488,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -590,7 +590,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -649,9 +649,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -1028,7 +1025,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P200"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1571,7 +1568,7 @@
     <row r="33" ht="36" customHeight="1">
       <c r="A33" s="8" t="inlineStr">
         <is>
-          <t>Transaction method: FCA(USD)</t>
+          <t>Transaction method: DAF(USD)</t>
         </is>
       </c>
       <c r="B33" s="8" t="n"/>
@@ -1696,165 +1693,6 @@
       <c r="E41" s="22" t="n"/>
       <c r="F41" s="2" t="n"/>
     </row>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
-    <row r="200"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="C36:E36"/>
@@ -1876,7 +1714,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P200"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2099,12 +1937,12 @@
       <c r="E10" s="32" t="n"/>
       <c r="F10" s="40" t="inlineStr">
         <is>
-          <t>FCA :</t>
+          <t>DAF :</t>
         </is>
       </c>
       <c r="G10" s="41" t="inlineStr">
         <is>
-          <t>BAVET, SVAYRIENG</t>
+          <t>BAVET</t>
         </is>
       </c>
       <c r="H10" s="2" t="n"/>
@@ -2917,159 +2755,6 @@
       <c r="N47" s="68" t="n"/>
       <c r="O47" s="68" t="n"/>
     </row>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
-    <row r="200"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="B39:C39"/>
@@ -3094,7 +2779,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T200"/>
+  <dimension ref="A1:T83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3263,7 +2948,7 @@
       </c>
       <c r="I7" s="78" t="inlineStr">
         <is>
-          <t>JFREF</t>
+          <t>CLF2025-150</t>
         </is>
       </c>
       <c r="J7" s="2" t="n"/>
@@ -3301,7 +2986,7 @@
       </c>
       <c r="I8" s="80" t="inlineStr">
         <is>
-          <t>JFINV</t>
+          <t>JF25027</t>
         </is>
       </c>
       <c r="J8" s="2" t="n"/>
@@ -3335,7 +3020,7 @@
       </c>
       <c r="I9" s="39" t="inlineStr">
         <is>
-          <t>JFTIME</t>
+          <t>26/05/2025</t>
         </is>
       </c>
       <c r="J9" s="2" t="n"/>
@@ -3364,12 +3049,12 @@
       <c r="G10" s="26" t="n"/>
       <c r="H10" s="40" t="inlineStr">
         <is>
-          <t>FCA :</t>
+          <t>DAF :</t>
         </is>
       </c>
       <c r="I10" s="81" t="inlineStr">
         <is>
-          <t>BAVET, SVAY RIENG</t>
+          <t>BAVET</t>
         </is>
       </c>
       <c r="J10" s="2" t="n"/>
@@ -4586,7 +4271,6 @@
         <v/>
       </c>
     </row>
-    <row r="55"/>
     <row r="56" ht="27" customHeight="1">
       <c r="A56" s="55" t="inlineStr">
         <is>
@@ -5205,8 +4889,8 @@
       </c>
       <c r="B78" s="104" t="n"/>
       <c r="C78" s="104" t="n"/>
-      <c r="D78" s="105" t="n"/>
-      <c r="E78" s="106" t="n"/>
+      <c r="D78" s="41" t="n"/>
+      <c r="E78" s="105" t="n"/>
       <c r="F78" s="26" t="n"/>
       <c r="G78" s="26" t="n"/>
       <c r="H78" s="26" t="n"/>
@@ -5229,15 +4913,15 @@
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B79" s="107" t="inlineStr">
+      <c r="B79" s="106" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="E79" s="108" t="n"/>
-      <c r="F79" s="108" t="n"/>
-      <c r="G79" s="108" t="n"/>
+      <c r="E79" s="107" t="n"/>
+      <c r="F79" s="107" t="n"/>
+      <c r="G79" s="107" t="n"/>
       <c r="H79" s="26" t="n"/>
       <c r="I79" s="2" t="n"/>
       <c r="J79" s="2" t="n"/>
@@ -5253,16 +4937,16 @@
       <c r="T79" s="2" t="n"/>
     </row>
     <row r="80" ht="51.75" customHeight="1">
-      <c r="A80" s="107" t="inlineStr">
+      <c r="A80" s="106" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
                                           /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="E80" s="108" t="n"/>
-      <c r="F80" s="108" t="n"/>
-      <c r="G80" s="108" t="n"/>
-      <c r="H80" s="108" t="n"/>
+      <c r="E80" s="107" t="n"/>
+      <c r="F80" s="107" t="n"/>
+      <c r="G80" s="107" t="n"/>
+      <c r="H80" s="107" t="n"/>
       <c r="I80" s="2" t="n"/>
       <c r="J80" s="2" t="n"/>
       <c r="K80" s="2" t="n"/>
@@ -5330,7 +5014,7 @@
     </row>
     <row r="83" ht="27" customHeight="1">
       <c r="A83" s="2" t="n"/>
-      <c r="B83" s="109" t="n"/>
+      <c r="B83" s="108" t="n"/>
       <c r="C83" s="2" t="n"/>
       <c r="D83" s="2" t="n"/>
       <c r="E83" s="52" t="n"/>
@@ -5354,123 +5038,6 @@
       <c r="S83" s="2" t="n"/>
       <c r="T83" s="2" t="n"/>
     </row>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
-    <row r="200"/>
   </sheetData>
   <mergeCells count="80">
     <mergeCell ref="A64:B64"/>

</xml_diff>

<commit_message>
finish with the template state builder shifting cell and exception for value that cant be shift when using skip in daf
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -28,6 +28,15 @@
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -127,15 +136,6 @@
     </font>
     <font>
       <name val="Times New Roman"/>
-      <b val="1"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
       <charset val="134"/>
       <color theme="1"/>
       <sz val="10"/>
@@ -160,6 +160,15 @@
     </font>
     <font>
       <name val="Times New Roman"/>
+      <b val="1"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
       <charset val="134"/>
       <sz val="20"/>
     </font>
@@ -178,15 +187,6 @@
       <name val="Times New Roman"/>
       <charset val="134"/>
       <sz val="15"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <b val="1"/>
-      <sz val="16"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="14"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -219,29 +219,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -303,6 +285,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="00000000"/>
       </left>
@@ -335,37 +335,6 @@
       <right style="thin">
         <color rgb="00000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
       <top style="thin">
         <color rgb="00000000"/>
       </top>
@@ -378,61 +347,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="25" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="21" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="26" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -450,106 +419,106 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -564,102 +533,99 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="29" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1033,15 +999,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="17.6640625" customWidth="1" min="1" max="1"/>
-    <col width="33.109375" customWidth="1" min="2" max="2"/>
-    <col width="42.5546875" customWidth="1" min="3" max="3"/>
-    <col width="34.5546875" customWidth="1" min="4" max="4"/>
-    <col width="47.5546875" customWidth="1" min="5" max="5"/>
-    <col width="28.6640625" customWidth="1" min="6" max="6"/>
+    <col width="17.7109375" customWidth="1" min="1" max="1"/>
+    <col width="33.140625" customWidth="1" min="2" max="2"/>
+    <col width="42.5703125" customWidth="1" min="3" max="3"/>
+    <col width="34.5703125" customWidth="1" min="4" max="4"/>
+    <col width="47.5703125" customWidth="1" min="5" max="5"/>
+    <col width="28.7109375" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45.9" customHeight="1">
+    <row r="1" ht="45.95" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>SALES CONTRACT</t>
@@ -1066,9 +1032,10 @@
           <t>DATE:</t>
         </is>
       </c>
-      <c r="E3" s="6">
-        <f>Invoice!G9</f>
-        <v/>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>26/05/2025</t>
+        </is>
       </c>
       <c r="F3" s="2" t="n"/>
     </row>
@@ -1081,9 +1048,10 @@
           <t>CONTRACT NO.:</t>
         </is>
       </c>
-      <c r="E4" s="7">
-        <f>Invoice!G8</f>
-        <v/>
+      <c r="E4" s="7" t="inlineStr">
+        <is>
+          <t>JF25027</t>
+        </is>
       </c>
       <c r="F4" s="2" t="n"/>
     </row>
@@ -1189,7 +1157,7 @@
       <c r="E12" s="8" t="n"/>
       <c r="F12" s="2" t="n"/>
     </row>
-    <row r="13" ht="60.9" customHeight="1">
+    <row r="13" ht="60.95" customHeight="1">
       <c r="A13" s="13" t="inlineStr">
         <is>
           <t>EMAll:jyangbin4720@dingtalk.com jialy@kukahome.com dailin@kukahome.com huanggf@kukahome.com zhangzp@kukahome.com</t>
@@ -1197,7 +1165,7 @@
       </c>
       <c r="F13" s="2" t="n"/>
     </row>
-    <row r="14" ht="54.9" customHeight="1">
+    <row r="14" ht="54.95" customHeight="1">
       <c r="A14" s="14" t="inlineStr">
         <is>
           <t>The undersigned Sellers 、Buyers and Beneficiary have agreed to close the  following transactions according to the terms and conditions Stipulated below:</t>
@@ -1577,7 +1545,7 @@
       <c r="E33" s="8" t="n"/>
       <c r="F33" s="2" t="n"/>
     </row>
-    <row r="34" ht="20.4" customHeight="1">
+    <row r="34" ht="20.45" customHeight="1">
       <c r="A34" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">Beneficiary bank information: </t>
@@ -1593,7 +1561,7 @@
       <c r="E34" s="8" t="n"/>
       <c r="F34" s="2" t="n"/>
     </row>
-    <row r="35" ht="45.9" customHeight="1">
+    <row r="35" ht="45.95" customHeight="1">
       <c r="A35" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">Beneficiary Bank' s Name: </t>
@@ -1637,7 +1605,7 @@
       </c>
       <c r="F37" s="2" t="n"/>
     </row>
-    <row r="38" ht="19.2" customHeight="1">
+    <row r="38" ht="19.15" customHeight="1">
       <c r="A38" s="8" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：</t>
@@ -1653,7 +1621,7 @@
       <c r="E38" s="8" t="n"/>
       <c r="F38" s="2" t="n"/>
     </row>
-    <row r="39" ht="45.9" customHeight="1">
+    <row r="39" ht="45.95" customHeight="1">
       <c r="A39" s="8" t="n"/>
       <c r="B39" s="8" t="n"/>
       <c r="C39" s="8" t="n"/>
@@ -1722,18 +1690,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="24.33203125" customWidth="1" min="1" max="1"/>
-    <col width="28.109375" customWidth="1" min="2" max="2"/>
-    <col width="21.6640625" customWidth="1" min="3" max="3"/>
-    <col width="18.33203125" customWidth="1" min="4" max="4"/>
-    <col width="15.6640625" customWidth="1" min="5" max="5"/>
-    <col width="16.44140625" customWidth="1" min="6" max="6"/>
-    <col width="24.88671875" customWidth="1" min="7" max="7"/>
-    <col width="25.109375" customWidth="1" min="8" max="8"/>
-    <col width="15.5546875" customWidth="1" min="9" max="9"/>
-    <col width="10.33203125" customWidth="1" min="10" max="10"/>
+    <col width="24.28515625" customWidth="1" min="1" max="1"/>
+    <col width="28.140625" customWidth="1" min="2" max="2"/>
+    <col width="21.7109375" customWidth="1" min="3" max="3"/>
+    <col width="18.28515625" customWidth="1" min="4" max="4"/>
+    <col width="15.7109375" customWidth="1" min="5" max="5"/>
+    <col width="16.42578125" customWidth="1" min="6" max="6"/>
+    <col width="24.85546875" customWidth="1" min="7" max="7"/>
+    <col width="25.140625" customWidth="1" min="8" max="8"/>
+    <col width="15.5703125" customWidth="1" min="9" max="9"/>
+    <col width="10.28515625" customWidth="1" min="10" max="10"/>
     <col width="13" customWidth="1" min="11" max="11"/>
-    <col width="12.44140625" customWidth="1" min="12" max="12"/>
+    <col width="12.42578125" customWidth="1" min="12" max="12"/>
     <col width="13" customWidth="1" min="13" max="13"/>
     <col width="13" customWidth="1" min="14" max="14"/>
     <col width="13" customWidth="1" min="15" max="15"/>
@@ -1852,9 +1820,10 @@
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="G7" s="34">
-        <f>'Packing list'!I7</f>
-        <v/>
+      <c r="G7" s="34" t="inlineStr">
+        <is>
+          <t>CLF2025-150</t>
+        </is>
       </c>
       <c r="H7" s="2" t="n"/>
       <c r="I7" s="2" t="n"/>
@@ -1884,9 +1853,10 @@
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="G8" s="38">
-        <f>'Packing list'!I8</f>
-        <v/>
+      <c r="G8" s="38" t="inlineStr">
+        <is>
+          <t>JF25027</t>
+        </is>
       </c>
       <c r="H8" s="2" t="n"/>
       <c r="I8" s="2" t="n"/>
@@ -1912,9 +1882,10 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="G9" s="39">
-        <f>'Packing list'!I9</f>
-        <v/>
+      <c r="G9" s="39" t="inlineStr">
+        <is>
+          <t>26/05/2025</t>
+        </is>
       </c>
       <c r="H9" s="2" t="n"/>
       <c r="I9" s="2" t="n"/>
@@ -2779,7 +2750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T83"/>
+  <dimension ref="A1:T85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2787,23 +2758,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25.44140625" customWidth="1" min="1" max="1"/>
-    <col width="22.88671875" customWidth="1" min="2" max="2"/>
-    <col width="19.44140625" customWidth="1" min="3" max="3"/>
-    <col width="26.6640625" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
-    <col width="13.6640625" customWidth="1" min="7" max="7"/>
-    <col width="15.5546875" customWidth="1" min="8" max="8"/>
-    <col width="23.6640625" customWidth="1" min="9" max="9"/>
-    <col width="12.44140625" customWidth="1" min="10" max="10"/>
-    <col width="12.88671875" customWidth="1" min="11" max="11"/>
-    <col width="12.5546875" customWidth="1" min="12" max="12"/>
-    <col width="13" customWidth="1" min="13" max="13"/>
-    <col width="12.5546875" customWidth="1" min="14" max="14"/>
-    <col width="13" customWidth="1" min="15" max="15"/>
-    <col width="12.5546875" customWidth="1" min="16" max="16"/>
-    <col width="13" customWidth="1" min="17" max="17"/>
+    <col width="25.42578125" customWidth="1" min="1" max="1"/>
+    <col width="22.85546875" customWidth="1" min="2" max="2"/>
+    <col width="19.42578125" customWidth="1" min="3" max="3"/>
+    <col width="26.7109375" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="13.7109375" customWidth="1" min="8" max="8"/>
+    <col width="15.5703125" customWidth="1" min="9" max="9"/>
+    <col width="23.7109375" customWidth="1" min="10" max="10"/>
+    <col width="12.42578125" customWidth="1" min="11" max="11"/>
+    <col width="12.85546875" customWidth="1" min="12" max="12"/>
+    <col width="12.5703125" customWidth="1" min="13" max="13"/>
+    <col width="13" customWidth="1" min="14" max="14"/>
+    <col width="12.5703125" customWidth="1" min="15" max="15"/>
+    <col width="13" customWidth="1" min="16" max="16"/>
+    <col width="12.5703125" customWidth="1" min="17" max="17"/>
     <col width="13" customWidth="1" min="18" max="18"/>
     <col width="13" customWidth="1" min="19" max="19"/>
     <col width="13" customWidth="1" min="20" max="20"/>
@@ -2815,7 +2786,6 @@
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="J1" s="2" t="n"/>
       <c r="K1" s="2" t="n"/>
       <c r="L1" s="2" t="n"/>
       <c r="M1" s="2" t="n"/>
@@ -2833,7 +2803,6 @@
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
         </is>
       </c>
-      <c r="J2" s="2" t="n"/>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n"/>
       <c r="M2" s="2" t="n"/>
@@ -2851,7 +2820,6 @@
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
       </c>
-      <c r="J3" s="2" t="n"/>
       <c r="K3" s="2" t="n"/>
       <c r="L3" s="2" t="n"/>
       <c r="M3" s="2" t="n"/>
@@ -2869,7 +2837,6 @@
           <t>VAT:L001-901903209</t>
         </is>
       </c>
-      <c r="J4" s="2" t="n"/>
       <c r="K4" s="2" t="n"/>
       <c r="L4" s="2" t="n"/>
       <c r="M4" s="2" t="n"/>
@@ -2895,7 +2862,6 @@
       <c r="G5" s="29" t="n"/>
       <c r="H5" s="29" t="n"/>
       <c r="I5" s="29" t="n"/>
-      <c r="J5" s="2" t="n"/>
       <c r="K5" s="2" t="n"/>
       <c r="L5" s="2" t="n"/>
       <c r="M5" s="2" t="n"/>
@@ -2921,7 +2887,6 @@
       <c r="G6" s="31" t="n"/>
       <c r="H6" s="31" t="n"/>
       <c r="I6" s="31" t="n"/>
-      <c r="J6" s="2" t="n"/>
       <c r="K6" s="2" t="n"/>
       <c r="L6" s="2" t="n"/>
       <c r="M6" s="2" t="n"/>
@@ -2951,7 +2916,6 @@
           <t>CLF2025-150</t>
         </is>
       </c>
-      <c r="J7" s="2" t="n"/>
       <c r="K7" s="2" t="n"/>
       <c r="L7" s="2" t="n"/>
       <c r="M7" s="2" t="n"/>
@@ -2989,7 +2953,6 @@
           <t>JF25027</t>
         </is>
       </c>
-      <c r="J8" s="2" t="n"/>
       <c r="K8" s="2" t="n"/>
       <c r="L8" s="2" t="n"/>
       <c r="M8" s="2" t="n"/>
@@ -3023,7 +2986,6 @@
           <t>26/05/2025</t>
         </is>
       </c>
-      <c r="J9" s="2" t="n"/>
       <c r="K9" s="2" t="n"/>
       <c r="L9" s="2" t="n"/>
       <c r="M9" s="2" t="n"/>
@@ -3057,7 +3019,6 @@
           <t>BAVET</t>
         </is>
       </c>
-      <c r="J10" s="2" t="n"/>
       <c r="K10" s="2" t="n"/>
       <c r="L10" s="2" t="n"/>
       <c r="M10" s="2" t="n"/>
@@ -3083,7 +3044,6 @@
       <c r="G11" s="26" t="n"/>
       <c r="H11" s="26" t="n"/>
       <c r="I11" s="26" t="n"/>
-      <c r="J11" s="2" t="n"/>
       <c r="K11" s="2" t="n"/>
       <c r="L11" s="2" t="n"/>
       <c r="M11" s="2" t="n"/>
@@ -3100,14 +3060,13 @@
       <c r="B12" s="77" t="n"/>
       <c r="C12" s="32" t="n"/>
       <c r="D12" s="32" t="n"/>
-      <c r="E12" s="26" t="n"/>
+      <c r="E12" s="32" t="n"/>
       <c r="F12" s="26" t="n"/>
       <c r="G12" s="26" t="n"/>
       <c r="H12" s="26" t="n"/>
       <c r="I12" s="26" t="n"/>
-      <c r="J12" s="2" t="n"/>
-      <c r="K12" s="2" t="n"/>
-      <c r="L12" s="2" t="n"/>
+      <c r="K12" s="26" t="n"/>
+      <c r="L12" s="82" t="n"/>
       <c r="M12" s="2" t="n"/>
       <c r="N12" s="2" t="n"/>
       <c r="O12" s="2" t="n"/>
@@ -3123,7 +3082,7 @@
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="82" t="inlineStr">
+      <c r="B13" s="83" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
@@ -3131,11 +3090,10 @@
       <c r="C13" s="2" t="n"/>
       <c r="D13" s="2" t="n"/>
       <c r="E13" s="2" t="n"/>
-      <c r="F13" s="83" t="n"/>
-      <c r="G13" s="83" t="n"/>
-      <c r="H13" s="83" t="n"/>
+      <c r="F13" s="84" t="n"/>
+      <c r="G13" s="84" t="n"/>
+      <c r="H13" s="84" t="n"/>
       <c r="I13" s="45" t="n"/>
-      <c r="J13" s="2" t="n"/>
       <c r="K13" s="2" t="n"/>
       <c r="L13" s="2" t="n"/>
       <c r="M13" s="2" t="n"/>
@@ -3149,19 +3107,18 @@
     </row>
     <row r="14" ht="25.5" customHeight="1">
       <c r="A14" s="32" t="n"/>
-      <c r="B14" s="84" t="inlineStr">
+      <c r="B14" s="85" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
       <c r="C14" s="47" t="n"/>
       <c r="D14" s="47" t="n"/>
-      <c r="E14" s="85" t="n"/>
-      <c r="F14" s="85" t="n"/>
-      <c r="G14" s="85" t="n"/>
-      <c r="H14" s="85" t="n"/>
+      <c r="E14" s="86" t="n"/>
+      <c r="F14" s="86" t="n"/>
+      <c r="G14" s="86" t="n"/>
+      <c r="H14" s="86" t="n"/>
       <c r="I14" s="2" t="n"/>
-      <c r="J14" s="2" t="n"/>
       <c r="K14" s="2" t="n"/>
       <c r="L14" s="2" t="n"/>
       <c r="M14" s="2" t="n"/>
@@ -3175,7 +3132,7 @@
     </row>
     <row r="15" ht="21" customHeight="1">
       <c r="A15" s="32" t="n"/>
-      <c r="B15" s="86" t="inlineStr">
+      <c r="B15" s="87" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
         </is>
@@ -3187,7 +3144,6 @@
       <c r="G15" s="45" t="n"/>
       <c r="H15" s="45" t="n"/>
       <c r="I15" s="2" t="n"/>
-      <c r="J15" s="2" t="n"/>
       <c r="K15" s="2" t="n"/>
       <c r="L15" s="2" t="n"/>
       <c r="M15" s="2" t="n"/>
@@ -3213,7 +3169,6 @@
       <c r="G16" s="45" t="n"/>
       <c r="H16" s="45" t="n"/>
       <c r="I16" s="2" t="n"/>
-      <c r="J16" s="2" t="n"/>
       <c r="K16" s="2" t="n"/>
       <c r="L16" s="2" t="n"/>
       <c r="M16" s="2" t="n"/>
@@ -3239,7 +3194,6 @@
       <c r="G17" s="45" t="n"/>
       <c r="H17" s="45" t="n"/>
       <c r="I17" s="2" t="n"/>
-      <c r="J17" s="2" t="n"/>
       <c r="K17" s="2" t="n"/>
       <c r="L17" s="2" t="n"/>
       <c r="M17" s="2" t="n"/>
@@ -3265,7 +3219,6 @@
       <c r="G18" s="26" t="n"/>
       <c r="H18" s="26" t="n"/>
       <c r="I18" s="2" t="n"/>
-      <c r="J18" s="2" t="n"/>
       <c r="K18" s="2" t="n"/>
       <c r="L18" s="2" t="n"/>
       <c r="M18" s="2" t="n"/>
@@ -3295,7 +3248,6 @@
       <c r="G19" s="2" t="n"/>
       <c r="H19" s="2" t="n"/>
       <c r="I19" s="2" t="n"/>
-      <c r="J19" s="2" t="n"/>
       <c r="K19" s="2" t="n"/>
       <c r="L19" s="2" t="n"/>
       <c r="M19" s="2" t="n"/>
@@ -3309,7 +3261,7 @@
     </row>
     <row r="20" ht="27.75" customHeight="1">
       <c r="A20" s="53" t="n"/>
-      <c r="B20" s="87" t="n"/>
+      <c r="B20" s="88" t="n"/>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
@@ -3317,7 +3269,6 @@
       <c r="G20" s="2" t="n"/>
       <c r="H20" s="2" t="n"/>
       <c r="I20" s="2" t="n"/>
-      <c r="J20" s="2" t="n"/>
       <c r="K20" s="2" t="n"/>
       <c r="L20" s="2" t="n"/>
       <c r="M20" s="2" t="n"/>
@@ -3335,922 +3286,909 @@
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B21" s="88" t="n"/>
+      <c r="B21" s="55" t="inlineStr">
+        <is>
+          <t>P.O Nº</t>
+        </is>
+      </c>
       <c r="C21" s="55" t="inlineStr">
         <is>
-          <t>P.O Nº</t>
+          <t>ITEM Nº</t>
         </is>
       </c>
       <c r="D21" s="55" t="inlineStr">
         <is>
-          <t>ITEM Nº</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="E21" s="55" t="inlineStr">
         <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="F21" s="55" t="inlineStr">
-        <is>
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="G21" s="89" t="n"/>
+      <c r="F21" s="89" t="n"/>
+      <c r="G21" s="56" t="inlineStr">
+        <is>
+          <t>N.W (kgs)</t>
+        </is>
+      </c>
       <c r="H21" s="56" t="inlineStr">
         <is>
-          <t>N.W (kgs)</t>
-        </is>
-      </c>
-      <c r="I21" s="56" t="inlineStr">
-        <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="J21" s="90" t="inlineStr">
+      <c r="I21" s="90" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
-      <c r="K21" s="2" t="n"/>
-      <c r="L21" s="2" t="n"/>
-      <c r="M21" s="2" t="n"/>
-      <c r="N21" s="2" t="n"/>
-      <c r="O21" s="2" t="n"/>
-      <c r="P21" s="2" t="n"/>
-      <c r="Q21" s="2" t="n"/>
-      <c r="R21" s="2" t="n"/>
-      <c r="S21" s="2" t="n"/>
-      <c r="T21" s="2" t="n"/>
     </row>
     <row r="22" ht="27" customHeight="1">
-      <c r="A22" s="91" t="n"/>
-      <c r="B22" s="92" t="n"/>
+      <c r="A22" s="62" t="n"/>
+      <c r="B22" s="62" t="n"/>
       <c r="C22" s="62" t="n"/>
       <c r="D22" s="62" t="n"/>
-      <c r="E22" s="62" t="n"/>
-      <c r="F22" s="93" t="inlineStr">
+      <c r="E22" s="91" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="G22" s="56" t="inlineStr">
+      <c r="F22" s="56" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
+      <c r="G22" s="62" t="n"/>
       <c r="H22" s="62" t="n"/>
       <c r="I22" s="62" t="n"/>
-      <c r="J22" s="62" t="n"/>
     </row>
     <row r="23" ht="27" customHeight="1">
-      <c r="A23" s="94" t="inlineStr">
+      <c r="A23" s="92" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B23" s="95" t="n"/>
-      <c r="C23" s="96" t="inlineStr">
+      <c r="B23" s="93" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="D23" s="96" t="inlineStr">
+      <c r="C23" s="93" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="E23" s="59" t="inlineStr">
+      <c r="D23" s="59" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="F23" s="97" t="n">
+      <c r="E23" s="94" t="n">
         <v>122</v>
       </c>
+      <c r="F23" s="60" t="n">
+        <v>6461.7</v>
+      </c>
       <c r="G23" s="60" t="n">
-        <v>6461.7</v>
+        <v>467.8306</v>
       </c>
       <c r="H23" s="60" t="n">
-        <v>467.8306</v>
-      </c>
-      <c r="I23" s="60" t="n">
         <v>512.1048</v>
       </c>
-      <c r="J23" s="98" t="n">
+      <c r="I23" s="95" t="n">
         <v>1.8312</v>
       </c>
     </row>
     <row r="24" ht="27" customHeight="1">
-      <c r="A24" s="94" t="inlineStr">
+      <c r="A24" s="92" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B24" s="95" t="n"/>
-      <c r="C24" s="96" t="inlineStr">
+      <c r="B24" s="93" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="D24" s="96" t="inlineStr">
+      <c r="C24" s="93" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
-      <c r="E24" s="61" t="n"/>
-      <c r="F24" s="97" t="n">
+      <c r="D24" s="61" t="n"/>
+      <c r="E24" s="94" t="n">
         <v>2</v>
       </c>
+      <c r="F24" s="60" t="n">
+        <v>77.90000000000001</v>
+      </c>
       <c r="G24" s="60" t="n">
-        <v>77.90000000000001</v>
+        <v>7.6694</v>
       </c>
       <c r="H24" s="60" t="n">
-        <v>7.6694</v>
-      </c>
-      <c r="I24" s="60" t="n">
         <v>8.395200000000001</v>
       </c>
-      <c r="J24" s="98" t="n">
+      <c r="I24" s="95" t="n">
         <v>0.03</v>
       </c>
     </row>
     <row r="25" ht="27" customHeight="1">
-      <c r="A25" s="94" t="inlineStr">
+      <c r="A25" s="92" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B25" s="95" t="n"/>
-      <c r="C25" s="96" t="inlineStr">
+      <c r="B25" s="93" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="D25" s="96" t="inlineStr">
+      <c r="C25" s="93" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
-      <c r="E25" s="61" t="n"/>
-      <c r="F25" s="97" t="n">
+      <c r="D25" s="61" t="n"/>
+      <c r="E25" s="94" t="n">
         <v>190</v>
       </c>
+      <c r="F25" s="60" t="n">
+        <v>10009.4</v>
+      </c>
       <c r="G25" s="60" t="n">
+        <v>757</v>
+      </c>
+      <c r="H25" s="60" t="n">
+        <v>802</v>
+      </c>
+      <c r="I25" s="95" t="n">
+        <v>2.4552</v>
+      </c>
+    </row>
+    <row r="26" ht="27" customHeight="1">
+      <c r="A26" s="92" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="B26" s="93" t="inlineStr">
+        <is>
+          <t>9000678762</t>
+        </is>
+      </c>
+      <c r="C26" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U756071</t>
+        </is>
+      </c>
+      <c r="D26" s="61" t="n"/>
+      <c r="E26" s="94" t="n">
+        <v>208</v>
+      </c>
+      <c r="F26" s="60" t="n">
+        <v>10940.1</v>
+      </c>
+      <c r="G26" s="60" t="n">
+        <v>842.2056</v>
+      </c>
+      <c r="H26" s="60" t="n">
+        <v>885.9439</v>
+      </c>
+      <c r="I26" s="95" t="n">
+        <v>2.6943</v>
+      </c>
+    </row>
+    <row r="27" ht="27" customHeight="1">
+      <c r="B27" s="93" t="inlineStr">
+        <is>
+          <t>9000678762</t>
+        </is>
+      </c>
+      <c r="C27" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U756071</t>
+        </is>
+      </c>
+      <c r="D27" s="61" t="n"/>
+      <c r="E27" s="94" t="n">
+        <v>6</v>
+      </c>
+      <c r="F27" s="60" t="n">
+        <v>241.9</v>
+      </c>
+      <c r="G27" s="60" t="n">
+        <v>24.2944</v>
+      </c>
+      <c r="H27" s="60" t="n">
+        <v>25.5561</v>
+      </c>
+      <c r="I27" s="95" t="n">
+        <v>0.07770000000000001</v>
+      </c>
+    </row>
+    <row r="28" ht="27" customHeight="1">
+      <c r="B28" s="93" t="n">
+        <v>9000697761</v>
+      </c>
+      <c r="C28" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D28" s="61" t="n"/>
+      <c r="E28" s="94" t="n">
+        <v>154</v>
+      </c>
+      <c r="F28" s="60" t="n">
+        <v>7788.7</v>
+      </c>
+      <c r="G28" s="60" t="n">
+        <v>617.7907</v>
+      </c>
+      <c r="H28" s="60" t="n">
+        <v>658.0814</v>
+      </c>
+      <c r="I28" s="95" t="n">
+        <v>2.0564</v>
+      </c>
+    </row>
+    <row r="29" ht="27" customHeight="1">
+      <c r="B29" s="93" t="n">
+        <v>9000697761</v>
+      </c>
+      <c r="C29" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D29" s="61" t="n"/>
+      <c r="E29" s="94" t="n">
+        <v>18</v>
+      </c>
+      <c r="F29" s="60" t="n">
+        <v>711.1</v>
+      </c>
+      <c r="G29" s="60" t="n">
+        <v>72.2093</v>
+      </c>
+      <c r="H29" s="60" t="n">
+        <v>76.9186</v>
+      </c>
+      <c r="I29" s="95" t="n">
+        <v>0.2404</v>
+      </c>
+    </row>
+    <row r="30" ht="27" customHeight="1">
+      <c r="B30" s="93" t="n">
+        <v>9000697761</v>
+      </c>
+      <c r="C30" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D30" s="61" t="n"/>
+      <c r="E30" s="94" t="n">
+        <v>195</v>
+      </c>
+      <c r="F30" s="60" t="n">
+        <v>10033.3</v>
+      </c>
+      <c r="G30" s="60" t="n">
+        <v>814.5</v>
+      </c>
+      <c r="H30" s="60" t="n">
+        <v>859.5</v>
+      </c>
+      <c r="I30" s="95" t="n">
+        <v>2.376</v>
+      </c>
+    </row>
+    <row r="31" ht="27" customHeight="1">
+      <c r="B31" s="93" t="n">
+        <v>9000697761</v>
+      </c>
+      <c r="C31" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D31" s="61" t="n"/>
+      <c r="E31" s="94" t="n">
+        <v>200</v>
+      </c>
+      <c r="F31" s="60" t="n">
+        <v>10334.8</v>
+      </c>
+      <c r="G31" s="60" t="n">
+        <v>740.5286</v>
+      </c>
+      <c r="H31" s="60" t="n">
+        <v>780.1762</v>
+      </c>
+      <c r="I31" s="95" t="n">
+        <v>2.2678</v>
+      </c>
+    </row>
+    <row r="32" ht="27" customHeight="1">
+      <c r="B32" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C32" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D32" s="61" t="n"/>
+      <c r="E32" s="94" t="n">
+        <v>27</v>
+      </c>
+      <c r="F32" s="60" t="n">
+        <v>1065.4</v>
+      </c>
+      <c r="G32" s="60" t="n">
+        <v>99.9714</v>
+      </c>
+      <c r="H32" s="60" t="n">
+        <v>105.3238</v>
+      </c>
+      <c r="I32" s="95" t="n">
+        <v>0.3062</v>
+      </c>
+    </row>
+    <row r="33" ht="27" customHeight="1">
+      <c r="B33" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C33" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D33" s="61" t="n"/>
+      <c r="E33" s="94" t="n">
+        <v>169</v>
+      </c>
+      <c r="F33" s="60" t="n">
+        <v>8660.5</v>
+      </c>
+      <c r="G33" s="60" t="n">
+        <v>693.3828999999999</v>
+      </c>
+      <c r="H33" s="60" t="n">
+        <v>736.84</v>
+      </c>
+      <c r="I33" s="95" t="n">
+        <v>2.2181</v>
+      </c>
+    </row>
+    <row r="34" ht="27" customHeight="1">
+      <c r="B34" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C34" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D34" s="61" t="n"/>
+      <c r="E34" s="94" t="n">
+        <v>6</v>
+      </c>
+      <c r="F34" s="60" t="n">
+        <v>236</v>
+      </c>
+      <c r="G34" s="60" t="n">
+        <v>24.6171</v>
+      </c>
+      <c r="H34" s="60" t="n">
+        <v>26.16</v>
+      </c>
+      <c r="I34" s="95" t="n">
+        <v>0.07870000000000001</v>
+      </c>
+    </row>
+    <row r="35" ht="27" customHeight="1">
+      <c r="B35" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C35" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528062</t>
+        </is>
+      </c>
+      <c r="D35" s="61" t="n"/>
+      <c r="E35" s="94" t="n">
+        <v>195</v>
+      </c>
+      <c r="F35" s="60" t="n">
+        <v>10057.4</v>
+      </c>
+      <c r="G35" s="60" t="n">
+        <v>814.5</v>
+      </c>
+      <c r="H35" s="60" t="n">
+        <v>859.5</v>
+      </c>
+      <c r="I35" s="95" t="n">
+        <v>2.376</v>
+      </c>
+    </row>
+    <row r="36" ht="27" customHeight="1">
+      <c r="B36" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C36" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D36" s="61" t="n"/>
+      <c r="E36" s="94" t="n">
+        <v>195</v>
+      </c>
+      <c r="F36" s="60" t="n">
+        <v>10176.8</v>
+      </c>
+      <c r="G36" s="60" t="n">
+        <v>830.5</v>
+      </c>
+      <c r="H36" s="60" t="n">
+        <v>875.5</v>
+      </c>
+      <c r="I36" s="95" t="n">
+        <v>2.6136</v>
+      </c>
+    </row>
+    <row r="37" ht="27" customHeight="1">
+      <c r="B37" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C37" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D37" s="61" t="n"/>
+      <c r="E37" s="94" t="n">
+        <v>215</v>
+      </c>
+      <c r="F37" s="60" t="n">
+        <v>11117</v>
+      </c>
+      <c r="G37" s="60" t="n">
+        <v>901.5</v>
+      </c>
+      <c r="H37" s="60" t="n">
+        <v>946.5</v>
+      </c>
+      <c r="I37" s="95" t="n">
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="38" ht="27" customHeight="1">
+      <c r="B38" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C38" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D38" s="61" t="n"/>
+      <c r="E38" s="94" t="n">
+        <v>215</v>
+      </c>
+      <c r="F38" s="60" t="n">
+        <v>11227</v>
+      </c>
+      <c r="G38" s="60" t="n">
+        <v>918</v>
+      </c>
+      <c r="H38" s="60" t="n">
+        <v>963</v>
+      </c>
+      <c r="I38" s="95" t="n">
+        <v>2.6136</v>
+      </c>
+    </row>
+    <row r="39" ht="27" customHeight="1">
+      <c r="B39" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C39" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D39" s="61" t="n"/>
+      <c r="E39" s="94" t="n">
+        <v>192</v>
+      </c>
+      <c r="F39" s="60" t="n">
+        <v>9879.4</v>
+      </c>
+      <c r="G39" s="60" t="n">
+        <v>795.0291</v>
+      </c>
+      <c r="H39" s="60" t="n">
+        <v>836.9709</v>
+      </c>
+      <c r="I39" s="95" t="n">
+        <v>2.4729</v>
+      </c>
+    </row>
+    <row r="40" ht="27" customHeight="1">
+      <c r="B40" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C40" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D40" s="61" t="n"/>
+      <c r="E40" s="94" t="n">
+        <v>14</v>
+      </c>
+      <c r="F40" s="60" t="n">
+        <v>561</v>
+      </c>
+      <c r="G40" s="60" t="n">
+        <v>57.9709</v>
+      </c>
+      <c r="H40" s="60" t="n">
+        <v>61.0291</v>
+      </c>
+      <c r="I40" s="95" t="n">
+        <v>0.1803</v>
+      </c>
+    </row>
+    <row r="41" ht="27" customHeight="1">
+      <c r="B41" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C41" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D41" s="61" t="n"/>
+      <c r="E41" s="94" t="n">
+        <v>97</v>
+      </c>
+      <c r="F41" s="60" t="n">
+        <v>5016.1</v>
+      </c>
+      <c r="G41" s="60" t="n">
+        <v>408</v>
+      </c>
+      <c r="H41" s="60" t="n">
+        <v>453</v>
+      </c>
+      <c r="I41" s="95" t="n">
+        <v>1.782</v>
+      </c>
+    </row>
+    <row r="42" ht="27" customHeight="1">
+      <c r="B42" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C42" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D42" s="61" t="n"/>
+      <c r="E42" s="94" t="n">
+        <v>97</v>
+      </c>
+      <c r="F42" s="60" t="n">
+        <v>5022.5</v>
+      </c>
+      <c r="G42" s="60" t="n">
+        <v>407</v>
+      </c>
+      <c r="H42" s="60" t="n">
+        <v>452</v>
+      </c>
+      <c r="I42" s="95" t="n">
+        <v>1.8216</v>
+      </c>
+    </row>
+    <row r="43" ht="27" customHeight="1">
+      <c r="B43" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C43" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D43" s="61" t="n"/>
+      <c r="E43" s="94" t="n">
+        <v>184</v>
+      </c>
+      <c r="F43" s="60" t="n">
+        <v>9583.5</v>
+      </c>
+      <c r="G43" s="60" t="n">
+        <v>773.7684</v>
+      </c>
+      <c r="H43" s="60" t="n">
+        <v>817.3474</v>
+      </c>
+      <c r="I43" s="95" t="n">
+        <v>2.6461</v>
+      </c>
+    </row>
+    <row r="44" ht="27" customHeight="1">
+      <c r="B44" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C44" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D44" s="61" t="n"/>
+      <c r="E44" s="94" t="n">
+        <v>6</v>
+      </c>
+      <c r="F44" s="60" t="n">
+        <v>237.8</v>
+      </c>
+      <c r="G44" s="60" t="n">
+        <v>25.2316</v>
+      </c>
+      <c r="H44" s="60" t="n">
+        <v>26.6526</v>
+      </c>
+      <c r="I44" s="95" t="n">
+        <v>0.0863</v>
+      </c>
+    </row>
+    <row r="45" ht="27" customHeight="1">
+      <c r="B45" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C45" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D45" s="61" t="n"/>
+      <c r="E45" s="94" t="n">
+        <v>185</v>
+      </c>
+      <c r="F45" s="60" t="n">
+        <v>9782.9</v>
+      </c>
+      <c r="G45" s="60" t="n">
+        <v>786.25</v>
+      </c>
+      <c r="H45" s="60" t="n">
+        <v>830.0658</v>
+      </c>
+      <c r="I45" s="95" t="n">
+        <v>2.5063</v>
+      </c>
+    </row>
+    <row r="46" ht="27" customHeight="1">
+      <c r="B46" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C46" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D46" s="61" t="n"/>
+      <c r="E46" s="94" t="n">
+        <v>5</v>
+      </c>
+      <c r="F46" s="60" t="n">
+        <v>199</v>
+      </c>
+      <c r="G46" s="60" t="n">
+        <v>21.25</v>
+      </c>
+      <c r="H46" s="60" t="n">
+        <v>22.4342</v>
+      </c>
+      <c r="I46" s="95" t="n">
+        <v>0.0677</v>
+      </c>
+    </row>
+    <row r="47" ht="27" customHeight="1">
+      <c r="B47" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C47" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D47" s="61" t="n"/>
+      <c r="E47" s="94" t="n">
+        <v>190</v>
+      </c>
+      <c r="F47" s="60" t="n">
         <v>10009.4</v>
       </c>
-      <c r="H25" s="60" t="n">
-        <v>757</v>
-      </c>
-      <c r="I25" s="60" t="n">
-        <v>802</v>
-      </c>
-      <c r="J25" s="98" t="n">
-        <v>2.4552</v>
-      </c>
-    </row>
-    <row r="26" ht="27" customHeight="1">
-      <c r="A26" s="94" t="inlineStr">
-        <is>
-          <t>MADE IN CAMBODIA</t>
-        </is>
-      </c>
-      <c r="B26" s="95" t="n"/>
-      <c r="C26" s="96" t="inlineStr">
-        <is>
-          <t>9000678762</t>
-        </is>
-      </c>
-      <c r="D26" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U756071</t>
-        </is>
-      </c>
-      <c r="E26" s="61" t="n"/>
-      <c r="F26" s="97" t="n">
-        <v>208</v>
-      </c>
-      <c r="G26" s="60" t="n">
-        <v>10940.1</v>
-      </c>
-      <c r="H26" s="60" t="n">
-        <v>842.2056</v>
-      </c>
-      <c r="I26" s="60" t="n">
-        <v>885.9439</v>
-      </c>
-      <c r="J26" s="98" t="n">
-        <v>2.6943</v>
-      </c>
-    </row>
-    <row r="27" ht="27" customHeight="1">
-      <c r="C27" s="96" t="inlineStr">
-        <is>
-          <t>9000678762</t>
-        </is>
-      </c>
-      <c r="D27" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U756071</t>
-        </is>
-      </c>
-      <c r="E27" s="61" t="n"/>
-      <c r="F27" s="97" t="n">
-        <v>6</v>
-      </c>
-      <c r="G27" s="60" t="n">
-        <v>241.9</v>
-      </c>
-      <c r="H27" s="60" t="n">
-        <v>24.2944</v>
-      </c>
-      <c r="I27" s="60" t="n">
-        <v>25.5561</v>
-      </c>
-      <c r="J27" s="98" t="n">
-        <v>0.07770000000000001</v>
-      </c>
-    </row>
-    <row r="28" ht="27" customHeight="1">
-      <c r="C28" s="96" t="n">
-        <v>9000697761</v>
-      </c>
-      <c r="D28" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528062</t>
-        </is>
-      </c>
-      <c r="E28" s="61" t="n"/>
-      <c r="F28" s="97" t="n">
-        <v>154</v>
-      </c>
-      <c r="G28" s="60" t="n">
-        <v>7788.7</v>
-      </c>
-      <c r="H28" s="60" t="n">
-        <v>617.7907</v>
-      </c>
-      <c r="I28" s="60" t="n">
-        <v>658.0814</v>
-      </c>
-      <c r="J28" s="98" t="n">
-        <v>2.0564</v>
-      </c>
-    </row>
-    <row r="29" ht="27" customHeight="1">
-      <c r="C29" s="96" t="n">
-        <v>9000697761</v>
-      </c>
-      <c r="D29" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528062</t>
-        </is>
-      </c>
-      <c r="E29" s="61" t="n"/>
-      <c r="F29" s="97" t="n">
-        <v>18</v>
-      </c>
-      <c r="G29" s="60" t="n">
-        <v>711.1</v>
-      </c>
-      <c r="H29" s="60" t="n">
-        <v>72.2093</v>
-      </c>
-      <c r="I29" s="60" t="n">
-        <v>76.9186</v>
-      </c>
-      <c r="J29" s="98" t="n">
-        <v>0.2404</v>
-      </c>
-    </row>
-    <row r="30" ht="27" customHeight="1">
-      <c r="C30" s="96" t="n">
-        <v>9000697761</v>
-      </c>
-      <c r="D30" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528062</t>
-        </is>
-      </c>
-      <c r="E30" s="61" t="n"/>
-      <c r="F30" s="97" t="n">
+      <c r="G47" s="60" t="n">
+        <v>824</v>
+      </c>
+      <c r="H47" s="60" t="n">
+        <v>869</v>
+      </c>
+      <c r="I47" s="95" t="n">
+        <v>2.574</v>
+      </c>
+    </row>
+    <row r="48" ht="27" customHeight="1">
+      <c r="B48" s="93" t="n">
+        <v>9000699450</v>
+      </c>
+      <c r="C48" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D48" s="61" t="n"/>
+      <c r="E48" s="94" t="n">
         <v>195</v>
       </c>
-      <c r="G30" s="60" t="n">
-        <v>10033.3</v>
-      </c>
-      <c r="H30" s="60" t="n">
-        <v>814.5</v>
-      </c>
-      <c r="I30" s="60" t="n">
-        <v>859.5</v>
-      </c>
-      <c r="J30" s="98" t="n">
-        <v>2.376</v>
-      </c>
-    </row>
-    <row r="31" ht="27" customHeight="1">
-      <c r="C31" s="96" t="n">
-        <v>9000697761</v>
-      </c>
-      <c r="D31" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528062</t>
-        </is>
-      </c>
-      <c r="E31" s="61" t="n"/>
-      <c r="F31" s="97" t="n">
-        <v>200</v>
-      </c>
-      <c r="G31" s="60" t="n">
-        <v>10334.8</v>
-      </c>
-      <c r="H31" s="60" t="n">
-        <v>740.5286</v>
-      </c>
-      <c r="I31" s="60" t="n">
-        <v>780.1762</v>
-      </c>
-      <c r="J31" s="98" t="n">
-        <v>2.2678</v>
-      </c>
-    </row>
-    <row r="32" ht="27" customHeight="1">
-      <c r="C32" s="96" t="n">
+      <c r="F48" s="60" t="n">
+        <v>10072.6</v>
+      </c>
+      <c r="G48" s="60" t="n">
+        <v>821</v>
+      </c>
+      <c r="H48" s="60" t="n">
+        <v>866</v>
+      </c>
+      <c r="I48" s="95" t="n">
+        <v>2.574</v>
+      </c>
+    </row>
+    <row r="49" ht="27" customHeight="1">
+      <c r="B49" s="93" t="n">
         <v>9000699450</v>
       </c>
-      <c r="D32" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528062</t>
-        </is>
-      </c>
-      <c r="E32" s="61" t="n"/>
-      <c r="F32" s="97" t="n">
-        <v>27</v>
-      </c>
-      <c r="G32" s="60" t="n">
-        <v>1065.4</v>
-      </c>
-      <c r="H32" s="60" t="n">
-        <v>99.9714</v>
-      </c>
-      <c r="I32" s="60" t="n">
-        <v>105.3238</v>
-      </c>
-      <c r="J32" s="98" t="n">
-        <v>0.3062</v>
-      </c>
-    </row>
-    <row r="33" ht="27" customHeight="1">
-      <c r="C33" s="96" t="n">
+      <c r="C49" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D49" s="61" t="n"/>
+      <c r="E49" s="94" t="n">
+        <v>195</v>
+      </c>
+      <c r="F49" s="60" t="n">
+        <v>10117.1</v>
+      </c>
+      <c r="G49" s="60" t="n">
+        <v>825.5</v>
+      </c>
+      <c r="H49" s="60" t="n">
+        <v>870.5</v>
+      </c>
+      <c r="I49" s="95" t="n">
+        <v>2.4948</v>
+      </c>
+    </row>
+    <row r="50" ht="27" customHeight="1">
+      <c r="B50" s="93" t="n">
         <v>9000699450</v>
       </c>
-      <c r="D33" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528062</t>
-        </is>
-      </c>
-      <c r="E33" s="61" t="n"/>
-      <c r="F33" s="97" t="n">
-        <v>169</v>
-      </c>
-      <c r="G33" s="60" t="n">
-        <v>8660.5</v>
-      </c>
-      <c r="H33" s="60" t="n">
-        <v>693.3828999999999</v>
-      </c>
-      <c r="I33" s="60" t="n">
-        <v>736.84</v>
-      </c>
-      <c r="J33" s="98" t="n">
-        <v>2.2181</v>
-      </c>
-    </row>
-    <row r="34" ht="27" customHeight="1">
-      <c r="C34" s="96" t="n">
+      <c r="C50" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D50" s="61" t="n"/>
+      <c r="E50" s="94" t="n">
+        <v>89</v>
+      </c>
+      <c r="F50" s="60" t="n">
+        <v>4707.4</v>
+      </c>
+      <c r="G50" s="60" t="n">
+        <v>376.5385</v>
+      </c>
+      <c r="H50" s="60" t="n">
+        <v>415.0481</v>
+      </c>
+      <c r="I50" s="95" t="n">
+        <v>1.4572</v>
+      </c>
+    </row>
+    <row r="51" ht="27" customHeight="1">
+      <c r="B51" s="93" t="n">
         <v>9000699450</v>
       </c>
-      <c r="D34" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528062</t>
-        </is>
-      </c>
-      <c r="E34" s="61" t="n"/>
-      <c r="F34" s="97" t="n">
-        <v>6</v>
-      </c>
-      <c r="G34" s="60" t="n">
-        <v>236</v>
-      </c>
-      <c r="H34" s="60" t="n">
-        <v>24.6171</v>
-      </c>
-      <c r="I34" s="60" t="n">
-        <v>26.16</v>
-      </c>
-      <c r="J34" s="98" t="n">
-        <v>0.07870000000000001</v>
-      </c>
-    </row>
-    <row r="35" ht="27" customHeight="1">
-      <c r="C35" s="96" t="n">
+      <c r="C51" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D51" s="61" t="n"/>
+      <c r="E51" s="94" t="n">
+        <v>8</v>
+      </c>
+      <c r="F51" s="60" t="n">
+        <v>322.8</v>
+      </c>
+      <c r="G51" s="60" t="n">
+        <v>33.8462</v>
+      </c>
+      <c r="H51" s="60" t="n">
+        <v>37.3077</v>
+      </c>
+      <c r="I51" s="95" t="n">
+        <v>0.131</v>
+      </c>
+    </row>
+    <row r="52" ht="27" customHeight="1">
+      <c r="B52" s="93" t="n">
         <v>9000699450</v>
       </c>
-      <c r="D35" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528062</t>
-        </is>
-      </c>
-      <c r="E35" s="61" t="n"/>
-      <c r="F35" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G35" s="60" t="n">
-        <v>10057.4</v>
-      </c>
-      <c r="H35" s="60" t="n">
-        <v>814.5</v>
-      </c>
-      <c r="I35" s="60" t="n">
-        <v>859.5</v>
-      </c>
-      <c r="J35" s="98" t="n">
-        <v>2.376</v>
-      </c>
-    </row>
-    <row r="36" ht="27" customHeight="1">
-      <c r="C36" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D36" s="96" t="inlineStr">
+      <c r="C52" s="93" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="E36" s="61" t="n"/>
-      <c r="F36" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G36" s="60" t="n">
-        <v>10176.8</v>
-      </c>
-      <c r="H36" s="60" t="n">
-        <v>830.5</v>
-      </c>
-      <c r="I36" s="60" t="n">
-        <v>875.5</v>
-      </c>
-      <c r="J36" s="98" t="n">
-        <v>2.6136</v>
-      </c>
-    </row>
-    <row r="37" ht="27" customHeight="1">
-      <c r="C37" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D37" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E37" s="61" t="n"/>
-      <c r="F37" s="97" t="n">
-        <v>215</v>
-      </c>
-      <c r="G37" s="60" t="n">
-        <v>11117</v>
-      </c>
-      <c r="H37" s="60" t="n">
-        <v>901.5</v>
-      </c>
-      <c r="I37" s="60" t="n">
-        <v>946.5</v>
-      </c>
-      <c r="J37" s="98" t="n">
-        <v>2.97</v>
-      </c>
-    </row>
-    <row r="38" ht="27" customHeight="1">
-      <c r="C38" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D38" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E38" s="61" t="n"/>
-      <c r="F38" s="97" t="n">
-        <v>215</v>
-      </c>
-      <c r="G38" s="60" t="n">
-        <v>11227</v>
-      </c>
-      <c r="H38" s="60" t="n">
-        <v>918</v>
-      </c>
-      <c r="I38" s="60" t="n">
-        <v>963</v>
-      </c>
-      <c r="J38" s="98" t="n">
-        <v>2.6136</v>
-      </c>
-    </row>
-    <row r="39" ht="27" customHeight="1">
-      <c r="C39" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D39" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E39" s="61" t="n"/>
-      <c r="F39" s="97" t="n">
-        <v>192</v>
-      </c>
-      <c r="G39" s="60" t="n">
-        <v>9879.4</v>
-      </c>
-      <c r="H39" s="60" t="n">
-        <v>795.0291</v>
-      </c>
-      <c r="I39" s="60" t="n">
-        <v>836.9709</v>
-      </c>
-      <c r="J39" s="98" t="n">
-        <v>2.4729</v>
-      </c>
-    </row>
-    <row r="40" ht="27" customHeight="1">
-      <c r="C40" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D40" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E40" s="61" t="n"/>
-      <c r="F40" s="97" t="n">
-        <v>14</v>
-      </c>
-      <c r="G40" s="60" t="n">
-        <v>561</v>
-      </c>
-      <c r="H40" s="60" t="n">
-        <v>57.9709</v>
-      </c>
-      <c r="I40" s="60" t="n">
-        <v>61.0291</v>
-      </c>
-      <c r="J40" s="98" t="n">
-        <v>0.1803</v>
-      </c>
-    </row>
-    <row r="41" ht="27" customHeight="1">
-      <c r="C41" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D41" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E41" s="61" t="n"/>
-      <c r="F41" s="97" t="n">
-        <v>97</v>
-      </c>
-      <c r="G41" s="60" t="n">
-        <v>5016.1</v>
-      </c>
-      <c r="H41" s="60" t="n">
-        <v>408</v>
-      </c>
-      <c r="I41" s="60" t="n">
-        <v>453</v>
-      </c>
-      <c r="J41" s="98" t="n">
-        <v>1.782</v>
-      </c>
-    </row>
-    <row r="42" ht="27" customHeight="1">
-      <c r="C42" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D42" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E42" s="61" t="n"/>
-      <c r="F42" s="97" t="n">
-        <v>97</v>
-      </c>
-      <c r="G42" s="60" t="n">
-        <v>5022.5</v>
-      </c>
-      <c r="H42" s="60" t="n">
-        <v>407</v>
-      </c>
-      <c r="I42" s="60" t="n">
-        <v>452</v>
-      </c>
-      <c r="J42" s="98" t="n">
-        <v>1.8216</v>
-      </c>
-    </row>
-    <row r="43" ht="27" customHeight="1">
-      <c r="C43" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D43" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E43" s="61" t="n"/>
-      <c r="F43" s="97" t="n">
-        <v>184</v>
-      </c>
-      <c r="G43" s="60" t="n">
-        <v>9583.5</v>
-      </c>
-      <c r="H43" s="60" t="n">
-        <v>773.7684</v>
-      </c>
-      <c r="I43" s="60" t="n">
-        <v>817.3474</v>
-      </c>
-      <c r="J43" s="98" t="n">
-        <v>2.6461</v>
-      </c>
-    </row>
-    <row r="44" ht="27" customHeight="1">
-      <c r="C44" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D44" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E44" s="61" t="n"/>
-      <c r="F44" s="97" t="n">
-        <v>6</v>
-      </c>
-      <c r="G44" s="60" t="n">
-        <v>237.8</v>
-      </c>
-      <c r="H44" s="60" t="n">
-        <v>25.2316</v>
-      </c>
-      <c r="I44" s="60" t="n">
-        <v>26.6526</v>
-      </c>
-      <c r="J44" s="98" t="n">
-        <v>0.0863</v>
-      </c>
-    </row>
-    <row r="45" ht="27" customHeight="1">
-      <c r="C45" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D45" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E45" s="61" t="n"/>
-      <c r="F45" s="97" t="n">
-        <v>185</v>
-      </c>
-      <c r="G45" s="60" t="n">
-        <v>9782.9</v>
-      </c>
-      <c r="H45" s="60" t="n">
-        <v>786.25</v>
-      </c>
-      <c r="I45" s="60" t="n">
-        <v>830.0658</v>
-      </c>
-      <c r="J45" s="98" t="n">
-        <v>2.5063</v>
-      </c>
-    </row>
-    <row r="46" ht="27" customHeight="1">
-      <c r="C46" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D46" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E46" s="61" t="n"/>
-      <c r="F46" s="97" t="n">
-        <v>5</v>
-      </c>
-      <c r="G46" s="60" t="n">
-        <v>199</v>
-      </c>
-      <c r="H46" s="60" t="n">
-        <v>21.25</v>
-      </c>
-      <c r="I46" s="60" t="n">
-        <v>22.4342</v>
-      </c>
-      <c r="J46" s="98" t="n">
-        <v>0.0677</v>
-      </c>
-    </row>
-    <row r="47" ht="27" customHeight="1">
-      <c r="C47" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D47" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E47" s="61" t="n"/>
-      <c r="F47" s="97" t="n">
-        <v>190</v>
-      </c>
-      <c r="G47" s="60" t="n">
-        <v>10009.4</v>
-      </c>
-      <c r="H47" s="60" t="n">
-        <v>824</v>
-      </c>
-      <c r="I47" s="60" t="n">
-        <v>869</v>
-      </c>
-      <c r="J47" s="98" t="n">
-        <v>2.574</v>
-      </c>
-    </row>
-    <row r="48" ht="27" customHeight="1">
-      <c r="C48" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D48" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E48" s="61" t="n"/>
-      <c r="F48" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G48" s="60" t="n">
-        <v>10072.6</v>
-      </c>
-      <c r="H48" s="60" t="n">
-        <v>821</v>
-      </c>
-      <c r="I48" s="60" t="n">
-        <v>866</v>
-      </c>
-      <c r="J48" s="98" t="n">
-        <v>2.574</v>
-      </c>
-    </row>
-    <row r="49" ht="27" customHeight="1">
-      <c r="C49" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D49" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E49" s="61" t="n"/>
-      <c r="F49" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G49" s="60" t="n">
-        <v>10117.1</v>
-      </c>
-      <c r="H49" s="60" t="n">
-        <v>825.5</v>
-      </c>
-      <c r="I49" s="60" t="n">
-        <v>870.5</v>
-      </c>
-      <c r="J49" s="98" t="n">
-        <v>2.4948</v>
-      </c>
-    </row>
-    <row r="50" ht="27" customHeight="1">
-      <c r="C50" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D50" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E50" s="61" t="n"/>
-      <c r="F50" s="97" t="n">
-        <v>89</v>
-      </c>
-      <c r="G50" s="60" t="n">
-        <v>4707.4</v>
-      </c>
-      <c r="H50" s="60" t="n">
-        <v>376.5385</v>
-      </c>
-      <c r="I50" s="60" t="n">
-        <v>415.0481</v>
-      </c>
-      <c r="J50" s="98" t="n">
-        <v>1.4572</v>
-      </c>
-    </row>
-    <row r="51" ht="27" customHeight="1">
-      <c r="C51" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D51" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E51" s="61" t="n"/>
-      <c r="F51" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="G51" s="60" t="n">
-        <v>322.8</v>
-      </c>
-      <c r="H51" s="60" t="n">
-        <v>33.8462</v>
-      </c>
-      <c r="I51" s="60" t="n">
-        <v>37.3077</v>
-      </c>
-      <c r="J51" s="98" t="n">
-        <v>0.131</v>
-      </c>
-    </row>
-    <row r="52" ht="27" customHeight="1">
-      <c r="C52" s="96" t="n">
-        <v>9000699450</v>
-      </c>
-      <c r="D52" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E52" s="62" t="n"/>
-      <c r="F52" s="97" t="n">
+      <c r="D52" s="62" t="n"/>
+      <c r="E52" s="94" t="n">
         <v>7</v>
       </c>
+      <c r="F52" s="60" t="n">
+        <v>367.3</v>
+      </c>
       <c r="G52" s="60" t="n">
-        <v>367.3</v>
+        <v>29.6154</v>
       </c>
       <c r="H52" s="60" t="n">
-        <v>29.6154</v>
-      </c>
-      <c r="I52" s="60" t="n">
         <v>32.6442</v>
       </c>
-      <c r="J52" s="98" t="n">
+      <c r="I52" s="95" t="n">
         <v>0.1146</v>
       </c>
     </row>
     <row r="53" ht="27" customHeight="1">
-      <c r="A53" s="99" t="n"/>
-      <c r="C53" s="55" t="inlineStr">
+      <c r="A53" s="96" t="n"/>
+      <c r="B53" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
         </is>
       </c>
+      <c r="C53" s="55" t="n"/>
       <c r="D53" s="55" t="n"/>
-      <c r="E53" s="55" t="n"/>
-      <c r="F53" s="93" t="n"/>
+      <c r="E53" s="91" t="n"/>
+      <c r="F53" s="56" t="n"/>
       <c r="G53" s="56" t="n"/>
       <c r="H53" s="56" t="n"/>
-      <c r="I53" s="56" t="n"/>
-      <c r="J53" s="90" t="n"/>
+      <c r="I53" s="90" t="n"/>
     </row>
     <row r="54" ht="27" customHeight="1">
       <c r="A54" s="55" t="n"/>
-      <c r="B54" s="89" t="n"/>
+      <c r="B54" s="55" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
       <c r="C54" s="55" t="inlineStr">
         <is>
-          <t>TOTAL:</t>
-        </is>
-      </c>
-      <c r="D54" s="55" t="inlineStr">
-        <is>
           <t>20 PALLETS</t>
         </is>
       </c>
-      <c r="E54" s="55" t="n"/>
-      <c r="F54" s="93">
+      <c r="D54" s="55" t="n"/>
+      <c r="E54" s="91">
+        <f>SUM(E23:E52)</f>
+        <v/>
+      </c>
+      <c r="F54" s="56">
         <f>SUM(F23:F52)</f>
         <v/>
       </c>
@@ -4262,14 +4200,10 @@
         <f>SUM(H23:H52)</f>
         <v/>
       </c>
-      <c r="I54" s="56">
+      <c r="I54" s="90">
         <f>SUM(I23:I52)</f>
         <v/>
       </c>
-      <c r="J54" s="90">
-        <f>SUM(J23:J52)</f>
-        <v/>
-      </c>
     </row>
     <row r="56" ht="27" customHeight="1">
       <c r="A56" s="55" t="inlineStr">
@@ -4277,490 +4211,487 @@
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B56" s="88" t="n"/>
+      <c r="B56" s="55" t="inlineStr">
+        <is>
+          <t>P.O Nº</t>
+        </is>
+      </c>
       <c r="C56" s="55" t="inlineStr">
         <is>
-          <t>P.O Nº</t>
+          <t>ITEM Nº</t>
         </is>
       </c>
       <c r="D56" s="55" t="inlineStr">
         <is>
-          <t>ITEM Nº</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="E56" s="55" t="inlineStr">
         <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="F56" s="55" t="inlineStr">
-        <is>
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="G56" s="89" t="n"/>
+      <c r="F56" s="89" t="n"/>
+      <c r="G56" s="56" t="inlineStr">
+        <is>
+          <t>N.W (kgs)</t>
+        </is>
+      </c>
       <c r="H56" s="56" t="inlineStr">
         <is>
-          <t>N.W (kgs)</t>
-        </is>
-      </c>
-      <c r="I56" s="56" t="inlineStr">
-        <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="J56" s="90" t="inlineStr">
+      <c r="I56" s="90" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
     <row r="57" ht="27" customHeight="1">
-      <c r="A57" s="91" t="n"/>
-      <c r="B57" s="92" t="n"/>
+      <c r="A57" s="62" t="n"/>
+      <c r="B57" s="62" t="n"/>
       <c r="C57" s="62" t="n"/>
       <c r="D57" s="62" t="n"/>
-      <c r="E57" s="62" t="n"/>
-      <c r="F57" s="93" t="inlineStr">
+      <c r="E57" s="91" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="G57" s="56" t="inlineStr">
+      <c r="F57" s="56" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
+      <c r="G57" s="62" t="n"/>
       <c r="H57" s="62" t="n"/>
       <c r="I57" s="62" t="n"/>
-      <c r="J57" s="62" t="n"/>
     </row>
     <row r="58" ht="27" customHeight="1">
-      <c r="A58" s="94" t="inlineStr">
+      <c r="A58" s="92" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B58" s="95" t="n"/>
-      <c r="C58" s="96" t="n">
+      <c r="B58" s="93" t="n">
         <v>9000701604</v>
       </c>
-      <c r="D58" s="96" t="inlineStr">
+      <c r="C58" s="93" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="E58" s="59" t="inlineStr">
+      <c r="D58" s="59" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="F58" s="97" t="n">
+      <c r="E58" s="94" t="n">
         <v>195</v>
       </c>
+      <c r="F58" s="60" t="n">
+        <v>10187.1</v>
+      </c>
       <c r="G58" s="60" t="n">
-        <v>10187.1</v>
+        <v>842.5</v>
       </c>
       <c r="H58" s="60" t="n">
-        <v>842.5</v>
-      </c>
-      <c r="I58" s="60" t="n">
         <v>887.5</v>
       </c>
-      <c r="J58" s="98" t="n">
+      <c r="I58" s="95" t="n">
         <v>2.6532</v>
       </c>
     </row>
     <row r="59" ht="27" customHeight="1">
-      <c r="A59" s="94" t="inlineStr">
+      <c r="A59" s="92" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B59" s="95" t="n"/>
-      <c r="C59" s="96" t="n">
+      <c r="B59" s="93" t="n">
         <v>9000701604</v>
       </c>
-      <c r="D59" s="96" t="inlineStr">
+      <c r="C59" s="93" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="E59" s="61" t="n"/>
-      <c r="F59" s="97" t="n">
+      <c r="D59" s="61" t="n"/>
+      <c r="E59" s="94" t="n">
         <v>195</v>
       </c>
+      <c r="F59" s="60" t="n">
+        <v>10219.2</v>
+      </c>
       <c r="G59" s="60" t="n">
-        <v>10219.2</v>
+        <v>846</v>
       </c>
       <c r="H59" s="60" t="n">
-        <v>846</v>
-      </c>
-      <c r="I59" s="60" t="n">
         <v>891</v>
       </c>
-      <c r="J59" s="98" t="n">
+      <c r="I59" s="95" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="60" ht="27" customHeight="1">
-      <c r="A60" s="94" t="inlineStr">
+      <c r="A60" s="92" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B60" s="95" t="n"/>
-      <c r="C60" s="96" t="n">
+      <c r="B60" s="93" t="n">
         <v>9000701604</v>
       </c>
-      <c r="D60" s="96" t="inlineStr">
+      <c r="C60" s="93" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="E60" s="61" t="n"/>
-      <c r="F60" s="97" t="n">
+      <c r="D60" s="61" t="n"/>
+      <c r="E60" s="94" t="n">
         <v>207</v>
       </c>
+      <c r="F60" s="60" t="n">
+        <v>10773.3</v>
+      </c>
       <c r="G60" s="60" t="n">
-        <v>10773.3</v>
+        <v>883.7671</v>
       </c>
       <c r="H60" s="60" t="n">
-        <v>883.7671</v>
-      </c>
-      <c r="I60" s="60" t="n">
         <v>926.3013999999999</v>
       </c>
-      <c r="J60" s="98" t="n">
+      <c r="I60" s="95" t="n">
         <v>2.8447</v>
       </c>
     </row>
     <row r="61" ht="27" customHeight="1">
-      <c r="A61" s="94" t="inlineStr">
+      <c r="A61" s="92" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B61" s="95" t="n"/>
-      <c r="C61" s="96" t="n">
+      <c r="B61" s="93" t="n">
         <v>9000701604</v>
       </c>
-      <c r="D61" s="96" t="inlineStr">
+      <c r="C61" s="93" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="E61" s="61" t="n"/>
-      <c r="F61" s="97" t="n">
+      <c r="D61" s="61" t="n"/>
+      <c r="E61" s="94" t="n">
         <v>12</v>
       </c>
+      <c r="F61" s="60" t="n">
+        <v>479.1</v>
+      </c>
       <c r="G61" s="60" t="n">
-        <v>479.1</v>
+        <v>51.2329</v>
       </c>
       <c r="H61" s="60" t="n">
-        <v>51.2329</v>
-      </c>
-      <c r="I61" s="60" t="n">
         <v>53.6986</v>
       </c>
-      <c r="J61" s="98" t="n">
+      <c r="I61" s="95" t="n">
         <v>0.1649</v>
       </c>
     </row>
     <row r="62" ht="27" customHeight="1">
-      <c r="C62" s="96" t="n">
+      <c r="B62" s="93" t="n">
         <v>9000701604</v>
       </c>
-      <c r="D62" s="96" t="inlineStr">
+      <c r="C62" s="93" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="E62" s="61" t="n"/>
-      <c r="F62" s="97" t="n">
+      <c r="D62" s="61" t="n"/>
+      <c r="E62" s="94" t="n">
         <v>195</v>
       </c>
+      <c r="F62" s="60" t="n">
+        <v>10215.8</v>
+      </c>
       <c r="G62" s="60" t="n">
-        <v>10215.8</v>
+        <v>840</v>
       </c>
       <c r="H62" s="60" t="n">
+        <v>885</v>
+      </c>
+      <c r="I62" s="95" t="n">
+        <v>2.6136</v>
+      </c>
+    </row>
+    <row r="63" ht="27" customHeight="1">
+      <c r="B63" s="93" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C63" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D63" s="61" t="n"/>
+      <c r="E63" s="94" t="n">
+        <v>195</v>
+      </c>
+      <c r="F63" s="60" t="n">
+        <v>10237.5</v>
+      </c>
+      <c r="G63" s="60" t="n">
+        <v>863.5</v>
+      </c>
+      <c r="H63" s="60" t="n">
+        <v>908.5</v>
+      </c>
+      <c r="I63" s="95" t="n">
+        <v>2.6928</v>
+      </c>
+    </row>
+    <row r="64" ht="27" customHeight="1">
+      <c r="B64" s="93" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C64" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D64" s="61" t="n"/>
+      <c r="E64" s="94" t="n">
+        <v>195</v>
+      </c>
+      <c r="F64" s="60" t="n">
+        <v>10196.1</v>
+      </c>
+      <c r="G64" s="60" t="n">
+        <v>849</v>
+      </c>
+      <c r="H64" s="60" t="n">
+        <v>894</v>
+      </c>
+      <c r="I64" s="95" t="n">
+        <v>2.6136</v>
+      </c>
+    </row>
+    <row r="65" ht="27" customHeight="1">
+      <c r="B65" s="93" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C65" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D65" s="61" t="n"/>
+      <c r="E65" s="94" t="n">
+        <v>175</v>
+      </c>
+      <c r="F65" s="60" t="n">
+        <v>9097.6</v>
+      </c>
+      <c r="G65" s="60" t="n">
+        <v>739.443</v>
+      </c>
+      <c r="H65" s="60" t="n">
+        <v>780.2461</v>
+      </c>
+      <c r="I65" s="95" t="n">
+        <v>2.3339</v>
+      </c>
+    </row>
+    <row r="66" ht="27" customHeight="1">
+      <c r="B66" s="93" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C66" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D66" s="61" t="n"/>
+      <c r="E66" s="94" t="n">
+        <v>18</v>
+      </c>
+      <c r="F66" s="60" t="n">
+        <v>726</v>
+      </c>
+      <c r="G66" s="60" t="n">
+        <v>76.057</v>
+      </c>
+      <c r="H66" s="60" t="n">
+        <v>80.2539</v>
+      </c>
+      <c r="I66" s="95" t="n">
+        <v>0.2401</v>
+      </c>
+    </row>
+    <row r="67" ht="27" customHeight="1">
+      <c r="B67" s="93" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C67" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D67" s="61" t="n"/>
+      <c r="E67" s="94" t="n">
+        <v>195</v>
+      </c>
+      <c r="F67" s="60" t="n">
+        <v>10110.4</v>
+      </c>
+      <c r="G67" s="60" t="n">
         <v>840</v>
       </c>
-      <c r="I62" s="60" t="n">
+      <c r="H67" s="60" t="n">
         <v>885</v>
       </c>
-      <c r="J62" s="98" t="n">
+      <c r="I67" s="95" t="n">
+        <v>2.574</v>
+      </c>
+    </row>
+    <row r="68" ht="27" customHeight="1">
+      <c r="B68" s="93" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C68" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D68" s="61" t="n"/>
+      <c r="E68" s="94" t="n">
+        <v>195</v>
+      </c>
+      <c r="F68" s="60" t="n">
+        <v>10165.7</v>
+      </c>
+      <c r="G68" s="60" t="n">
+        <v>844.5</v>
+      </c>
+      <c r="H68" s="60" t="n">
+        <v>889.5</v>
+      </c>
+      <c r="I68" s="95" t="n">
+        <v>2.772</v>
+      </c>
+    </row>
+    <row r="69" ht="27" customHeight="1">
+      <c r="B69" s="93" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="C69" s="93" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="D69" s="61" t="n"/>
+      <c r="E69" s="94" t="n">
+        <v>195</v>
+      </c>
+      <c r="F69" s="60" t="n">
+        <v>10222.1</v>
+      </c>
+      <c r="G69" s="60" t="n">
+        <v>843</v>
+      </c>
+      <c r="H69" s="60" t="n">
+        <v>888</v>
+      </c>
+      <c r="I69" s="95" t="n">
         <v>2.6136</v>
       </c>
     </row>
-    <row r="63" ht="27" customHeight="1">
-      <c r="C63" s="96" t="n">
-        <v>9000701604</v>
-      </c>
-      <c r="D63" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E63" s="61" t="n"/>
-      <c r="F63" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G63" s="60" t="n">
-        <v>10237.5</v>
-      </c>
-      <c r="H63" s="60" t="n">
-        <v>863.5</v>
-      </c>
-      <c r="I63" s="60" t="n">
-        <v>908.5</v>
-      </c>
-      <c r="J63" s="98" t="n">
-        <v>2.6928</v>
-      </c>
-    </row>
-    <row r="64" ht="27" customHeight="1">
-      <c r="C64" s="96" t="n">
-        <v>9000701604</v>
-      </c>
-      <c r="D64" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E64" s="61" t="n"/>
-      <c r="F64" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G64" s="60" t="n">
-        <v>10196.1</v>
-      </c>
-      <c r="H64" s="60" t="n">
-        <v>849</v>
-      </c>
-      <c r="I64" s="60" t="n">
-        <v>894</v>
-      </c>
-      <c r="J64" s="98" t="n">
-        <v>2.6136</v>
-      </c>
-    </row>
-    <row r="65" ht="27" customHeight="1">
-      <c r="C65" s="96" t="n">
-        <v>9000701604</v>
-      </c>
-      <c r="D65" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E65" s="61" t="n"/>
-      <c r="F65" s="97" t="n">
-        <v>175</v>
-      </c>
-      <c r="G65" s="60" t="n">
-        <v>9097.6</v>
-      </c>
-      <c r="H65" s="60" t="n">
-        <v>739.443</v>
-      </c>
-      <c r="I65" s="60" t="n">
-        <v>780.2461</v>
-      </c>
-      <c r="J65" s="98" t="n">
-        <v>2.3339</v>
-      </c>
-    </row>
-    <row r="66" ht="27" customHeight="1">
-      <c r="C66" s="96" t="n">
-        <v>9000701604</v>
-      </c>
-      <c r="D66" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E66" s="61" t="n"/>
-      <c r="F66" s="97" t="n">
-        <v>18</v>
-      </c>
-      <c r="G66" s="60" t="n">
-        <v>726</v>
-      </c>
-      <c r="H66" s="60" t="n">
-        <v>76.057</v>
-      </c>
-      <c r="I66" s="60" t="n">
-        <v>80.2539</v>
-      </c>
-      <c r="J66" s="98" t="n">
-        <v>0.2401</v>
-      </c>
-    </row>
-    <row r="67" ht="27" customHeight="1">
-      <c r="C67" s="96" t="n">
-        <v>9000701604</v>
-      </c>
-      <c r="D67" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E67" s="61" t="n"/>
-      <c r="F67" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G67" s="60" t="n">
-        <v>10110.4</v>
-      </c>
-      <c r="H67" s="60" t="n">
-        <v>840</v>
-      </c>
-      <c r="I67" s="60" t="n">
-        <v>885</v>
-      </c>
-      <c r="J67" s="98" t="n">
-        <v>2.574</v>
-      </c>
-    </row>
-    <row r="68" ht="27" customHeight="1">
-      <c r="C68" s="96" t="n">
-        <v>9000701604</v>
-      </c>
-      <c r="D68" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E68" s="61" t="n"/>
-      <c r="F68" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G68" s="60" t="n">
-        <v>10165.7</v>
-      </c>
-      <c r="H68" s="60" t="n">
-        <v>844.5</v>
-      </c>
-      <c r="I68" s="60" t="n">
-        <v>889.5</v>
-      </c>
-      <c r="J68" s="98" t="n">
-        <v>2.772</v>
-      </c>
-    </row>
-    <row r="69" ht="27" customHeight="1">
-      <c r="C69" s="96" t="n">
-        <v>9000701604</v>
-      </c>
-      <c r="D69" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E69" s="61" t="n"/>
-      <c r="F69" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G69" s="60" t="n">
-        <v>10222.1</v>
-      </c>
-      <c r="H69" s="60" t="n">
-        <v>843</v>
-      </c>
-      <c r="I69" s="60" t="n">
-        <v>888</v>
-      </c>
-      <c r="J69" s="98" t="n">
-        <v>2.6136</v>
-      </c>
-    </row>
     <row r="70" ht="27" customHeight="1">
-      <c r="C70" s="96" t="inlineStr">
+      <c r="B70" s="93" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="D70" s="96" t="inlineStr">
+      <c r="C70" s="93" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="E70" s="61" t="n"/>
-      <c r="F70" s="97" t="n">
+      <c r="D70" s="61" t="n"/>
+      <c r="E70" s="94" t="n">
         <v>106</v>
       </c>
+      <c r="F70" s="60" t="n">
+        <v>5345</v>
+      </c>
       <c r="G70" s="60" t="n">
-        <v>5345</v>
+        <v>381.211</v>
       </c>
       <c r="H70" s="60" t="n">
-        <v>381.211</v>
-      </c>
-      <c r="I70" s="60" t="n">
         <v>424.9725</v>
       </c>
-      <c r="J70" s="98" t="n">
+      <c r="I70" s="95" t="n">
         <v>2.0795</v>
       </c>
     </row>
     <row r="71" ht="27" customHeight="1">
-      <c r="C71" s="96" t="inlineStr">
+      <c r="B71" s="93" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="D71" s="96" t="inlineStr">
+      <c r="C71" s="93" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="E71" s="62" t="n"/>
-      <c r="F71" s="97" t="n">
+      <c r="D71" s="62" t="n"/>
+      <c r="E71" s="94" t="n">
         <v>3</v>
       </c>
+      <c r="F71" s="60" t="n">
+        <v>121</v>
+      </c>
       <c r="G71" s="60" t="n">
-        <v>121</v>
+        <v>10.789</v>
       </c>
       <c r="H71" s="60" t="n">
-        <v>10.789</v>
-      </c>
-      <c r="I71" s="60" t="n">
         <v>12.0275</v>
       </c>
-      <c r="J71" s="98" t="n">
+      <c r="I71" s="95" t="n">
         <v>0.0589</v>
       </c>
     </row>
     <row r="72" ht="27" customHeight="1">
-      <c r="A72" s="99" t="n"/>
-      <c r="C72" s="55" t="inlineStr">
+      <c r="A72" s="96" t="n"/>
+      <c r="B72" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
         </is>
       </c>
+      <c r="C72" s="55" t="n"/>
       <c r="D72" s="55" t="n"/>
-      <c r="E72" s="55" t="n"/>
-      <c r="F72" s="93" t="n"/>
+      <c r="E72" s="91" t="n"/>
+      <c r="F72" s="56" t="n"/>
       <c r="G72" s="56" t="n"/>
       <c r="H72" s="56" t="n"/>
-      <c r="I72" s="56" t="n"/>
-      <c r="J72" s="90" t="n"/>
+      <c r="I72" s="90" t="n"/>
     </row>
     <row r="73" ht="27" customHeight="1">
       <c r="A73" s="55" t="n"/>
-      <c r="B73" s="89" t="n"/>
+      <c r="B73" s="55" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
       <c r="C73" s="55" t="inlineStr">
         <is>
-          <t>TOTAL:</t>
-        </is>
-      </c>
-      <c r="D73" s="55" t="inlineStr">
-        <is>
           <t>11 PALLETS</t>
         </is>
       </c>
-      <c r="E73" s="55" t="n"/>
-      <c r="F73" s="93">
+      <c r="D73" s="55" t="n"/>
+      <c r="E73" s="91">
+        <f>SUM(E58:E71)</f>
+        <v/>
+      </c>
+      <c r="F73" s="56">
         <f>SUM(F58:F71)</f>
         <v/>
       </c>
@@ -4772,46 +4703,42 @@
         <f>SUM(H58:H71)</f>
         <v/>
       </c>
-      <c r="I73" s="56">
+      <c r="I73" s="90">
         <f>SUM(I58:I71)</f>
         <v/>
       </c>
-      <c r="J73" s="90">
-        <f>SUM(J58:J71)</f>
+    </row>
+    <row r="74" ht="27" customHeight="1">
+      <c r="A74" s="97" t="n"/>
+      <c r="B74" s="97" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C74" s="97" t="inlineStr">
+        <is>
+          <t>31 PALLETS</t>
+        </is>
+      </c>
+      <c r="D74" s="97" t="n"/>
+      <c r="E74" s="98">
+        <f>SUM(E23:E52,E58:E71)</f>
         <v/>
       </c>
-    </row>
-    <row r="74" ht="27" customHeight="1">
-      <c r="A74" s="100" t="n"/>
-      <c r="C74" s="100" t="inlineStr">
-        <is>
-          <t>TOTAL OF:</t>
-        </is>
-      </c>
-      <c r="D74" s="100" t="inlineStr">
-        <is>
-          <t>31 PALLETS</t>
-        </is>
-      </c>
-      <c r="E74" s="100" t="n"/>
-      <c r="F74" s="101">
+      <c r="F74" s="99">
         <f>SUM(F23:F52,F58:F71)</f>
         <v/>
       </c>
-      <c r="G74" s="102">
+      <c r="G74" s="99">
         <f>SUM(G23:G52,G58:G71)</f>
         <v/>
       </c>
-      <c r="H74" s="102">
+      <c r="H74" s="99">
         <f>SUM(H23:H52,H58:H71)</f>
         <v/>
       </c>
-      <c r="I74" s="102">
+      <c r="I74" s="100">
         <f>SUM(I23:I52,I58:I71)</f>
-        <v/>
-      </c>
-      <c r="J74" s="103">
-        <f>SUM(J23:J52,J58:J71)</f>
         <v/>
       </c>
     </row>
@@ -4825,7 +4752,6 @@
       <c r="G75" s="2" t="n"/>
       <c r="H75" s="2" t="n"/>
       <c r="I75" s="2" t="n"/>
-      <c r="J75" s="2" t="n"/>
       <c r="K75" s="2" t="n"/>
       <c r="L75" s="2" t="n"/>
       <c r="M75" s="2" t="n"/>
@@ -4847,7 +4773,6 @@
       <c r="G76" s="2" t="n"/>
       <c r="H76" s="2" t="n"/>
       <c r="I76" s="2" t="n"/>
-      <c r="J76" s="2" t="n"/>
       <c r="K76" s="2" t="n"/>
       <c r="L76" s="2" t="n"/>
       <c r="M76" s="2" t="n"/>
@@ -4861,7 +4786,7 @@
     </row>
     <row r="77" ht="27" customHeight="1">
       <c r="A77" s="53" t="n"/>
-      <c r="B77" s="87" t="n"/>
+      <c r="B77" s="88" t="n"/>
       <c r="C77" s="2" t="n"/>
       <c r="D77" s="2" t="n"/>
       <c r="E77" s="2" t="n"/>
@@ -4869,7 +4794,6 @@
       <c r="G77" s="2" t="n"/>
       <c r="H77" s="2" t="n"/>
       <c r="I77" s="2" t="n"/>
-      <c r="J77" s="2" t="n"/>
       <c r="K77" s="2" t="n"/>
       <c r="L77" s="2" t="n"/>
       <c r="M77" s="2" t="n"/>
@@ -4882,20 +4806,19 @@
       <c r="T77" s="2" t="n"/>
     </row>
     <row r="78" ht="27" customHeight="1">
-      <c r="A78" s="104" t="inlineStr">
+      <c r="A78" s="101" t="inlineStr">
         <is>
           <t>Country of Original Cambodia</t>
         </is>
       </c>
-      <c r="B78" s="104" t="n"/>
-      <c r="C78" s="104" t="n"/>
+      <c r="B78" s="101" t="n"/>
+      <c r="C78" s="101" t="n"/>
       <c r="D78" s="41" t="n"/>
-      <c r="E78" s="105" t="n"/>
+      <c r="E78" s="102" t="n"/>
       <c r="F78" s="26" t="n"/>
       <c r="G78" s="26" t="n"/>
       <c r="H78" s="26" t="n"/>
       <c r="I78" s="2" t="n"/>
-      <c r="J78" s="2" t="n"/>
       <c r="K78" s="2" t="n"/>
       <c r="L78" s="2" t="n"/>
       <c r="M78" s="2" t="n"/>
@@ -4913,18 +4836,17 @@
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B79" s="106" t="inlineStr">
+      <c r="B79" s="103" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="E79" s="107" t="n"/>
-      <c r="F79" s="107" t="n"/>
-      <c r="G79" s="107" t="n"/>
+      <c r="E79" s="104" t="n"/>
+      <c r="F79" s="104" t="n"/>
+      <c r="G79" s="104" t="n"/>
       <c r="H79" s="26" t="n"/>
       <c r="I79" s="2" t="n"/>
-      <c r="J79" s="2" t="n"/>
       <c r="K79" s="2" t="n"/>
       <c r="L79" s="2" t="n"/>
       <c r="M79" s="2" t="n"/>
@@ -4937,18 +4859,17 @@
       <c r="T79" s="2" t="n"/>
     </row>
     <row r="80" ht="51.75" customHeight="1">
-      <c r="A80" s="106" t="inlineStr">
+      <c r="A80" s="103" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
                                           /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="E80" s="107" t="n"/>
-      <c r="F80" s="107" t="n"/>
-      <c r="G80" s="107" t="n"/>
-      <c r="H80" s="107" t="n"/>
+      <c r="E80" s="104" t="n"/>
+      <c r="F80" s="104" t="n"/>
+      <c r="G80" s="104" t="n"/>
+      <c r="H80" s="104" t="n"/>
       <c r="I80" s="2" t="n"/>
-      <c r="J80" s="2" t="n"/>
       <c r="K80" s="2" t="n"/>
       <c r="L80" s="2" t="n"/>
       <c r="M80" s="2" t="n"/>
@@ -4974,7 +4895,6 @@
       <c r="G81" s="50" t="n"/>
       <c r="H81" s="50" t="n"/>
       <c r="I81" s="2" t="n"/>
-      <c r="J81" s="2" t="n"/>
       <c r="K81" s="2" t="n"/>
       <c r="L81" s="2" t="n"/>
       <c r="M81" s="2" t="n"/>
@@ -5000,7 +4920,6 @@
       <c r="G82" s="50" t="n"/>
       <c r="H82" s="50" t="n"/>
       <c r="I82" s="2" t="n"/>
-      <c r="J82" s="2" t="n"/>
       <c r="K82" s="2" t="n"/>
       <c r="L82" s="2" t="n"/>
       <c r="M82" s="2" t="n"/>
@@ -5014,19 +4933,18 @@
     </row>
     <row r="83" ht="27" customHeight="1">
       <c r="A83" s="2" t="n"/>
-      <c r="B83" s="108" t="n"/>
+      <c r="B83" s="105" t="n"/>
       <c r="C83" s="2" t="n"/>
       <c r="D83" s="2" t="n"/>
       <c r="E83" s="52" t="n"/>
       <c r="F83" s="2" t="n"/>
-      <c r="G83" s="26" t="inlineStr">
+      <c r="G83" s="2" t="n"/>
+      <c r="H83" s="26" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="H83" s="52" t="n"/>
       <c r="I83" s="2" t="n"/>
-      <c r="J83" s="2" t="n"/>
       <c r="K83" s="2" t="n"/>
       <c r="L83" s="2" t="n"/>
       <c r="M83" s="2" t="n"/>
@@ -5038,88 +4956,121 @@
       <c r="S83" s="2" t="n"/>
       <c r="T83" s="2" t="n"/>
     </row>
+    <row r="84" ht="27" customHeight="1">
+      <c r="A84" s="2" t="n"/>
+      <c r="B84" s="2" t="n"/>
+      <c r="C84" s="2" t="n"/>
+      <c r="D84" s="2" t="n"/>
+      <c r="E84" s="2" t="n"/>
+      <c r="F84" s="2" t="n"/>
+      <c r="G84" s="2" t="n"/>
+      <c r="H84" s="2" t="n"/>
+      <c r="I84" s="2" t="n"/>
+      <c r="K84" s="2" t="n"/>
+      <c r="L84" s="2" t="n"/>
+      <c r="M84" s="2" t="n"/>
+      <c r="N84" s="2" t="n"/>
+      <c r="O84" s="2" t="n"/>
+      <c r="P84" s="2" t="n"/>
+      <c r="Q84" s="2" t="n"/>
+      <c r="R84" s="2" t="n"/>
+      <c r="S84" s="2" t="n"/>
+      <c r="T84" s="2" t="n"/>
+    </row>
+    <row r="85" ht="27" customHeight="1">
+      <c r="A85" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B85" s="2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C85" s="2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E85" s="52" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F85" s="52" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G85" s="52" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="H85" s="52" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I85" s="52" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="K85" s="52" t="inlineStr">
+        <is>
+          <t>J</t>
+        </is>
+      </c>
+      <c r="L85" s="2" t="n"/>
+      <c r="M85" s="2" t="n"/>
+      <c r="N85" s="2" t="n"/>
+      <c r="O85" s="2" t="n"/>
+      <c r="P85" s="2" t="n"/>
+      <c r="Q85" s="2" t="n"/>
+      <c r="R85" s="2" t="n"/>
+      <c r="S85" s="2" t="n"/>
+      <c r="T85" s="2" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="80">
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A51:B51"/>
+  <mergeCells count="31">
+    <mergeCell ref="D23:D52"/>
+    <mergeCell ref="B74"/>
+    <mergeCell ref="B72:C72"/>
     <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="D58:D71"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C74"/>
-    <mergeCell ref="E58:E71"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="E23:E52"/>
     <mergeCell ref="I56:I57"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A56:A57"/>
     <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="B54"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="B73"/>
+    <mergeCell ref="G56:G57"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C54"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="G21:G22"/>
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="J56:J57"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix the weight summary add on footer_builder
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -303,14 +303,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -343,11 +335,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -515,9 +515,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -579,7 +576,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -598,7 +595,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1682,7 +1679,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2519,225 +2516,242 @@
       </c>
     </row>
     <row r="37" ht="35" customHeight="1">
-      <c r="A37" s="63" t="n"/>
+      <c r="A37" s="54" t="n"/>
       <c r="B37" s="54" t="inlineStr">
         <is>
-          <t>HS.CODE: 4107.12.00</t>
-        </is>
-      </c>
-      <c r="C37" s="54" t="n"/>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="C37" s="54" t="inlineStr">
+        <is>
+          <t>31 PALLETS</t>
+        </is>
+      </c>
       <c r="D37" s="55" t="n"/>
-      <c r="E37" s="56" t="n"/>
+      <c r="E37" s="56">
+        <f>SUM(E22:E36)</f>
+        <v/>
+      </c>
       <c r="F37" s="56" t="n"/>
-      <c r="G37" s="56" t="n"/>
+      <c r="G37" s="56">
+        <f>SUM(G22:G36)</f>
+        <v/>
+      </c>
     </row>
     <row r="38" ht="35" customHeight="1">
       <c r="A38" s="54" t="n"/>
       <c r="B38" s="54" t="inlineStr">
         <is>
-          <t>TOTAL:</t>
-        </is>
-      </c>
-      <c r="C38" s="54" t="inlineStr">
-        <is>
-          <t>31 PALLETS</t>
-        </is>
+          <t>NW(KGS)</t>
+        </is>
+      </c>
+      <c r="C38" s="56" t="n">
+        <v>14811.5001</v>
       </c>
       <c r="D38" s="55" t="n"/>
-      <c r="E38" s="56">
-        <f>SUM(E22:E36)</f>
-        <v/>
-      </c>
+      <c r="E38" s="56" t="n"/>
       <c r="F38" s="56" t="n"/>
-      <c r="G38" s="56">
-        <f>SUM(G22:G36)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" ht="61.5" customHeight="1">
-      <c r="A39" s="64" t="inlineStr">
+      <c r="G38" s="56" t="n"/>
+    </row>
+    <row r="39" ht="35" customHeight="1">
+      <c r="A39" s="54" t="n"/>
+      <c r="B39" s="54" t="inlineStr">
+        <is>
+          <t>GW(KGS):</t>
+        </is>
+      </c>
+      <c r="C39" s="56" t="n">
+        <v>15711.5</v>
+      </c>
+      <c r="D39" s="55" t="n"/>
+      <c r="E39" s="56" t="n"/>
+      <c r="F39" s="56" t="n"/>
+      <c r="G39" s="56" t="n"/>
+    </row>
+    <row r="40" ht="61.5" customHeight="1">
+      <c r="A40" s="63" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B39" s="65" t="inlineStr">
+      <c r="B40" s="64" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D39" s="65" t="n"/>
-      <c r="E39" s="65" t="n"/>
-      <c r="F39" s="32" t="n"/>
-      <c r="G39" s="26" t="n"/>
-      <c r="H39" s="2" t="n"/>
-      <c r="I39" s="2" t="n"/>
-      <c r="J39" s="2" t="n"/>
-      <c r="K39" s="2" t="n"/>
-      <c r="L39" s="66" t="n"/>
-      <c r="M39" s="67" t="n"/>
-      <c r="N39" s="68" t="n"/>
-      <c r="O39" s="68" t="n"/>
-    </row>
-    <row r="40" ht="42" customHeight="1">
-      <c r="A40" s="69" t="inlineStr">
-        <is>
-          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
-                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-      <c r="D40" s="69" t="n"/>
-      <c r="E40" s="69" t="n"/>
-      <c r="F40" s="69" t="n"/>
+      <c r="D40" s="64" t="n"/>
+      <c r="E40" s="64" t="n"/>
+      <c r="F40" s="32" t="n"/>
       <c r="G40" s="26" t="n"/>
       <c r="H40" s="2" t="n"/>
       <c r="I40" s="2" t="n"/>
       <c r="J40" s="2" t="n"/>
       <c r="K40" s="2" t="n"/>
-      <c r="L40" s="66" t="n"/>
-      <c r="M40" s="67" t="n"/>
-      <c r="N40" s="68" t="n"/>
-      <c r="O40" s="68" t="n"/>
-    </row>
-    <row r="41" ht="24.75" customHeight="1">
-      <c r="A41" s="70" t="inlineStr">
-        <is>
-          <t>A/C NO:100001100764430</t>
-        </is>
-      </c>
+      <c r="L40" s="65" t="n"/>
+      <c r="M40" s="66" t="n"/>
+      <c r="N40" s="67" t="n"/>
+      <c r="O40" s="67" t="n"/>
+    </row>
+    <row r="41" ht="42" customHeight="1">
+      <c r="A41" s="68" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="D41" s="68" t="n"/>
+      <c r="E41" s="68" t="n"/>
+      <c r="F41" s="68" t="n"/>
+      <c r="G41" s="26" t="n"/>
       <c r="H41" s="2" t="n"/>
       <c r="I41" s="2" t="n"/>
       <c r="J41" s="2" t="n"/>
       <c r="K41" s="2" t="n"/>
-      <c r="L41" s="66" t="n"/>
-      <c r="M41" s="67" t="n"/>
-      <c r="N41" s="68" t="n"/>
-      <c r="O41" s="68" t="n"/>
-    </row>
-    <row r="42" ht="27" customHeight="1">
-      <c r="A42" s="70" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+      <c r="L41" s="65" t="n"/>
+      <c r="M41" s="66" t="n"/>
+      <c r="N41" s="67" t="n"/>
+      <c r="O41" s="67" t="n"/>
+    </row>
+    <row r="42" ht="24.75" customHeight="1">
+      <c r="A42" s="69" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
         </is>
       </c>
       <c r="H42" s="2" t="n"/>
       <c r="I42" s="2" t="n"/>
       <c r="J42" s="2" t="n"/>
       <c r="K42" s="2" t="n"/>
-      <c r="L42" s="66" t="n"/>
-      <c r="M42" s="67" t="n"/>
-      <c r="N42" s="68" t="n"/>
-      <c r="O42" s="68" t="n"/>
-    </row>
-    <row r="43" ht="61.5" customHeight="1">
-      <c r="A43" s="2" t="n"/>
-      <c r="B43" s="2" t="n"/>
-      <c r="C43" s="2" t="n"/>
-      <c r="D43" s="2" t="n"/>
-      <c r="E43" s="71" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
-      <c r="F43" s="71" t="n"/>
-      <c r="G43" s="71" t="n"/>
-      <c r="H43" s="71" t="n"/>
+      <c r="L42" s="65" t="n"/>
+      <c r="M42" s="66" t="n"/>
+      <c r="N42" s="67" t="n"/>
+      <c r="O42" s="67" t="n"/>
+    </row>
+    <row r="43" ht="27" customHeight="1">
+      <c r="A43" s="69" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="H43" s="2" t="n"/>
       <c r="I43" s="2" t="n"/>
       <c r="J43" s="2" t="n"/>
       <c r="K43" s="2" t="n"/>
-      <c r="L43" s="66" t="n"/>
-      <c r="M43" s="67" t="n"/>
-      <c r="N43" s="68" t="n"/>
-      <c r="O43" s="68" t="n"/>
-    </row>
-    <row r="44" ht="42" customHeight="1">
+      <c r="L43" s="65" t="n"/>
+      <c r="M43" s="66" t="n"/>
+      <c r="N43" s="67" t="n"/>
+      <c r="O43" s="67" t="n"/>
+    </row>
+    <row r="44" ht="61.5" customHeight="1">
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="2" t="n"/>
       <c r="C44" s="2" t="n"/>
-      <c r="D44" s="72" t="n"/>
-      <c r="E44" s="73" t="n"/>
-      <c r="F44" s="74" t="inlineStr">
-        <is>
-          <t>Sign &amp; Stamp</t>
-        </is>
-      </c>
-      <c r="G44" s="75" t="n"/>
-      <c r="H44" s="2" t="n"/>
+      <c r="D44" s="2" t="n"/>
+      <c r="E44" s="70" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="F44" s="70" t="n"/>
+      <c r="G44" s="70" t="n"/>
+      <c r="H44" s="70" t="n"/>
       <c r="I44" s="2" t="n"/>
       <c r="J44" s="2" t="n"/>
       <c r="K44" s="2" t="n"/>
-      <c r="L44" s="66" t="n"/>
-      <c r="M44" s="67" t="n"/>
-      <c r="N44" s="68" t="n"/>
-      <c r="O44" s="68" t="n"/>
-    </row>
-    <row r="45" ht="24.75" customHeight="1">
+      <c r="L44" s="65" t="n"/>
+      <c r="M44" s="66" t="n"/>
+      <c r="N44" s="67" t="n"/>
+      <c r="O44" s="67" t="n"/>
+    </row>
+    <row r="45" ht="42" customHeight="1">
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="n"/>
       <c r="C45" s="2" t="n"/>
-      <c r="D45" s="72" t="n"/>
-      <c r="E45" s="73" t="n"/>
-      <c r="F45" s="73" t="n"/>
-      <c r="G45" s="75" t="n"/>
+      <c r="D45" s="71" t="n"/>
+      <c r="E45" s="72" t="n"/>
+      <c r="F45" s="73" t="inlineStr">
+        <is>
+          <t>Sign &amp; Stamp</t>
+        </is>
+      </c>
+      <c r="G45" s="74" t="n"/>
       <c r="H45" s="2" t="n"/>
       <c r="I45" s="2" t="n"/>
       <c r="J45" s="2" t="n"/>
       <c r="K45" s="2" t="n"/>
-      <c r="L45" s="66" t="n"/>
-      <c r="M45" s="67" t="n"/>
-      <c r="N45" s="68" t="n"/>
-      <c r="O45" s="68" t="n"/>
-    </row>
-    <row r="46" ht="27" customHeight="1">
+      <c r="L45" s="65" t="n"/>
+      <c r="M45" s="66" t="n"/>
+      <c r="N45" s="67" t="n"/>
+      <c r="O45" s="67" t="n"/>
+    </row>
+    <row r="46" ht="24.75" customHeight="1">
       <c r="A46" s="2" t="n"/>
       <c r="B46" s="2" t="n"/>
       <c r="C46" s="2" t="n"/>
-      <c r="D46" s="72" t="n"/>
-      <c r="E46" s="73" t="n"/>
-      <c r="F46" s="73" t="n"/>
-      <c r="G46" s="75" t="n"/>
+      <c r="D46" s="71" t="n"/>
+      <c r="E46" s="72" t="n"/>
+      <c r="F46" s="72" t="n"/>
+      <c r="G46" s="74" t="n"/>
       <c r="H46" s="2" t="n"/>
       <c r="I46" s="2" t="n"/>
       <c r="J46" s="2" t="n"/>
       <c r="K46" s="2" t="n"/>
-      <c r="L46" s="66" t="n"/>
-      <c r="M46" s="67" t="n"/>
-      <c r="N46" s="68" t="n"/>
-      <c r="O46" s="68" t="n"/>
-    </row>
-    <row r="47" ht="21" customHeight="1">
+      <c r="L46" s="65" t="n"/>
+      <c r="M46" s="66" t="n"/>
+      <c r="N46" s="67" t="n"/>
+      <c r="O46" s="67" t="n"/>
+    </row>
+    <row r="47" ht="27" customHeight="1">
       <c r="A47" s="2" t="n"/>
       <c r="B47" s="2" t="n"/>
       <c r="C47" s="2" t="n"/>
-      <c r="D47" s="72" t="n"/>
-      <c r="E47" s="73" t="n"/>
-      <c r="F47" s="76" t="inlineStr">
-        <is>
-          <t>ZENG XUELI</t>
-        </is>
-      </c>
-      <c r="G47" s="76" t="n"/>
+      <c r="D47" s="71" t="n"/>
+      <c r="E47" s="72" t="n"/>
+      <c r="F47" s="72" t="n"/>
+      <c r="G47" s="74" t="n"/>
       <c r="H47" s="2" t="n"/>
       <c r="I47" s="2" t="n"/>
       <c r="J47" s="2" t="n"/>
       <c r="K47" s="2" t="n"/>
-      <c r="L47" s="66" t="n"/>
-      <c r="M47" s="67" t="n"/>
-      <c r="N47" s="68" t="n"/>
-      <c r="O47" s="68" t="n"/>
+      <c r="L47" s="65" t="n"/>
+      <c r="M47" s="66" t="n"/>
+      <c r="N47" s="67" t="n"/>
+      <c r="O47" s="67" t="n"/>
+    </row>
+    <row r="48" ht="21" customHeight="1">
+      <c r="A48" s="2" t="n"/>
+      <c r="B48" s="2" t="n"/>
+      <c r="C48" s="2" t="n"/>
+      <c r="D48" s="71" t="n"/>
+      <c r="E48" s="72" t="n"/>
+      <c r="F48" s="75" t="inlineStr">
+        <is>
+          <t>ZENG XUELI</t>
+        </is>
+      </c>
+      <c r="G48" s="75" t="n"/>
+      <c r="H48" s="2" t="n"/>
+      <c r="I48" s="2" t="n"/>
+      <c r="J48" s="2" t="n"/>
+      <c r="K48" s="2" t="n"/>
+      <c r="L48" s="65" t="n"/>
+      <c r="M48" s="66" t="n"/>
+      <c r="N48" s="67" t="n"/>
+      <c r="O48" s="67" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A41:C41"/>
     <mergeCell ref="D22:D36"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A42:G42"/>
-    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A43:G43"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2900,7 +2914,7 @@
     </row>
     <row r="7" ht="18" customHeight="1">
       <c r="A7" s="32" t="n"/>
-      <c r="B7" s="77" t="n"/>
+      <c r="B7" s="76" t="n"/>
       <c r="C7" s="32" t="n"/>
       <c r="D7" s="32" t="n"/>
       <c r="E7" s="26" t="n"/>
@@ -2911,7 +2925,7 @@
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="I7" s="78" t="inlineStr">
+      <c r="I7" s="77" t="inlineStr">
         <is>
           <t>CLF2025-150</t>
         </is>
@@ -2933,7 +2947,7 @@
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="79" t="inlineStr">
+      <c r="B8" s="78" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
@@ -2948,7 +2962,7 @@
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="I8" s="80" t="inlineStr">
+      <c r="I8" s="79" t="inlineStr">
         <is>
           <t>JF25027</t>
         </is>
@@ -2966,7 +2980,7 @@
     </row>
     <row r="9" ht="21" customHeight="1">
       <c r="A9" s="32" t="n"/>
-      <c r="B9" s="77" t="inlineStr">
+      <c r="B9" s="76" t="inlineStr">
         <is>
           <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages,</t>
         </is>
@@ -2999,7 +3013,7 @@
     </row>
     <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="32" t="n"/>
-      <c r="B10" s="77" t="inlineStr">
+      <c r="B10" s="76" t="inlineStr">
         <is>
           <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
         </is>
@@ -3014,7 +3028,7 @@
           <t>DAF :</t>
         </is>
       </c>
-      <c r="I10" s="81" t="inlineStr">
+      <c r="I10" s="80" t="inlineStr">
         <is>
           <t>BAVET</t>
         </is>
@@ -3032,7 +3046,7 @@
     </row>
     <row r="11" ht="20.25" customHeight="1">
       <c r="A11" s="32" t="n"/>
-      <c r="B11" s="77" t="inlineStr">
+      <c r="B11" s="76" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
@@ -3057,7 +3071,7 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="n"/>
-      <c r="B12" s="77" t="n"/>
+      <c r="B12" s="76" t="n"/>
       <c r="C12" s="32" t="n"/>
       <c r="D12" s="32" t="n"/>
       <c r="E12" s="32" t="n"/>
@@ -3066,7 +3080,7 @@
       <c r="H12" s="26" t="n"/>
       <c r="I12" s="26" t="n"/>
       <c r="K12" s="26" t="n"/>
-      <c r="L12" s="82" t="n"/>
+      <c r="L12" s="81" t="n"/>
       <c r="M12" s="2" t="n"/>
       <c r="N12" s="2" t="n"/>
       <c r="O12" s="2" t="n"/>
@@ -3082,7 +3096,7 @@
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="83" t="inlineStr">
+      <c r="B13" s="82" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
@@ -3090,9 +3104,9 @@
       <c r="C13" s="2" t="n"/>
       <c r="D13" s="2" t="n"/>
       <c r="E13" s="2" t="n"/>
-      <c r="F13" s="84" t="n"/>
-      <c r="G13" s="84" t="n"/>
-      <c r="H13" s="84" t="n"/>
+      <c r="F13" s="83" t="n"/>
+      <c r="G13" s="83" t="n"/>
+      <c r="H13" s="83" t="n"/>
       <c r="I13" s="45" t="n"/>
       <c r="K13" s="2" t="n"/>
       <c r="L13" s="2" t="n"/>
@@ -3107,17 +3121,17 @@
     </row>
     <row r="14" ht="25.5" customHeight="1">
       <c r="A14" s="32" t="n"/>
-      <c r="B14" s="85" t="inlineStr">
+      <c r="B14" s="84" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
       <c r="C14" s="47" t="n"/>
       <c r="D14" s="47" t="n"/>
-      <c r="E14" s="86" t="n"/>
-      <c r="F14" s="86" t="n"/>
-      <c r="G14" s="86" t="n"/>
-      <c r="H14" s="86" t="n"/>
+      <c r="E14" s="85" t="n"/>
+      <c r="F14" s="85" t="n"/>
+      <c r="G14" s="85" t="n"/>
+      <c r="H14" s="85" t="n"/>
       <c r="I14" s="2" t="n"/>
       <c r="K14" s="2" t="n"/>
       <c r="L14" s="2" t="n"/>
@@ -3132,7 +3146,7 @@
     </row>
     <row r="15" ht="21" customHeight="1">
       <c r="A15" s="32" t="n"/>
-      <c r="B15" s="87" t="inlineStr">
+      <c r="B15" s="86" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
         </is>
@@ -3236,7 +3250,7 @@
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B19" s="77" t="inlineStr">
+      <c r="B19" s="76" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
         </is>
@@ -3261,7 +3275,7 @@
     </row>
     <row r="20" ht="27.75" customHeight="1">
       <c r="A20" s="53" t="n"/>
-      <c r="B20" s="88" t="n"/>
+      <c r="B20" s="87" t="n"/>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
@@ -3306,7 +3320,7 @@
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F21" s="89" t="n"/>
+      <c r="F21" s="88" t="n"/>
       <c r="G21" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -3317,7 +3331,7 @@
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I21" s="90" t="inlineStr">
+      <c r="I21" s="89" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
@@ -3328,7 +3342,7 @@
       <c r="B22" s="62" t="n"/>
       <c r="C22" s="62" t="n"/>
       <c r="D22" s="62" t="n"/>
-      <c r="E22" s="91" t="inlineStr">
+      <c r="E22" s="90" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
@@ -3343,17 +3357,17 @@
       <c r="I22" s="62" t="n"/>
     </row>
     <row r="23" ht="27" customHeight="1">
-      <c r="A23" s="92" t="inlineStr">
+      <c r="A23" s="91" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B23" s="93" t="inlineStr">
+      <c r="B23" s="92" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="C23" s="93" t="inlineStr">
+      <c r="C23" s="92" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
@@ -3363,7 +3377,7 @@
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E23" s="94" t="n">
+      <c r="E23" s="93" t="n">
         <v>122</v>
       </c>
       <c r="F23" s="60" t="n">
@@ -3375,28 +3389,28 @@
       <c r="H23" s="60" t="n">
         <v>512.1048</v>
       </c>
-      <c r="I23" s="95" t="n">
+      <c r="I23" s="94" t="n">
         <v>1.8312</v>
       </c>
     </row>
     <row r="24" ht="27" customHeight="1">
-      <c r="A24" s="92" t="inlineStr">
+      <c r="A24" s="91" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B24" s="93" t="inlineStr">
+      <c r="B24" s="92" t="inlineStr">
         <is>
           <t>9000675121</t>
         </is>
       </c>
-      <c r="C24" s="93" t="inlineStr">
+      <c r="C24" s="92" t="inlineStr">
         <is>
           <t>01.10.W653191</t>
         </is>
       </c>
       <c r="D24" s="61" t="n"/>
-      <c r="E24" s="94" t="n">
+      <c r="E24" s="93" t="n">
         <v>2</v>
       </c>
       <c r="F24" s="60" t="n">
@@ -3408,28 +3422,28 @@
       <c r="H24" s="60" t="n">
         <v>8.395200000000001</v>
       </c>
-      <c r="I24" s="95" t="n">
+      <c r="I24" s="94" t="n">
         <v>0.03</v>
       </c>
     </row>
     <row r="25" ht="27" customHeight="1">
-      <c r="A25" s="92" t="inlineStr">
+      <c r="A25" s="91" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B25" s="93" t="inlineStr">
+      <c r="B25" s="92" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C25" s="93" t="inlineStr">
+      <c r="C25" s="92" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
       <c r="D25" s="61" t="n"/>
-      <c r="E25" s="94" t="n">
+      <c r="E25" s="93" t="n">
         <v>190</v>
       </c>
       <c r="F25" s="60" t="n">
@@ -3441,28 +3455,28 @@
       <c r="H25" s="60" t="n">
         <v>802</v>
       </c>
-      <c r="I25" s="95" t="n">
+      <c r="I25" s="94" t="n">
         <v>2.4552</v>
       </c>
     </row>
     <row r="26" ht="27" customHeight="1">
-      <c r="A26" s="92" t="inlineStr">
+      <c r="A26" s="91" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B26" s="93" t="inlineStr">
+      <c r="B26" s="92" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C26" s="93" t="inlineStr">
+      <c r="C26" s="92" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
       <c r="D26" s="61" t="n"/>
-      <c r="E26" s="94" t="n">
+      <c r="E26" s="93" t="n">
         <v>208</v>
       </c>
       <c r="F26" s="60" t="n">
@@ -3474,23 +3488,23 @@
       <c r="H26" s="60" t="n">
         <v>885.9439</v>
       </c>
-      <c r="I26" s="95" t="n">
+      <c r="I26" s="94" t="n">
         <v>2.6943</v>
       </c>
     </row>
     <row r="27" ht="27" customHeight="1">
-      <c r="B27" s="93" t="inlineStr">
+      <c r="B27" s="92" t="inlineStr">
         <is>
           <t>9000678762</t>
         </is>
       </c>
-      <c r="C27" s="93" t="inlineStr">
+      <c r="C27" s="92" t="inlineStr">
         <is>
           <t>01.10.U756071</t>
         </is>
       </c>
       <c r="D27" s="61" t="n"/>
-      <c r="E27" s="94" t="n">
+      <c r="E27" s="93" t="n">
         <v>6</v>
       </c>
       <c r="F27" s="60" t="n">
@@ -3502,21 +3516,21 @@
       <c r="H27" s="60" t="n">
         <v>25.5561</v>
       </c>
-      <c r="I27" s="95" t="n">
+      <c r="I27" s="94" t="n">
         <v>0.07770000000000001</v>
       </c>
     </row>
     <row r="28" ht="27" customHeight="1">
-      <c r="B28" s="93" t="n">
+      <c r="B28" s="92" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C28" s="93" t="inlineStr">
+      <c r="C28" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
       <c r="D28" s="61" t="n"/>
-      <c r="E28" s="94" t="n">
+      <c r="E28" s="93" t="n">
         <v>154</v>
       </c>
       <c r="F28" s="60" t="n">
@@ -3528,21 +3542,21 @@
       <c r="H28" s="60" t="n">
         <v>658.0814</v>
       </c>
-      <c r="I28" s="95" t="n">
+      <c r="I28" s="94" t="n">
         <v>2.0564</v>
       </c>
     </row>
     <row r="29" ht="27" customHeight="1">
-      <c r="B29" s="93" t="n">
+      <c r="B29" s="92" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C29" s="93" t="inlineStr">
+      <c r="C29" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
       <c r="D29" s="61" t="n"/>
-      <c r="E29" s="94" t="n">
+      <c r="E29" s="93" t="n">
         <v>18</v>
       </c>
       <c r="F29" s="60" t="n">
@@ -3554,21 +3568,21 @@
       <c r="H29" s="60" t="n">
         <v>76.9186</v>
       </c>
-      <c r="I29" s="95" t="n">
+      <c r="I29" s="94" t="n">
         <v>0.2404</v>
       </c>
     </row>
     <row r="30" ht="27" customHeight="1">
-      <c r="B30" s="93" t="n">
+      <c r="B30" s="92" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C30" s="93" t="inlineStr">
+      <c r="C30" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
       <c r="D30" s="61" t="n"/>
-      <c r="E30" s="94" t="n">
+      <c r="E30" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F30" s="60" t="n">
@@ -3580,21 +3594,21 @@
       <c r="H30" s="60" t="n">
         <v>859.5</v>
       </c>
-      <c r="I30" s="95" t="n">
+      <c r="I30" s="94" t="n">
         <v>2.376</v>
       </c>
     </row>
     <row r="31" ht="27" customHeight="1">
-      <c r="B31" s="93" t="n">
+      <c r="B31" s="92" t="n">
         <v>9000697761</v>
       </c>
-      <c r="C31" s="93" t="inlineStr">
+      <c r="C31" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
       <c r="D31" s="61" t="n"/>
-      <c r="E31" s="94" t="n">
+      <c r="E31" s="93" t="n">
         <v>200</v>
       </c>
       <c r="F31" s="60" t="n">
@@ -3606,21 +3620,21 @@
       <c r="H31" s="60" t="n">
         <v>780.1762</v>
       </c>
-      <c r="I31" s="95" t="n">
+      <c r="I31" s="94" t="n">
         <v>2.2678</v>
       </c>
     </row>
     <row r="32" ht="27" customHeight="1">
-      <c r="B32" s="93" t="n">
+      <c r="B32" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C32" s="93" t="inlineStr">
+      <c r="C32" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
       <c r="D32" s="61" t="n"/>
-      <c r="E32" s="94" t="n">
+      <c r="E32" s="93" t="n">
         <v>27</v>
       </c>
       <c r="F32" s="60" t="n">
@@ -3632,21 +3646,21 @@
       <c r="H32" s="60" t="n">
         <v>105.3238</v>
       </c>
-      <c r="I32" s="95" t="n">
+      <c r="I32" s="94" t="n">
         <v>0.3062</v>
       </c>
     </row>
     <row r="33" ht="27" customHeight="1">
-      <c r="B33" s="93" t="n">
+      <c r="B33" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C33" s="93" t="inlineStr">
+      <c r="C33" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
       <c r="D33" s="61" t="n"/>
-      <c r="E33" s="94" t="n">
+      <c r="E33" s="93" t="n">
         <v>169</v>
       </c>
       <c r="F33" s="60" t="n">
@@ -3658,21 +3672,21 @@
       <c r="H33" s="60" t="n">
         <v>736.84</v>
       </c>
-      <c r="I33" s="95" t="n">
+      <c r="I33" s="94" t="n">
         <v>2.2181</v>
       </c>
     </row>
     <row r="34" ht="27" customHeight="1">
-      <c r="B34" s="93" t="n">
+      <c r="B34" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C34" s="93" t="inlineStr">
+      <c r="C34" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
       <c r="D34" s="61" t="n"/>
-      <c r="E34" s="94" t="n">
+      <c r="E34" s="93" t="n">
         <v>6</v>
       </c>
       <c r="F34" s="60" t="n">
@@ -3684,21 +3698,21 @@
       <c r="H34" s="60" t="n">
         <v>26.16</v>
       </c>
-      <c r="I34" s="95" t="n">
+      <c r="I34" s="94" t="n">
         <v>0.07870000000000001</v>
       </c>
     </row>
     <row r="35" ht="27" customHeight="1">
-      <c r="B35" s="93" t="n">
+      <c r="B35" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C35" s="93" t="inlineStr">
+      <c r="C35" s="92" t="inlineStr">
         <is>
           <t>01.10.U528062</t>
         </is>
       </c>
       <c r="D35" s="61" t="n"/>
-      <c r="E35" s="94" t="n">
+      <c r="E35" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F35" s="60" t="n">
@@ -3710,21 +3724,21 @@
       <c r="H35" s="60" t="n">
         <v>859.5</v>
       </c>
-      <c r="I35" s="95" t="n">
+      <c r="I35" s="94" t="n">
         <v>2.376</v>
       </c>
     </row>
     <row r="36" ht="27" customHeight="1">
-      <c r="B36" s="93" t="n">
+      <c r="B36" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C36" s="93" t="inlineStr">
+      <c r="C36" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D36" s="61" t="n"/>
-      <c r="E36" s="94" t="n">
+      <c r="E36" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F36" s="60" t="n">
@@ -3736,21 +3750,21 @@
       <c r="H36" s="60" t="n">
         <v>875.5</v>
       </c>
-      <c r="I36" s="95" t="n">
+      <c r="I36" s="94" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="37" ht="27" customHeight="1">
-      <c r="B37" s="93" t="n">
+      <c r="B37" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C37" s="93" t="inlineStr">
+      <c r="C37" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D37" s="61" t="n"/>
-      <c r="E37" s="94" t="n">
+      <c r="E37" s="93" t="n">
         <v>215</v>
       </c>
       <c r="F37" s="60" t="n">
@@ -3762,21 +3776,21 @@
       <c r="H37" s="60" t="n">
         <v>946.5</v>
       </c>
-      <c r="I37" s="95" t="n">
+      <c r="I37" s="94" t="n">
         <v>2.97</v>
       </c>
     </row>
     <row r="38" ht="27" customHeight="1">
-      <c r="B38" s="93" t="n">
+      <c r="B38" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C38" s="93" t="inlineStr">
+      <c r="C38" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D38" s="61" t="n"/>
-      <c r="E38" s="94" t="n">
+      <c r="E38" s="93" t="n">
         <v>215</v>
       </c>
       <c r="F38" s="60" t="n">
@@ -3788,21 +3802,21 @@
       <c r="H38" s="60" t="n">
         <v>963</v>
       </c>
-      <c r="I38" s="95" t="n">
+      <c r="I38" s="94" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="39" ht="27" customHeight="1">
-      <c r="B39" s="93" t="n">
+      <c r="B39" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C39" s="93" t="inlineStr">
+      <c r="C39" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D39" s="61" t="n"/>
-      <c r="E39" s="94" t="n">
+      <c r="E39" s="93" t="n">
         <v>192</v>
       </c>
       <c r="F39" s="60" t="n">
@@ -3814,21 +3828,21 @@
       <c r="H39" s="60" t="n">
         <v>836.9709</v>
       </c>
-      <c r="I39" s="95" t="n">
+      <c r="I39" s="94" t="n">
         <v>2.4729</v>
       </c>
     </row>
     <row r="40" ht="27" customHeight="1">
-      <c r="B40" s="93" t="n">
+      <c r="B40" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C40" s="93" t="inlineStr">
+      <c r="C40" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D40" s="61" t="n"/>
-      <c r="E40" s="94" t="n">
+      <c r="E40" s="93" t="n">
         <v>14</v>
       </c>
       <c r="F40" s="60" t="n">
@@ -3840,21 +3854,21 @@
       <c r="H40" s="60" t="n">
         <v>61.0291</v>
       </c>
-      <c r="I40" s="95" t="n">
+      <c r="I40" s="94" t="n">
         <v>0.1803</v>
       </c>
     </row>
     <row r="41" ht="27" customHeight="1">
-      <c r="B41" s="93" t="n">
+      <c r="B41" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C41" s="93" t="inlineStr">
+      <c r="C41" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D41" s="61" t="n"/>
-      <c r="E41" s="94" t="n">
+      <c r="E41" s="93" t="n">
         <v>97</v>
       </c>
       <c r="F41" s="60" t="n">
@@ -3866,21 +3880,21 @@
       <c r="H41" s="60" t="n">
         <v>453</v>
       </c>
-      <c r="I41" s="95" t="n">
+      <c r="I41" s="94" t="n">
         <v>1.782</v>
       </c>
     </row>
     <row r="42" ht="27" customHeight="1">
-      <c r="B42" s="93" t="n">
+      <c r="B42" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C42" s="93" t="inlineStr">
+      <c r="C42" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D42" s="61" t="n"/>
-      <c r="E42" s="94" t="n">
+      <c r="E42" s="93" t="n">
         <v>97</v>
       </c>
       <c r="F42" s="60" t="n">
@@ -3892,21 +3906,21 @@
       <c r="H42" s="60" t="n">
         <v>452</v>
       </c>
-      <c r="I42" s="95" t="n">
+      <c r="I42" s="94" t="n">
         <v>1.8216</v>
       </c>
     </row>
     <row r="43" ht="27" customHeight="1">
-      <c r="B43" s="93" t="n">
+      <c r="B43" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C43" s="93" t="inlineStr">
+      <c r="C43" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D43" s="61" t="n"/>
-      <c r="E43" s="94" t="n">
+      <c r="E43" s="93" t="n">
         <v>184</v>
       </c>
       <c r="F43" s="60" t="n">
@@ -3918,21 +3932,21 @@
       <c r="H43" s="60" t="n">
         <v>817.3474</v>
       </c>
-      <c r="I43" s="95" t="n">
+      <c r="I43" s="94" t="n">
         <v>2.6461</v>
       </c>
     </row>
     <row r="44" ht="27" customHeight="1">
-      <c r="B44" s="93" t="n">
+      <c r="B44" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C44" s="93" t="inlineStr">
+      <c r="C44" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D44" s="61" t="n"/>
-      <c r="E44" s="94" t="n">
+      <c r="E44" s="93" t="n">
         <v>6</v>
       </c>
       <c r="F44" s="60" t="n">
@@ -3944,21 +3958,21 @@
       <c r="H44" s="60" t="n">
         <v>26.6526</v>
       </c>
-      <c r="I44" s="95" t="n">
+      <c r="I44" s="94" t="n">
         <v>0.0863</v>
       </c>
     </row>
     <row r="45" ht="27" customHeight="1">
-      <c r="B45" s="93" t="n">
+      <c r="B45" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C45" s="93" t="inlineStr">
+      <c r="C45" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D45" s="61" t="n"/>
-      <c r="E45" s="94" t="n">
+      <c r="E45" s="93" t="n">
         <v>185</v>
       </c>
       <c r="F45" s="60" t="n">
@@ -3970,21 +3984,21 @@
       <c r="H45" s="60" t="n">
         <v>830.0658</v>
       </c>
-      <c r="I45" s="95" t="n">
+      <c r="I45" s="94" t="n">
         <v>2.5063</v>
       </c>
     </row>
     <row r="46" ht="27" customHeight="1">
-      <c r="B46" s="93" t="n">
+      <c r="B46" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C46" s="93" t="inlineStr">
+      <c r="C46" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D46" s="61" t="n"/>
-      <c r="E46" s="94" t="n">
+      <c r="E46" s="93" t="n">
         <v>5</v>
       </c>
       <c r="F46" s="60" t="n">
@@ -3996,21 +4010,21 @@
       <c r="H46" s="60" t="n">
         <v>22.4342</v>
       </c>
-      <c r="I46" s="95" t="n">
+      <c r="I46" s="94" t="n">
         <v>0.0677</v>
       </c>
     </row>
     <row r="47" ht="27" customHeight="1">
-      <c r="B47" s="93" t="n">
+      <c r="B47" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C47" s="93" t="inlineStr">
+      <c r="C47" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D47" s="61" t="n"/>
-      <c r="E47" s="94" t="n">
+      <c r="E47" s="93" t="n">
         <v>190</v>
       </c>
       <c r="F47" s="60" t="n">
@@ -4022,21 +4036,21 @@
       <c r="H47" s="60" t="n">
         <v>869</v>
       </c>
-      <c r="I47" s="95" t="n">
+      <c r="I47" s="94" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="48" ht="27" customHeight="1">
-      <c r="B48" s="93" t="n">
+      <c r="B48" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C48" s="93" t="inlineStr">
+      <c r="C48" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D48" s="61" t="n"/>
-      <c r="E48" s="94" t="n">
+      <c r="E48" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F48" s="60" t="n">
@@ -4048,21 +4062,21 @@
       <c r="H48" s="60" t="n">
         <v>866</v>
       </c>
-      <c r="I48" s="95" t="n">
+      <c r="I48" s="94" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="49" ht="27" customHeight="1">
-      <c r="B49" s="93" t="n">
+      <c r="B49" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C49" s="93" t="inlineStr">
+      <c r="C49" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D49" s="61" t="n"/>
-      <c r="E49" s="94" t="n">
+      <c r="E49" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F49" s="60" t="n">
@@ -4074,21 +4088,21 @@
       <c r="H49" s="60" t="n">
         <v>870.5</v>
       </c>
-      <c r="I49" s="95" t="n">
+      <c r="I49" s="94" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="50" ht="27" customHeight="1">
-      <c r="B50" s="93" t="n">
+      <c r="B50" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C50" s="93" t="inlineStr">
+      <c r="C50" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D50" s="61" t="n"/>
-      <c r="E50" s="94" t="n">
+      <c r="E50" s="93" t="n">
         <v>89</v>
       </c>
       <c r="F50" s="60" t="n">
@@ -4100,21 +4114,21 @@
       <c r="H50" s="60" t="n">
         <v>415.0481</v>
       </c>
-      <c r="I50" s="95" t="n">
+      <c r="I50" s="94" t="n">
         <v>1.4572</v>
       </c>
     </row>
     <row r="51" ht="27" customHeight="1">
-      <c r="B51" s="93" t="n">
+      <c r="B51" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C51" s="93" t="inlineStr">
+      <c r="C51" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D51" s="61" t="n"/>
-      <c r="E51" s="94" t="n">
+      <c r="E51" s="93" t="n">
         <v>8</v>
       </c>
       <c r="F51" s="60" t="n">
@@ -4126,21 +4140,21 @@
       <c r="H51" s="60" t="n">
         <v>37.3077</v>
       </c>
-      <c r="I51" s="95" t="n">
+      <c r="I51" s="94" t="n">
         <v>0.131</v>
       </c>
     </row>
     <row r="52" ht="27" customHeight="1">
-      <c r="B52" s="93" t="n">
+      <c r="B52" s="92" t="n">
         <v>9000699450</v>
       </c>
-      <c r="C52" s="93" t="inlineStr">
+      <c r="C52" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D52" s="62" t="n"/>
-      <c r="E52" s="94" t="n">
+      <c r="E52" s="93" t="n">
         <v>7</v>
       </c>
       <c r="F52" s="60" t="n">
@@ -4152,12 +4166,12 @@
       <c r="H52" s="60" t="n">
         <v>32.6442</v>
       </c>
-      <c r="I52" s="95" t="n">
+      <c r="I52" s="94" t="n">
         <v>0.1146</v>
       </c>
     </row>
     <row r="53" ht="27" customHeight="1">
-      <c r="A53" s="96" t="n"/>
+      <c r="A53" s="95" t="n"/>
       <c r="B53" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
@@ -4165,11 +4179,11 @@
       </c>
       <c r="C53" s="55" t="n"/>
       <c r="D53" s="55" t="n"/>
-      <c r="E53" s="91" t="n"/>
+      <c r="E53" s="90" t="n"/>
       <c r="F53" s="56" t="n"/>
       <c r="G53" s="56" t="n"/>
       <c r="H53" s="56" t="n"/>
-      <c r="I53" s="90" t="n"/>
+      <c r="I53" s="89" t="n"/>
     </row>
     <row r="54" ht="27" customHeight="1">
       <c r="A54" s="55" t="n"/>
@@ -4184,7 +4198,7 @@
         </is>
       </c>
       <c r="D54" s="55" t="n"/>
-      <c r="E54" s="91">
+      <c r="E54" s="90">
         <f>SUM(E23:E52)</f>
         <v/>
       </c>
@@ -4200,7 +4214,7 @@
         <f>SUM(H23:H52)</f>
         <v/>
       </c>
-      <c r="I54" s="90">
+      <c r="I54" s="89">
         <f>SUM(I23:I52)</f>
         <v/>
       </c>
@@ -4231,7 +4245,7 @@
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F56" s="89" t="n"/>
+      <c r="F56" s="88" t="n"/>
       <c r="G56" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -4242,7 +4256,7 @@
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I56" s="90" t="inlineStr">
+      <c r="I56" s="89" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
@@ -4253,7 +4267,7 @@
       <c r="B57" s="62" t="n"/>
       <c r="C57" s="62" t="n"/>
       <c r="D57" s="62" t="n"/>
-      <c r="E57" s="91" t="inlineStr">
+      <c r="E57" s="90" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
@@ -4268,15 +4282,15 @@
       <c r="I57" s="62" t="n"/>
     </row>
     <row r="58" ht="27" customHeight="1">
-      <c r="A58" s="92" t="inlineStr">
+      <c r="A58" s="91" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B58" s="93" t="n">
+      <c r="B58" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C58" s="93" t="inlineStr">
+      <c r="C58" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
@@ -4286,7 +4300,7 @@
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E58" s="94" t="n">
+      <c r="E58" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F58" s="60" t="n">
@@ -4298,26 +4312,26 @@
       <c r="H58" s="60" t="n">
         <v>887.5</v>
       </c>
-      <c r="I58" s="95" t="n">
+      <c r="I58" s="94" t="n">
         <v>2.6532</v>
       </c>
     </row>
     <row r="59" ht="27" customHeight="1">
-      <c r="A59" s="92" t="inlineStr">
+      <c r="A59" s="91" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
       </c>
-      <c r="B59" s="93" t="n">
+      <c r="B59" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C59" s="93" t="inlineStr">
+      <c r="C59" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D59" s="61" t="n"/>
-      <c r="E59" s="94" t="n">
+      <c r="E59" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F59" s="60" t="n">
@@ -4329,26 +4343,26 @@
       <c r="H59" s="60" t="n">
         <v>891</v>
       </c>
-      <c r="I59" s="95" t="n">
+      <c r="I59" s="94" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="60" ht="27" customHeight="1">
-      <c r="A60" s="92" t="inlineStr">
+      <c r="A60" s="91" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
       </c>
-      <c r="B60" s="93" t="n">
+      <c r="B60" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C60" s="93" t="inlineStr">
+      <c r="C60" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D60" s="61" t="n"/>
-      <c r="E60" s="94" t="n">
+      <c r="E60" s="93" t="n">
         <v>207</v>
       </c>
       <c r="F60" s="60" t="n">
@@ -4360,26 +4374,26 @@
       <c r="H60" s="60" t="n">
         <v>926.3013999999999</v>
       </c>
-      <c r="I60" s="95" t="n">
+      <c r="I60" s="94" t="n">
         <v>2.8447</v>
       </c>
     </row>
     <row r="61" ht="27" customHeight="1">
-      <c r="A61" s="92" t="inlineStr">
+      <c r="A61" s="91" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B61" s="93" t="n">
+      <c r="B61" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C61" s="93" t="inlineStr">
+      <c r="C61" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D61" s="61" t="n"/>
-      <c r="E61" s="94" t="n">
+      <c r="E61" s="93" t="n">
         <v>12</v>
       </c>
       <c r="F61" s="60" t="n">
@@ -4391,21 +4405,21 @@
       <c r="H61" s="60" t="n">
         <v>53.6986</v>
       </c>
-      <c r="I61" s="95" t="n">
+      <c r="I61" s="94" t="n">
         <v>0.1649</v>
       </c>
     </row>
     <row r="62" ht="27" customHeight="1">
-      <c r="B62" s="93" t="n">
+      <c r="B62" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C62" s="93" t="inlineStr">
+      <c r="C62" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D62" s="61" t="n"/>
-      <c r="E62" s="94" t="n">
+      <c r="E62" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F62" s="60" t="n">
@@ -4417,21 +4431,21 @@
       <c r="H62" s="60" t="n">
         <v>885</v>
       </c>
-      <c r="I62" s="95" t="n">
+      <c r="I62" s="94" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="63" ht="27" customHeight="1">
-      <c r="B63" s="93" t="n">
+      <c r="B63" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C63" s="93" t="inlineStr">
+      <c r="C63" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D63" s="61" t="n"/>
-      <c r="E63" s="94" t="n">
+      <c r="E63" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F63" s="60" t="n">
@@ -4443,21 +4457,21 @@
       <c r="H63" s="60" t="n">
         <v>908.5</v>
       </c>
-      <c r="I63" s="95" t="n">
+      <c r="I63" s="94" t="n">
         <v>2.6928</v>
       </c>
     </row>
     <row r="64" ht="27" customHeight="1">
-      <c r="B64" s="93" t="n">
+      <c r="B64" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C64" s="93" t="inlineStr">
+      <c r="C64" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D64" s="61" t="n"/>
-      <c r="E64" s="94" t="n">
+      <c r="E64" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F64" s="60" t="n">
@@ -4469,21 +4483,21 @@
       <c r="H64" s="60" t="n">
         <v>894</v>
       </c>
-      <c r="I64" s="95" t="n">
+      <c r="I64" s="94" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="65" ht="27" customHeight="1">
-      <c r="B65" s="93" t="n">
+      <c r="B65" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C65" s="93" t="inlineStr">
+      <c r="C65" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D65" s="61" t="n"/>
-      <c r="E65" s="94" t="n">
+      <c r="E65" s="93" t="n">
         <v>175</v>
       </c>
       <c r="F65" s="60" t="n">
@@ -4495,21 +4509,21 @@
       <c r="H65" s="60" t="n">
         <v>780.2461</v>
       </c>
-      <c r="I65" s="95" t="n">
+      <c r="I65" s="94" t="n">
         <v>2.3339</v>
       </c>
     </row>
     <row r="66" ht="27" customHeight="1">
-      <c r="B66" s="93" t="n">
+      <c r="B66" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C66" s="93" t="inlineStr">
+      <c r="C66" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D66" s="61" t="n"/>
-      <c r="E66" s="94" t="n">
+      <c r="E66" s="93" t="n">
         <v>18</v>
       </c>
       <c r="F66" s="60" t="n">
@@ -4521,21 +4535,21 @@
       <c r="H66" s="60" t="n">
         <v>80.2539</v>
       </c>
-      <c r="I66" s="95" t="n">
+      <c r="I66" s="94" t="n">
         <v>0.2401</v>
       </c>
     </row>
     <row r="67" ht="27" customHeight="1">
-      <c r="B67" s="93" t="n">
+      <c r="B67" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C67" s="93" t="inlineStr">
+      <c r="C67" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D67" s="61" t="n"/>
-      <c r="E67" s="94" t="n">
+      <c r="E67" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F67" s="60" t="n">
@@ -4547,21 +4561,21 @@
       <c r="H67" s="60" t="n">
         <v>885</v>
       </c>
-      <c r="I67" s="95" t="n">
+      <c r="I67" s="94" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="68" ht="27" customHeight="1">
-      <c r="B68" s="93" t="n">
+      <c r="B68" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C68" s="93" t="inlineStr">
+      <c r="C68" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D68" s="61" t="n"/>
-      <c r="E68" s="94" t="n">
+      <c r="E68" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F68" s="60" t="n">
@@ -4573,21 +4587,21 @@
       <c r="H68" s="60" t="n">
         <v>889.5</v>
       </c>
-      <c r="I68" s="95" t="n">
+      <c r="I68" s="94" t="n">
         <v>2.772</v>
       </c>
     </row>
     <row r="69" ht="27" customHeight="1">
-      <c r="B69" s="93" t="n">
+      <c r="B69" s="92" t="n">
         <v>9000701604</v>
       </c>
-      <c r="C69" s="93" t="inlineStr">
+      <c r="C69" s="92" t="inlineStr">
         <is>
           <t>01.10.U528073</t>
         </is>
       </c>
       <c r="D69" s="61" t="n"/>
-      <c r="E69" s="94" t="n">
+      <c r="E69" s="93" t="n">
         <v>195</v>
       </c>
       <c r="F69" s="60" t="n">
@@ -4599,23 +4613,23 @@
       <c r="H69" s="60" t="n">
         <v>888</v>
       </c>
-      <c r="I69" s="95" t="n">
+      <c r="I69" s="94" t="n">
         <v>2.6136</v>
       </c>
     </row>
     <row r="70" ht="27" customHeight="1">
-      <c r="B70" s="93" t="inlineStr">
+      <c r="B70" s="92" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="C70" s="93" t="inlineStr">
+      <c r="C70" s="92" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
       <c r="D70" s="61" t="n"/>
-      <c r="E70" s="94" t="n">
+      <c r="E70" s="93" t="n">
         <v>106</v>
       </c>
       <c r="F70" s="60" t="n">
@@ -4627,23 +4641,23 @@
       <c r="H70" s="60" t="n">
         <v>424.9725</v>
       </c>
-      <c r="I70" s="95" t="n">
+      <c r="I70" s="94" t="n">
         <v>2.0795</v>
       </c>
     </row>
     <row r="71" ht="27" customHeight="1">
-      <c r="B71" s="93" t="inlineStr">
+      <c r="B71" s="92" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="C71" s="93" t="inlineStr">
+      <c r="C71" s="92" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
       <c r="D71" s="62" t="n"/>
-      <c r="E71" s="94" t="n">
+      <c r="E71" s="93" t="n">
         <v>3</v>
       </c>
       <c r="F71" s="60" t="n">
@@ -4655,12 +4669,12 @@
       <c r="H71" s="60" t="n">
         <v>12.0275</v>
       </c>
-      <c r="I71" s="95" t="n">
+      <c r="I71" s="94" t="n">
         <v>0.0589</v>
       </c>
     </row>
     <row r="72" ht="27" customHeight="1">
-      <c r="A72" s="96" t="n"/>
+      <c r="A72" s="95" t="n"/>
       <c r="B72" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
@@ -4668,11 +4682,11 @@
       </c>
       <c r="C72" s="55" t="n"/>
       <c r="D72" s="55" t="n"/>
-      <c r="E72" s="91" t="n"/>
+      <c r="E72" s="90" t="n"/>
       <c r="F72" s="56" t="n"/>
       <c r="G72" s="56" t="n"/>
       <c r="H72" s="56" t="n"/>
-      <c r="I72" s="90" t="n"/>
+      <c r="I72" s="89" t="n"/>
     </row>
     <row r="73" ht="27" customHeight="1">
       <c r="A73" s="55" t="n"/>
@@ -4687,7 +4701,7 @@
         </is>
       </c>
       <c r="D73" s="55" t="n"/>
-      <c r="E73" s="91">
+      <c r="E73" s="90">
         <f>SUM(E58:E71)</f>
         <v/>
       </c>
@@ -4703,41 +4717,41 @@
         <f>SUM(H58:H71)</f>
         <v/>
       </c>
-      <c r="I73" s="90">
+      <c r="I73" s="89">
         <f>SUM(I58:I71)</f>
         <v/>
       </c>
     </row>
     <row r="74" ht="27" customHeight="1">
-      <c r="A74" s="97" t="n"/>
-      <c r="B74" s="97" t="inlineStr">
+      <c r="A74" s="96" t="n"/>
+      <c r="B74" s="96" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="C74" s="97" t="inlineStr">
+      <c r="C74" s="96" t="inlineStr">
         <is>
           <t>31 PALLETS</t>
         </is>
       </c>
-      <c r="D74" s="97" t="n"/>
-      <c r="E74" s="98">
+      <c r="D74" s="96" t="n"/>
+      <c r="E74" s="97">
         <f>SUM(E23:E52,E58:E71)</f>
         <v/>
       </c>
-      <c r="F74" s="99">
+      <c r="F74" s="98">
         <f>SUM(F23:F52,F58:F71)</f>
         <v/>
       </c>
-      <c r="G74" s="99">
+      <c r="G74" s="98">
         <f>SUM(G23:G52,G58:G71)</f>
         <v/>
       </c>
-      <c r="H74" s="99">
+      <c r="H74" s="98">
         <f>SUM(H23:H52,H58:H71)</f>
         <v/>
       </c>
-      <c r="I74" s="100">
+      <c r="I74" s="99">
         <f>SUM(I23:I52,I58:I71)</f>
         <v/>
       </c>
@@ -4786,7 +4800,7 @@
     </row>
     <row r="77" ht="27" customHeight="1">
       <c r="A77" s="53" t="n"/>
-      <c r="B77" s="88" t="n"/>
+      <c r="B77" s="87" t="n"/>
       <c r="C77" s="2" t="n"/>
       <c r="D77" s="2" t="n"/>
       <c r="E77" s="2" t="n"/>
@@ -4806,15 +4820,15 @@
       <c r="T77" s="2" t="n"/>
     </row>
     <row r="78" ht="27" customHeight="1">
-      <c r="A78" s="101" t="inlineStr">
+      <c r="A78" s="100" t="inlineStr">
         <is>
           <t>Country of Original Cambodia</t>
         </is>
       </c>
-      <c r="B78" s="101" t="n"/>
-      <c r="C78" s="101" t="n"/>
+      <c r="B78" s="100" t="n"/>
+      <c r="C78" s="100" t="n"/>
       <c r="D78" s="41" t="n"/>
-      <c r="E78" s="102" t="n"/>
+      <c r="E78" s="101" t="n"/>
       <c r="F78" s="26" t="n"/>
       <c r="G78" s="26" t="n"/>
       <c r="H78" s="26" t="n"/>
@@ -4831,20 +4845,20 @@
       <c r="T78" s="2" t="n"/>
     </row>
     <row r="79" ht="65.25" customHeight="1">
-      <c r="A79" s="64" t="inlineStr">
+      <c r="A79" s="63" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B79" s="103" t="inlineStr">
+      <c r="B79" s="102" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="E79" s="104" t="n"/>
-      <c r="F79" s="104" t="n"/>
-      <c r="G79" s="104" t="n"/>
+      <c r="E79" s="103" t="n"/>
+      <c r="F79" s="103" t="n"/>
+      <c r="G79" s="103" t="n"/>
       <c r="H79" s="26" t="n"/>
       <c r="I79" s="2" t="n"/>
       <c r="K79" s="2" t="n"/>
@@ -4859,16 +4873,16 @@
       <c r="T79" s="2" t="n"/>
     </row>
     <row r="80" ht="51.75" customHeight="1">
-      <c r="A80" s="103" t="inlineStr">
+      <c r="A80" s="102" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
                                           /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="E80" s="104" t="n"/>
-      <c r="F80" s="104" t="n"/>
-      <c r="G80" s="104" t="n"/>
-      <c r="H80" s="104" t="n"/>
+      <c r="E80" s="103" t="n"/>
+      <c r="F80" s="103" t="n"/>
+      <c r="G80" s="103" t="n"/>
+      <c r="H80" s="103" t="n"/>
       <c r="I80" s="2" t="n"/>
       <c r="K80" s="2" t="n"/>
       <c r="L80" s="2" t="n"/>
@@ -4882,14 +4896,14 @@
       <c r="T80" s="2" t="n"/>
     </row>
     <row r="81" ht="27" customHeight="1">
-      <c r="A81" s="70" t="inlineStr">
+      <c r="A81" s="69" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
-      <c r="B81" s="70" t="n"/>
-      <c r="C81" s="70" t="n"/>
-      <c r="D81" s="70" t="n"/>
+      <c r="B81" s="69" t="n"/>
+      <c r="C81" s="69" t="n"/>
+      <c r="D81" s="69" t="n"/>
       <c r="E81" s="50" t="n"/>
       <c r="F81" s="50" t="n"/>
       <c r="G81" s="50" t="n"/>
@@ -4907,14 +4921,14 @@
       <c r="T81" s="2" t="n"/>
     </row>
     <row r="82" ht="27" customHeight="1">
-      <c r="A82" s="70" t="inlineStr">
+      <c r="A82" s="69" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
       </c>
-      <c r="B82" s="70" t="n"/>
-      <c r="C82" s="70" t="n"/>
-      <c r="D82" s="70" t="n"/>
+      <c r="B82" s="69" t="n"/>
+      <c r="C82" s="69" t="n"/>
+      <c r="D82" s="69" t="n"/>
       <c r="E82" s="50" t="n"/>
       <c r="F82" s="50" t="n"/>
       <c r="G82" s="50" t="n"/>
@@ -4933,7 +4947,7 @@
     </row>
     <row r="83" ht="27" customHeight="1">
       <c r="A83" s="2" t="n"/>
-      <c r="B83" s="105" t="n"/>
+      <c r="B83" s="104" t="n"/>
       <c r="C83" s="2" t="n"/>
       <c r="D83" s="2" t="n"/>
       <c r="E83" s="52" t="n"/>

</xml_diff>

<commit_message>
after refactoring and reoviing the style lecacy
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -2169,7 +2169,7 @@
         </is>
       </c>
       <c r="C29" s="56" t="n">
-        <v>7822</v>
+        <v>0</v>
       </c>
       <c r="D29" s="55" t="n"/>
       <c r="E29" s="56" t="n"/>
@@ -2184,7 +2184,7 @@
         </is>
       </c>
       <c r="C30" s="56" t="n">
-        <v>8407</v>
+        <v>0</v>
       </c>
       <c r="D30" s="55" t="n"/>
       <c r="E30" s="56" t="n"/>
@@ -2386,7 +2386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T72"/>
+  <dimension ref="A1:T71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4113,33 +4113,25 @@
       </c>
     </row>
     <row r="61" ht="27" customHeight="1">
-      <c r="A61" s="94" t="n"/>
-      <c r="B61" s="94" t="inlineStr">
-        <is>
-          <t>TOTAL OF BUFFALO LEATHER</t>
-        </is>
-      </c>
-      <c r="C61" s="94" t="n"/>
-      <c r="D61" s="94" t="inlineStr">
-        <is>
-          <t>26 PALLETS</t>
-        </is>
-      </c>
-      <c r="E61" s="95" t="n">
-        <v>6304</v>
-      </c>
-      <c r="F61" s="96" t="n">
-        <v>237879.6</v>
-      </c>
-      <c r="G61" s="96" t="n">
-        <v>15644</v>
-      </c>
-      <c r="H61" s="96" t="n">
-        <v>16814</v>
-      </c>
-      <c r="I61" s="97" t="n">
-        <v>59.47920000000001</v>
-      </c>
+      <c r="A61" s="2" t="n"/>
+      <c r="B61" s="2" t="n"/>
+      <c r="C61" s="2" t="n"/>
+      <c r="D61" s="2" t="n"/>
+      <c r="E61" s="2" t="n"/>
+      <c r="F61" s="2" t="n"/>
+      <c r="G61" s="2" t="n"/>
+      <c r="H61" s="2" t="n"/>
+      <c r="I61" s="2" t="n"/>
+      <c r="K61" s="2" t="n"/>
+      <c r="L61" s="2" t="n"/>
+      <c r="M61" s="2" t="n"/>
+      <c r="N61" s="2" t="n"/>
+      <c r="O61" s="2" t="n"/>
+      <c r="P61" s="2" t="n"/>
+      <c r="Q61" s="2" t="n"/>
+      <c r="R61" s="2" t="n"/>
+      <c r="S61" s="2" t="n"/>
+      <c r="T61" s="2" t="n"/>
     </row>
     <row r="62" ht="27" customHeight="1">
       <c r="A62" s="2" t="n"/>
@@ -4163,8 +4155,8 @@
       <c r="T62" s="2" t="n"/>
     </row>
     <row r="63" ht="27" customHeight="1">
-      <c r="A63" s="2" t="n"/>
-      <c r="B63" s="2" t="n"/>
+      <c r="A63" s="53" t="n"/>
+      <c r="B63" s="85" t="n"/>
       <c r="C63" s="2" t="n"/>
       <c r="D63" s="2" t="n"/>
       <c r="E63" s="2" t="n"/>
@@ -4184,14 +4176,18 @@
       <c r="T63" s="2" t="n"/>
     </row>
     <row r="64" ht="27" customHeight="1">
-      <c r="A64" s="53" t="n"/>
-      <c r="B64" s="85" t="n"/>
-      <c r="C64" s="2" t="n"/>
-      <c r="D64" s="2" t="n"/>
-      <c r="E64" s="2" t="n"/>
-      <c r="F64" s="2" t="n"/>
-      <c r="G64" s="2" t="n"/>
-      <c r="H64" s="2" t="n"/>
+      <c r="A64" s="98" t="inlineStr">
+        <is>
+          <t>Country of Original Cambodia</t>
+        </is>
+      </c>
+      <c r="B64" s="98" t="n"/>
+      <c r="C64" s="98" t="n"/>
+      <c r="D64" s="41" t="n"/>
+      <c r="E64" s="99" t="n"/>
+      <c r="F64" s="26" t="n"/>
+      <c r="G64" s="26" t="n"/>
+      <c r="H64" s="26" t="n"/>
       <c r="I64" s="2" t="n"/>
       <c r="K64" s="2" t="n"/>
       <c r="L64" s="2" t="n"/>
@@ -4204,18 +4200,21 @@
       <c r="S64" s="2" t="n"/>
       <c r="T64" s="2" t="n"/>
     </row>
-    <row r="65" ht="27" customHeight="1">
-      <c r="A65" s="98" t="inlineStr">
-        <is>
-          <t>Country of Original Cambodia</t>
-        </is>
-      </c>
-      <c r="B65" s="98" t="n"/>
-      <c r="C65" s="98" t="n"/>
-      <c r="D65" s="41" t="n"/>
-      <c r="E65" s="99" t="n"/>
-      <c r="F65" s="26" t="n"/>
-      <c r="G65" s="26" t="n"/>
+    <row r="65" ht="65.25" customHeight="1">
+      <c r="A65" s="61" t="inlineStr">
+        <is>
+          <t>Manufacture:</t>
+        </is>
+      </c>
+      <c r="B65" s="100" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
+XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="E65" s="101" t="n"/>
+      <c r="F65" s="101" t="n"/>
+      <c r="G65" s="101" t="n"/>
       <c r="H65" s="26" t="n"/>
       <c r="I65" s="2" t="n"/>
       <c r="K65" s="2" t="n"/>
@@ -4229,22 +4228,17 @@
       <c r="S65" s="2" t="n"/>
       <c r="T65" s="2" t="n"/>
     </row>
-    <row r="66" ht="65.25" customHeight="1">
-      <c r="A66" s="61" t="inlineStr">
-        <is>
-          <t>Manufacture:</t>
-        </is>
-      </c>
-      <c r="B66" s="100" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
-XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
+    <row r="66" ht="51.75" customHeight="1">
+      <c r="A66" s="100" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
+                                          /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
       <c r="E66" s="101" t="n"/>
       <c r="F66" s="101" t="n"/>
       <c r="G66" s="101" t="n"/>
-      <c r="H66" s="26" t="n"/>
+      <c r="H66" s="101" t="n"/>
       <c r="I66" s="2" t="n"/>
       <c r="K66" s="2" t="n"/>
       <c r="L66" s="2" t="n"/>
@@ -4257,17 +4251,19 @@
       <c r="S66" s="2" t="n"/>
       <c r="T66" s="2" t="n"/>
     </row>
-    <row r="67" ht="51.75" customHeight="1">
-      <c r="A67" s="100" t="inlineStr">
-        <is>
-          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
-                                          /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-      <c r="E67" s="101" t="n"/>
-      <c r="F67" s="101" t="n"/>
-      <c r="G67" s="101" t="n"/>
-      <c r="H67" s="101" t="n"/>
+    <row r="67" ht="27" customHeight="1">
+      <c r="A67" s="67" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+      <c r="B67" s="67" t="n"/>
+      <c r="C67" s="67" t="n"/>
+      <c r="D67" s="67" t="n"/>
+      <c r="E67" s="50" t="n"/>
+      <c r="F67" s="50" t="n"/>
+      <c r="G67" s="50" t="n"/>
+      <c r="H67" s="50" t="n"/>
       <c r="I67" s="2" t="n"/>
       <c r="K67" s="2" t="n"/>
       <c r="L67" s="2" t="n"/>
@@ -4283,7 +4279,7 @@
     <row r="68" ht="27" customHeight="1">
       <c r="A68" s="67" t="inlineStr">
         <is>
-          <t>A/C NO:100001100764430</t>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
       </c>
       <c r="B68" s="67" t="n"/>
@@ -4306,18 +4302,18 @@
       <c r="T68" s="2" t="n"/>
     </row>
     <row r="69" ht="27" customHeight="1">
-      <c r="A69" s="67" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
-        </is>
-      </c>
-      <c r="B69" s="67" t="n"/>
-      <c r="C69" s="67" t="n"/>
-      <c r="D69" s="67" t="n"/>
-      <c r="E69" s="50" t="n"/>
-      <c r="F69" s="50" t="n"/>
-      <c r="G69" s="50" t="n"/>
-      <c r="H69" s="50" t="n"/>
+      <c r="A69" s="2" t="n"/>
+      <c r="B69" s="102" t="n"/>
+      <c r="C69" s="2" t="n"/>
+      <c r="D69" s="2" t="n"/>
+      <c r="E69" s="52" t="n"/>
+      <c r="F69" s="2" t="n"/>
+      <c r="G69" s="2" t="n"/>
+      <c r="H69" s="26" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
       <c r="I69" s="2" t="n"/>
       <c r="K69" s="2" t="n"/>
       <c r="L69" s="2" t="n"/>
@@ -4332,17 +4328,13 @@
     </row>
     <row r="70" ht="27" customHeight="1">
       <c r="A70" s="2" t="n"/>
-      <c r="B70" s="102" t="n"/>
+      <c r="B70" s="2" t="n"/>
       <c r="C70" s="2" t="n"/>
       <c r="D70" s="2" t="n"/>
-      <c r="E70" s="52" t="n"/>
+      <c r="E70" s="2" t="n"/>
       <c r="F70" s="2" t="n"/>
       <c r="G70" s="2" t="n"/>
-      <c r="H70" s="26" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
+      <c r="H70" s="2" t="n"/>
       <c r="I70" s="2" t="n"/>
       <c r="K70" s="2" t="n"/>
       <c r="L70" s="2" t="n"/>
@@ -4356,16 +4348,56 @@
       <c r="T70" s="2" t="n"/>
     </row>
     <row r="71" ht="27" customHeight="1">
-      <c r="A71" s="2" t="n"/>
-      <c r="B71" s="2" t="n"/>
-      <c r="C71" s="2" t="n"/>
-      <c r="D71" s="2" t="n"/>
-      <c r="E71" s="2" t="n"/>
-      <c r="F71" s="2" t="n"/>
-      <c r="G71" s="2" t="n"/>
-      <c r="H71" s="2" t="n"/>
-      <c r="I71" s="2" t="n"/>
-      <c r="K71" s="2" t="n"/>
+      <c r="A71" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B71" s="2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E71" s="52" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F71" s="52" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G71" s="52" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="H71" s="52" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="I71" s="52" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="K71" s="52" t="inlineStr">
+        <is>
+          <t>J</t>
+        </is>
+      </c>
       <c r="L71" s="2" t="n"/>
       <c r="M71" s="2" t="n"/>
       <c r="N71" s="2" t="n"/>
@@ -4376,67 +4408,6 @@
       <c r="S71" s="2" t="n"/>
       <c r="T71" s="2" t="n"/>
     </row>
-    <row r="72" ht="27" customHeight="1">
-      <c r="A72" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B72" s="2" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C72" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D72" s="2" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="E72" s="52" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="F72" s="52" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="G72" s="52" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="H72" s="52" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="I72" s="52" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="K72" s="52" t="inlineStr">
-        <is>
-          <t>J</t>
-        </is>
-      </c>
-      <c r="L72" s="2" t="n"/>
-      <c r="M72" s="2" t="n"/>
-      <c r="N72" s="2" t="n"/>
-      <c r="O72" s="2" t="n"/>
-      <c r="P72" s="2" t="n"/>
-      <c r="Q72" s="2" t="n"/>
-      <c r="R72" s="2" t="n"/>
-      <c r="S72" s="2" t="n"/>
-      <c r="T72" s="2" t="n"/>
-    </row>
   </sheetData>
   <mergeCells count="29">
     <mergeCell ref="D21:D22"/>
@@ -4446,13 +4417,13 @@
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="I41:I42"/>
     <mergeCell ref="B58:C58"/>
-    <mergeCell ref="A67:D67"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B65:D65"/>
     <mergeCell ref="B59"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A21:A22"/>
@@ -4460,7 +4431,7 @@
     <mergeCell ref="B39"/>
     <mergeCell ref="G41:G42"/>
     <mergeCell ref="B60"/>
-    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="A66:D66"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="G21:G22"/>

</xml_diff>

<commit_message>
refactor: change the code do calculation into of footer and data builder into the new files call calculation, and the resolver will now handle the distribution via context
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -2169,7 +2169,7 @@
         </is>
       </c>
       <c r="C29" s="56" t="n">
-        <v>0</v>
+        <v>7822</v>
       </c>
       <c r="D29" s="55" t="n"/>
       <c r="E29" s="56" t="n"/>
@@ -2184,7 +2184,7 @@
         </is>
       </c>
       <c r="C30" s="56" t="n">
-        <v>0</v>
+        <v>8407</v>
       </c>
       <c r="D30" s="55" t="n"/>
       <c r="E30" s="56" t="n"/>

</xml_diff>

<commit_message>
fix global caluclation not pass into the footer
</commit_message>
<xml_diff>
--- a/result_test2.xlsx
+++ b/result_test2.xlsx
@@ -2169,7 +2169,7 @@
         </is>
       </c>
       <c r="C29" s="56" t="n">
-        <v>0</v>
+        <v>7822</v>
       </c>
       <c r="D29" s="55" t="n"/>
       <c r="E29" s="56" t="n"/>
@@ -2184,7 +2184,7 @@
         </is>
       </c>
       <c r="C30" s="56" t="n">
-        <v>0</v>
+        <v>8407</v>
       </c>
       <c r="D30" s="55" t="n"/>
       <c r="E30" s="56" t="n"/>

</xml_diff>